<commit_message>
Premiere préparation du site local
</commit_message>
<xml_diff>
--- a/excel/Itineraires.xlsx
+++ b/excel/Itineraires.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brunogauthier/Documents/guide2024/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A06D2B46-4363-E644-8DDB-FDE57763EAE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDEF4594-ABD7-0D47-92F3-895E883EEEA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9240" yWindow="3100" windowWidth="59240" windowHeight="22740" tabRatio="758" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="40880" yWindow="3140" windowWidth="59240" windowHeight="22740" tabRatio="758" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="23" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="914" uniqueCount="419">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="917" uniqueCount="420">
   <si>
     <t>GPM</t>
   </si>
@@ -1319,15 +1319,17 @@
   <si>
     <t>Stage 7 - Senneterre</t>
   </si>
+  <si>
+    <t>Entrée sur le circuit d'arrivée &lt;br/&gt;14e Avenue E</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
-    <numFmt numFmtId="170" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
   <fonts count="32" x14ac:knownFonts="1">
     <font>
@@ -1793,7 +1795,7 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="170" fontId="24" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="24" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
@@ -20518,7 +20520,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31D78861-6A86-448A-A85A-2A1E287D1373}">
   <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
@@ -20823,7 +20825,7 @@
   <dimension ref="A1:AM14"/>
   <sheetViews>
     <sheetView topLeftCell="C1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="K16" sqref="K16"/>
+      <selection activeCell="N1" sqref="N1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -20906,7 +20908,7 @@
       <c r="M1" t="s">
         <v>90</v>
       </c>
-      <c r="N1" t="s">
+      <c r="N1" s="16" t="s">
         <v>110</v>
       </c>
       <c r="O1" t="s">
@@ -21897,8 +21899,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{371307C5-CDC8-4A0E-8E08-E5295E5C8E14}">
   <dimension ref="A1:D46"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18:D18"/>
+    <sheetView topLeftCell="A10" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23:D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
@@ -22563,10 +22565,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:K38"/>
+  <dimension ref="A1:K39"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView topLeftCell="A8" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="A33" sqref="A33:D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
@@ -23107,99 +23109,115 @@
         <v>129.5</v>
       </c>
       <c r="B33" s="37" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C33" s="37" t="s">
-        <v>338</v>
-      </c>
-      <c r="D33" s="37" t="str">
-        <f>C33</f>
-        <v>2e Avenue O</v>
+        <v>419</v>
+      </c>
+      <c r="D33" s="37" t="s">
+        <v>372</v>
       </c>
       <c r="F33" s="21"/>
       <c r="K33" s="35"/>
     </row>
     <row r="34" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A34" s="36">
-        <v>129.69999999999999</v>
+        <v>129.6</v>
       </c>
       <c r="B34" s="37" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C34" s="37" t="s">
-        <v>221</v>
+        <v>338</v>
       </c>
       <c r="D34" s="37" t="str">
         <f>C34</f>
-        <v>1re Rue O</v>
+        <v>2e Avenue O</v>
       </c>
       <c r="F34" s="21"/>
       <c r="K34" s="35"/>
     </row>
-    <row r="35" spans="1:11" ht="26" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A35" s="36">
-        <v>129.80000000000001</v>
+        <v>129.69999999999999</v>
       </c>
       <c r="B35" s="37" t="s">
-        <v>113</v>
-      </c>
-      <c r="C35" s="4" t="s">
-        <v>343</v>
-      </c>
-      <c r="D35" s="17" t="s">
-        <v>340</v>
+        <v>74</v>
+      </c>
+      <c r="C35" s="37" t="s">
+        <v>221</v>
+      </c>
+      <c r="D35" s="37" t="str">
+        <f>C35</f>
+        <v>1re Rue O</v>
       </c>
       <c r="F35" s="21"/>
       <c r="K35" s="35"/>
     </row>
-    <row r="36" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:11" ht="26" x14ac:dyDescent="0.2">
       <c r="A36" s="36">
-        <v>130.1</v>
+        <v>129.80000000000001</v>
       </c>
       <c r="B36" s="37" t="s">
-        <v>73</v>
-      </c>
-      <c r="C36" s="37" t="s">
-        <v>341</v>
-      </c>
-      <c r="D36" s="37" t="str">
-        <f>C36</f>
-        <v>5e Avenue O</v>
+        <v>113</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>343</v>
+      </c>
+      <c r="D36" s="17" t="s">
+        <v>340</v>
       </c>
       <c r="F36" s="21"/>
       <c r="K36" s="35"/>
     </row>
     <row r="37" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A37" s="36">
-        <v>130.30000000000001</v>
+        <v>130.1</v>
       </c>
       <c r="B37" s="37" t="s">
         <v>73</v>
       </c>
       <c r="C37" s="37" t="s">
-        <v>223</v>
+        <v>341</v>
       </c>
       <c r="D37" s="37" t="str">
         <f>C37</f>
-        <v>Rue Principale N</v>
+        <v>5e Avenue O</v>
       </c>
       <c r="F37" s="21"/>
       <c r="K37" s="35"/>
     </row>
-    <row r="38" spans="1:11" ht="13" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A38" s="36">
+        <v>130.30000000000001</v>
+      </c>
+      <c r="B38" s="37" t="s">
+        <v>73</v>
+      </c>
+      <c r="C38" s="37" t="s">
+        <v>223</v>
+      </c>
+      <c r="D38" s="37" t="str">
+        <f>C38</f>
+        <v>Rue Principale N</v>
+      </c>
+      <c r="F38" s="21"/>
+      <c r="K38" s="35"/>
+    </row>
+    <row r="39" spans="1:11" ht="13" x14ac:dyDescent="0.15">
+      <c r="A39" s="36">
         <v>130.6</v>
       </c>
-      <c r="B38" s="37" t="s">
+      <c r="B39" s="37" t="s">
         <v>44</v>
       </c>
-      <c r="C38" s="38" t="s">
+      <c r="C39" s="38" t="s">
         <v>111</v>
       </c>
-      <c r="D38" s="39" t="s">
+      <c r="D39" s="39" t="s">
         <v>200</v>
       </c>
-      <c r="F38" s="21"/>
+      <c r="F39" s="21"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -24344,8 +24362,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E156DDD-44B2-497E-B657-8831DB081CFE}">
   <dimension ref="A1:F42"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7:XFD7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="11" x14ac:dyDescent="0.15"/>

</xml_diff>

<commit_message>
Récupération Étape 5 Senneterre 2023 avant annulation
Pour premier jet 2024, à valider plus tard.
</commit_message>
<xml_diff>
--- a/excel/Itineraires.xlsx
+++ b/excel/Itineraires.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brunogauthier/Documents/guide2024/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDEF4594-ABD7-0D47-92F3-895E883EEEA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D93BCCE4-3AA0-E54A-85CA-DA8F655B3B83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40880" yWindow="3140" windowWidth="59240" windowHeight="22740" tabRatio="758" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="68300" yWindow="560" windowWidth="34040" windowHeight="28180" tabRatio="758" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="23" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="917" uniqueCount="420">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="922" uniqueCount="404">
   <si>
     <t>GPM</t>
   </si>
@@ -494,22 +494,7 @@
     <t>Stage 3 - ITT</t>
   </si>
   <si>
-    <t>https://ridewithgps.com/routes/42268563</t>
-  </si>
-  <si>
-    <t>https://ridewithgps.com/routes/42268538</t>
-  </si>
-  <si>
     <t>https://ridewithgps.com/routes/42268527</t>
-  </si>
-  <si>
-    <t>https://ridewithgps.com/routes/42268509</t>
-  </si>
-  <si>
-    <t>https://ridewithgps.com/routes/42183412</t>
-  </si>
-  <si>
-    <t>https://ridewithgps.com/routes/42099075</t>
   </si>
   <si>
     <t>Boulevard du Collège</t>
@@ -1197,45 +1182,9 @@
     <t>Zone déchêts (sur 200m)</t>
   </si>
   <si>
-    <t>Sprint de la Mairesse de Senneterre $250&lt;br/&gt;Église de Ste-Gertrude</t>
-  </si>
-  <si>
-    <t>Senneterre Mayor's sprint $250&lt;br/&gt;Ste-Gertrude church</t>
-  </si>
-  <si>
     <t>Preissac Mayor's sprint $250&lt;br/&gt;Gas Station Preissac</t>
   </si>
   <si>
-    <t>Points GPM&lt;br/&gt; Sommet Preissac</t>
-  </si>
-  <si>
-    <t>KOM Points&lt;br/&gt;Preissac Summit</t>
-  </si>
-  <si>
-    <t>Sprint bonification temps et points&lt;br/&gt;Intersection chemin St-Luc</t>
-  </si>
-  <si>
-    <t>Bonification Sprint - times and points&lt;br/&gt;Intersection chemin St-Luc</t>
-  </si>
-  <si>
-    <t>Senneterre Mayor's sprint $250&lt;br/&gt;Shell gas station</t>
-  </si>
-  <si>
-    <t>Sprint de la Mairesse de Senneterre $250&lt;br/&gt;Station-service Shell</t>
-  </si>
-  <si>
-    <t>Rue des Quatre-Coins</t>
-  </si>
-  <si>
-    <t>https://ridewithgps.com/routes/43489600</t>
-  </si>
-  <si>
-    <t>Zone déchets (après le pont, sur 200 m)</t>
-  </si>
-  <si>
-    <t>Trash zone (after the bridge, on 200 m)</t>
-  </si>
-  <si>
     <t>Pont de bois</t>
   </si>
   <si>
@@ -1251,9 +1200,6 @@
     <t>Amos - Val-d'Or</t>
   </si>
   <si>
-    <t>Senneterre - Senneterre</t>
-  </si>
-  <si>
     <t xml:space="preserve">Val-d'Or - Val-d'Or </t>
   </si>
   <si>
@@ -1321,6 +1267,12 @@
   </si>
   <si>
     <t>Entrée sur le circuit d'arrivée &lt;br/&gt;14e Avenue E</t>
+  </si>
+  <si>
+    <t>Senneterre - VD - Senneterre</t>
+  </si>
+  <si>
+    <t>https://ridewithgps.com/routes/42268449</t>
   </si>
 </sst>
 </file>
@@ -2588,10 +2540,10 @@
         <v>64</v>
       </c>
       <c r="C2" s="50" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="D2" s="51" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="F2" s="21"/>
     </row>
@@ -2603,10 +2555,10 @@
         <v>74</v>
       </c>
       <c r="C3" s="54" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="D3" s="54" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="F3" s="21"/>
     </row>
@@ -2618,7 +2570,7 @@
         <v>73</v>
       </c>
       <c r="C4" s="54" t="s">
-        <v>354</v>
+        <v>349</v>
       </c>
       <c r="D4" s="35" t="str">
         <f>C4</f>
@@ -2633,7 +2585,7 @@
         <v>73</v>
       </c>
       <c r="C5" s="54" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="D5" s="35" t="str">
         <f>C5</f>
@@ -2648,10 +2600,10 @@
         <v>74</v>
       </c>
       <c r="C6" s="54" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="D6" s="35" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -2690,10 +2642,10 @@
         <v>72</v>
       </c>
       <c r="C9" s="54" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="D9" s="54" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
@@ -2704,7 +2656,7 @@
         <v>5</v>
       </c>
       <c r="C10" s="54" t="s">
-        <v>358</v>
+        <v>353</v>
       </c>
       <c r="D10" s="54" t="str">
         <f>C10</f>
@@ -2719,10 +2671,10 @@
         <v>82</v>
       </c>
       <c r="C11" s="53" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="D11" s="53" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
@@ -2733,10 +2685,10 @@
         <v>25</v>
       </c>
       <c r="C12" s="54" t="s">
-        <v>359</v>
+        <v>354</v>
       </c>
       <c r="D12" s="35" t="s">
-        <v>360</v>
+        <v>355</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
@@ -2747,10 +2699,10 @@
         <v>25</v>
       </c>
       <c r="C13" s="54" t="s">
-        <v>361</v>
+        <v>356</v>
       </c>
       <c r="D13" s="35" t="s">
-        <v>362</v>
+        <v>357</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
@@ -2761,7 +2713,7 @@
         <v>5</v>
       </c>
       <c r="C14" s="54" t="s">
-        <v>357</v>
+        <v>352</v>
       </c>
       <c r="D14" s="35" t="str">
         <f>C14</f>
@@ -2790,10 +2742,10 @@
         <v>79</v>
       </c>
       <c r="C16" s="54" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="D16" s="35" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
@@ -2804,10 +2756,10 @@
         <v>25</v>
       </c>
       <c r="C17" s="54" t="s">
+        <v>182</v>
+      </c>
+      <c r="D17" s="35" t="s">
         <v>187</v>
-      </c>
-      <c r="D17" s="35" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
@@ -2832,7 +2784,7 @@
         <v>5</v>
       </c>
       <c r="C19" s="54" t="s">
-        <v>334</v>
+        <v>329</v>
       </c>
       <c r="D19" s="35" t="str">
         <f>C19</f>
@@ -2847,10 +2799,10 @@
         <v>71</v>
       </c>
       <c r="C20" s="53" t="s">
-        <v>355</v>
+        <v>350</v>
       </c>
       <c r="D20" s="53" t="s">
-        <v>356</v>
+        <v>351</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
@@ -2858,13 +2810,13 @@
         <v>49.2</v>
       </c>
       <c r="B21" s="55" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="C21" s="54" t="s">
-        <v>377</v>
+        <v>372</v>
       </c>
       <c r="D21" s="54" t="s">
-        <v>374</v>
+        <v>369</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
@@ -2903,7 +2855,7 @@
         <v>5</v>
       </c>
       <c r="C24" s="54" t="s">
-        <v>336</v>
+        <v>331</v>
       </c>
       <c r="D24" s="35" t="str">
         <f>C24</f>
@@ -2918,10 +2870,10 @@
         <v>82</v>
       </c>
       <c r="C25" s="53" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="D25" s="53" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
@@ -2932,10 +2884,10 @@
         <v>25</v>
       </c>
       <c r="C26" s="54" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="D26" s="35" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
@@ -2946,7 +2898,7 @@
         <v>5</v>
       </c>
       <c r="C27" s="54" t="s">
-        <v>337</v>
+        <v>332</v>
       </c>
       <c r="D27" s="35" t="str">
         <f>C27</f>
@@ -2964,7 +2916,7 @@
         <v>112</v>
       </c>
       <c r="D28" s="75" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
@@ -2990,10 +2942,10 @@
         <v>74</v>
       </c>
       <c r="C30" s="54" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="D30" s="35" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
@@ -3004,7 +2956,7 @@
         <v>73</v>
       </c>
       <c r="C31" s="54" t="s">
-        <v>338</v>
+        <v>333</v>
       </c>
       <c r="D31" s="35" t="str">
         <f t="shared" ref="D31:D47" si="0">C31</f>
@@ -3019,7 +2971,7 @@
         <v>74</v>
       </c>
       <c r="C32" s="54" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="D32" s="35" t="str">
         <f t="shared" si="0"/>
@@ -3034,7 +2986,7 @@
         <v>73</v>
       </c>
       <c r="C33" s="54" t="s">
-        <v>341</v>
+        <v>336</v>
       </c>
       <c r="D33" s="35" t="str">
         <f t="shared" si="0"/>
@@ -3049,7 +3001,7 @@
         <v>73</v>
       </c>
       <c r="C34" s="54" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="D34" s="35" t="str">
         <f t="shared" si="0"/>
@@ -3064,10 +3016,10 @@
         <v>82</v>
       </c>
       <c r="C35" s="53" t="s">
-        <v>303</v>
+        <v>298</v>
       </c>
       <c r="D35" s="60" t="s">
-        <v>307</v>
+        <v>302</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
@@ -3078,7 +3030,7 @@
         <v>74</v>
       </c>
       <c r="C36" s="54" t="s">
-        <v>363</v>
+        <v>358</v>
       </c>
       <c r="D36" s="35" t="str">
         <f>C36</f>
@@ -3093,7 +3045,7 @@
         <v>74</v>
       </c>
       <c r="C37" s="54" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="D37" s="35" t="str">
         <f t="shared" si="0"/>
@@ -3108,7 +3060,7 @@
         <v>73</v>
       </c>
       <c r="C38" s="54" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="D38" s="35" t="str">
         <f t="shared" si="0"/>
@@ -3123,7 +3075,7 @@
         <v>73</v>
       </c>
       <c r="C39" s="54" t="s">
-        <v>364</v>
+        <v>359</v>
       </c>
       <c r="D39" s="35" t="str">
         <f t="shared" si="0"/>
@@ -3138,7 +3090,7 @@
         <v>73</v>
       </c>
       <c r="C40" s="54" t="s">
-        <v>315</v>
+        <v>310</v>
       </c>
       <c r="D40" s="35" t="str">
         <f t="shared" si="0"/>
@@ -3153,7 +3105,7 @@
         <v>73</v>
       </c>
       <c r="C41" s="54" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="D41" s="35" t="str">
         <f t="shared" si="0"/>
@@ -3168,7 +3120,7 @@
         <v>74</v>
       </c>
       <c r="C42" s="54" t="s">
-        <v>365</v>
+        <v>360</v>
       </c>
       <c r="D42" s="35" t="str">
         <f t="shared" si="0"/>
@@ -3183,7 +3135,7 @@
         <v>73</v>
       </c>
       <c r="C43" s="54" t="s">
-        <v>338</v>
+        <v>333</v>
       </c>
       <c r="D43" s="35" t="str">
         <f t="shared" si="0"/>
@@ -3198,10 +3150,10 @@
         <v>79</v>
       </c>
       <c r="C44" s="54" t="s">
-        <v>375</v>
+        <v>370</v>
       </c>
       <c r="D44" s="35" t="s">
-        <v>376</v>
+        <v>371</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
@@ -3212,7 +3164,7 @@
         <v>74</v>
       </c>
       <c r="C45" s="54" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="D45" s="35" t="str">
         <f t="shared" si="0"/>
@@ -3227,7 +3179,7 @@
         <v>73</v>
       </c>
       <c r="C46" s="54" t="s">
-        <v>341</v>
+        <v>336</v>
       </c>
       <c r="D46" s="35" t="str">
         <f t="shared" si="0"/>
@@ -3242,7 +3194,7 @@
         <v>73</v>
       </c>
       <c r="C47" s="54" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="D47" s="35" t="str">
         <f t="shared" si="0"/>
@@ -3258,10 +3210,10 @@
         <v>82</v>
       </c>
       <c r="C48" s="53" t="s">
-        <v>302</v>
+        <v>297</v>
       </c>
       <c r="D48" s="60" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
     </row>
     <row r="49" spans="1:16384" x14ac:dyDescent="0.2">
@@ -3272,10 +3224,10 @@
         <v>79</v>
       </c>
       <c r="C49" s="54" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="D49" s="35" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
     </row>
     <row r="50" spans="1:16384" x14ac:dyDescent="0.2">
@@ -3287,10 +3239,10 @@
         <v>82</v>
       </c>
       <c r="C50" s="53" t="s">
+        <v>299</v>
+      </c>
+      <c r="D50" s="60" t="s">
         <v>304</v>
-      </c>
-      <c r="D50" s="60" t="s">
-        <v>309</v>
       </c>
     </row>
     <row r="51" spans="1:16384" x14ac:dyDescent="0.2">
@@ -3302,10 +3254,10 @@
         <v>82</v>
       </c>
       <c r="C51" s="53" t="s">
+        <v>300</v>
+      </c>
+      <c r="D51" s="60" t="s">
         <v>305</v>
-      </c>
-      <c r="D51" s="60" t="s">
-        <v>310</v>
       </c>
     </row>
     <row r="52" spans="1:16384" x14ac:dyDescent="0.2">
@@ -3317,10 +3269,10 @@
         <v>82</v>
       </c>
       <c r="C52" s="53" t="s">
+        <v>301</v>
+      </c>
+      <c r="D52" s="60" t="s">
         <v>306</v>
-      </c>
-      <c r="D52" s="60" t="s">
-        <v>311</v>
       </c>
     </row>
     <row r="53" spans="1:16384" x14ac:dyDescent="0.2">
@@ -3331,10 +3283,10 @@
         <v>113</v>
       </c>
       <c r="C53" s="54" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="D53" s="35" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="E53" s="57"/>
       <c r="F53" s="55"/>
@@ -19729,7 +19681,7 @@
         <v>111</v>
       </c>
       <c r="D54" s="60" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
     </row>
     <row r="55" spans="1:16384" x14ac:dyDescent="0.2">
@@ -20028,10 +19980,10 @@
         <v>64</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -20042,10 +19994,10 @@
         <v>77</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>318</v>
+        <v>313</v>
       </c>
       <c r="D3" s="15" t="s">
-        <v>319</v>
+        <v>314</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -20059,7 +20011,7 @@
         <v>10</v>
       </c>
       <c r="D4" s="15" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -20070,10 +20022,10 @@
         <v>5</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="D5" s="18" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="26" x14ac:dyDescent="0.15">
@@ -20084,10 +20036,10 @@
         <v>71</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
       <c r="D6" s="19" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -20098,7 +20050,7 @@
         <v>74</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>320</v>
+        <v>315</v>
       </c>
       <c r="D7" s="15" t="str">
         <f>C7</f>
@@ -20113,10 +20065,10 @@
         <v>79</v>
       </c>
       <c r="C8" s="37" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="D8" s="37" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -20127,10 +20079,10 @@
         <v>72</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
       <c r="D9" s="19" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -20141,10 +20093,10 @@
         <v>5</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="D10" s="15" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="26" x14ac:dyDescent="0.15">
@@ -20155,10 +20107,10 @@
         <v>82</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="D11" s="17" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="26" x14ac:dyDescent="0.15">
@@ -20169,10 +20121,10 @@
         <v>71</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>321</v>
+        <v>316</v>
       </c>
       <c r="D12" s="19" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -20180,13 +20132,13 @@
         <v>71</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="D13" s="18" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -20197,10 +20149,10 @@
         <v>83</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
       <c r="D14" s="15" t="s">
-        <v>347</v>
+        <v>342</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -20214,7 +20166,7 @@
         <v>22</v>
       </c>
       <c r="D15" s="15" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -20228,7 +20180,7 @@
         <v>22</v>
       </c>
       <c r="D16" s="15" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -20239,10 +20191,10 @@
         <v>83</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
       <c r="D17" s="15" t="s">
-        <v>347</v>
+        <v>342</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -20253,10 +20205,10 @@
         <v>72</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
       <c r="D18" s="17" t="s">
-        <v>279</v>
+        <v>274</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -20267,7 +20219,7 @@
         <v>74</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>322</v>
+        <v>317</v>
       </c>
       <c r="D19" s="15" t="str">
         <f>C19</f>
@@ -20282,10 +20234,10 @@
         <v>5</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>267</v>
+        <v>262</v>
       </c>
       <c r="D20" s="15" t="s">
-        <v>267</v>
+        <v>262</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="26" x14ac:dyDescent="0.15">
@@ -20296,10 +20248,10 @@
         <v>82</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="D21" s="17" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -20310,10 +20262,10 @@
         <v>79</v>
       </c>
       <c r="C22" s="54" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="D22" s="35" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -20338,10 +20290,10 @@
         <v>75</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>348</v>
+        <v>343</v>
       </c>
       <c r="D24" s="15" t="s">
-        <v>349</v>
+        <v>344</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -20352,7 +20304,7 @@
         <v>73</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>323</v>
+        <v>318</v>
       </c>
       <c r="D25" s="15" t="str">
         <f>C25</f>
@@ -20367,10 +20319,10 @@
         <v>73</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
       <c r="D26" s="15" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -20381,10 +20333,10 @@
         <v>73</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="D27" s="15" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -20395,10 +20347,10 @@
         <v>73</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
       <c r="D28" s="15" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="26" x14ac:dyDescent="0.15">
@@ -20409,10 +20361,10 @@
         <v>113</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>324</v>
+        <v>319</v>
       </c>
       <c r="D29" s="15" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="26" x14ac:dyDescent="0.15">
@@ -20423,10 +20375,10 @@
         <v>76</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="D30" s="18" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="39" x14ac:dyDescent="0.15">
@@ -20437,10 +20389,10 @@
         <v>44</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>316</v>
+        <v>311</v>
       </c>
       <c r="D31" s="17" t="s">
-        <v>317</v>
+        <v>312</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="12" x14ac:dyDescent="0.15">
@@ -20564,7 +20516,7 @@
         <v>80</v>
       </c>
       <c r="B3" s="16" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="C3" s="16" t="s">
         <v>6</v>
@@ -20592,7 +20544,7 @@
         <v>44</v>
       </c>
       <c r="B5" s="16" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="C5" s="16" t="s">
         <v>7</v>
@@ -20634,7 +20586,7 @@
         <v>71</v>
       </c>
       <c r="B8" s="16" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="C8" s="16" t="s">
         <v>8</v>
@@ -20662,7 +20614,7 @@
         <v>82</v>
       </c>
       <c r="B10" s="16" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="C10" s="16" t="s">
         <v>9</v>
@@ -20774,7 +20726,7 @@
         <v>79</v>
       </c>
       <c r="B18" s="16" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="C18" t="s">
         <v>84</v>
@@ -20799,16 +20751,16 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A20" s="16" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="B20" s="16" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="C20" s="16" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="D20" s="16" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
   </sheetData>
@@ -20824,8 +20776,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF8C653E-9E00-4EDF-9978-201805372337}">
   <dimension ref="A1:AM14"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="N1" sqref="N1"/>
+    <sheetView tabSelected="1" topLeftCell="N1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="T19" sqref="T19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -21004,7 +20956,7 @@
         <v>86</v>
       </c>
       <c r="F2" s="16" t="s">
-        <v>394</v>
+        <v>377</v>
       </c>
       <c r="G2" s="61" t="str">
         <f>CONCATENATE(Tableau2[[#This Row],[Distance_Route]], " km + (",Tableau2[[#This Row],[Nb_tours]]," x ",Tableau2[[#This Row],[KM_par_tours]]," km) = ",Tableau2[[#This Row],[Distance_totale]]," km")</f>
@@ -21050,9 +21002,7 @@
         <f>IF(R2&gt;0,R2-2,"")</f>
         <v>42</v>
       </c>
-      <c r="T2" s="29" t="s">
-        <v>153</v>
-      </c>
+      <c r="T2" s="29"/>
       <c r="U2" t="str">
         <f>TEXT(_xlfn.CONCAT(Tableau2[[#This Row],[Heure_dep]],":",Tableau2[[#This Row],[min_dep]]), "HH:MM")</f>
         <v>16:45</v>
@@ -21083,32 +21033,32 @@
         <v>0.80965909090909083</v>
       </c>
       <c r="AC2" s="31" t="s">
-        <v>399</v>
+        <v>381</v>
       </c>
       <c r="AD2" s="31" t="s">
-        <v>400</v>
+        <v>382</v>
       </c>
       <c r="AE2" s="31" t="s">
-        <v>401</v>
+        <v>383</v>
       </c>
       <c r="AF2" s="31" t="s">
         <v>132</v>
       </c>
       <c r="AG2" s="31" t="s">
-        <v>405</v>
+        <v>387</v>
       </c>
       <c r="AH2" s="31" t="str">
         <f>Tableau2[[#This Row],[LieuDepFR]]</f>
         <v>CEGEP</v>
       </c>
       <c r="AI2" s="31" t="s">
-        <v>408</v>
+        <v>390</v>
       </c>
       <c r="AJ2" s="16" t="s">
-        <v>409</v>
+        <v>391</v>
       </c>
       <c r="AK2" s="16" t="s">
-        <v>414</v>
+        <v>396</v>
       </c>
       <c r="AL2" s="30"/>
       <c r="AM2" s="30"/>
@@ -21131,7 +21081,7 @@
         <v>86</v>
       </c>
       <c r="F3" s="16" t="s">
-        <v>395</v>
+        <v>378</v>
       </c>
       <c r="G3" s="61" t="str">
         <f>CONCATENATE(Tableau2[[#This Row],[Distance_Route]], " km + (",Tableau2[[#This Row],[Nb_tours]]," x ",Tableau2[[#This Row],[KM_par_tours]]," km) = ",Tableau2[[#This Row],[Distance_totale]]," km")</f>
@@ -21177,9 +21127,7 @@
         <f>IF(R3&gt;0,R3-2,"")</f>
         <v>42</v>
       </c>
-      <c r="T3" s="29" t="s">
-        <v>155</v>
-      </c>
+      <c r="T3" s="29"/>
       <c r="U3" t="str">
         <f>TEXT(_xlfn.CONCAT(Tableau2[[#This Row],[Heure_dep]],":",Tableau2[[#This Row],[min_dep]]), "HH:MM")</f>
         <v>17:00</v>
@@ -21213,7 +21161,7 @@
         <v>126</v>
       </c>
       <c r="AD3" s="31" t="s">
-        <v>400</v>
+        <v>382</v>
       </c>
       <c r="AE3" s="31" t="s">
         <v>138</v>
@@ -21222,20 +21170,20 @@
         <v>129</v>
       </c>
       <c r="AG3" s="31" t="s">
-        <v>405</v>
+        <v>387</v>
       </c>
       <c r="AH3" s="31" t="str">
         <f>Tableau2[[#This Row],[LieuDepFR]]</f>
         <v>Cathédrale</v>
       </c>
       <c r="AI3" s="31" t="s">
-        <v>408</v>
+        <v>390</v>
       </c>
       <c r="AJ3" s="16" t="s">
-        <v>410</v>
+        <v>392</v>
       </c>
       <c r="AK3" s="16" t="s">
-        <v>415</v>
+        <v>397</v>
       </c>
       <c r="AL3" s="30"/>
       <c r="AM3" s="30"/>
@@ -21258,7 +21206,7 @@
         <v>86</v>
       </c>
       <c r="F4" s="16" t="s">
-        <v>393</v>
+        <v>376</v>
       </c>
       <c r="G4" s="61" t="str">
         <f>CONCATENATE(Tableau2[[#This Row],[Distance_totale]]," km")</f>
@@ -21303,9 +21251,7 @@
       <c r="S4" s="24">
         <v>42</v>
       </c>
-      <c r="T4" s="29" t="s">
-        <v>150</v>
-      </c>
+      <c r="T4" s="29"/>
       <c r="U4" t="str">
         <f>TEXT(_xlfn.CONCAT(Tableau2[[#This Row],[Heure_dep]],":",Tableau2[[#This Row],[min_dep]]), "HH:MM")</f>
         <v>09:00</v>
@@ -21336,16 +21282,16 @@
         <v>0.38260869565217392</v>
       </c>
       <c r="AC4" s="31" t="s">
-        <v>400</v>
+        <v>382</v>
       </c>
       <c r="AD4" s="31" t="s">
-        <v>400</v>
+        <v>382</v>
       </c>
       <c r="AE4" s="31" t="s">
-        <v>402</v>
+        <v>384</v>
       </c>
       <c r="AF4" s="31" t="s">
-        <v>406</v>
+        <v>388</v>
       </c>
       <c r="AG4" s="31" t="str">
         <f>Tableau2[[#This Row],[LieuDepFR]]</f>
@@ -21439,7 +21385,7 @@
         <v>44</v>
       </c>
       <c r="T5" s="29" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="U5" t="str">
         <f>TEXT(_xlfn.CONCAT(Tableau2[[#This Row],[Heure_dep]],":",Tableau2[[#This Row],[min_dep]]), "HH:MM")</f>
@@ -21480,14 +21426,14 @@
         <v>143</v>
       </c>
       <c r="AF5" s="32" t="s">
-        <v>407</v>
+        <v>389</v>
       </c>
       <c r="AG5" s="31" t="str">
         <f>Tableau2[[#This Row],[LieuDepFR]]</f>
         <v>TBD</v>
       </c>
       <c r="AH5" s="31" t="s">
-        <v>407</v>
+        <v>389</v>
       </c>
       <c r="AI5" s="30" t="str">
         <f>Tableau2[[#This Row],[LieuDepEN]]</f>
@@ -21520,7 +21466,7 @@
         <v>86</v>
       </c>
       <c r="F6" s="16" t="s">
-        <v>396</v>
+        <v>402</v>
       </c>
       <c r="G6" s="61" t="str">
         <f>CONCATENATE(Tableau2[[#This Row],[Distance_totale]]," km")</f>
@@ -21557,17 +21503,17 @@
         <v>140</v>
       </c>
       <c r="Q6">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="R6">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="S6" s="24">
         <f t="shared" ref="S6" si="1">IF(R6&gt;0,R6-2,"")</f>
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="T6" s="29" t="s">
-        <v>388</v>
+        <v>403</v>
       </c>
       <c r="U6" t="str">
         <f>TEXT(_xlfn.CONCAT(Tableau2[[#This Row],[Heure_dep]],":",Tableau2[[#This Row],[min_dep]]), "HH:MM")</f>
@@ -21592,11 +21538,11 @@
       </c>
       <c r="AA6" s="30" t="str">
         <f>TEXT((Tableau2[[#This Row],[KM_Total]]-Tableau2[[#This Row],[Distance_en_circuit]])/Tableau2[[#This Row],[Vit_moy]]/24+Tableau2[[#This Row],[Depart]],"HH:MM")</f>
-        <v>17:17</v>
+        <v>17:22</v>
       </c>
       <c r="AB6" s="30">
         <f>Tableau2[[#This Row],[KM_Total]]/Tableau2[[#This Row],[Vit_moy]]/24+Tableau2[[#This Row],[Depart]]</f>
-        <v>0.72064393939393945</v>
+        <v>0.72383720930232565</v>
       </c>
       <c r="AC6" s="31" t="s">
         <v>134</v>
@@ -21605,25 +21551,25 @@
         <v>134</v>
       </c>
       <c r="AE6" s="31" t="s">
-        <v>403</v>
+        <v>385</v>
       </c>
       <c r="AF6" s="31" t="s">
-        <v>405</v>
+        <v>387</v>
       </c>
       <c r="AG6" s="31" t="s">
-        <v>405</v>
+        <v>387</v>
       </c>
       <c r="AH6" s="31" t="s">
-        <v>408</v>
+        <v>390</v>
       </c>
       <c r="AI6" s="31" t="s">
-        <v>408</v>
+        <v>390</v>
       </c>
       <c r="AJ6" s="16" t="s">
-        <v>411</v>
+        <v>393</v>
       </c>
       <c r="AK6" s="16" t="s">
-        <v>416</v>
+        <v>398</v>
       </c>
       <c r="AL6" s="30"/>
       <c r="AM6" s="30"/>
@@ -21646,7 +21592,7 @@
         <v>86</v>
       </c>
       <c r="F7" s="61" t="s">
-        <v>397</v>
+        <v>379</v>
       </c>
       <c r="G7" s="61" t="str">
         <f>CONCATENATE(Tableau2[[#This Row],[Nb_tours]], " x ",Tableau2[[#This Row],[KM_par_tours]], " km = ",Tableau2[[#This Row],[Distance_totale]]," km")</f>
@@ -21693,9 +21639,7 @@
         <f t="shared" ref="S7:S8" si="2">IF(R7&gt;0,R7-2,"")</f>
         <v>42</v>
       </c>
-      <c r="T7" s="29" t="s">
-        <v>151</v>
-      </c>
+      <c r="T7" s="29"/>
       <c r="U7" t="str">
         <f>TEXT(_xlfn.CONCAT(Tableau2[[#This Row],[Heure_dep]],":",Tableau2[[#This Row],[min_dep]]), "HH:MM")</f>
         <v>16:30</v>
@@ -21726,32 +21670,32 @@
         <v>0.80568181818181817</v>
       </c>
       <c r="AC7" s="31" t="s">
-        <v>400</v>
+        <v>382</v>
       </c>
       <c r="AD7" s="31" t="s">
-        <v>400</v>
+        <v>382</v>
       </c>
       <c r="AE7" s="31" t="s">
-        <v>402</v>
+        <v>384</v>
       </c>
       <c r="AF7" s="77" t="s">
-        <v>405</v>
+        <v>387</v>
       </c>
       <c r="AG7" s="31" t="str">
         <f>Tableau2[[#This Row],[LieuDepFR]]</f>
         <v>Hôtel de Ville</v>
       </c>
       <c r="AH7" s="31" t="s">
-        <v>408</v>
+        <v>390</v>
       </c>
       <c r="AI7" s="31" t="s">
-        <v>408</v>
+        <v>390</v>
       </c>
       <c r="AJ7" s="16" t="s">
-        <v>412</v>
+        <v>394</v>
       </c>
       <c r="AK7" s="16" t="s">
-        <v>417</v>
+        <v>399</v>
       </c>
       <c r="AL7" s="30"/>
       <c r="AM7" s="30"/>
@@ -21774,7 +21718,7 @@
         <v>86</v>
       </c>
       <c r="F8" s="16" t="s">
-        <v>398</v>
+        <v>380</v>
       </c>
       <c r="G8" s="61" t="str">
         <f>CONCATENATE(Tableau2[[#This Row],[Distance_Route]], " km + (",Tableau2[[#This Row],[Nb_tours]]," x ",Tableau2[[#This Row],[KM_par_tours]]," km) = ",Tableau2[[#This Row],[Distance_totale]]," km")</f>
@@ -21820,9 +21764,7 @@
         <f t="shared" si="2"/>
         <v>42</v>
       </c>
-      <c r="T8" s="29" t="s">
-        <v>154</v>
-      </c>
+      <c r="T8" s="29"/>
       <c r="U8" t="str">
         <f>TEXT(_xlfn.CONCAT(Tableau2[[#This Row],[Heure_dep]],":",Tableau2[[#This Row],[min_dep]]), "HH:MM")</f>
         <v>14:00</v>
@@ -21856,28 +21798,28 @@
         <v>134</v>
       </c>
       <c r="AD8" s="31" t="s">
+        <v>382</v>
+      </c>
+      <c r="AE8" s="31" t="s">
+        <v>386</v>
+      </c>
+      <c r="AF8" s="31" t="s">
+        <v>387</v>
+      </c>
+      <c r="AG8" s="31" t="s">
+        <v>387</v>
+      </c>
+      <c r="AH8" s="31" t="s">
+        <v>390</v>
+      </c>
+      <c r="AI8" s="31" t="s">
+        <v>390</v>
+      </c>
+      <c r="AJ8" s="16" t="s">
+        <v>395</v>
+      </c>
+      <c r="AK8" s="16" t="s">
         <v>400</v>
-      </c>
-      <c r="AE8" s="31" t="s">
-        <v>404</v>
-      </c>
-      <c r="AF8" s="31" t="s">
-        <v>405</v>
-      </c>
-      <c r="AG8" s="31" t="s">
-        <v>405</v>
-      </c>
-      <c r="AH8" s="31" t="s">
-        <v>408</v>
-      </c>
-      <c r="AI8" s="31" t="s">
-        <v>408</v>
-      </c>
-      <c r="AJ8" s="16" t="s">
-        <v>413</v>
-      </c>
-      <c r="AK8" s="16" t="s">
-        <v>418</v>
       </c>
       <c r="AL8" s="30"/>
       <c r="AM8" s="30"/>
@@ -21887,10 +21829,13 @@
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="T6" r:id="rId1" xr:uid="{4FDD5E38-AE51-BB40-AA8B-9E6AE8398E4F}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
@@ -21933,10 +21878,10 @@
         <v>64</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -21947,10 +21892,10 @@
         <v>74</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="D3" s="15" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -21961,10 +21906,10 @@
         <v>73</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="D4" s="15" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -21975,7 +21920,7 @@
         <v>25</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="D5" s="15" t="s">
         <v>21</v>
@@ -21989,10 +21934,10 @@
         <v>83</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>366</v>
+        <v>361</v>
       </c>
       <c r="D6" s="15" t="s">
-        <v>369</v>
+        <v>364</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -22017,7 +21962,7 @@
         <v>5</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="D8" s="15" t="str">
         <f>C8</f>
@@ -22032,10 +21977,10 @@
         <v>72</v>
       </c>
       <c r="C9" s="63" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="D9" s="63" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -22046,10 +21991,10 @@
         <v>79</v>
       </c>
       <c r="C10" s="34" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="D10" s="34" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -22060,7 +22005,7 @@
         <v>5</v>
       </c>
       <c r="C11" s="64" t="s">
-        <v>367</v>
+        <v>362</v>
       </c>
       <c r="D11" s="64" t="str">
         <f>C11</f>
@@ -22075,10 +22020,10 @@
         <v>71</v>
       </c>
       <c r="C12" s="63" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="D12" s="63" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -22089,10 +22034,10 @@
         <v>74</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="D13" s="15" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -22103,10 +22048,10 @@
         <v>72</v>
       </c>
       <c r="C14" s="63" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="D14" s="63" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -22117,7 +22062,7 @@
         <v>25</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="D15" s="15" t="s">
         <v>21</v>
@@ -22131,10 +22076,10 @@
         <v>5</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="D16" s="17" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="26" x14ac:dyDescent="0.15">
@@ -22145,10 +22090,10 @@
         <v>71</v>
       </c>
       <c r="C17" s="63" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="D17" s="63" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -22156,13 +22101,13 @@
         <v>82.8</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>373</v>
+        <v>368</v>
       </c>
       <c r="D18" s="18" t="s">
-        <v>374</v>
+        <v>369</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -22173,10 +22118,10 @@
         <v>73</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="D19" s="18" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -22201,10 +22146,10 @@
         <v>79</v>
       </c>
       <c r="C21" s="34" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="D21" s="34" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="26" x14ac:dyDescent="0.15">
@@ -22215,10 +22160,10 @@
         <v>83</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>368</v>
+        <v>363</v>
       </c>
       <c r="D22" s="15" t="s">
-        <v>370</v>
+        <v>365</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -22229,10 +22174,10 @@
         <v>74</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>371</v>
+        <v>366</v>
       </c>
       <c r="D23" s="18" t="s">
-        <v>372</v>
+        <v>367</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -22243,10 +22188,10 @@
         <v>73</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="D24" s="15" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -22257,10 +22202,10 @@
         <v>74</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="D25" s="17" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -22271,10 +22216,10 @@
         <v>73</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="D26" s="17" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -22285,10 +22230,10 @@
         <v>74</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="D27" s="17" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -22299,10 +22244,10 @@
         <v>73</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="D28" s="17" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -22313,10 +22258,10 @@
         <v>73</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="D29" s="17" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -22327,10 +22272,10 @@
         <v>82</v>
       </c>
       <c r="C30" s="64" t="s">
-        <v>301</v>
+        <v>296</v>
       </c>
       <c r="D30" s="65" t="s">
-        <v>297</v>
+        <v>292</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -22341,10 +22286,10 @@
         <v>74</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>314</v>
+        <v>309</v>
       </c>
       <c r="D31" s="15" t="s">
-        <v>314</v>
+        <v>309</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -22355,10 +22300,10 @@
         <v>74</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="D32" s="15" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -22369,10 +22314,10 @@
         <v>73</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="D33" s="15" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -22383,10 +22328,10 @@
         <v>73</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="D34" s="15" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -22397,10 +22342,10 @@
         <v>73</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>315</v>
+        <v>310</v>
       </c>
       <c r="D35" s="15" t="s">
-        <v>315</v>
+        <v>310</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -22411,10 +22356,10 @@
         <v>73</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="D36" s="15" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -22425,10 +22370,10 @@
         <v>74</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="D37" s="15" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -22439,10 +22384,10 @@
         <v>73</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="D38" s="15" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -22453,10 +22398,10 @@
         <v>74</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="D39" s="15" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -22467,10 +22412,10 @@
         <v>73</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="D40" s="15" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -22481,10 +22426,10 @@
         <v>73</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="D41" s="15" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -22495,10 +22440,10 @@
         <v>77</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="D42" s="17" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -22509,10 +22454,10 @@
         <v>82</v>
       </c>
       <c r="C43" s="64" t="s">
-        <v>299</v>
+        <v>294</v>
       </c>
       <c r="D43" s="65" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -22523,10 +22468,10 @@
         <v>81</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>294</v>
+        <v>289</v>
       </c>
       <c r="D44" s="17" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="26" x14ac:dyDescent="0.15">
@@ -22537,10 +22482,10 @@
         <v>113</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>339</v>
+        <v>334</v>
       </c>
       <c r="D45" s="17" t="s">
-        <v>340</v>
+        <v>335</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="13" x14ac:dyDescent="0.15">
@@ -22554,7 +22499,7 @@
         <v>111</v>
       </c>
       <c r="D46" s="65" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
     </row>
   </sheetData>
@@ -22606,10 +22551,10 @@
         <v>64</v>
       </c>
       <c r="C2" s="38" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="D2" s="39" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="F2" s="21"/>
       <c r="K2" s="35"/>
@@ -22622,7 +22567,7 @@
         <v>73</v>
       </c>
       <c r="C3" s="37" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="D3" s="37" t="str">
         <f>C3</f>
@@ -22639,7 +22584,7 @@
         <v>74</v>
       </c>
       <c r="C4" s="37" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="D4" s="37" t="str">
         <f t="shared" ref="D4:D7" si="0">C4</f>
@@ -22656,7 +22601,7 @@
         <v>74</v>
       </c>
       <c r="C5" s="37" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="D5" s="37" t="str">
         <f t="shared" si="0"/>
@@ -22673,7 +22618,7 @@
         <v>73</v>
       </c>
       <c r="C6" s="37" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="D6" s="37" t="str">
         <f t="shared" si="0"/>
@@ -22690,7 +22635,7 @@
         <v>73</v>
       </c>
       <c r="C7" s="37" t="s">
-        <v>344</v>
+        <v>339</v>
       </c>
       <c r="D7" s="37" t="str">
         <f t="shared" si="0"/>
@@ -22707,10 +22652,10 @@
         <v>74</v>
       </c>
       <c r="C8" s="37" t="s">
-        <v>328</v>
+        <v>323</v>
       </c>
       <c r="D8" s="37" t="s">
-        <v>329</v>
+        <v>324</v>
       </c>
       <c r="F8" s="21"/>
       <c r="K8" s="35"/>
@@ -22739,10 +22684,10 @@
         <v>83</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>330</v>
+        <v>325</v>
       </c>
       <c r="D10" s="15" t="s">
-        <v>331</v>
+        <v>326</v>
       </c>
       <c r="F10" s="21"/>
       <c r="K10" s="35"/>
@@ -22755,10 +22700,10 @@
         <v>72</v>
       </c>
       <c r="C11" s="38" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="D11" s="38" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="F11" s="21"/>
       <c r="K11" s="35"/>
@@ -22771,7 +22716,7 @@
         <v>5</v>
       </c>
       <c r="C12" s="76" t="s">
-        <v>332</v>
+        <v>327</v>
       </c>
       <c r="D12" s="76" t="str">
         <f>C12</f>
@@ -22788,10 +22733,10 @@
         <v>82</v>
       </c>
       <c r="C13" s="38" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="D13" s="39" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="F13" s="21"/>
       <c r="K13" s="34"/>
@@ -22804,10 +22749,10 @@
         <v>79</v>
       </c>
       <c r="C14" s="37" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="D14" s="37" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="F14" s="21"/>
       <c r="K14" s="34"/>
@@ -22820,10 +22765,10 @@
         <v>72</v>
       </c>
       <c r="C15" s="38" t="s">
-        <v>312</v>
+        <v>307</v>
       </c>
       <c r="D15" s="38" t="s">
-        <v>313</v>
+        <v>308</v>
       </c>
       <c r="F15" s="21"/>
       <c r="K15" s="35"/>
@@ -22836,10 +22781,10 @@
         <v>5</v>
       </c>
       <c r="C16" s="76" t="s">
-        <v>333</v>
+        <v>328</v>
       </c>
       <c r="D16" s="76" t="s">
-        <v>333</v>
+        <v>328</v>
       </c>
       <c r="F16" s="21"/>
       <c r="K16" s="34"/>
@@ -22852,10 +22797,10 @@
         <v>71</v>
       </c>
       <c r="C17" s="38" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="D17" s="38" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="F17" s="21"/>
       <c r="K17" s="35"/>
@@ -22868,7 +22813,7 @@
         <v>73</v>
       </c>
       <c r="C18" s="37" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
       <c r="D18" s="37" t="str">
         <f>C18</f>
@@ -22885,7 +22830,7 @@
         <v>5</v>
       </c>
       <c r="C19" s="76" t="s">
-        <v>334</v>
+        <v>329</v>
       </c>
       <c r="D19" s="76" t="str">
         <f>C19</f>
@@ -22899,13 +22844,13 @@
         <v>82</v>
       </c>
       <c r="B20" s="37" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>373</v>
+        <v>368</v>
       </c>
       <c r="D20" s="18" t="s">
-        <v>374</v>
+        <v>369</v>
       </c>
       <c r="F20" s="21"/>
       <c r="K20" s="35"/>
@@ -22918,10 +22863,10 @@
         <v>74</v>
       </c>
       <c r="C21" s="37" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="D21" s="37" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="F21" s="21"/>
       <c r="K21" s="35"/>
@@ -22950,10 +22895,10 @@
         <v>73</v>
       </c>
       <c r="C23" s="37" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="D23" s="37" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="F23" s="21"/>
       <c r="K23" s="35"/>
@@ -22982,7 +22927,7 @@
         <v>5</v>
       </c>
       <c r="C25" s="76" t="s">
-        <v>336</v>
+        <v>331</v>
       </c>
       <c r="D25" s="76" t="str">
         <f>C25</f>
@@ -22999,10 +22944,10 @@
         <v>82</v>
       </c>
       <c r="C26" s="38" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="D26" s="39" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="F26" s="21"/>
       <c r="K26" s="35"/>
@@ -23031,7 +22976,7 @@
         <v>5</v>
       </c>
       <c r="C28" s="76" t="s">
-        <v>337</v>
+        <v>332</v>
       </c>
       <c r="D28" s="76" t="str">
         <f>C28</f>
@@ -23048,10 +22993,10 @@
         <v>79</v>
       </c>
       <c r="C29" s="37" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="D29" s="37" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="F29" s="21"/>
       <c r="K29" s="34"/>
@@ -23067,7 +23012,7 @@
         <v>112</v>
       </c>
       <c r="D30" s="38" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="F30" s="21"/>
       <c r="K30" s="35"/>
@@ -23083,7 +23028,7 @@
         <v>87</v>
       </c>
       <c r="D31" s="37" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="F31" s="21"/>
       <c r="K31" s="35"/>
@@ -23096,10 +23041,10 @@
         <v>74</v>
       </c>
       <c r="C32" s="37" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="D32" s="37" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="F32" s="21"/>
       <c r="K32" s="35"/>
@@ -23112,10 +23057,10 @@
         <v>74</v>
       </c>
       <c r="C33" s="37" t="s">
-        <v>419</v>
+        <v>401</v>
       </c>
       <c r="D33" s="37" t="s">
-        <v>372</v>
+        <v>367</v>
       </c>
       <c r="F33" s="21"/>
       <c r="K33" s="35"/>
@@ -23128,7 +23073,7 @@
         <v>73</v>
       </c>
       <c r="C34" s="37" t="s">
-        <v>338</v>
+        <v>333</v>
       </c>
       <c r="D34" s="37" t="str">
         <f>C34</f>
@@ -23145,7 +23090,7 @@
         <v>74</v>
       </c>
       <c r="C35" s="37" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="D35" s="37" t="str">
         <f>C35</f>
@@ -23162,10 +23107,10 @@
         <v>113</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
       <c r="D36" s="17" t="s">
-        <v>340</v>
+        <v>335</v>
       </c>
       <c r="F36" s="21"/>
       <c r="K36" s="35"/>
@@ -23178,7 +23123,7 @@
         <v>73</v>
       </c>
       <c r="C37" s="37" t="s">
-        <v>341</v>
+        <v>336</v>
       </c>
       <c r="D37" s="37" t="str">
         <f>C37</f>
@@ -23195,7 +23140,7 @@
         <v>73</v>
       </c>
       <c r="C38" s="37" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="D38" s="37" t="str">
         <f>C38</f>
@@ -23215,7 +23160,7 @@
         <v>111</v>
       </c>
       <c r="D39" s="39" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="F39" s="21"/>
     </row>
@@ -23263,10 +23208,10 @@
         <v>80</v>
       </c>
       <c r="C2" s="71" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="D2" s="71" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="19" x14ac:dyDescent="0.15">
@@ -23277,7 +23222,7 @@
         <v>73</v>
       </c>
       <c r="C3" s="71" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="D3" s="71" t="str">
         <f>C3</f>
@@ -23292,7 +23237,7 @@
         <v>78</v>
       </c>
       <c r="C4" s="71" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="D4" s="71" t="s">
         <v>54</v>
@@ -23306,7 +23251,7 @@
         <v>74</v>
       </c>
       <c r="C5" s="71" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="D5" s="71" t="str">
         <f>C5</f>
@@ -23321,7 +23266,7 @@
         <v>44</v>
       </c>
       <c r="C6" s="71" t="s">
-        <v>342</v>
+        <v>337</v>
       </c>
       <c r="D6" s="71" t="s">
         <v>44</v>
@@ -23389,10 +23334,10 @@
         <v>64</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>283</v>
+        <v>278</v>
       </c>
       <c r="F2" s="21"/>
     </row>
@@ -23404,7 +23349,7 @@
         <v>74</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>284</v>
+        <v>279</v>
       </c>
       <c r="D3" s="15" t="str">
         <f>C3</f>
@@ -23420,10 +23365,10 @@
         <v>83</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>326</v>
+        <v>321</v>
       </c>
       <c r="D4" s="15" t="s">
-        <v>327</v>
+        <v>322</v>
       </c>
       <c r="F4" s="21"/>
     </row>
@@ -23450,10 +23395,10 @@
         <v>82</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="D6" s="18" t="s">
-        <v>286</v>
+        <v>281</v>
       </c>
       <c r="F6" s="21"/>
     </row>
@@ -23465,7 +23410,7 @@
         <v>5</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>287</v>
+        <v>282</v>
       </c>
       <c r="D7" s="15" t="str">
         <f>C7</f>
@@ -23497,10 +23442,10 @@
         <v>74</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="D9" s="19" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="F9" s="21"/>
     </row>
@@ -23512,7 +23457,7 @@
         <v>74</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
       <c r="D10" s="15" t="str">
         <f>C10</f>
@@ -23528,7 +23473,7 @@
         <v>73</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="D11" s="17" t="str">
         <f>C11</f>
@@ -23544,10 +23489,10 @@
         <v>5</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>287</v>
+        <v>282</v>
       </c>
       <c r="D12" s="15" t="s">
-        <v>287</v>
+        <v>282</v>
       </c>
       <c r="F12" s="21"/>
     </row>
@@ -23559,10 +23504,10 @@
         <v>82</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="D13" s="18" t="s">
-        <v>286</v>
+        <v>281</v>
       </c>
       <c r="F13" s="21"/>
     </row>
@@ -23590,10 +23535,10 @@
         <v>83</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="D15" s="17" t="s">
-        <v>289</v>
+        <v>284</v>
       </c>
       <c r="F15" s="21"/>
     </row>
@@ -23605,7 +23550,7 @@
         <v>74</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>290</v>
+        <v>285</v>
       </c>
       <c r="D16" s="18" t="str">
         <f>C16</f>
@@ -23621,7 +23566,7 @@
         <v>74</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
       <c r="D17" s="18" t="str">
         <f>C17</f>
@@ -23637,10 +23582,10 @@
         <v>113</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>292</v>
+        <v>287</v>
       </c>
       <c r="D18" s="18" t="s">
-        <v>293</v>
+        <v>288</v>
       </c>
       <c r="F18" s="21"/>
     </row>
@@ -23652,10 +23597,10 @@
         <v>44</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="D19" s="15" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="F19" s="21"/>
     </row>
@@ -23839,7 +23784,7 @@
   <dimension ref="A1:F42"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
@@ -23865,420 +23810,454 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="13" x14ac:dyDescent="0.15">
-      <c r="A2" s="72">
+      <c r="A2" s="13">
         <v>0</v>
       </c>
       <c r="B2" s="13" t="s">
         <v>64</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>238</v>
+        <v>254</v>
       </c>
       <c r="F2" s="21"/>
     </row>
-    <row r="3" spans="1:6" ht="26" x14ac:dyDescent="0.15">
-      <c r="A3" s="9">
-        <v>1.6</v>
+    <row r="3" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+      <c r="A3" s="7">
+        <v>0.7</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>350</v>
+        <v>313</v>
       </c>
       <c r="D3" s="15" t="s">
-        <v>351</v>
+        <v>314</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="13" x14ac:dyDescent="0.15">
-      <c r="A4" s="9">
-        <v>3</v>
+      <c r="A4" s="7">
+        <v>5</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>239</v>
+        <v>10</v>
       </c>
       <c r="D4" s="15" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="13" x14ac:dyDescent="0.15">
-      <c r="A5" s="9">
-        <v>3.0009999999999999</v>
+      <c r="A5" s="7">
+        <v>8.8000000000000007</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" s="17" t="s">
-        <v>240</v>
+        <v>5</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>255</v>
+      </c>
+      <c r="D5" s="18" t="s">
+        <v>255</v>
       </c>
       <c r="F5" s="21"/>
     </row>
-    <row r="6" spans="1:6" ht="13" x14ac:dyDescent="0.15">
-      <c r="A6" s="9">
-        <v>20.100000000000001</v>
+    <row r="6" spans="1:6" ht="26" x14ac:dyDescent="0.15">
+      <c r="A6" s="7">
+        <v>9.3000000000000007</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>254</v>
-      </c>
-      <c r="D6" s="15" t="s">
-        <v>254</v>
+        <v>71</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>256</v>
+      </c>
+      <c r="D6" s="19" t="s">
+        <v>257</v>
       </c>
       <c r="F6" s="21"/>
     </row>
-    <row r="7" spans="1:6" ht="26" x14ac:dyDescent="0.15">
-      <c r="A7" s="9">
-        <v>20.2</v>
+    <row r="7" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+      <c r="A7" s="7">
+        <v>29.6</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>378</v>
-      </c>
-      <c r="D7" s="17" t="s">
-        <v>379</v>
+        <v>74</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>315</v>
+      </c>
+      <c r="D7" s="15" t="str">
+        <f>C7</f>
+        <v>Route 397</v>
       </c>
       <c r="F7" s="21"/>
     </row>
     <row r="8" spans="1:6" ht="13" x14ac:dyDescent="0.15">
-      <c r="A8" s="9">
-        <v>33</v>
+      <c r="A8" s="7">
+        <v>35</v>
       </c>
       <c r="B8" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="C8" s="5" t="s">
-        <v>170</v>
-      </c>
-      <c r="D8" s="15" t="s">
-        <v>171</v>
+      <c r="C8" s="37" t="s">
+        <v>165</v>
+      </c>
+      <c r="D8" s="37" t="s">
+        <v>166</v>
       </c>
       <c r="F8" s="21"/>
     </row>
     <row r="9" spans="1:6" ht="13" x14ac:dyDescent="0.15">
-      <c r="A9" s="9">
-        <v>36.299999999999997</v>
+      <c r="A9" s="7">
+        <v>38</v>
       </c>
       <c r="B9" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>258</v>
+      </c>
+      <c r="D9" s="19" t="s">
+        <v>259</v>
+      </c>
+      <c r="F9" s="21"/>
+    </row>
+    <row r="10" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+      <c r="A10" s="7">
+        <v>55.8</v>
+      </c>
+      <c r="B10" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="5" t="s">
-        <v>250</v>
-      </c>
-      <c r="D9" s="15" t="s">
-        <v>250</v>
-      </c>
-      <c r="F9" s="21"/>
-    </row>
-    <row r="10" spans="1:6" ht="13" x14ac:dyDescent="0.15">
-      <c r="A10" s="9">
-        <v>45.5</v>
-      </c>
-      <c r="B10" s="7" t="s">
+      <c r="C10" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="D10" s="15" t="s">
+        <v>202</v>
+      </c>
+      <c r="F10" s="21"/>
+    </row>
+    <row r="11" spans="1:6" ht="26" x14ac:dyDescent="0.15">
+      <c r="A11" s="7">
+        <v>56.5</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>263</v>
+      </c>
+      <c r="D11" s="17" t="s">
+        <v>264</v>
+      </c>
+      <c r="F11" s="21"/>
+    </row>
+    <row r="12" spans="1:6" ht="26" x14ac:dyDescent="0.15">
+      <c r="A12" s="7">
+        <v>67.3</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>316</v>
+      </c>
+      <c r="D12" s="19" t="s">
+        <v>260</v>
+      </c>
+      <c r="F12" s="21"/>
+    </row>
+    <row r="13" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+      <c r="A13" s="7">
+        <v>71</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>272</v>
+      </c>
+      <c r="D13" s="18" t="s">
+        <v>271</v>
+      </c>
+      <c r="F13" s="21"/>
+    </row>
+    <row r="14" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+      <c r="A14" s="7">
+        <v>72.3</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>341</v>
+      </c>
+      <c r="D14" s="15" t="s">
+        <v>342</v>
+      </c>
+      <c r="F14" s="21"/>
+    </row>
+    <row r="15" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+      <c r="A15" s="7">
+        <v>72.8</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D15" s="15" t="s">
+        <v>261</v>
+      </c>
+      <c r="F15" s="21"/>
+    </row>
+    <row r="16" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+      <c r="A16" s="7">
+        <v>73.900000000000006</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D16" s="15" t="s">
+        <v>261</v>
+      </c>
+      <c r="F16" s="21"/>
+    </row>
+    <row r="17" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+      <c r="A17" s="7">
+        <v>74.8</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>341</v>
+      </c>
+      <c r="D17" s="15" t="s">
+        <v>342</v>
+      </c>
+      <c r="F17" s="21"/>
+    </row>
+    <row r="18" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+      <c r="A18" s="7">
+        <v>96.1</v>
+      </c>
+      <c r="B18" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="C10" s="4" t="s">
-        <v>381</v>
-      </c>
-      <c r="D10" s="17" t="s">
-        <v>382</v>
-      </c>
-      <c r="F10" s="21"/>
-    </row>
-    <row r="11" spans="1:6" ht="13" x14ac:dyDescent="0.15">
-      <c r="A11" s="9">
-        <v>53.4</v>
-      </c>
-      <c r="B11" s="7" t="s">
-        <v>166</v>
-      </c>
-      <c r="C11" s="8" t="s">
-        <v>389</v>
-      </c>
-      <c r="D11" s="18" t="s">
-        <v>390</v>
-      </c>
-      <c r="F11" s="21"/>
-    </row>
-    <row r="12" spans="1:6" ht="13" x14ac:dyDescent="0.15">
-      <c r="A12" s="9">
-        <v>59.4</v>
-      </c>
-      <c r="B12" s="7" t="s">
+      <c r="C18" s="4" t="s">
+        <v>273</v>
+      </c>
+      <c r="D18" s="17" t="s">
+        <v>274</v>
+      </c>
+      <c r="F18" s="21"/>
+    </row>
+    <row r="19" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+      <c r="A19" s="7">
+        <v>103.3</v>
+      </c>
+      <c r="B19" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="C12" s="5" t="s">
-        <v>246</v>
-      </c>
-      <c r="D12" s="15" t="s">
-        <v>246</v>
-      </c>
-      <c r="F12" s="21"/>
-    </row>
-    <row r="13" spans="1:6" ht="13" x14ac:dyDescent="0.15">
-      <c r="A13" s="9">
-        <v>62.5</v>
-      </c>
-      <c r="B13" s="7" t="s">
+      <c r="C19" s="5" t="s">
+        <v>317</v>
+      </c>
+      <c r="D19" s="15" t="str">
+        <f>C19</f>
+        <v>Route 113</v>
+      </c>
+      <c r="F19" s="21"/>
+    </row>
+    <row r="20" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+      <c r="A20" s="7">
+        <v>116.6</v>
+      </c>
+      <c r="B20" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C13" s="5" t="s">
-        <v>143</v>
-      </c>
-      <c r="D13" s="15" t="s">
-        <v>143</v>
-      </c>
-      <c r="F13" s="21"/>
-    </row>
-    <row r="14" spans="1:6" ht="26" x14ac:dyDescent="0.15">
-      <c r="A14" s="9">
-        <v>62.9</v>
-      </c>
-      <c r="B14" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>247</v>
-      </c>
-      <c r="D14" s="17" t="s">
-        <v>248</v>
-      </c>
-      <c r="F14" s="21"/>
-    </row>
-    <row r="15" spans="1:6" ht="13" x14ac:dyDescent="0.15">
-      <c r="A15" s="9">
-        <v>76.099999999999994</v>
-      </c>
-      <c r="B15" s="7" t="s">
+      <c r="C20" s="5" t="s">
+        <v>262</v>
+      </c>
+      <c r="D20" s="15" t="s">
+        <v>262</v>
+      </c>
+      <c r="F20" s="21"/>
+    </row>
+    <row r="21" spans="1:6" ht="26" x14ac:dyDescent="0.15">
+      <c r="A21" s="7">
+        <v>117</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>266</v>
+      </c>
+      <c r="D21" s="17" t="s">
+        <v>265</v>
+      </c>
+      <c r="F21" s="21"/>
+    </row>
+    <row r="22" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A22" s="7">
+        <v>125</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="C22" s="54" t="s">
+        <v>164</v>
+      </c>
+      <c r="D22" s="35" t="s">
+        <v>163</v>
+      </c>
+      <c r="F22" s="21"/>
+    </row>
+    <row r="23" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+      <c r="A23" s="7">
+        <v>139</v>
+      </c>
+      <c r="B23" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C15" s="5" t="s">
-        <v>243</v>
-      </c>
-      <c r="D15" s="15" t="s">
-        <v>243</v>
-      </c>
-      <c r="F15" s="21"/>
-    </row>
-    <row r="16" spans="1:6" ht="26" x14ac:dyDescent="0.15">
-      <c r="A16" s="9">
-        <v>76.3</v>
-      </c>
-      <c r="B16" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>386</v>
-      </c>
-      <c r="D16" s="17" t="s">
-        <v>385</v>
-      </c>
-      <c r="F16" s="21"/>
-    </row>
-    <row r="17" spans="1:6" ht="13" x14ac:dyDescent="0.15">
-      <c r="A17" s="9">
-        <v>76.599999999999994</v>
-      </c>
-      <c r="B17" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>387</v>
-      </c>
-      <c r="D17" s="15" t="str">
-        <f>C17</f>
-        <v>Rue des Quatre-Coins</v>
-      </c>
-      <c r="F17" s="21"/>
-    </row>
-    <row r="18" spans="1:6" ht="13" x14ac:dyDescent="0.15">
-      <c r="A18" s="9">
-        <v>76.900000000000006</v>
-      </c>
-      <c r="B18" s="7" t="s">
+      <c r="C23" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="D23" s="15" t="s">
+        <v>134</v>
+      </c>
+      <c r="F23" s="21"/>
+    </row>
+    <row r="24" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+      <c r="A24" s="7">
+        <v>139.30000000000001</v>
+      </c>
+      <c r="B24" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="C18" s="5" t="s">
-        <v>249</v>
-      </c>
-      <c r="D18" s="15" t="s">
-        <v>249</v>
-      </c>
-      <c r="F18" s="21"/>
-    </row>
-    <row r="19" spans="1:6" ht="26" x14ac:dyDescent="0.15">
-      <c r="A19" s="9">
-        <v>88.9</v>
-      </c>
-      <c r="B19" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>383</v>
-      </c>
-      <c r="D19" s="17" t="s">
-        <v>384</v>
-      </c>
-      <c r="F19" s="21"/>
-    </row>
-    <row r="20" spans="1:6" ht="13" x14ac:dyDescent="0.15">
-      <c r="A20" s="9">
-        <v>98.9</v>
-      </c>
-      <c r="B20" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="C20" s="5" t="s">
-        <v>169</v>
-      </c>
-      <c r="D20" s="15" t="s">
-        <v>168</v>
-      </c>
-      <c r="F20" s="21"/>
-    </row>
-    <row r="21" spans="1:6" ht="13" x14ac:dyDescent="0.15">
-      <c r="A21" s="9">
-        <v>101.2</v>
-      </c>
-      <c r="B21" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>256</v>
-      </c>
-      <c r="D21" s="17" t="s">
-        <v>257</v>
-      </c>
-      <c r="F21" s="21"/>
-    </row>
-    <row r="22" spans="1:6" ht="13" x14ac:dyDescent="0.15">
-      <c r="A22" s="9">
-        <v>105.71</v>
-      </c>
-      <c r="B22" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C22" s="5" t="s">
-        <v>241</v>
-      </c>
-      <c r="D22" s="15" t="s">
-        <v>241</v>
-      </c>
-      <c r="F22" s="21"/>
-    </row>
-    <row r="23" spans="1:6" ht="13" x14ac:dyDescent="0.15">
-      <c r="A23" s="9">
-        <v>115.9</v>
-      </c>
-      <c r="B23" s="7" t="s">
+      <c r="C24" s="5" t="s">
+        <v>343</v>
+      </c>
+      <c r="D24" s="15" t="s">
+        <v>344</v>
+      </c>
+      <c r="F24" s="21"/>
+    </row>
+    <row r="25" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+      <c r="A25" s="7">
+        <v>139.80000000000001</v>
+      </c>
+      <c r="B25" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="C23" s="5" t="s">
-        <v>167</v>
-      </c>
-      <c r="D23" s="15" t="s">
-        <v>167</v>
-      </c>
-      <c r="F23" s="21"/>
-    </row>
-    <row r="24" spans="1:6" ht="39" x14ac:dyDescent="0.15">
-      <c r="A24" s="9">
-        <v>117.3</v>
-      </c>
-      <c r="B24" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="C24" s="5" t="s">
-        <v>352</v>
-      </c>
-      <c r="D24" s="15" t="s">
-        <v>353</v>
-      </c>
-      <c r="F24" s="21"/>
-    </row>
-    <row r="25" spans="1:6" ht="13" x14ac:dyDescent="0.15">
-      <c r="A25" s="9">
-        <v>118.6</v>
-      </c>
-      <c r="B25" s="7" t="s">
-        <v>25</v>
-      </c>
       <c r="C25" s="5" t="s">
-        <v>205</v>
-      </c>
-      <c r="D25" s="15" t="s">
-        <v>21</v>
+        <v>318</v>
+      </c>
+      <c r="D25" s="15" t="str">
+        <f>C25</f>
+        <v>10e Avenue/ Route 386</v>
       </c>
       <c r="F25" s="21"/>
     </row>
-    <row r="26" spans="1:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="A26" s="9">
-        <v>118.8</v>
+    <row r="26" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+      <c r="A26" s="7">
+        <v>140.5</v>
       </c>
       <c r="B26" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>267</v>
+      </c>
+      <c r="D26" s="15" t="s">
+        <v>267</v>
+      </c>
+      <c r="F26" s="21"/>
+    </row>
+    <row r="27" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+      <c r="A27" s="7">
+        <v>142.1</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>268</v>
+      </c>
+      <c r="D27" s="15" t="s">
+        <v>268</v>
+      </c>
+      <c r="F27" s="21"/>
+    </row>
+    <row r="28" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+      <c r="A28" s="7">
+        <v>143.80000000000001</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>269</v>
+      </c>
+      <c r="D28" s="15" t="s">
+        <v>269</v>
+      </c>
+      <c r="F28" s="21"/>
+    </row>
+    <row r="29" spans="1:6" ht="26" x14ac:dyDescent="0.15">
+      <c r="A29" s="7">
+        <v>144.6</v>
+      </c>
+      <c r="B29" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="C26" s="73" t="s">
-        <v>280</v>
-      </c>
-      <c r="D26" s="74" t="s">
-        <v>281</v>
-      </c>
-      <c r="F26" s="21"/>
-    </row>
-    <row r="27" spans="1:6" ht="13" x14ac:dyDescent="0.15">
-      <c r="A27" s="9">
-        <v>118.9</v>
-      </c>
-      <c r="B27" s="7" t="s">
+      <c r="C29" s="5" t="s">
+        <v>319</v>
+      </c>
+      <c r="D29" s="15" t="s">
+        <v>320</v>
+      </c>
+      <c r="F29" s="21"/>
+    </row>
+    <row r="30" spans="1:6" ht="26" x14ac:dyDescent="0.15">
+      <c r="A30" s="7">
+        <v>144.9</v>
+      </c>
+      <c r="B30" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="C30" s="8" t="s">
+        <v>270</v>
+      </c>
+      <c r="D30" s="18" t="s">
+        <v>270</v>
+      </c>
+      <c r="F30" s="21"/>
+    </row>
+    <row r="31" spans="1:6" ht="39" x14ac:dyDescent="0.15">
+      <c r="A31" s="7">
+        <v>145</v>
+      </c>
+      <c r="B31" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="C27" s="4" t="s">
-        <v>255</v>
-      </c>
-      <c r="D27" s="17" t="s">
-        <v>200</v>
-      </c>
-      <c r="F27" s="21"/>
-    </row>
-    <row r="28" spans="1:6" ht="12" x14ac:dyDescent="0.15">
-      <c r="A28" s="3"/>
-      <c r="B28" s="7"/>
-      <c r="C28" s="5"/>
-      <c r="D28" s="15"/>
-      <c r="F28" s="21"/>
-    </row>
-    <row r="29" spans="1:6" ht="12" x14ac:dyDescent="0.15">
-      <c r="A29" s="3"/>
-      <c r="B29" s="7"/>
-      <c r="C29" s="5"/>
-      <c r="D29" s="15"/>
-      <c r="F29" s="21"/>
-    </row>
-    <row r="30" spans="1:6" ht="12" x14ac:dyDescent="0.15">
-      <c r="A30" s="3"/>
-      <c r="B30" s="7"/>
-      <c r="C30" s="5"/>
-      <c r="D30" s="15"/>
-      <c r="F30" s="21"/>
-    </row>
-    <row r="31" spans="1:6" ht="12" x14ac:dyDescent="0.15">
-      <c r="A31" s="3"/>
-      <c r="B31" s="7"/>
-      <c r="C31" s="5"/>
-      <c r="D31" s="15"/>
+      <c r="C31" s="4" t="s">
+        <v>311</v>
+      </c>
+      <c r="D31" s="17" t="s">
+        <v>312</v>
+      </c>
       <c r="F31" s="21"/>
     </row>
     <row r="32" spans="1:6" ht="12" x14ac:dyDescent="0.15">
@@ -24362,7 +24341,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E156DDD-44B2-497E-B657-8831DB081CFE}">
   <dimension ref="A1:F42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="A7" sqref="A7:XFD7"/>
     </sheetView>
   </sheetViews>
@@ -24396,10 +24375,10 @@
         <v>64</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="F2" s="21"/>
     </row>
@@ -24411,10 +24390,10 @@
         <v>73</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>350</v>
+        <v>345</v>
       </c>
       <c r="D3" s="15" t="s">
-        <v>351</v>
+        <v>346</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="13" x14ac:dyDescent="0.15">
@@ -24425,10 +24404,10 @@
         <v>74</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="D4" s="15" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="13" x14ac:dyDescent="0.15">
@@ -24442,7 +24421,7 @@
         <v>10</v>
       </c>
       <c r="D5" s="17" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="F5" s="21"/>
     </row>
@@ -24454,10 +24433,10 @@
         <v>5</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="D6" s="15" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="F6" s="21"/>
     </row>
@@ -24469,10 +24448,10 @@
         <v>72</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="D7" s="17" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
       <c r="F7" s="21"/>
     </row>
@@ -24484,10 +24463,10 @@
         <v>82</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="D8" s="17" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="F8" s="21"/>
     </row>
@@ -24499,10 +24478,10 @@
         <v>79</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="D9" s="15" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="F9" s="21"/>
     </row>
@@ -24514,10 +24493,10 @@
         <v>5</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="D10" s="15" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="F10" s="21"/>
     </row>
@@ -24529,10 +24508,10 @@
         <v>71</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
       <c r="D11" s="17" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
       <c r="F11" s="21"/>
     </row>
@@ -24544,10 +24523,10 @@
         <v>76</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="D12" s="15" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="F12" s="21"/>
     </row>
@@ -24574,10 +24553,10 @@
         <v>71</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="D14" s="17" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
       <c r="F14" s="21"/>
     </row>
@@ -24589,10 +24568,10 @@
         <v>73</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="D15" s="15" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="F15" s="21"/>
     </row>
@@ -24604,10 +24583,10 @@
         <v>5</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="D16" s="15" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="F16" s="21"/>
     </row>
@@ -24619,10 +24598,10 @@
         <v>72</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="D17" s="17" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="F17" s="21"/>
     </row>
@@ -24634,10 +24613,10 @@
         <v>82</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="D18" s="17" t="s">
-        <v>380</v>
+        <v>373</v>
       </c>
       <c r="F18" s="21"/>
     </row>
@@ -24646,13 +24625,13 @@
         <v>82.5</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>373</v>
+        <v>368</v>
       </c>
       <c r="D19" s="18" t="s">
-        <v>374</v>
+        <v>369</v>
       </c>
       <c r="F19" s="21"/>
     </row>
@@ -24664,10 +24643,10 @@
         <v>25</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>391</v>
+        <v>374</v>
       </c>
       <c r="D20" s="18" t="s">
-        <v>392</v>
+        <v>375</v>
       </c>
       <c r="F20" s="21"/>
     </row>
@@ -24679,10 +24658,10 @@
         <v>5</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="D21" s="15" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="F21" s="21"/>
     </row>
@@ -24694,10 +24673,10 @@
         <v>79</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="D22" s="15" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="F22" s="21"/>
     </row>
@@ -24709,10 +24688,10 @@
         <v>77</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="D23" s="15" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="F23" s="21"/>
     </row>
@@ -24724,10 +24703,10 @@
         <v>83</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>352</v>
+        <v>347</v>
       </c>
       <c r="D24" s="15" t="s">
-        <v>353</v>
+        <v>348</v>
       </c>
       <c r="F24" s="21"/>
     </row>
@@ -24739,7 +24718,7 @@
         <v>25</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="D25" s="15" t="s">
         <v>21</v>
@@ -24754,10 +24733,10 @@
         <v>113</v>
       </c>
       <c r="C26" s="73" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
       <c r="D26" s="74" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="F26" s="21"/>
     </row>
@@ -24769,10 +24748,10 @@
         <v>44</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="D27" s="17" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="F27" s="21"/>
     </row>

</xml_diff>

<commit_message>
Fin mise à jour initiale 2024
- import des gpx selon programmation préliminaire
- update sites
- guide organisateur mis en attente (conflit avec les gpx préliminaires sans POI)
</commit_message>
<xml_diff>
--- a/excel/Itineraires.xlsx
+++ b/excel/Itineraires.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brunogauthier/Documents/guide2024/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1F7E69F-B20E-0F43-B735-494E43AE28B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60B7F859-9C04-4D46-9ADE-44586E9280E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="68360" yWindow="500" windowWidth="34040" windowHeight="28180" tabRatio="758" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="927" uniqueCount="410">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="925" uniqueCount="411">
   <si>
     <t>GPM</t>
   </si>
@@ -1209,9 +1209,6 @@
     <t>(via 117)</t>
   </si>
   <si>
-    <t>xx</t>
-  </si>
-  <si>
     <t>(via Val-d'Or)</t>
   </si>
   <si>
@@ -1291,6 +1288,12 @@
   </si>
   <si>
     <t>Mineralogical Museum of A-T</t>
+  </si>
+  <si>
+    <t>Mont Bell</t>
+  </si>
+  <si>
+    <t>Mount Bell</t>
   </si>
 </sst>
 </file>
@@ -20789,7 +20792,7 @@
   <dimension ref="A1:AM14"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="AA1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="AF18" sqref="AF18"/>
+      <selection activeCell="AE6" sqref="AE6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -21015,7 +21018,7 @@
         <v>42</v>
       </c>
       <c r="T2" s="29" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="U2" t="str">
         <f>TEXT(_xlfn.CONCAT(Tableau2[[#This Row],[Heure_dep]],":",Tableau2[[#This Row],[min_dep]]), "HH:MM")</f>
@@ -21059,20 +21062,20 @@
         <v>131</v>
       </c>
       <c r="AG2" s="31" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="AH2" s="31" t="str">
         <f>Tableau2[[#This Row],[LieuDepFR]]</f>
         <v>CEGEP</v>
       </c>
       <c r="AI2" s="31" t="s">
+        <v>386</v>
+      </c>
+      <c r="AJ2" s="16" t="s">
         <v>387</v>
       </c>
-      <c r="AJ2" s="16" t="s">
-        <v>388</v>
-      </c>
       <c r="AK2" s="16" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="AL2" s="30"/>
       <c r="AM2" s="30"/>
@@ -21142,7 +21145,7 @@
         <v>42</v>
       </c>
       <c r="T3" s="29" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="U3" t="str">
         <f>TEXT(_xlfn.CONCAT(Tableau2[[#This Row],[Heure_dep]],":",Tableau2[[#This Row],[min_dep]]), "HH:MM")</f>
@@ -21186,20 +21189,20 @@
         <v>128</v>
       </c>
       <c r="AG3" s="31" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="AH3" s="31" t="str">
         <f>Tableau2[[#This Row],[LieuDepFR]]</f>
         <v>Cathédrale</v>
       </c>
       <c r="AI3" s="31" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="AJ3" s="16" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="AK3" s="16" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="AL3" s="30"/>
       <c r="AM3" s="30"/>
@@ -21268,7 +21271,7 @@
         <v>42</v>
       </c>
       <c r="T4" s="29" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="U4" t="str">
         <f>TEXT(_xlfn.CONCAT(Tableau2[[#This Row],[Heure_dep]],":",Tableau2[[#This Row],[min_dep]]), "HH:MM")</f>
@@ -21305,11 +21308,9 @@
       <c r="AD4" s="31" t="s">
         <v>380</v>
       </c>
-      <c r="AE4" s="31" t="s">
-        <v>382</v>
-      </c>
+      <c r="AE4" s="31"/>
       <c r="AF4" s="31" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="AG4" s="31" t="str">
         <f>Tableau2[[#This Row],[LieuDepFR]]</f>
@@ -21356,7 +21357,7 @@
         <v>85</v>
       </c>
       <c r="F5" s="16" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="G5" s="60" t="str">
         <f>CONCATENATE(Tableau2[[#This Row],[Distance_totale]]," km")</f>
@@ -21403,7 +21404,7 @@
         <v>44</v>
       </c>
       <c r="T5" s="29" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="U5" t="str">
         <f>TEXT(_xlfn.CONCAT(Tableau2[[#This Row],[Heure_dep]],":",Tableau2[[#This Row],[min_dep]]), "HH:MM")</f>
@@ -21444,14 +21445,14 @@
         <v>142</v>
       </c>
       <c r="AF5" s="31" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="AG5" s="31" t="str">
         <f>Tableau2[[#This Row],[LieuDepFR]]</f>
         <v>Musée minéralogique de l'A-T</v>
       </c>
       <c r="AH5" s="31" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="AI5" s="30" t="str">
         <f>Tableau2[[#This Row],[LieuDepEN]]</f>
@@ -21484,7 +21485,7 @@
         <v>85</v>
       </c>
       <c r="F6" s="16" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="G6" s="60" t="str">
         <f>CONCATENATE(Tableau2[[#This Row],[Distance_totale]]," km")</f>
@@ -21531,7 +21532,7 @@
         <v>41</v>
       </c>
       <c r="T6" s="29" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="U6" t="str">
         <f>TEXT(_xlfn.CONCAT(Tableau2[[#This Row],[Heure_dep]],":",Tableau2[[#This Row],[min_dep]]), "HH:MM")</f>
@@ -21569,25 +21570,25 @@
         <v>133</v>
       </c>
       <c r="AE6" s="31" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="AF6" s="31" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="AG6" s="31" t="s">
-        <v>385</v>
+        <v>409</v>
       </c>
       <c r="AH6" s="31" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="AI6" s="31" t="s">
-        <v>387</v>
+        <v>410</v>
       </c>
       <c r="AJ6" s="16" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="AK6" s="16" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="AL6" s="30"/>
       <c r="AM6" s="30"/>
@@ -21658,7 +21659,7 @@
         <v>42</v>
       </c>
       <c r="T7" s="29" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="U7" t="str">
         <f>TEXT(_xlfn.CONCAT(Tableau2[[#This Row],[Heure_dep]],":",Tableau2[[#This Row],[min_dep]]), "HH:MM")</f>
@@ -21695,27 +21696,25 @@
       <c r="AD7" s="31" t="s">
         <v>380</v>
       </c>
-      <c r="AE7" s="31" t="s">
-        <v>382</v>
-      </c>
+      <c r="AE7" s="31"/>
       <c r="AF7" s="76" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="AG7" s="31" t="str">
         <f>Tableau2[[#This Row],[LieuDepFR]]</f>
         <v>Hôtel de Ville</v>
       </c>
       <c r="AH7" s="31" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="AI7" s="31" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="AJ7" s="16" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="AK7" s="16" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="AL7" s="30"/>
       <c r="AM7" s="30"/>
@@ -21785,7 +21784,7 @@
         <v>42</v>
       </c>
       <c r="T8" s="29" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="U8" t="str">
         <f>TEXT(_xlfn.CONCAT(Tableau2[[#This Row],[Heure_dep]],":",Tableau2[[#This Row],[min_dep]]), "HH:MM")</f>
@@ -21823,25 +21822,25 @@
         <v>380</v>
       </c>
       <c r="AE8" s="31" t="s">
+        <v>383</v>
+      </c>
+      <c r="AF8" s="31" t="s">
         <v>384</v>
       </c>
-      <c r="AF8" s="31" t="s">
-        <v>385</v>
-      </c>
       <c r="AG8" s="31" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="AH8" s="31" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="AI8" s="31" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="AJ8" s="16" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="AK8" s="16" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="AL8" s="30"/>
       <c r="AM8" s="30"/>
@@ -23080,7 +23079,7 @@
         <v>73</v>
       </c>
       <c r="C33" s="36" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="D33" s="36" t="s">
         <v>365</v>

</xml_diff>

<commit_message>
Corrections page Cyclo & upload seulement fichier requis pour pipeline
</commit_message>
<xml_diff>
--- a/excel/Itineraires.xlsx
+++ b/excel/Itineraires.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brunogauthier/Documents/guide2024/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24D76139-C8DF-244B-B69C-12AF45BAC38D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A963DD3A-499D-1D42-8E40-AD6A74857999}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="64160" yWindow="560" windowWidth="38160" windowHeight="19860" tabRatio="758" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="64160" yWindow="560" windowWidth="38160" windowHeight="19860" tabRatio="758" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="23" r:id="rId1"/>
@@ -6786,8 +6786,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{371307C5-CDC8-4A0E-8E08-E5295E5C8E14}">
   <dimension ref="A1:G326"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7:E7"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
@@ -6852,7 +6852,7 @@
     </row>
     <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.2">
       <c r="A3" s="30">
-        <v>0.03</v>
+        <v>5.0999999999999997E-2</v>
       </c>
       <c r="B3" s="29" t="s">
         <v>72</v>
@@ -6878,7 +6878,7 @@
     </row>
     <row r="4" spans="1:7" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" s="30">
-        <v>0.12</v>
+        <v>0.151</v>
       </c>
       <c r="B4" s="29" t="s">
         <v>73</v>
@@ -9246,7 +9246,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{999478FB-CEE0-EF4A-8215-89FD317FBCF5}">
   <dimension ref="A1:G321"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
@@ -12032,7 +12032,7 @@
         <v>333</v>
       </c>
       <c r="E8" s="23" t="str">
-        <f t="shared" ref="E8:E18" si="0">D8</f>
+        <f t="shared" ref="E8:E17" si="0">D8</f>
         <v>Boulevard Sabourin</v>
       </c>
       <c r="F8" s="47" t="str">

</xml_diff>

<commit_message>
Ajout élévation 5 et code
</commit_message>
<xml_diff>
--- a/excel/Itineraires.xlsx
+++ b/excel/Itineraires.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brunogauthier/Documents/guide2024/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10BB5FA1-9059-944D-8204-DF66FBB05144}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{172294A5-F7B2-6042-9A72-6239693D4E94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="64160" yWindow="560" windowWidth="38160" windowHeight="19860" tabRatio="758" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3071,8 +3071,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BF2EC7B-8CF4-1449-B844-A73E16F738A4}">
   <dimension ref="A1:G322"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="D47" sqref="D47"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="B54" sqref="B54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
@@ -4064,7 +4064,7 @@
     <row r="41" spans="1:7" ht="15" x14ac:dyDescent="0.2">
       <c r="A41" s="30">
         <f>$A$46-20</f>
-        <v>101</v>
+        <v>101.3</v>
       </c>
       <c r="B41" s="29" t="s">
         <v>78</v>
@@ -4149,7 +4149,8 @@
     </row>
     <row r="45" spans="1:7" ht="14" x14ac:dyDescent="0.2">
       <c r="A45" s="37">
-        <v>120.94</v>
+        <f>$A$46-0.1</f>
+        <v>121.2</v>
       </c>
       <c r="B45" s="31" t="s">
         <v>110</v>
@@ -4168,7 +4169,7 @@
     </row>
     <row r="46" spans="1:7" ht="15" x14ac:dyDescent="0.2">
       <c r="A46" s="37">
-        <v>121</v>
+        <v>121.3</v>
       </c>
       <c r="B46" s="31" t="s">
         <v>43</v>
@@ -6542,7 +6543,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF8C653E-9E00-4EDF-9978-201805372337}">
   <dimension ref="A1:AM14"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
@@ -10076,8 +10077,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{999478FB-CEE0-EF4A-8215-89FD317FBCF5}">
   <dimension ref="A1:G321"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView topLeftCell="A12" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
@@ -18596,8 +18597,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA4CF35A-AE95-4D4B-80F8-FB6E5D8CEEB2}">
   <dimension ref="A1:I48"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32:XFD36"/>
+    <sheetView topLeftCell="A11" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
@@ -19524,8 +19525,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AEBDB8C-6DC2-3445-97F3-86408AFF8E25}">
   <dimension ref="A1:G321"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView topLeftCell="A9" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
@@ -20029,8 +20030,8 @@
     </row>
     <row r="20" spans="1:7" ht="15" x14ac:dyDescent="0.2">
       <c r="A20" s="30">
-        <f>A19+6.42</f>
-        <v>27.22</v>
+        <f>A19+6.52</f>
+        <v>27.32</v>
       </c>
       <c r="B20" s="29" t="s">
         <v>71</v>
@@ -20159,8 +20160,8 @@
     </row>
     <row r="25" spans="1:7" ht="15" x14ac:dyDescent="0.2">
       <c r="A25" s="30">
-        <f>A24+6.42</f>
-        <v>58.42</v>
+        <f>A24+6.52</f>
+        <v>58.519999999999996</v>
       </c>
       <c r="B25" s="29" t="s">
         <v>71</v>
@@ -20263,8 +20264,8 @@
     </row>
     <row r="29" spans="1:7" ht="15" x14ac:dyDescent="0.2">
       <c r="A29" s="30">
-        <f>A28+6.42</f>
-        <v>89.62</v>
+        <f>A28+6.52</f>
+        <v>89.72</v>
       </c>
       <c r="B29" s="29" t="s">
         <v>71</v>

</xml_diff>

<commit_message>
Correction sprint maire Senneterre placé en double, ref #2.
Correction gpx, fichier excel
Correction carte statique full de l'étape 5
Manque correction élévations full des étapes 5 et 7 pour éliminer le
point bleu (correction manuelle requise pour arriver aux bons profils)
</commit_message>
<xml_diff>
--- a/excel/Itineraires.xlsx
+++ b/excel/Itineraires.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10414"/>
   <workbookPr date1904="1" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brunogauthier/Documents/guide2024/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{172294A5-F7B2-6042-9A72-6239693D4E94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD36A0CF-5C2E-104A-8054-BC6B503D76C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="64160" yWindow="560" windowWidth="38160" windowHeight="19860" tabRatio="758" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28760" yWindow="2220" windowWidth="38160" windowHeight="19860" tabRatio="758" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="23" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1199" uniqueCount="615">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1196" uniqueCount="613">
   <si>
     <t>GPM</t>
   </si>
@@ -568,12 +568,6 @@
     <t>Obaska</t>
   </si>
   <si>
-    <t>Sprint du maire de Senneterre 250$&lt;br/&gt;(École St-Isidore)</t>
-  </si>
-  <si>
-    <t>Senneterre Mayor's sprint 250$&lt;br/&gt;(École St-Isidore)</t>
-  </si>
-  <si>
     <t>Senneterre Mayor's sprint 250$&lt;br/&gt;(Camping le Huard)</t>
   </si>
   <si>
@@ -1654,12 +1648,6 @@
     <t>Sprint de la Mairesse 250$ / Mayor Sprint</t>
   </si>
   <si>
-    <t>Début 2e tour (9 tours à faire)&lt;br/&gt;Sprint de la Mairesse de Senneterre (250$)</t>
-  </si>
-  <si>
-    <t>Start of 2nd lap (9 laps to go)&lt;br/&gt;Senneterre Mayor's sprint (250$)</t>
-  </si>
-  <si>
     <t>straigth</t>
   </si>
   <si>
@@ -1886,6 +1874,12 @@
   </si>
   <si>
     <t>Round about 1st exit on the left (reverse of normal traffic)&lt;br&gt;7e rue</t>
+  </si>
+  <si>
+    <t>Début 2e tour (9 tours à faire)</t>
+  </si>
+  <si>
+    <t>Start of 2nd lap (9 laps to go)</t>
   </si>
 </sst>
 </file>
@@ -3038,27 +3032,27 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A6" s="4" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A7" s="4" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A8" s="4" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A9" s="4" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A10" s="4" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
     </row>
   </sheetData>
@@ -3071,8 +3065,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BF2EC7B-8CF4-1449-B844-A73E16F738A4}">
   <dimension ref="A1:G322"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B54" sqref="B54"/>
+    <sheetView topLeftCell="A20" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
@@ -3095,7 +3089,7 @@
         <v>19</v>
       </c>
       <c r="C1" s="39" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="D1" s="40" t="s">
         <v>17</v>
@@ -3104,10 +3098,10 @@
         <v>18</v>
       </c>
       <c r="F1" s="41" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="G1" s="41" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="15" x14ac:dyDescent="0.2">
@@ -3118,13 +3112,13 @@
         <v>63</v>
       </c>
       <c r="C2" s="29" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="D2" s="23" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="E2" s="23" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="F2" s="35" t="str">
         <f>VLOOKUP(B2,Lexique!A:F,5,)</f>
@@ -3143,13 +3137,13 @@
         <v>76</v>
       </c>
       <c r="C3" s="29" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="D3" s="23" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="E3" s="23" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="F3" s="35" t="str">
         <f>VLOOKUP(B3,Lexique!A:F,5,)</f>
@@ -3168,13 +3162,13 @@
         <v>73</v>
       </c>
       <c r="C4" s="29" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="D4" s="23" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="E4" s="23" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="F4" s="35" t="str">
         <f>VLOOKUP(B4,Lexique!A:F,5,)</f>
@@ -3193,13 +3187,13 @@
         <v>75</v>
       </c>
       <c r="C5" s="29" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="D5" s="23" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="E5" s="23" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="F5" s="35" t="str">
         <f>VLOOKUP(B5,Lexique!A:F,5,)</f>
@@ -3218,13 +3212,13 @@
         <v>75</v>
       </c>
       <c r="C6" s="29" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="D6" s="23" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="E6" s="23" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="F6" s="35" t="str">
         <f>VLOOKUP(B6,Lexique!A:F,5,)</f>
@@ -3243,7 +3237,7 @@
         <v>25</v>
       </c>
       <c r="C7" s="29" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="D7" s="23" t="s">
         <v>2</v>
@@ -3268,7 +3262,7 @@
         <v>79</v>
       </c>
       <c r="C8" s="29" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="D8" s="23" t="s">
         <v>10</v>
@@ -3293,7 +3287,7 @@
         <v>25</v>
       </c>
       <c r="C9" s="29" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="D9" s="23" t="s">
         <v>2</v>
@@ -3319,7 +3313,7 @@
         <v>78</v>
       </c>
       <c r="C10" s="29" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="D10" s="23" t="s">
         <v>155</v>
@@ -3344,7 +3338,7 @@
         <v>72</v>
       </c>
       <c r="C11" s="29" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="D11" s="23" t="s">
         <v>165</v>
@@ -3369,7 +3363,7 @@
         <v>76</v>
       </c>
       <c r="C12" s="29" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="D12" s="23" t="s">
         <v>165</v>
@@ -3394,13 +3388,13 @@
         <v>71</v>
       </c>
       <c r="C13" s="29" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="D13" s="23" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="E13" s="23" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="F13" s="35" t="str">
         <f>VLOOKUP(B13,Lexique!A:F,5,)</f>
@@ -3419,7 +3413,7 @@
         <v>25</v>
       </c>
       <c r="C14" s="29" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="D14" s="23" t="s">
         <v>2</v>
@@ -3444,13 +3438,13 @@
         <v>5</v>
       </c>
       <c r="C15" s="29" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="D15" s="23" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="E15" s="23" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="F15" s="35" t="str">
         <f>VLOOKUP(B15,Lexique!A:F,5,)</f>
@@ -3469,13 +3463,13 @@
         <v>82</v>
       </c>
       <c r="C16" s="29" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="D16" s="44" t="s">
-        <v>611</v>
+        <v>607</v>
       </c>
       <c r="E16" s="62" t="s">
-        <v>612</v>
+        <v>608</v>
       </c>
       <c r="F16" s="35" t="str">
         <f>VLOOKUP(B16,Lexique!A:F,5,)</f>
@@ -3494,13 +3488,13 @@
         <v>25</v>
       </c>
       <c r="C17" s="29" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="D17" s="24" t="s">
         <v>22</v>
       </c>
       <c r="E17" s="25" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="F17" s="35" t="str">
         <f>VLOOKUP(B17,Lexique!A:F,5,)</f>
@@ -3519,13 +3513,13 @@
         <v>25</v>
       </c>
       <c r="C18" s="29" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="D18" s="24" t="s">
         <v>22</v>
       </c>
       <c r="E18" s="25" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="F18" s="35" t="str">
         <f>VLOOKUP(B18,Lexique!A:F,5,)</f>
@@ -3544,13 +3538,13 @@
         <v>25</v>
       </c>
       <c r="C19" s="29" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="D19" s="24" t="s">
         <v>22</v>
       </c>
       <c r="E19" s="25" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="F19" s="35" t="str">
         <f>VLOOKUP(B19,Lexique!A:F,5,)</f>
@@ -3569,13 +3563,13 @@
         <v>82</v>
       </c>
       <c r="C20" s="29" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="D20" s="44" t="s">
-        <v>613</v>
+        <v>609</v>
       </c>
       <c r="E20" s="62" t="s">
-        <v>614</v>
+        <v>610</v>
       </c>
       <c r="F20" s="35" t="str">
         <f>VLOOKUP(B20,Lexique!A:F,5,)</f>
@@ -3594,13 +3588,13 @@
         <v>72</v>
       </c>
       <c r="C21" s="29" t="s">
+        <v>514</v>
+      </c>
+      <c r="D21" s="25" t="s">
+        <v>515</v>
+      </c>
+      <c r="E21" s="25" t="s">
         <v>516</v>
-      </c>
-      <c r="D21" s="25" t="s">
-        <v>517</v>
-      </c>
-      <c r="E21" s="25" t="s">
-        <v>518</v>
       </c>
       <c r="F21" s="35" t="str">
         <f>VLOOKUP(B21,Lexique!A:F,5,)</f>
@@ -3619,13 +3613,13 @@
         <v>76</v>
       </c>
       <c r="C22" s="29" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="D22" s="23" t="s">
-        <v>610</v>
+        <v>606</v>
       </c>
       <c r="E22" s="23" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="F22" s="35" t="str">
         <f>VLOOKUP(B22,Lexique!A:F,5,)</f>
@@ -3644,13 +3638,13 @@
         <v>73</v>
       </c>
       <c r="C23" s="29" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="D23" s="23" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="E23" s="23" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="F23" s="35" t="str">
         <f>VLOOKUP(B23,Lexique!A:F,5,)</f>
@@ -3669,13 +3663,13 @@
         <v>72</v>
       </c>
       <c r="C24" s="29" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="D24" s="23" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="E24" s="23" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="F24" s="35" t="str">
         <f>VLOOKUP(B24,Lexique!A:F,5,)</f>
@@ -3694,13 +3688,13 @@
         <v>73</v>
       </c>
       <c r="C25" s="29" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="D25" s="23" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="E25" s="23" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="F25" s="35" t="str">
         <f>VLOOKUP(B25,Lexique!A:F,5,)</f>
@@ -3719,13 +3713,13 @@
         <v>71</v>
       </c>
       <c r="C26" s="29" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="D26" s="23" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="E26" s="23" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="F26" s="35" t="str">
         <f>VLOOKUP(B26,Lexique!A:F,5,)</f>
@@ -3744,13 +3738,13 @@
         <v>73</v>
       </c>
       <c r="C27" s="29" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="D27" s="26" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="E27" s="26" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="F27" s="35" t="str">
         <f>VLOOKUP(B27,Lexique!A:F,5,)</f>
@@ -3769,13 +3763,13 @@
         <v>72</v>
       </c>
       <c r="C28" s="29" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D28" s="23" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="E28" s="23" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="F28" s="35" t="str">
         <f>VLOOKUP(B28,Lexique!A:F,5,)</f>
@@ -3794,13 +3788,13 @@
         <v>73</v>
       </c>
       <c r="C29" s="29" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="D29" s="23" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="E29" s="23" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="F29" s="35" t="str">
         <f>VLOOKUP(B29,Lexique!A:F,5,)</f>
@@ -3819,13 +3813,13 @@
         <v>73</v>
       </c>
       <c r="C30" s="29" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="D30" s="24" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="E30" s="24" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="F30" s="35" t="str">
         <f>VLOOKUP(B30,Lexique!A:F,5,)</f>
@@ -3844,13 +3838,13 @@
         <v>72</v>
       </c>
       <c r="C31" s="29" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="D31" s="23" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="E31" s="23" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="F31" s="35" t="str">
         <f>VLOOKUP(B31,Lexique!A:F,5,)</f>
@@ -3869,13 +3863,13 @@
         <v>73</v>
       </c>
       <c r="C32" s="29" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="D32" s="24" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="E32" s="24" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="F32" s="35" t="str">
         <f>VLOOKUP(B32,Lexique!A:F,5,)</f>
@@ -3894,13 +3888,13 @@
         <v>73</v>
       </c>
       <c r="C33" s="29" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="D33" s="23" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="E33" s="23" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="F33" s="35" t="str">
         <f>VLOOKUP(B33,Lexique!A:F,5,)</f>
@@ -3911,30 +3905,30 @@
         <v>Nom route / rue</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="30" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:7" ht="15" x14ac:dyDescent="0.2">
       <c r="A34" s="30">
         <f>A22+5.175</f>
         <v>74.424999999999997</v>
       </c>
       <c r="B34" s="29" t="s">
-        <v>81</v>
-      </c>
-      <c r="C34" s="29" t="s">
-        <v>536</v>
+        <v>76</v>
+      </c>
+      <c r="C34" s="32" t="s">
+        <v>535</v>
       </c>
       <c r="D34" s="23" t="s">
-        <v>537</v>
+        <v>611</v>
       </c>
       <c r="E34" s="23" t="s">
-        <v>538</v>
+        <v>612</v>
       </c>
       <c r="F34" s="35" t="str">
         <f>VLOOKUP(B34,Lexique!A:F,5,)</f>
-        <v>Sprint du maire Ville $250&lt;br/&gt; Lieu précis Ville</v>
+        <v>Nom route / rue</v>
       </c>
       <c r="G34" s="35" t="str">
         <f>VLOOKUP(B34,Lexique!A:F,6,)</f>
-        <v>Ville Mayor's sprint $250&lt;br/&gt; Lieu précis Ville</v>
+        <v>Nom route / rue</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="15" x14ac:dyDescent="0.2">
@@ -3946,13 +3940,13 @@
         <v>76</v>
       </c>
       <c r="C35" s="32" t="s">
-        <v>539</v>
+        <v>535</v>
       </c>
       <c r="D35" s="23" t="s">
-        <v>540</v>
+        <v>536</v>
       </c>
       <c r="E35" s="23" t="s">
-        <v>541</v>
+        <v>537</v>
       </c>
       <c r="F35" s="35" t="str">
         <f>VLOOKUP(B35,Lexique!A:F,5,)</f>
@@ -3975,10 +3969,10 @@
         <v>4</v>
       </c>
       <c r="D36" s="27" t="s">
-        <v>542</v>
+        <v>538</v>
       </c>
       <c r="E36" s="27" t="s">
-        <v>543</v>
+        <v>539</v>
       </c>
       <c r="F36" s="35"/>
       <c r="G36" s="35"/>
@@ -3995,10 +3989,10 @@
         <v>5</v>
       </c>
       <c r="D37" s="27" t="s">
-        <v>544</v>
+        <v>540</v>
       </c>
       <c r="E37" s="27" t="s">
-        <v>545</v>
+        <v>541</v>
       </c>
       <c r="F37" s="35"/>
       <c r="G37" s="35"/>
@@ -4011,13 +4005,13 @@
         <v>71</v>
       </c>
       <c r="C38" s="32" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="D38" s="23" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="E38" s="23" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="F38" s="35"/>
       <c r="G38" s="35"/>
@@ -4034,10 +4028,10 @@
         <v>6</v>
       </c>
       <c r="D39" s="27" t="s">
-        <v>546</v>
+        <v>542</v>
       </c>
       <c r="E39" s="27" t="s">
-        <v>547</v>
+        <v>543</v>
       </c>
       <c r="F39" s="35"/>
       <c r="G39" s="35"/>
@@ -4050,13 +4044,13 @@
         <v>70</v>
       </c>
       <c r="C40" s="32" t="s">
-        <v>548</v>
+        <v>544</v>
       </c>
       <c r="D40" s="27" t="s">
-        <v>549</v>
+        <v>545</v>
       </c>
       <c r="E40" s="27" t="s">
-        <v>550</v>
+        <v>546</v>
       </c>
       <c r="F40" s="35"/>
       <c r="G40" s="35"/>
@@ -4070,7 +4064,7 @@
         <v>78</v>
       </c>
       <c r="C41" s="29" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="D41" s="23" t="s">
         <v>154</v>
@@ -4096,13 +4090,13 @@
         <v>76</v>
       </c>
       <c r="C42" s="32" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="D42" s="27" t="s">
-        <v>552</v>
+        <v>548</v>
       </c>
       <c r="E42" s="27" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="F42" s="35"/>
       <c r="G42" s="35"/>
@@ -4116,13 +4110,13 @@
         <v>81</v>
       </c>
       <c r="C43" s="32" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="D43" s="23" t="s">
-        <v>554</v>
+        <v>550</v>
       </c>
       <c r="E43" s="23" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
       <c r="F43" s="35"/>
       <c r="G43" s="35"/>
@@ -4136,13 +4130,13 @@
         <v>76</v>
       </c>
       <c r="C44" s="32" t="s">
-        <v>556</v>
+        <v>552</v>
       </c>
       <c r="D44" s="27" t="s">
-        <v>557</v>
+        <v>553</v>
       </c>
       <c r="E44" s="27" t="s">
-        <v>558</v>
+        <v>554</v>
       </c>
       <c r="F44" s="35"/>
       <c r="G44" s="35"/>
@@ -4156,13 +4150,13 @@
         <v>110</v>
       </c>
       <c r="C45" s="32" t="s">
-        <v>559</v>
+        <v>555</v>
       </c>
       <c r="D45" s="27" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="E45" s="27" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="F45" s="35"/>
       <c r="G45" s="35"/>
@@ -4175,7 +4169,7 @@
         <v>43</v>
       </c>
       <c r="C46" s="32" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="D46" s="23" t="s">
         <v>166</v>
@@ -6139,10 +6133,10 @@
         <v>38</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="F1" s="22" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.15">
@@ -6159,10 +6153,10 @@
         <v>40</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.15">
@@ -6199,10 +6193,10 @@
         <v>42</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.15">
@@ -6239,10 +6233,10 @@
         <v>25</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.15">
@@ -6259,10 +6253,10 @@
         <v>5</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.15">
@@ -6279,10 +6273,10 @@
         <v>44</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.15">
@@ -6299,10 +6293,10 @@
         <v>45</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.15">
@@ -6319,10 +6313,10 @@
         <v>46</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="14" x14ac:dyDescent="0.15">
@@ -6339,7 +6333,7 @@
         <v>47</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="F11" t="str">
         <f>Tableau1[[#This Row],[Texte_REF_FR]]</f>
@@ -6360,7 +6354,7 @@
         <v>48</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="F12" t="str">
         <f>Tableau1[[#This Row],[Texte_REF_FR]]</f>
@@ -6381,7 +6375,7 @@
         <v>49</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="F13" t="str">
         <f>Tableau1[[#This Row],[Texte_REF_FR]]</f>
@@ -6402,7 +6396,7 @@
         <v>50</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="F14" t="str">
         <f>Tableau1[[#This Row],[Texte_REF_FR]]</f>
@@ -6423,7 +6417,7 @@
         <v>51</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="F15" t="str">
         <f>Tableau1[[#This Row],[Texte_REF_FR]]</f>
@@ -6444,10 +6438,10 @@
         <v>52</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.15">
@@ -6484,10 +6478,10 @@
         <v>84</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.15">
@@ -6504,10 +6498,10 @@
         <v>112</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.15">
@@ -6524,10 +6518,10 @@
         <v>151</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
   </sheetData>
@@ -6723,7 +6717,7 @@
         <v>85</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="G2" s="19" t="str">
         <f>CONCATENATE(Tableau2[[#This Row],[Distance_Route]], " km + (",Tableau2[[#This Row],[Nb_tours]]," x ",Tableau2[[#This Row],[KM_par_tours]]," km) = ",Tableau2[[#This Row],[Distance_totale]]," km")</f>
@@ -6770,7 +6764,7 @@
         <v>42</v>
       </c>
       <c r="T2" s="14" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="U2" t="str">
         <f>TEXT(_xlfn.CONCAT(Tableau2[[#This Row],[Heure_dep]],":",Tableau2[[#This Row],[min_dep]]), "HH:MM")</f>
@@ -6802,32 +6796,32 @@
         <v>0.81022727272727268</v>
       </c>
       <c r="AC2" s="16" t="s">
+        <v>212</v>
+      </c>
+      <c r="AD2" s="16" t="s">
+        <v>213</v>
+      </c>
+      <c r="AE2" s="16" t="s">
         <v>214</v>
-      </c>
-      <c r="AD2" s="16" t="s">
-        <v>215</v>
-      </c>
-      <c r="AE2" s="16" t="s">
-        <v>216</v>
       </c>
       <c r="AF2" s="16" t="s">
         <v>129</v>
       </c>
       <c r="AG2" s="16" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="AH2" s="16" t="str">
         <f>Tableau2[[#This Row],[LieuDepFR]]</f>
         <v>CEGEP</v>
       </c>
       <c r="AI2" s="16" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="AJ2" s="4" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="AK2" s="4" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="AL2" s="15"/>
       <c r="AM2" s="15"/>
@@ -6850,7 +6844,7 @@
         <v>85</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="G3" s="19" t="str">
         <f>CONCATENATE(Tableau2[[#This Row],[Distance_Route]], " km + (",Tableau2[[#This Row],[Nb_tours]]," x ",Tableau2[[#This Row],[KM_par_tours]]," km) = ",Tableau2[[#This Row],[Distance_totale]]," km")</f>
@@ -6897,7 +6891,7 @@
         <v>42</v>
       </c>
       <c r="T3" s="14" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="U3" t="str">
         <f>TEXT(_xlfn.CONCAT(Tableau2[[#This Row],[Heure_dep]],":",Tableau2[[#This Row],[min_dep]]), "HH:MM")</f>
@@ -6932,7 +6926,7 @@
         <v>123</v>
       </c>
       <c r="AD3" s="16" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="AE3" s="16" t="s">
         <v>135</v>
@@ -6941,20 +6935,20 @@
         <v>126</v>
       </c>
       <c r="AG3" s="16" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="AH3" s="16" t="str">
         <f>Tableau2[[#This Row],[LieuDepFR]]</f>
         <v>Cathédrale</v>
       </c>
       <c r="AI3" s="16" t="s">
+        <v>219</v>
+      </c>
+      <c r="AJ3" s="4" t="s">
         <v>221</v>
       </c>
-      <c r="AJ3" s="4" t="s">
-        <v>223</v>
-      </c>
       <c r="AK3" s="4" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="AL3" s="15"/>
       <c r="AM3" s="15"/>
@@ -6977,7 +6971,7 @@
         <v>85</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="G4" s="19" t="str">
         <f>CONCATENATE(Tableau2[[#This Row],[Distance_totale]]," km")</f>
@@ -7023,7 +7017,7 @@
         <v>42</v>
       </c>
       <c r="T4" s="14" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="U4" t="str">
         <f>TEXT(_xlfn.CONCAT(Tableau2[[#This Row],[Heure_dep]],":",Tableau2[[#This Row],[min_dep]]), "HH:MM")</f>
@@ -7055,14 +7049,14 @@
         <v>0.382518115942029</v>
       </c>
       <c r="AC4" s="16" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="AD4" s="16" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="AE4" s="16"/>
       <c r="AF4" s="16" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="AG4" s="16" t="str">
         <f>Tableau2[[#This Row],[LieuDepFR]]</f>
@@ -7109,7 +7103,7 @@
         <v>85</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="G5" s="19" t="str">
         <f>CONCATENATE(Tableau2[[#This Row],[Distance_totale]]," km")</f>
@@ -7156,7 +7150,7 @@
         <v>44</v>
       </c>
       <c r="T5" s="14" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="U5" t="str">
         <f>TEXT(_xlfn.CONCAT(Tableau2[[#This Row],[Heure_dep]],":",Tableau2[[#This Row],[min_dep]]), "HH:MM")</f>
@@ -7197,14 +7191,14 @@
         <v>140</v>
       </c>
       <c r="AF5" s="16" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="AG5" s="16" t="str">
         <f>Tableau2[[#This Row],[LieuDepFR]]</f>
         <v>Musée minéralogique de l'A-T</v>
       </c>
       <c r="AH5" s="16" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="AI5" s="15" t="str">
         <f>Tableau2[[#This Row],[LieuDepEN]]</f>
@@ -7237,7 +7231,7 @@
         <v>85</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="G6" s="19" t="str">
         <f>CONCATENATE(Tableau2[[#This Row],[Distance_totale]]," km")</f>
@@ -7284,7 +7278,7 @@
         <v>41</v>
       </c>
       <c r="T6" s="14" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="U6" t="str">
         <f>TEXT(_xlfn.CONCAT(Tableau2[[#This Row],[Heure_dep]],":",Tableau2[[#This Row],[min_dep]]), "HH:MM")</f>
@@ -7322,25 +7316,25 @@
         <v>131</v>
       </c>
       <c r="AE6" s="16" t="s">
+        <v>215</v>
+      </c>
+      <c r="AF6" s="16" t="s">
         <v>217</v>
       </c>
-      <c r="AF6" s="16" t="s">
+      <c r="AG6" s="16" t="s">
+        <v>237</v>
+      </c>
+      <c r="AH6" s="16" t="s">
         <v>219</v>
       </c>
-      <c r="AG6" s="16" t="s">
-        <v>239</v>
-      </c>
-      <c r="AH6" s="16" t="s">
-        <v>221</v>
-      </c>
       <c r="AI6" s="16" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="AJ6" s="4" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="AK6" s="4" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="AL6" s="15"/>
       <c r="AM6" s="15"/>
@@ -7363,7 +7357,7 @@
         <v>85</v>
       </c>
       <c r="F7" s="19" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="G7" s="19" t="str">
         <f>CONCATENATE(Tableau2[[#This Row],[Nb_tours]], " x ",Tableau2[[#This Row],[KM_par_tours]], " km = ",Tableau2[[#This Row],[Distance_totale]]," km")</f>
@@ -7411,7 +7405,7 @@
         <v>42</v>
       </c>
       <c r="T7" s="14" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="U7" t="str">
         <f>TEXT(_xlfn.CONCAT(Tableau2[[#This Row],[Heure_dep]],":",Tableau2[[#This Row],[min_dep]]), "HH:MM")</f>
@@ -7443,30 +7437,30 @@
         <v>0.80568181818181817</v>
       </c>
       <c r="AC7" s="16" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="AD7" s="16" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="AE7" s="16"/>
       <c r="AF7" s="21" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="AG7" s="16" t="str">
         <f>Tableau2[[#This Row],[LieuDepFR]]</f>
         <v>Hôtel de Ville</v>
       </c>
       <c r="AH7" s="16" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="AI7" s="16" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="AJ7" s="4" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="AK7" s="4" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="AL7" s="15"/>
       <c r="AM7" s="15"/>
@@ -7489,7 +7483,7 @@
         <v>85</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="G8" s="19" t="str">
         <f>CONCATENATE(Tableau2[[#This Row],[Distance_Route]], " km + (",Tableau2[[#This Row],[Nb_tours]]," x ",Tableau2[[#This Row],[KM_par_tours]]," km) = ",Tableau2[[#This Row],[Distance_totale]]," km")</f>
@@ -7536,7 +7530,7 @@
         <v>42</v>
       </c>
       <c r="T8" s="14" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="U8" t="str">
         <f>TEXT(_xlfn.CONCAT(Tableau2[[#This Row],[Heure_dep]],":",Tableau2[[#This Row],[min_dep]]), "HH:MM")</f>
@@ -7571,28 +7565,28 @@
         <v>131</v>
       </c>
       <c r="AD8" s="16" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="AE8" s="16" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="AF8" s="16" t="s">
+        <v>217</v>
+      </c>
+      <c r="AG8" s="16" t="s">
+        <v>217</v>
+      </c>
+      <c r="AH8" s="16" t="s">
         <v>219</v>
       </c>
-      <c r="AG8" s="16" t="s">
+      <c r="AI8" s="16" t="s">
         <v>219</v>
       </c>
-      <c r="AH8" s="16" t="s">
-        <v>221</v>
-      </c>
-      <c r="AI8" s="16" t="s">
-        <v>221</v>
-      </c>
       <c r="AJ8" s="4" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="AK8" s="4" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="AL8" s="15"/>
       <c r="AM8" s="15"/>
@@ -7641,7 +7635,7 @@
         <v>19</v>
       </c>
       <c r="C1" s="39" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="D1" s="40" t="s">
         <v>17</v>
@@ -7650,10 +7644,10 @@
         <v>18</v>
       </c>
       <c r="F1" s="41" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="G1" s="41" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="15" x14ac:dyDescent="0.2">
@@ -7664,13 +7658,13 @@
         <v>63</v>
       </c>
       <c r="C2" s="29" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="D2" s="23" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="E2" s="23" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="F2" s="35" t="str">
         <f>VLOOKUP(B2,Lexique!A:F,5,)</f>
@@ -7689,7 +7683,7 @@
         <v>72</v>
       </c>
       <c r="C3" s="29" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="D3" s="23" t="s">
         <v>147</v>
@@ -7715,7 +7709,7 @@
         <v>73</v>
       </c>
       <c r="C4" s="29" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="D4" s="23" t="s">
         <v>148</v>
@@ -7741,7 +7735,7 @@
         <v>72</v>
       </c>
       <c r="C5" s="29" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="D5" s="23" t="s">
         <v>149</v>
@@ -7767,10 +7761,10 @@
         <v>73</v>
       </c>
       <c r="C6" s="29" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="D6" s="23" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="E6" s="23" t="str">
         <f>D6</f>
@@ -7793,13 +7787,13 @@
         <v>82</v>
       </c>
       <c r="C7" s="29" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="D7" s="23" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="E7" s="23" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="F7" s="35" t="str">
         <f>VLOOKUP(B7,Lexique!A:F,5,)</f>
@@ -7818,7 +7812,7 @@
         <v>79</v>
       </c>
       <c r="C8" s="29" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="D8" s="23" t="s">
         <v>10</v>
@@ -7843,13 +7837,13 @@
         <v>5</v>
       </c>
       <c r="C9" s="29" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D9" s="23" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="E9" s="23" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="F9" s="35" t="str">
         <f>VLOOKUP(B9,Lexique!A:F,5,)</f>
@@ -7918,13 +7912,13 @@
         <v>5</v>
       </c>
       <c r="C12" s="29" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="D12" s="23" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="E12" s="25" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="F12" s="35" t="str">
         <f>VLOOKUP(B12,Lexique!A:F,5,)</f>
@@ -7968,13 +7962,13 @@
         <v>71</v>
       </c>
       <c r="C14" s="29" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="D14" s="25" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="E14" s="25" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="F14" s="35" t="str">
         <f>VLOOKUP(B14,Lexique!A:F,5,)</f>
@@ -7993,7 +7987,7 @@
         <v>78</v>
       </c>
       <c r="C15" s="29" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="D15" s="23" t="s">
         <v>155</v>
@@ -8043,13 +8037,13 @@
         <v>70</v>
       </c>
       <c r="C17" s="29" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="D17" s="43" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="E17" s="43" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="F17" s="35" t="str">
         <f>VLOOKUP(B17,Lexique!A:F,5,)</f>
@@ -8068,10 +8062,10 @@
         <v>5</v>
       </c>
       <c r="C18" s="29" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="D18" s="23" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="E18" s="23" t="s">
         <v>140</v>
@@ -8093,13 +8087,13 @@
         <v>81</v>
       </c>
       <c r="C19" s="29" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="D19" s="23" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="E19" s="23" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="F19" s="35" t="str">
         <f>VLOOKUP(B19,Lexique!A:F,5,)</f>
@@ -8118,13 +8112,13 @@
         <v>5</v>
       </c>
       <c r="C20" s="29" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="D20" s="23" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="E20" s="23" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="F20" s="35" t="str">
         <f>VLOOKUP(B20,Lexique!A:F,5,)</f>
@@ -8143,7 +8137,7 @@
         <v>75</v>
       </c>
       <c r="C21" s="29" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="D21" s="24" t="s">
         <v>165</v>
@@ -8169,7 +8163,7 @@
         <v>75</v>
       </c>
       <c r="C22" s="29" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="D22" s="23" t="s">
         <v>165</v>
@@ -8195,13 +8189,13 @@
         <v>70</v>
       </c>
       <c r="C23" s="29" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="D23" s="43" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="E23" s="43" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="F23" s="35" t="str">
         <f>VLOOKUP(B23,Lexique!A:F,5,)</f>
@@ -8220,13 +8214,13 @@
         <v>5</v>
       </c>
       <c r="C24" s="29" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="D24" s="23" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="E24" s="44" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="F24" s="35" t="str">
         <f>VLOOKUP(B24,Lexique!A:F,5,)</f>
@@ -8245,13 +8239,13 @@
         <v>82</v>
       </c>
       <c r="C25" s="29" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="D25" s="23" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="E25" s="23" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="F25" s="35" t="str">
         <f>VLOOKUP(B25,Lexique!A:F,5,)</f>
@@ -8270,13 +8264,13 @@
         <v>25</v>
       </c>
       <c r="C26" s="29" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="D26" s="23" t="s">
         <v>22</v>
       </c>
       <c r="E26" s="23" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="F26" s="35" t="str">
         <f>VLOOKUP(B26,Lexique!A:F,5,)</f>
@@ -8295,13 +8289,13 @@
         <v>152</v>
       </c>
       <c r="C27" s="29" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="D27" s="23" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="E27" s="23" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="F27" s="35" t="str">
         <f>VLOOKUP(B27,Lexique!A:F,5,)</f>
@@ -8320,13 +8314,13 @@
         <v>5</v>
       </c>
       <c r="C28" s="29" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="D28" s="23" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E28" s="23" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="F28" s="35" t="str">
         <f>VLOOKUP(B28,Lexique!A:F,5,)</f>
@@ -8345,13 +8339,13 @@
         <v>81</v>
       </c>
       <c r="C29" s="29" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="D29" s="23" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="E29" s="23" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="F29" s="35" t="str">
         <f>VLOOKUP(B29,Lexique!A:F,5,)</f>
@@ -8370,13 +8364,13 @@
         <v>25</v>
       </c>
       <c r="C30" s="29" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="D30" s="24" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="E30" s="24" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="F30" s="35" t="str">
         <f>VLOOKUP(B30,Lexique!A:F,5,)</f>
@@ -8395,7 +8389,7 @@
         <v>78</v>
       </c>
       <c r="C31" s="29" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="D31" s="23" t="s">
         <v>154</v>
@@ -8420,13 +8414,13 @@
         <v>5</v>
       </c>
       <c r="C32" s="29" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="D32" s="23" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="E32" s="23" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="F32" s="35" t="str">
         <f>VLOOKUP(B32,Lexique!A:F,5,)</f>
@@ -8445,13 +8439,13 @@
         <v>82</v>
       </c>
       <c r="C33" s="29" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="D33" s="23" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="E33" s="23" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="F33" s="35" t="str">
         <f>VLOOKUP(B33,Lexique!A:F,5,)</f>
@@ -8470,10 +8464,10 @@
         <v>73</v>
       </c>
       <c r="C34" s="29" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="D34" s="23" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="E34" s="23" t="str">
         <f>D34</f>
@@ -8496,13 +8490,13 @@
         <v>71</v>
       </c>
       <c r="C35" s="29" t="s">
+        <v>424</v>
+      </c>
+      <c r="D35" s="25" t="s">
+        <v>425</v>
+      </c>
+      <c r="E35" s="25" t="s">
         <v>426</v>
-      </c>
-      <c r="D35" s="25" t="s">
-        <v>427</v>
-      </c>
-      <c r="E35" s="25" t="s">
-        <v>428</v>
       </c>
       <c r="F35" s="35" t="str">
         <f>VLOOKUP(B35,Lexique!A:F,5,)</f>
@@ -8521,10 +8515,10 @@
         <v>72</v>
       </c>
       <c r="C36" s="29" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="D36" s="23" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="E36" s="23" t="str">
         <f>D36</f>
@@ -8547,10 +8541,10 @@
         <v>73</v>
       </c>
       <c r="C37" s="29" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="D37" s="23" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="E37" s="23" t="str">
         <f>D37</f>
@@ -8573,13 +8567,13 @@
         <v>72</v>
       </c>
       <c r="C38" s="29" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="D38" s="23" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="E38" s="23" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="F38" s="35" t="str">
         <f>VLOOKUP(B38,Lexique!A:F,5,)</f>
@@ -8598,10 +8592,10 @@
         <v>73</v>
       </c>
       <c r="C39" s="29" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="D39" s="23" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="E39" s="23" t="str">
         <f>D39</f>
@@ -8624,10 +8618,10 @@
         <v>73</v>
       </c>
       <c r="C40" s="29" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="D40" s="23" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="E40" s="23" t="str">
         <f>D40</f>
@@ -8650,13 +8644,13 @@
         <v>76</v>
       </c>
       <c r="C41" s="29" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="D41" s="23" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="E41" s="23" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="F41" s="35" t="str">
         <f>VLOOKUP(B41,Lexique!A:F,5,)</f>
@@ -8675,10 +8669,10 @@
         <v>73</v>
       </c>
       <c r="C42" s="29" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="D42" s="23" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="E42" s="23" t="str">
         <f>D42</f>
@@ -8701,10 +8695,10 @@
         <v>72</v>
       </c>
       <c r="C43" s="29" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="D43" s="24" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="E43" s="23" t="str">
         <f t="shared" ref="E43:E49" si="0">D43</f>
@@ -8727,10 +8721,10 @@
         <v>73</v>
       </c>
       <c r="C44" s="29" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="D44" s="23" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="E44" s="23" t="str">
         <f t="shared" si="0"/>
@@ -8753,10 +8747,10 @@
         <v>73</v>
       </c>
       <c r="C45" s="29" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="D45" s="23" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="E45" s="23" t="str">
         <f t="shared" si="0"/>
@@ -8779,10 +8773,10 @@
         <v>73</v>
       </c>
       <c r="C46" s="29" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="D46" s="24" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="E46" s="23" t="str">
         <f t="shared" si="0"/>
@@ -8805,10 +8799,10 @@
         <v>72</v>
       </c>
       <c r="C47" s="32" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="D47" s="26" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="E47" s="23" t="str">
         <f t="shared" si="0"/>
@@ -8831,10 +8825,10 @@
         <v>73</v>
       </c>
       <c r="C48" s="32" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="D48" s="26" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="E48" s="23" t="str">
         <f t="shared" si="0"/>
@@ -8857,10 +8851,10 @@
         <v>73</v>
       </c>
       <c r="C49" s="32" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="D49" s="26" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="E49" s="23" t="str">
         <f t="shared" si="0"/>
@@ -8883,13 +8877,13 @@
         <v>76</v>
       </c>
       <c r="C50" s="32" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="D50" s="23" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="E50" s="23" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="F50" s="35" t="str">
         <f>VLOOKUP(B50,Lexique!A:F,5,)</f>
@@ -8908,13 +8902,13 @@
         <v>80</v>
       </c>
       <c r="C51" s="32" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="D51" s="26" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="E51" s="26" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="F51" s="35" t="str">
         <f>VLOOKUP(B51,Lexique!A:F,5,)</f>
@@ -8933,13 +8927,13 @@
         <v>110</v>
       </c>
       <c r="C52" s="32" t="s">
+        <v>349</v>
+      </c>
+      <c r="D52" s="26" t="s">
+        <v>350</v>
+      </c>
+      <c r="E52" s="26" t="s">
         <v>351</v>
-      </c>
-      <c r="D52" s="26" t="s">
-        <v>352</v>
-      </c>
-      <c r="E52" s="26" t="s">
-        <v>353</v>
       </c>
       <c r="F52" s="35" t="str">
         <f>VLOOKUP(B52,Lexique!A:F,5,)</f>
@@ -8958,7 +8952,7 @@
         <v>43</v>
       </c>
       <c r="C53" s="32" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="D53" s="26" t="s">
         <v>109</v>
@@ -10101,7 +10095,7 @@
         <v>19</v>
       </c>
       <c r="C1" s="39" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="D1" s="40" t="s">
         <v>17</v>
@@ -10110,10 +10104,10 @@
         <v>18</v>
       </c>
       <c r="F1" s="41" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="G1" s="41" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="15" x14ac:dyDescent="0.2">
@@ -10124,13 +10118,13 @@
         <v>63</v>
       </c>
       <c r="C2" s="29" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="D2" s="23" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="E2" s="23" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="F2" s="35" t="str">
         <f>VLOOKUP(B2,Lexique!A:F,5,)</f>
@@ -10155,7 +10149,7 @@
         <v>22</v>
       </c>
       <c r="E3" s="23" t="s">
-        <v>560</v>
+        <v>556</v>
       </c>
       <c r="F3" s="35" t="str">
         <f>VLOOKUP(B3,Lexique!A:F,5,)</f>
@@ -10174,13 +10168,13 @@
         <v>72</v>
       </c>
       <c r="C4" s="29" t="s">
-        <v>561</v>
+        <v>557</v>
       </c>
       <c r="D4" s="23" t="s">
-        <v>562</v>
+        <v>558</v>
       </c>
       <c r="E4" s="23" t="s">
-        <v>562</v>
+        <v>558</v>
       </c>
       <c r="F4" s="35" t="str">
         <f>VLOOKUP(B4,Lexique!A:F,5,)</f>
@@ -10199,13 +10193,13 @@
         <v>82</v>
       </c>
       <c r="C5" s="29" t="s">
-        <v>563</v>
+        <v>559</v>
       </c>
       <c r="D5" s="23" t="s">
-        <v>602</v>
+        <v>598</v>
       </c>
       <c r="E5" s="23" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
       <c r="F5" s="35" t="str">
         <f>VLOOKUP(B5,Lexique!A:F,5,)</f>
@@ -10224,13 +10218,13 @@
         <v>82</v>
       </c>
       <c r="C6" s="29" t="s">
-        <v>564</v>
+        <v>560</v>
       </c>
       <c r="D6" s="23" t="s">
-        <v>600</v>
+        <v>596</v>
       </c>
       <c r="E6" s="23" t="s">
-        <v>601</v>
+        <v>597</v>
       </c>
       <c r="F6" s="35" t="str">
         <f>VLOOKUP(B6,Lexique!A:F,5,)</f>
@@ -10249,7 +10243,7 @@
         <v>79</v>
       </c>
       <c r="C7" s="29" t="s">
-        <v>565</v>
+        <v>561</v>
       </c>
       <c r="D7" s="23" t="s">
         <v>10</v>
@@ -10274,13 +10268,13 @@
         <v>73</v>
       </c>
       <c r="C8" s="29" t="s">
-        <v>566</v>
+        <v>562</v>
       </c>
       <c r="D8" s="23" t="s">
-        <v>567</v>
+        <v>563</v>
       </c>
       <c r="E8" s="23" t="s">
-        <v>567</v>
+        <v>563</v>
       </c>
       <c r="F8" s="35" t="str">
         <f>VLOOKUP(B8,Lexique!A:F,5,)</f>
@@ -10299,10 +10293,10 @@
         <v>5</v>
       </c>
       <c r="C9" s="29" t="s">
-        <v>588</v>
+        <v>584</v>
       </c>
       <c r="D9" s="23" t="s">
-        <v>588</v>
+        <v>584</v>
       </c>
       <c r="E9" s="23" t="str">
         <f>D9</f>
@@ -10325,13 +10319,13 @@
         <v>81</v>
       </c>
       <c r="C10" s="29" t="s">
-        <v>568</v>
+        <v>564</v>
       </c>
       <c r="D10" s="23" t="s">
-        <v>590</v>
+        <v>586</v>
       </c>
       <c r="E10" s="24" t="s">
-        <v>589</v>
+        <v>585</v>
       </c>
       <c r="F10" s="35" t="str">
         <f>VLOOKUP(B10,Lexique!A:F,5,)</f>
@@ -10356,7 +10350,7 @@
         <v>12</v>
       </c>
       <c r="E11" s="23" t="s">
-        <v>569</v>
+        <v>565</v>
       </c>
       <c r="F11" s="35" t="str">
         <f>VLOOKUP(B11,Lexique!A:F,5,)</f>
@@ -10375,13 +10369,13 @@
         <v>71</v>
       </c>
       <c r="C12" s="29" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="D12" s="23" t="s">
-        <v>594</v>
+        <v>590</v>
       </c>
       <c r="E12" s="23" t="s">
-        <v>595</v>
+        <v>591</v>
       </c>
       <c r="F12" s="35" t="str">
         <f>VLOOKUP(B12,Lexique!A:F,5,)</f>
@@ -10401,7 +10395,7 @@
         <v>78</v>
       </c>
       <c r="C13" s="29" t="s">
-        <v>570</v>
+        <v>566</v>
       </c>
       <c r="D13" s="23" t="s">
         <v>155</v>
@@ -10426,13 +10420,13 @@
         <v>72</v>
       </c>
       <c r="C14" s="29" t="s">
-        <v>571</v>
+        <v>567</v>
       </c>
       <c r="D14" s="25" t="s">
-        <v>572</v>
+        <v>568</v>
       </c>
       <c r="E14" s="25" t="s">
-        <v>572</v>
+        <v>568</v>
       </c>
       <c r="F14" s="35" t="str">
         <f>VLOOKUP(B14,Lexique!A:F,5,)</f>
@@ -10451,7 +10445,7 @@
         <v>25</v>
       </c>
       <c r="C15" s="29" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="D15" s="23" t="s">
         <v>2</v>
@@ -10476,7 +10470,7 @@
         <v>25</v>
       </c>
       <c r="C16" s="29" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="D16" s="23" t="s">
         <v>2</v>
@@ -10501,13 +10495,13 @@
         <v>5</v>
       </c>
       <c r="C17" s="29" t="s">
-        <v>573</v>
+        <v>569</v>
       </c>
       <c r="D17" s="26" t="s">
-        <v>574</v>
+        <v>570</v>
       </c>
       <c r="E17" s="25" t="s">
-        <v>574</v>
+        <v>570</v>
       </c>
       <c r="F17" s="35" t="str">
         <f>VLOOKUP(B17,Lexique!A:F,5,)</f>
@@ -10526,13 +10520,13 @@
         <v>70</v>
       </c>
       <c r="C18" s="29" t="s">
-        <v>575</v>
+        <v>571</v>
       </c>
       <c r="D18" s="23" t="s">
-        <v>591</v>
+        <v>587</v>
       </c>
       <c r="E18" s="23" t="s">
-        <v>576</v>
+        <v>572</v>
       </c>
       <c r="F18" s="35" t="str">
         <f>VLOOKUP(B18,Lexique!A:F,5,)</f>
@@ -10557,7 +10551,7 @@
         <v>22</v>
       </c>
       <c r="E19" s="23" t="s">
-        <v>560</v>
+        <v>556</v>
       </c>
       <c r="F19" s="35" t="str">
         <f>VLOOKUP(B19,Lexique!A:F,5,)</f>
@@ -10576,13 +10570,13 @@
         <v>152</v>
       </c>
       <c r="C20" s="29" t="s">
-        <v>577</v>
+        <v>573</v>
       </c>
       <c r="D20" s="25" t="s">
-        <v>577</v>
+        <v>573</v>
       </c>
       <c r="E20" s="25" t="s">
-        <v>578</v>
+        <v>574</v>
       </c>
       <c r="F20" s="35" t="str">
         <f>VLOOKUP(B20,Lexique!A:F,5,)</f>
@@ -10601,13 +10595,13 @@
         <v>71</v>
       </c>
       <c r="C21" s="29" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="D21" s="23" t="s">
-        <v>596</v>
+        <v>592</v>
       </c>
       <c r="E21" s="23" t="s">
-        <v>597</v>
+        <v>593</v>
       </c>
       <c r="F21" s="35" t="str">
         <f>VLOOKUP(B21,Lexique!A:F,5,)</f>
@@ -10626,7 +10620,7 @@
         <v>25</v>
       </c>
       <c r="C22" s="29" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="D22" s="23" t="s">
         <v>2</v>
@@ -10651,7 +10645,7 @@
         <v>25</v>
       </c>
       <c r="C23" s="29" t="s">
-        <v>579</v>
+        <v>575</v>
       </c>
       <c r="D23" s="23" t="s">
         <v>2</v>
@@ -10676,13 +10670,13 @@
         <v>81</v>
       </c>
       <c r="C24" s="29" t="s">
-        <v>568</v>
+        <v>564</v>
       </c>
       <c r="D24" s="23" t="s">
-        <v>608</v>
+        <v>604</v>
       </c>
       <c r="E24" s="24" t="s">
-        <v>609</v>
+        <v>605</v>
       </c>
       <c r="F24" s="35" t="str">
         <f>VLOOKUP(B24,Lexique!A:F,5,)</f>
@@ -10702,7 +10696,7 @@
         <v>78</v>
       </c>
       <c r="C25" s="29" t="s">
-        <v>580</v>
+        <v>576</v>
       </c>
       <c r="D25" s="25" t="s">
         <v>154</v>
@@ -10727,10 +10721,10 @@
         <v>5</v>
       </c>
       <c r="C26" s="29" t="s">
-        <v>606</v>
+        <v>602</v>
       </c>
       <c r="D26" s="25" t="s">
-        <v>607</v>
+        <v>603</v>
       </c>
       <c r="E26" s="25" t="str">
         <f>D26</f>
@@ -10753,13 +10747,13 @@
         <v>82</v>
       </c>
       <c r="C27" s="29" t="s">
-        <v>581</v>
+        <v>577</v>
       </c>
       <c r="D27" s="23" t="s">
-        <v>598</v>
+        <v>594</v>
       </c>
       <c r="E27" s="23" t="s">
-        <v>599</v>
+        <v>595</v>
       </c>
       <c r="F27" s="35" t="str">
         <f>VLOOKUP(B27,Lexique!A:F,5,)</f>
@@ -10784,7 +10778,7 @@
         <v>22</v>
       </c>
       <c r="E28" s="23" t="s">
-        <v>560</v>
+        <v>556</v>
       </c>
       <c r="F28" s="35" t="str">
         <f>VLOOKUP(B28,Lexique!A:F,5,)</f>
@@ -10803,13 +10797,13 @@
         <v>72</v>
       </c>
       <c r="C29" s="29" t="s">
-        <v>582</v>
+        <v>578</v>
       </c>
       <c r="D29" s="25" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="E29" s="25" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="F29" s="35" t="str">
         <f>VLOOKUP(B29,Lexique!A:F,5,)</f>
@@ -10828,13 +10822,13 @@
         <v>76</v>
       </c>
       <c r="C30" s="29" t="s">
-        <v>583</v>
+        <v>579</v>
       </c>
       <c r="D30" s="23" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="E30" s="23" t="s">
-        <v>593</v>
+        <v>589</v>
       </c>
       <c r="F30" s="35" t="str">
         <f>VLOOKUP(B30,Lexique!A:F,5,)</f>
@@ -10853,13 +10847,13 @@
         <v>73</v>
       </c>
       <c r="C31" s="29" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="D31" s="23" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="E31" s="23" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="F31" s="35" t="str">
         <f>VLOOKUP(B31,Lexique!A:F,5,)</f>
@@ -10878,13 +10872,13 @@
         <v>72</v>
       </c>
       <c r="C32" s="29" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="D32" s="63" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="E32" s="28" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="F32" s="35" t="str">
         <f>VLOOKUP(B32,Lexique!A:F,5,)</f>
@@ -10903,13 +10897,13 @@
         <v>73</v>
       </c>
       <c r="C33" s="29" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="D33" s="23" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="E33" s="23" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="F33" s="35" t="str">
         <f>VLOOKUP(B33,Lexique!A:F,5,)</f>
@@ -10928,13 +10922,13 @@
         <v>71</v>
       </c>
       <c r="C34" s="29" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="D34" s="23" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="E34" s="23" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="F34" s="35" t="str">
         <f>VLOOKUP(B34,Lexique!A:F,5,)</f>
@@ -10953,13 +10947,13 @@
         <v>73</v>
       </c>
       <c r="C35" s="29" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="D35" s="26" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="E35" s="26" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="F35" s="35" t="str">
         <f>VLOOKUP(B35,Lexique!A:F,5,)</f>
@@ -10978,13 +10972,13 @@
         <v>73</v>
       </c>
       <c r="C36" s="29" t="s">
-        <v>584</v>
+        <v>580</v>
       </c>
       <c r="D36" s="23" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="E36" s="23" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="F36" s="35" t="str">
         <f>VLOOKUP(B36,Lexique!A:F,5,)</f>
@@ -11003,13 +10997,13 @@
         <v>72</v>
       </c>
       <c r="C37" s="29" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="D37" s="23" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="E37" s="23" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="F37" s="35" t="str">
         <f>VLOOKUP(B37,Lexique!A:F,5,)</f>
@@ -11028,13 +11022,13 @@
         <v>73</v>
       </c>
       <c r="C38" s="29" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="D38" s="24" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="E38" s="24" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="F38" s="35" t="str">
         <f>VLOOKUP(B38,Lexique!A:F,5,)</f>
@@ -11053,13 +11047,13 @@
         <v>73</v>
       </c>
       <c r="C39" s="29" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="D39" s="23" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="E39" s="23" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="F39" s="35" t="str">
         <f>VLOOKUP(B39,Lexique!A:F,5,)</f>
@@ -11078,13 +11072,13 @@
         <v>70</v>
       </c>
       <c r="C40" s="29" t="s">
-        <v>585</v>
+        <v>581</v>
       </c>
       <c r="D40" s="23" t="s">
-        <v>604</v>
+        <v>600</v>
       </c>
       <c r="E40" s="23" t="s">
-        <v>605</v>
+        <v>601</v>
       </c>
       <c r="F40" s="35" t="str">
         <f>VLOOKUP(B40,Lexique!A:F,5,)</f>
@@ -11103,13 +11097,13 @@
         <v>80</v>
       </c>
       <c r="C41" s="34" t="s">
-        <v>586</v>
+        <v>582</v>
       </c>
       <c r="D41" s="23" t="s">
-        <v>587</v>
+        <v>583</v>
       </c>
       <c r="E41" s="23" t="s">
-        <v>592</v>
+        <v>588</v>
       </c>
       <c r="F41" s="35" t="str">
         <f>VLOOKUP(B41,Lexique!A:F,5,)</f>
@@ -11128,13 +11122,13 @@
         <v>110</v>
       </c>
       <c r="C42" s="34" t="s">
-        <v>559</v>
+        <v>555</v>
       </c>
       <c r="D42" s="63" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="E42" s="27" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="F42" s="35" t="str">
         <f>VLOOKUP(B42,Lexique!A:F,5,)</f>
@@ -11153,7 +11147,7 @@
         <v>43</v>
       </c>
       <c r="C43" s="34" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="D43" s="63" t="s">
         <v>166</v>
@@ -13139,7 +13133,7 @@
         <v>19</v>
       </c>
       <c r="C1" s="39" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="D1" s="40" t="s">
         <v>17</v>
@@ -13148,10 +13142,10 @@
         <v>18</v>
       </c>
       <c r="F1" s="45" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="G1" s="45" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="15" x14ac:dyDescent="0.15">
@@ -13163,10 +13157,10 @@
       </c>
       <c r="C2" s="29"/>
       <c r="D2" s="23" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="E2" s="23" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="F2" s="47" t="str">
         <f>VLOOKUP(B2,Lexique!A:F,5,)</f>
@@ -13185,10 +13179,10 @@
         <v>72</v>
       </c>
       <c r="C3" s="29" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="D3" s="23" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="E3" s="23" t="str">
         <f>D3</f>
@@ -13211,13 +13205,13 @@
         <v>75</v>
       </c>
       <c r="C4" s="29" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="D4" s="23" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="E4" s="23" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="F4" s="47" t="str">
         <f>VLOOKUP(B4,Lexique!A:F,5,)</f>
@@ -13236,10 +13230,10 @@
         <v>73</v>
       </c>
       <c r="C5" s="29" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="D5" s="23" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="E5" s="23" t="str">
         <f>D5</f>
@@ -13262,13 +13256,13 @@
         <v>74</v>
       </c>
       <c r="C6" s="29" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="D6" s="23" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="E6" s="23" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="F6" s="47" t="str">
         <f>VLOOKUP(B6,Lexique!A:F,5,)</f>
@@ -13287,10 +13281,10 @@
         <v>76</v>
       </c>
       <c r="C7" s="29" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="D7" s="23" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="E7" s="23" t="str">
         <f>D7</f>
@@ -13313,10 +13307,10 @@
         <v>73</v>
       </c>
       <c r="C8" s="29" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="D8" s="23" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="E8" s="23" t="str">
         <f t="shared" ref="E8:E17" si="0">D8</f>
@@ -13339,13 +13333,13 @@
         <v>73</v>
       </c>
       <c r="C9" s="29" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="D9" s="23" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="E9" s="23" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="F9" s="47" t="str">
         <f>VLOOKUP(B9,Lexique!A:F,5,)</f>
@@ -13364,13 +13358,13 @@
         <v>77</v>
       </c>
       <c r="C10" s="29" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="D10" s="23" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="E10" s="23" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="F10" s="47" t="str">
         <f>VLOOKUP(B10,Lexique!A:F,5,)</f>
@@ -13389,13 +13383,13 @@
         <v>72</v>
       </c>
       <c r="C11" s="29" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="D11" s="49" t="s">
+        <v>379</v>
+      </c>
+      <c r="E11" s="23" t="s">
         <v>381</v>
-      </c>
-      <c r="E11" s="23" t="s">
-        <v>383</v>
       </c>
       <c r="F11" s="47" t="str">
         <f>VLOOKUP(B11,Lexique!A:F,5,)</f>
@@ -13414,13 +13408,13 @@
         <v>72</v>
       </c>
       <c r="C12" s="29" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="D12" s="23" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="E12" s="23" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="F12" s="47" t="str">
         <f>VLOOKUP(B12,Lexique!A:F,5,)</f>
@@ -13439,10 +13433,10 @@
         <v>76</v>
       </c>
       <c r="C13" s="29" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="D13" s="23" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="E13" s="23" t="str">
         <f t="shared" si="0"/>
@@ -13465,10 +13459,10 @@
         <v>72</v>
       </c>
       <c r="C14" s="29" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="D14" s="23" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="E14" s="23" t="str">
         <f t="shared" si="0"/>
@@ -13491,13 +13485,13 @@
         <v>75</v>
       </c>
       <c r="C15" s="29" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="D15" s="23" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="E15" s="23" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="F15" s="47" t="str">
         <f>VLOOKUP(B15,Lexique!A:F,5,)</f>
@@ -13516,10 +13510,10 @@
         <v>73</v>
       </c>
       <c r="C16" s="29" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="D16" s="49" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="E16" s="23" t="str">
         <f t="shared" si="0"/>
@@ -13542,10 +13536,10 @@
         <v>72</v>
       </c>
       <c r="C17" s="29" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="D17" s="50" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="E17" s="23" t="str">
         <f t="shared" si="0"/>
@@ -13568,10 +13562,10 @@
         <v>43</v>
       </c>
       <c r="C18" s="29" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="D18" s="23" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="E18" s="23" t="s">
         <v>43</v>
@@ -15815,7 +15809,7 @@
         <v>19</v>
       </c>
       <c r="C1" s="39" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="D1" s="40" t="s">
         <v>17</v>
@@ -15824,10 +15818,10 @@
         <v>18</v>
       </c>
       <c r="F1" s="41" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="G1" s="41" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.2">
@@ -15839,10 +15833,10 @@
       </c>
       <c r="C2" s="29"/>
       <c r="D2" s="23" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="E2" s="23" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="F2" s="35" t="str">
         <f>VLOOKUP(B2,Lexique!A:F,5,)</f>
@@ -15861,10 +15855,10 @@
         <v>73</v>
       </c>
       <c r="C3" s="29" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="D3" s="23" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="E3" s="23" t="str">
         <f>D3</f>
@@ -15887,10 +15881,10 @@
         <v>73</v>
       </c>
       <c r="C4" s="29" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="D4" s="23" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="E4" s="23" t="str">
         <f>D4</f>
@@ -15913,13 +15907,13 @@
         <v>75</v>
       </c>
       <c r="C5" s="29" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="D5" s="23" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="E5" s="23" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="F5" s="35" t="str">
         <f>VLOOKUP(B5,Lexique!A:F,5,)</f>
@@ -15938,7 +15932,7 @@
         <v>25</v>
       </c>
       <c r="C6" s="29" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="D6" s="23" t="s">
         <v>22</v>
@@ -15963,13 +15957,13 @@
         <v>82</v>
       </c>
       <c r="C7" s="29" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="D7" s="23" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="E7" s="23" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="F7" s="35" t="str">
         <f>VLOOKUP(B7,Lexique!A:F,5,)</f>
@@ -15988,7 +15982,7 @@
         <v>79</v>
       </c>
       <c r="C8" s="29" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="D8" s="23" t="s">
         <v>10</v>
@@ -16013,7 +16007,7 @@
         <v>74</v>
       </c>
       <c r="C9" s="29" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="D9" s="28" t="s">
         <v>165</v>
@@ -16039,13 +16033,13 @@
         <v>81</v>
       </c>
       <c r="C10" s="29" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="D10" s="23" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="E10" s="23" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="F10" s="35" t="str">
         <f>VLOOKUP(B10,Lexique!A:F,5,)</f>
@@ -16064,13 +16058,13 @@
         <v>5</v>
       </c>
       <c r="C11" s="29" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D11" s="23" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="E11" s="23" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="F11" s="35" t="str">
         <f>VLOOKUP(B11,Lexique!A:F,5,)</f>
@@ -16089,7 +16083,7 @@
         <v>74</v>
       </c>
       <c r="C12" s="29" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="D12" s="28" t="s">
         <v>165</v>
@@ -16140,13 +16134,13 @@
         <v>73</v>
       </c>
       <c r="C14" s="29" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="D14" s="23" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="E14" s="23" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="F14" s="35" t="str">
         <f>VLOOKUP(B14,Lexique!A:F,5,)</f>
@@ -16165,13 +16159,13 @@
         <v>73</v>
       </c>
       <c r="C15" s="29" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="D15" s="23" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="E15" s="24" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="F15" s="35" t="str">
         <f>VLOOKUP(B15,Lexique!A:F,5,)</f>
@@ -16190,7 +16184,7 @@
         <v>72</v>
       </c>
       <c r="C16" s="29" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="D16" s="24" t="s">
         <v>165</v>
@@ -16215,13 +16209,13 @@
         <v>5</v>
       </c>
       <c r="C17" s="29" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D17" s="23" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="E17" s="25" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="F17" s="35" t="str">
         <f>VLOOKUP(B17,Lexique!A:F,5,)</f>
@@ -16240,7 +16234,7 @@
         <v>75</v>
       </c>
       <c r="C18" s="29" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="D18" s="28" t="s">
         <v>165</v>
@@ -16266,13 +16260,13 @@
         <v>81</v>
       </c>
       <c r="C19" s="29" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="D19" s="23" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="E19" s="25" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="F19" s="35" t="str">
         <f>VLOOKUP(B19,Lexique!A:F,5,)</f>
@@ -16316,13 +16310,13 @@
         <v>82</v>
       </c>
       <c r="C21" s="29" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="D21" s="23" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="E21" s="23" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="F21" s="35" t="str">
         <f>VLOOKUP(B21,Lexique!A:F,5,)</f>
@@ -16341,7 +16335,7 @@
         <v>25</v>
       </c>
       <c r="C22" s="29" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="D22" s="23" t="s">
         <v>22</v>
@@ -16366,13 +16360,13 @@
         <v>75</v>
       </c>
       <c r="C23" s="29" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="D23" s="23" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="E23" s="23" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="F23" s="35" t="str">
         <f>VLOOKUP(B23,Lexique!A:F,5,)</f>
@@ -16391,13 +16385,13 @@
         <v>72</v>
       </c>
       <c r="C24" s="29" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="D24" s="28" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="E24" s="28" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="F24" s="35" t="str">
         <f>VLOOKUP(B24,Lexique!A:F,5,)</f>
@@ -16416,13 +16410,13 @@
         <v>110</v>
       </c>
       <c r="C25" s="29" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="D25" s="23" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="E25" s="23" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="F25" s="35" t="str">
         <f>VLOOKUP(B25,Lexique!A:F,5,)</f>
@@ -16441,10 +16435,10 @@
         <v>73</v>
       </c>
       <c r="C26" s="29" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="D26" s="23" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="E26" s="23" t="str">
         <f>D26</f>
@@ -16467,7 +16461,7 @@
         <v>43</v>
       </c>
       <c r="C27" s="29" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="D27" s="23" t="s">
         <v>166</v>
@@ -18595,10 +18589,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA4CF35A-AE95-4D4B-80F8-FB6E5D8CEEB2}">
-  <dimension ref="A1:I48"/>
+  <dimension ref="A1:I47"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
@@ -18620,7 +18614,7 @@
         <v>19</v>
       </c>
       <c r="C1" s="39" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="D1" s="39" t="s">
         <v>17</v>
@@ -18629,10 +18623,10 @@
         <v>18</v>
       </c>
       <c r="F1" s="41" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="G1" s="41" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="15" x14ac:dyDescent="0.2">
@@ -18644,10 +18638,10 @@
       </c>
       <c r="C2" s="29"/>
       <c r="D2" s="23" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="E2" s="23" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="F2" s="35" t="str">
         <f>VLOOKUP(B2,Lexique!A:F,5,)</f>
@@ -18668,10 +18662,10 @@
       </c>
       <c r="C3" s="29"/>
       <c r="D3" s="23" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="E3" s="23" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="F3" s="35" t="str">
         <f>VLOOKUP(B3,Lexique!A:F,5,)</f>
@@ -18762,7 +18756,7 @@
       </c>
       <c r="C7" s="29"/>
       <c r="D7" s="23" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="E7" s="23" t="str">
         <f>D7</f>
@@ -18852,103 +18846,103 @@
     </row>
     <row r="11" spans="1:9" ht="30" x14ac:dyDescent="0.2">
       <c r="A11" s="30">
-        <v>56.5</v>
+        <v>67.3</v>
       </c>
       <c r="B11" s="29" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="C11" s="29"/>
       <c r="D11" s="23" t="s">
-        <v>175</v>
+        <v>194</v>
       </c>
       <c r="E11" s="23" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="F11" s="35" t="str">
         <f>VLOOKUP(B11,Lexique!A:F,5,)</f>
-        <v>Sprint du maire Ville $250&lt;br/&gt; Lieu précis Ville</v>
+        <v>Sprint bonification temps et points&lt;br/&gt; Lieu précis Ville</v>
       </c>
       <c r="G11" s="35" t="str">
         <f>VLOOKUP(B11,Lexique!A:F,6,)</f>
-        <v>Ville Mayor's sprint $250&lt;br/&gt; Lieu précis Ville</v>
+        <v>Bonification Sprint - times and points&lt;br/&gt; Lieu précis Ville</v>
       </c>
       <c r="I11" s="6"/>
     </row>
-    <row r="12" spans="1:9" ht="30" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A12" s="30">
-        <v>67.3</v>
+        <v>71</v>
       </c>
       <c r="B12" s="29" t="s">
-        <v>70</v>
+        <v>152</v>
       </c>
       <c r="C12" s="29"/>
       <c r="D12" s="23" t="s">
-        <v>196</v>
+        <v>182</v>
       </c>
       <c r="E12" s="23" t="s">
-        <v>172</v>
+        <v>181</v>
       </c>
       <c r="F12" s="35" t="str">
         <f>VLOOKUP(B12,Lexique!A:F,5,)</f>
-        <v>Sprint bonification temps et points&lt;br/&gt; Lieu précis Ville</v>
+        <v>Zone déchets (sur xxx m)</v>
       </c>
       <c r="G12" s="35" t="str">
         <f>VLOOKUP(B12,Lexique!A:F,6,)</f>
-        <v>Bonification Sprint - times and points&lt;br/&gt; Lieu précis Ville</v>
+        <v>Trash zone (on xxx m)</v>
       </c>
       <c r="I12" s="6"/>
     </row>
     <row r="13" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A13" s="30">
-        <v>71</v>
+        <v>72.3</v>
       </c>
       <c r="B13" s="29" t="s">
-        <v>152</v>
+        <v>82</v>
       </c>
       <c r="C13" s="29"/>
       <c r="D13" s="23" t="s">
-        <v>184</v>
+        <v>201</v>
       </c>
       <c r="E13" s="23" t="s">
-        <v>183</v>
+        <v>202</v>
       </c>
       <c r="F13" s="35" t="str">
         <f>VLOOKUP(B13,Lexique!A:F,5,)</f>
-        <v>Zone déchets (sur xxx m)</v>
+        <v>Carrefour giratoire, Xe sortie tout droit/droite/gauche&lt;br/&gt;rue</v>
       </c>
       <c r="G13" s="35" t="str">
         <f>VLOOKUP(B13,Lexique!A:F,6,)</f>
-        <v>Trash zone (on xxx m)</v>
+        <v>Round about Xnd exit straight ahead/right/left&lt;br&gt; rue</v>
       </c>
       <c r="I13" s="6"/>
     </row>
     <row r="14" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A14" s="30">
-        <v>72.3</v>
+        <v>72.8</v>
       </c>
       <c r="B14" s="29" t="s">
-        <v>82</v>
+        <v>25</v>
       </c>
       <c r="C14" s="29"/>
       <c r="D14" s="23" t="s">
-        <v>203</v>
+        <v>22</v>
       </c>
       <c r="E14" s="23" t="s">
-        <v>204</v>
+        <v>173</v>
       </c>
       <c r="F14" s="35" t="str">
         <f>VLOOKUP(B14,Lexique!A:F,5,)</f>
-        <v>Carrefour giratoire, Xe sortie tout droit/droite/gauche&lt;br/&gt;rue</v>
+        <v>Voie ferrée oblique / Pont de bois</v>
       </c>
       <c r="G14" s="35" t="str">
         <f>VLOOKUP(B14,Lexique!A:F,6,)</f>
-        <v>Round about Xnd exit straight ahead/right/left&lt;br&gt; rue</v>
+        <v>Oblique railroad crossing / Wooden bridge</v>
       </c>
       <c r="I14" s="6"/>
     </row>
     <row r="15" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A15" s="30">
-        <v>72.8</v>
+        <v>73.900000000000006</v>
       </c>
       <c r="B15" s="29" t="s">
         <v>25</v>
@@ -18972,210 +18966,211 @@
     </row>
     <row r="16" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A16" s="30">
-        <v>73.900000000000006</v>
+        <v>74.8</v>
       </c>
       <c r="B16" s="29" t="s">
-        <v>25</v>
+        <v>82</v>
       </c>
       <c r="C16" s="29"/>
       <c r="D16" s="23" t="s">
-        <v>22</v>
+        <v>201</v>
       </c>
       <c r="E16" s="23" t="s">
-        <v>173</v>
+        <v>202</v>
       </c>
       <c r="F16" s="35" t="str">
         <f>VLOOKUP(B16,Lexique!A:F,5,)</f>
-        <v>Voie ferrée oblique / Pont de bois</v>
+        <v>Carrefour giratoire, Xe sortie tout droit/droite/gauche&lt;br/&gt;rue</v>
       </c>
       <c r="G16" s="35" t="str">
         <f>VLOOKUP(B16,Lexique!A:F,6,)</f>
-        <v>Oblique railroad crossing / Wooden bridge</v>
+        <v>Round about Xnd exit straight ahead/right/left&lt;br&gt; rue</v>
       </c>
       <c r="I16" s="6"/>
     </row>
     <row r="17" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A17" s="30">
-        <v>74.8</v>
+        <v>96.1</v>
       </c>
       <c r="B17" s="29" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
       <c r="C17" s="29"/>
       <c r="D17" s="23" t="s">
-        <v>203</v>
+        <v>183</v>
       </c>
       <c r="E17" s="23" t="s">
-        <v>204</v>
+        <v>184</v>
       </c>
       <c r="F17" s="35" t="str">
         <f>VLOOKUP(B17,Lexique!A:F,5,)</f>
-        <v>Carrefour giratoire, Xe sortie tout droit/droite/gauche&lt;br/&gt;rue</v>
+        <v>Points GPM&lt;br/&gt; Lieu précis Ville</v>
       </c>
       <c r="G17" s="35" t="str">
         <f>VLOOKUP(B17,Lexique!A:F,6,)</f>
-        <v>Round about Xnd exit straight ahead/right/left&lt;br&gt; rue</v>
+        <v>KOM Points&lt;br/&gt; Lieu précis Ville</v>
       </c>
       <c r="I17" s="6"/>
     </row>
     <row r="18" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A18" s="30">
-        <v>96.1</v>
+        <v>103.3</v>
       </c>
       <c r="B18" s="29" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C18" s="29"/>
       <c r="D18" s="23" t="s">
-        <v>185</v>
-      </c>
-      <c r="E18" s="23" t="s">
-        <v>186</v>
+        <v>195</v>
+      </c>
+      <c r="E18" s="23" t="str">
+        <f>D18</f>
+        <v>Route 113</v>
       </c>
       <c r="F18" s="35" t="str">
         <f>VLOOKUP(B18,Lexique!A:F,5,)</f>
-        <v>Points GPM&lt;br/&gt; Lieu précis Ville</v>
+        <v>Nom route / rue</v>
       </c>
       <c r="G18" s="35" t="str">
         <f>VLOOKUP(B18,Lexique!A:F,6,)</f>
-        <v>KOM Points&lt;br/&gt; Lieu précis Ville</v>
+        <v>Nom route / rue</v>
       </c>
       <c r="I18" s="6"/>
     </row>
     <row r="19" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A19" s="30">
-        <v>103.3</v>
+        <v>116.6</v>
       </c>
       <c r="B19" s="29" t="s">
-        <v>73</v>
+        <v>5</v>
       </c>
       <c r="C19" s="29"/>
       <c r="D19" s="23" t="s">
-        <v>197</v>
-      </c>
-      <c r="E19" s="23" t="str">
-        <f>D19</f>
-        <v>Route 113</v>
+        <v>174</v>
+      </c>
+      <c r="E19" s="23" t="s">
+        <v>174</v>
       </c>
       <c r="F19" s="35" t="str">
         <f>VLOOKUP(B19,Lexique!A:F,5,)</f>
-        <v>Nom route / rue</v>
+        <v>Ville</v>
       </c>
       <c r="G19" s="35" t="str">
         <f>VLOOKUP(B19,Lexique!A:F,6,)</f>
-        <v>Nom route / rue</v>
+        <v>Ville</v>
       </c>
       <c r="I19" s="6"/>
     </row>
-    <row r="20" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" ht="30" x14ac:dyDescent="0.2">
       <c r="A20" s="30">
-        <v>116.6</v>
+        <v>117</v>
       </c>
       <c r="B20" s="29" t="s">
-        <v>5</v>
+        <v>81</v>
       </c>
       <c r="C20" s="29"/>
       <c r="D20" s="23" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="E20" s="23" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="F20" s="35" t="str">
         <f>VLOOKUP(B20,Lexique!A:F,5,)</f>
-        <v>Ville</v>
+        <v>Sprint du maire Ville $250&lt;br/&gt; Lieu précis Ville</v>
       </c>
       <c r="G20" s="35" t="str">
         <f>VLOOKUP(B20,Lexique!A:F,6,)</f>
-        <v>Ville</v>
+        <v>Ville Mayor's sprint $250&lt;br/&gt; Lieu précis Ville</v>
       </c>
       <c r="I20" s="6"/>
     </row>
-    <row r="21" spans="1:9" ht="30" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A21" s="30">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="B21" s="29" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C21" s="29"/>
       <c r="D21" s="23" t="s">
-        <v>178</v>
+        <v>154</v>
       </c>
       <c r="E21" s="23" t="s">
-        <v>177</v>
+        <v>153</v>
       </c>
       <c r="F21" s="35" t="str">
         <f>VLOOKUP(B21,Lexique!A:F,5,)</f>
-        <v>Sprint du maire Ville $250&lt;br/&gt; Lieu précis Ville</v>
+        <v>Début du ravitaillement / Fin du ravitaillement</v>
       </c>
       <c r="G21" s="35" t="str">
         <f>VLOOKUP(B21,Lexique!A:F,6,)</f>
-        <v>Ville Mayor's sprint $250&lt;br/&gt; Lieu précis Ville</v>
+        <v>Feed open / Feed closed</v>
       </c>
       <c r="I21" s="6"/>
     </row>
     <row r="22" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A22" s="30">
-        <v>125</v>
+        <v>139</v>
       </c>
       <c r="B22" s="29" t="s">
-        <v>78</v>
+        <v>5</v>
       </c>
       <c r="C22" s="29"/>
       <c r="D22" s="23" t="s">
-        <v>154</v>
+        <v>131</v>
       </c>
       <c r="E22" s="23" t="s">
-        <v>153</v>
+        <v>131</v>
       </c>
       <c r="F22" s="35" t="str">
         <f>VLOOKUP(B22,Lexique!A:F,5,)</f>
-        <v>Début du ravitaillement / Fin du ravitaillement</v>
+        <v>Ville</v>
       </c>
       <c r="G22" s="35" t="str">
         <f>VLOOKUP(B22,Lexique!A:F,6,)</f>
-        <v>Feed open / Feed closed</v>
+        <v>Ville</v>
       </c>
       <c r="I22" s="6"/>
     </row>
     <row r="23" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A23" s="30">
-        <v>139</v>
+        <v>139.30000000000001</v>
       </c>
       <c r="B23" s="29" t="s">
-        <v>5</v>
+        <v>74</v>
       </c>
       <c r="C23" s="29"/>
       <c r="D23" s="23" t="s">
-        <v>131</v>
+        <v>203</v>
       </c>
       <c r="E23" s="23" t="s">
-        <v>131</v>
+        <v>204</v>
       </c>
       <c r="F23" s="35" t="str">
         <f>VLOOKUP(B23,Lexique!A:F,5,)</f>
-        <v>Ville</v>
+        <v>Nom route / rue</v>
       </c>
       <c r="G23" s="35" t="str">
         <f>VLOOKUP(B23,Lexique!A:F,6,)</f>
-        <v>Ville</v>
+        <v>Nom route / rue</v>
       </c>
       <c r="I23" s="6"/>
     </row>
     <row r="24" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A24" s="30">
-        <v>139.30000000000001</v>
+        <v>139.80000000000001</v>
       </c>
       <c r="B24" s="29" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C24" s="29"/>
       <c r="D24" s="23" t="s">
-        <v>205</v>
-      </c>
-      <c r="E24" s="23" t="s">
-        <v>206</v>
+        <v>196</v>
+      </c>
+      <c r="E24" s="23" t="str">
+        <f>D24</f>
+        <v>10e Avenue/ Route 386</v>
       </c>
       <c r="F24" s="35" t="str">
         <f>VLOOKUP(B24,Lexique!A:F,5,)</f>
@@ -19189,18 +19184,17 @@
     </row>
     <row r="25" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A25" s="30">
-        <v>139.80000000000001</v>
+        <v>140.5</v>
       </c>
       <c r="B25" s="29" t="s">
         <v>72</v>
       </c>
       <c r="C25" s="29"/>
       <c r="D25" s="23" t="s">
-        <v>198</v>
-      </c>
-      <c r="E25" s="23" t="str">
-        <f>D25</f>
-        <v>10e Avenue/ Route 386</v>
+        <v>177</v>
+      </c>
+      <c r="E25" s="23" t="s">
+        <v>177</v>
       </c>
       <c r="F25" s="35" t="str">
         <f>VLOOKUP(B25,Lexique!A:F,5,)</f>
@@ -19214,17 +19208,17 @@
     </row>
     <row r="26" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A26" s="30">
-        <v>140.5</v>
+        <v>142.1</v>
       </c>
       <c r="B26" s="29" t="s">
         <v>72</v>
       </c>
       <c r="C26" s="29"/>
       <c r="D26" s="23" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E26" s="23" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="F26" s="35" t="str">
         <f>VLOOKUP(B26,Lexique!A:F,5,)</f>
@@ -19238,17 +19232,17 @@
     </row>
     <row r="27" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A27" s="30">
-        <v>142.1</v>
+        <v>143.80000000000001</v>
       </c>
       <c r="B27" s="29" t="s">
         <v>72</v>
       </c>
       <c r="C27" s="29"/>
       <c r="D27" s="23" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E27" s="23" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="F27" s="35" t="str">
         <f>VLOOKUP(B27,Lexique!A:F,5,)</f>
@@ -19260,100 +19254,86 @@
       </c>
       <c r="I27" s="6"/>
     </row>
-    <row r="28" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9" ht="30" x14ac:dyDescent="0.2">
       <c r="A28" s="30">
-        <v>143.80000000000001</v>
+        <v>144.6</v>
       </c>
       <c r="B28" s="29" t="s">
-        <v>72</v>
+        <v>110</v>
       </c>
       <c r="C28" s="29"/>
       <c r="D28" s="23" t="s">
-        <v>181</v>
+        <v>197</v>
       </c>
       <c r="E28" s="23" t="s">
-        <v>181</v>
+        <v>198</v>
       </c>
       <c r="F28" s="35" t="str">
         <f>VLOOKUP(B28,Lexique!A:F,5,)</f>
-        <v>Nom route / rue</v>
+        <v>Déviation de la caravance&lt;br/&gt; À droite/gauche sur rue</v>
       </c>
       <c r="G28" s="35" t="str">
         <f>VLOOKUP(B28,Lexique!A:F,6,)</f>
-        <v>Nom route / rue</v>
+        <v>Caravan bypass&lt;br/&gt;Right/left on rue</v>
       </c>
       <c r="I28" s="6"/>
     </row>
-    <row r="29" spans="1:9" ht="30" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A29" s="30">
-        <v>144.6</v>
+        <v>144.9</v>
       </c>
       <c r="B29" s="29" t="s">
-        <v>110</v>
+        <v>75</v>
       </c>
       <c r="C29" s="29"/>
       <c r="D29" s="23" t="s">
-        <v>199</v>
+        <v>180</v>
       </c>
       <c r="E29" s="23" t="s">
-        <v>200</v>
+        <v>180</v>
       </c>
       <c r="F29" s="35" t="str">
         <f>VLOOKUP(B29,Lexique!A:F,5,)</f>
-        <v>Déviation de la caravance&lt;br/&gt; À droite/gauche sur rue</v>
+        <v>Nom route / rue</v>
       </c>
       <c r="G29" s="35" t="str">
         <f>VLOOKUP(B29,Lexique!A:F,6,)</f>
-        <v>Caravan bypass&lt;br/&gt;Right/left on rue</v>
+        <v>Nom route / rue</v>
       </c>
       <c r="I29" s="6"/>
     </row>
-    <row r="30" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:9" ht="30" x14ac:dyDescent="0.2">
       <c r="A30" s="30">
-        <v>144.9</v>
+        <v>145</v>
       </c>
       <c r="B30" s="29" t="s">
-        <v>75</v>
+        <v>43</v>
       </c>
       <c r="C30" s="29"/>
       <c r="D30" s="23" t="s">
-        <v>182</v>
+        <v>189</v>
       </c>
       <c r="E30" s="23" t="s">
-        <v>182</v>
+        <v>190</v>
       </c>
       <c r="F30" s="35" t="str">
         <f>VLOOKUP(B30,Lexique!A:F,5,)</f>
-        <v>Nom route / rue</v>
+        <v>Arrivée&lt;br/&gt;Bonification en temps et points</v>
       </c>
       <c r="G30" s="35" t="str">
         <f>VLOOKUP(B30,Lexique!A:F,6,)</f>
-        <v>Nom route / rue</v>
+        <v>Finish&lt;br/&gt;Time and points bonus</v>
       </c>
       <c r="I30" s="6"/>
     </row>
-    <row r="31" spans="1:9" ht="30" x14ac:dyDescent="0.2">
-      <c r="A31" s="30">
-        <v>145</v>
-      </c>
-      <c r="B31" s="29" t="s">
-        <v>43</v>
-      </c>
+    <row r="31" spans="1:9" ht="14" x14ac:dyDescent="0.2">
+      <c r="A31" s="30"/>
+      <c r="B31" s="29"/>
       <c r="C31" s="29"/>
-      <c r="D31" s="23" t="s">
-        <v>191</v>
-      </c>
-      <c r="E31" s="23" t="s">
-        <v>192</v>
-      </c>
-      <c r="F31" s="35" t="str">
-        <f>VLOOKUP(B31,Lexique!A:F,5,)</f>
-        <v>Arrivée&lt;br/&gt;Bonification en temps et points</v>
-      </c>
-      <c r="G31" s="35" t="str">
-        <f>VLOOKUP(B31,Lexique!A:F,6,)</f>
-        <v>Finish&lt;br/&gt;Time and points bonus</v>
-      </c>
+      <c r="D31" s="23"/>
+      <c r="E31" s="23"/>
+      <c r="F31" s="35"/>
+      <c r="G31" s="35"/>
       <c r="I31" s="6"/>
     </row>
     <row r="32" spans="1:9" ht="14" x14ac:dyDescent="0.2">
@@ -19446,17 +19426,16 @@
       <c r="G40" s="35"/>
       <c r="I40" s="6"/>
     </row>
-    <row r="41" spans="1:9" ht="14" x14ac:dyDescent="0.2">
-      <c r="A41" s="30"/>
-      <c r="B41" s="29"/>
-      <c r="C41" s="29"/>
+    <row r="41" spans="1:9" ht="47.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="36"/>
+      <c r="B41" s="31"/>
+      <c r="C41" s="32"/>
       <c r="D41" s="23"/>
       <c r="E41" s="23"/>
       <c r="F41" s="35"/>
       <c r="G41" s="35"/>
-      <c r="I41" s="6"/>
-    </row>
-    <row r="42" spans="1:9" ht="47.25" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="42" spans="1:9" ht="14" x14ac:dyDescent="0.2">
       <c r="A42" s="36"/>
       <c r="B42" s="31"/>
       <c r="C42" s="32"/>
@@ -19496,8 +19475,6 @@
       <c r="A46" s="36"/>
       <c r="B46" s="31"/>
       <c r="C46" s="32"/>
-      <c r="D46" s="23"/>
-      <c r="E46" s="23"/>
       <c r="F46" s="35"/>
       <c r="G46" s="35"/>
     </row>
@@ -19507,13 +19484,6 @@
       <c r="C47" s="32"/>
       <c r="F47" s="35"/>
       <c r="G47" s="35"/>
-    </row>
-    <row r="48" spans="1:9" ht="14" x14ac:dyDescent="0.2">
-      <c r="A48" s="36"/>
-      <c r="B48" s="31"/>
-      <c r="C48" s="32"/>
-      <c r="F48" s="35"/>
-      <c r="G48" s="35"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -19549,7 +19519,7 @@
         <v>19</v>
       </c>
       <c r="C1" s="39" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="D1" s="40" t="s">
         <v>17</v>
@@ -19558,10 +19528,10 @@
         <v>18</v>
       </c>
       <c r="F1" s="41" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="G1" s="41" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="15" x14ac:dyDescent="0.2">
@@ -19572,13 +19542,13 @@
         <v>79</v>
       </c>
       <c r="C2" s="29" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="D2" s="23" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="E2" s="23" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="F2" s="35" t="str">
         <f>VLOOKUP(B2,Lexique!A:F,5,)</f>
@@ -19597,10 +19567,10 @@
         <v>73</v>
       </c>
       <c r="C3" s="29" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="D3" s="23" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="E3" s="23" t="str">
         <f>D3</f>
@@ -19623,10 +19593,10 @@
         <v>72</v>
       </c>
       <c r="C4" s="29" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="D4" s="23" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="E4" s="23" t="str">
         <f>D4</f>
@@ -19649,10 +19619,10 @@
         <v>73</v>
       </c>
       <c r="C5" s="29" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="D5" s="23" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="E5" s="23" t="str">
         <f>D5</f>
@@ -19675,10 +19645,10 @@
         <v>72</v>
       </c>
       <c r="C6" s="29" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="D6" s="23" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="E6" s="23" t="str">
         <f>D6</f>
@@ -19701,13 +19671,13 @@
         <v>74</v>
       </c>
       <c r="C7" s="29" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="D7" s="23" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="E7" s="23" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="F7" s="35" t="str">
         <f>VLOOKUP(B7,Lexique!A:F,5,)</f>
@@ -19726,10 +19696,10 @@
         <v>74</v>
       </c>
       <c r="C8" s="29" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="D8" s="23" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="E8" s="23" t="str">
         <f>D8</f>
@@ -19752,13 +19722,13 @@
         <v>72</v>
       </c>
       <c r="C9" s="29" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="D9" s="23" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="E9" s="23" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="F9" s="35" t="str">
         <f>VLOOKUP(B9,Lexique!A:F,5,)</f>
@@ -19777,10 +19747,10 @@
         <v>73</v>
       </c>
       <c r="C10" s="29" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="D10" s="23" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="E10" s="24" t="str">
         <f>D10</f>
@@ -19803,10 +19773,10 @@
         <v>73</v>
       </c>
       <c r="C11" s="29" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="D11" s="24" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="E11" s="24" t="str">
         <f>D11</f>
@@ -19829,10 +19799,10 @@
         <v>73</v>
       </c>
       <c r="C12" s="29" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="D12" s="23" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="E12" s="25" t="str">
         <f>D12</f>
@@ -19855,10 +19825,10 @@
         <v>72</v>
       </c>
       <c r="C13" s="29" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="D13" s="23" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="E13" s="25" t="str">
         <f t="shared" ref="E13:E17" si="0">D13</f>
@@ -19881,10 +19851,10 @@
         <v>73</v>
       </c>
       <c r="C14" s="29" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="D14" s="25" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="E14" s="25" t="str">
         <f t="shared" si="0"/>
@@ -19907,10 +19877,10 @@
         <v>72</v>
       </c>
       <c r="C15" s="29" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="D15" s="23" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="E15" s="25" t="str">
         <f t="shared" si="0"/>
@@ -19933,10 +19903,10 @@
         <v>73</v>
       </c>
       <c r="C16" s="29" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="D16" s="24" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="E16" s="25" t="str">
         <f t="shared" si="0"/>
@@ -19959,10 +19929,10 @@
         <v>73</v>
       </c>
       <c r="C17" s="29" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="D17" s="43" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="E17" s="25" t="str">
         <f t="shared" si="0"/>
@@ -19985,13 +19955,13 @@
         <v>76</v>
       </c>
       <c r="C18" s="29" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="D18" s="23" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="E18" s="23" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="F18" s="35" t="str">
         <f>VLOOKUP(B18,Lexique!A:F,5,)</f>
@@ -20011,13 +19981,13 @@
         <v>76</v>
       </c>
       <c r="C19" s="29" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="D19" s="23" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="E19" s="23" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="F19" s="35" t="str">
         <f>VLOOKUP(B19,Lexique!A:F,5,)</f>
@@ -20037,13 +20007,13 @@
         <v>71</v>
       </c>
       <c r="C20" s="29" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="D20" s="25" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="E20" s="25" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="F20" s="35" t="str">
         <f>VLOOKUP(B20,Lexique!A:F,5,)</f>
@@ -20063,13 +20033,13 @@
         <v>76</v>
       </c>
       <c r="C21" s="29" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="D21" s="23" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="E21" s="23" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="F21" s="35" t="str">
         <f>VLOOKUP(B21,Lexique!A:F,5,)</f>
@@ -20089,7 +20059,7 @@
         <v>78</v>
       </c>
       <c r="C22" s="29" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="D22" s="23" t="s">
         <v>155</v>
@@ -20115,13 +20085,13 @@
         <v>70</v>
       </c>
       <c r="C23" s="29" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="D23" s="23" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="E23" s="23" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="F23" s="35" t="str">
         <f>VLOOKUP(B23,Lexique!A:F,5,)</f>
@@ -20141,13 +20111,13 @@
         <v>76</v>
       </c>
       <c r="C24" s="29" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="D24" s="23" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="E24" s="23" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="F24" s="35" t="str">
         <f>VLOOKUP(B24,Lexique!A:F,5,)</f>
@@ -20167,13 +20137,13 @@
         <v>71</v>
       </c>
       <c r="C25" s="29" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="D25" s="25" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="E25" s="25" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="F25" s="35" t="str">
         <f>VLOOKUP(B25,Lexique!A:F,5,)</f>
@@ -20193,13 +20163,13 @@
         <v>81</v>
       </c>
       <c r="C26" s="29" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="D26" s="23" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="E26" s="23" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="F26" s="35" t="str">
         <f>VLOOKUP(B26,Lexique!A:F,5,)</f>
@@ -20219,13 +20189,13 @@
         <v>76</v>
       </c>
       <c r="C27" s="29" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="D27" s="23" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="E27" s="23" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="F27" s="35" t="str">
         <f>VLOOKUP(B27,Lexique!A:F,5,)</f>
@@ -20245,13 +20215,13 @@
         <v>76</v>
       </c>
       <c r="C28" s="29" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="D28" s="23" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="E28" s="23" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="F28" s="35" t="str">
         <f>VLOOKUP(B28,Lexique!A:F,5,)</f>
@@ -20271,13 +20241,13 @@
         <v>71</v>
       </c>
       <c r="C29" s="29" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="D29" s="25" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="E29" s="25" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="F29" s="35" t="str">
         <f>VLOOKUP(B29,Lexique!A:F,5,)</f>
@@ -20297,13 +20267,13 @@
         <v>70</v>
       </c>
       <c r="C30" s="29" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="D30" s="23" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="E30" s="23" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="F30" s="35" t="str">
         <f>VLOOKUP(B30,Lexique!A:F,5,)</f>
@@ -20323,13 +20293,13 @@
         <v>81</v>
       </c>
       <c r="C31" s="29" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="D31" s="23" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="E31" s="23" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="F31" s="35" t="str">
         <f>VLOOKUP(B31,Lexique!A:F,5,)</f>
@@ -20349,7 +20319,7 @@
         <v>78</v>
       </c>
       <c r="C32" s="29" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="D32" s="23" t="s">
         <v>154</v>
@@ -20375,13 +20345,13 @@
         <v>80</v>
       </c>
       <c r="C33" s="29" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="D33" s="23" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="E33" s="23" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="F33" s="35" t="str">
         <f>VLOOKUP(B33,Lexique!A:F,5,)</f>
@@ -20402,10 +20372,10 @@
       </c>
       <c r="C34" s="29"/>
       <c r="D34" s="26" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="E34" s="26" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="F34" s="35" t="str">
         <f>VLOOKUP(B34,Lexique!A:F,5,)</f>
@@ -20425,7 +20395,7 @@
         <v>43</v>
       </c>
       <c r="C35" s="29" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="D35" s="26" t="s">
         <v>109</v>

</xml_diff>

<commit_message>
Modif commanditaires étapes dans logos et itineraires
</commit_message>
<xml_diff>
--- a/excel/Itineraires.xlsx
+++ b/excel/Itineraires.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brunogauthier/Documents/guide2024/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40EA46D0-6D35-AC4E-A8A0-63FDFB8E15BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C5E5B5D-A855-4046-89D9-1430DFD58F99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28760" yWindow="2220" windowWidth="38160" windowHeight="19860" tabRatio="758" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="35240" yWindow="3120" windowWidth="38160" windowHeight="19860" tabRatio="758" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="23" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1196" uniqueCount="613">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1196" uniqueCount="619">
   <si>
     <t>GPM</t>
   </si>
@@ -1881,6 +1881,24 @@
   </si>
   <si>
     <t>Start of 2nd lap (9 laps to go)</t>
+  </si>
+  <si>
+    <t>Desjardins</t>
+  </si>
+  <si>
+    <t>Gouvernement du Québec</t>
+  </si>
+  <si>
+    <t>Eldorado Gold</t>
+  </si>
+  <si>
+    <t>Agnico Eagle</t>
+  </si>
+  <si>
+    <t>CMAC Thyssen</t>
+  </si>
+  <si>
+    <t>Sûreté du Québec</t>
   </si>
 </sst>
 </file>
@@ -6538,8 +6556,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF8C653E-9E00-4EDF-9978-201805372337}">
   <dimension ref="A1:AM14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Z1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="AF12" sqref="AF12"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -6715,7 +6733,7 @@
         <v>44027</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>85</v>
+        <v>613</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>208</v>
@@ -6842,7 +6860,7 @@
         <v>44028</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>85</v>
+        <v>614</v>
       </c>
       <c r="F3" s="4" t="s">
         <v>209</v>
@@ -6969,7 +6987,7 @@
         <v>44029</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>85</v>
+        <v>615</v>
       </c>
       <c r="F4" s="4" t="s">
         <v>207</v>
@@ -7101,7 +7119,7 @@
         <v>44029</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>85</v>
+        <v>616</v>
       </c>
       <c r="F5" s="4" t="s">
         <v>232</v>
@@ -7229,7 +7247,7 @@
         <v>44030</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>85</v>
+        <v>617</v>
       </c>
       <c r="F6" s="4" t="s">
         <v>230</v>
@@ -7355,7 +7373,7 @@
         <v>44031</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>85</v>
+        <v>278</v>
       </c>
       <c r="F7" s="19" t="s">
         <v>210</v>
@@ -7481,7 +7499,7 @@
         <v>44032</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>85</v>
+        <v>618</v>
       </c>
       <c r="F8" s="4" t="s">
         <v>211</v>

</xml_diff>

<commit_message>
Premier test guide signalisation
</commit_message>
<xml_diff>
--- a/excel/Itineraires.xlsx
+++ b/excel/Itineraires.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10609"/>
   <workbookPr date1904="1" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brunogauthier/Documents/guide2024/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C5E5B5D-A855-4046-89D9-1430DFD58F99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DB74E8C-F022-3748-A47D-02CFA3F6181B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="35240" yWindow="3120" windowWidth="38160" windowHeight="19860" tabRatio="758" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" tabRatio="758" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="23" r:id="rId1"/>
@@ -1049,9 +1049,6 @@
     <t>7e rue</t>
   </si>
   <si>
-    <t>Entrée sur le circuit d’arrivée&lt;br/&gt;1er avenue</t>
-  </si>
-  <si>
     <t>Circuit finish entrance&lt;br/&gt;1ere avenue</t>
   </si>
   <si>
@@ -1899,6 +1896,9 @@
   </si>
   <si>
     <t>Sûreté du Québec</t>
+  </si>
+  <si>
+    <t>Entrée sur le circuit d’arrivée &lt;br/&gt;1er avenue</t>
   </si>
 </sst>
 </file>
@@ -3056,22 +3056,22 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A7" s="4" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A8" s="4" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A9" s="4" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A10" s="4" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
   </sheetData>
@@ -3134,10 +3134,10 @@
         <v>264</v>
       </c>
       <c r="D2" s="23" t="s">
+        <v>456</v>
+      </c>
+      <c r="E2" s="23" t="s">
         <v>457</v>
-      </c>
-      <c r="E2" s="23" t="s">
-        <v>458</v>
       </c>
       <c r="F2" s="35" t="str">
         <f>VLOOKUP(B2,Lexique!A:F,5,)</f>
@@ -3156,13 +3156,13 @@
         <v>76</v>
       </c>
       <c r="C3" s="29" t="s">
+        <v>495</v>
+      </c>
+      <c r="D3" s="23" t="s">
         <v>496</v>
       </c>
-      <c r="D3" s="23" t="s">
-        <v>497</v>
-      </c>
       <c r="E3" s="23" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="F3" s="35" t="str">
         <f>VLOOKUP(B3,Lexique!A:F,5,)</f>
@@ -3181,13 +3181,13 @@
         <v>73</v>
       </c>
       <c r="C4" s="29" t="s">
+        <v>497</v>
+      </c>
+      <c r="D4" s="23" t="s">
         <v>498</v>
       </c>
-      <c r="D4" s="23" t="s">
-        <v>499</v>
-      </c>
       <c r="E4" s="23" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="F4" s="35" t="str">
         <f>VLOOKUP(B4,Lexique!A:F,5,)</f>
@@ -3206,13 +3206,13 @@
         <v>75</v>
       </c>
       <c r="C5" s="29" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="D5" s="23" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="E5" s="23" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="F5" s="35" t="str">
         <f>VLOOKUP(B5,Lexique!A:F,5,)</f>
@@ -3231,13 +3231,13 @@
         <v>75</v>
       </c>
       <c r="C6" s="29" t="s">
+        <v>500</v>
+      </c>
+      <c r="D6" s="23" t="s">
         <v>501</v>
       </c>
-      <c r="D6" s="23" t="s">
-        <v>502</v>
-      </c>
       <c r="E6" s="23" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="F6" s="35" t="str">
         <f>VLOOKUP(B6,Lexique!A:F,5,)</f>
@@ -3256,7 +3256,7 @@
         <v>25</v>
       </c>
       <c r="C7" s="29" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="D7" s="23" t="s">
         <v>2</v>
@@ -3306,7 +3306,7 @@
         <v>25</v>
       </c>
       <c r="C9" s="29" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="D9" s="23" t="s">
         <v>2</v>
@@ -3332,7 +3332,7 @@
         <v>78</v>
       </c>
       <c r="C10" s="29" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D10" s="23" t="s">
         <v>155</v>
@@ -3357,7 +3357,7 @@
         <v>72</v>
       </c>
       <c r="C11" s="29" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="D11" s="23" t="s">
         <v>165</v>
@@ -3382,7 +3382,7 @@
         <v>76</v>
       </c>
       <c r="C12" s="29" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="D12" s="23" t="s">
         <v>165</v>
@@ -3410,10 +3410,10 @@
         <v>267</v>
       </c>
       <c r="D13" s="23" t="s">
+        <v>504</v>
+      </c>
+      <c r="E13" s="23" t="s">
         <v>505</v>
-      </c>
-      <c r="E13" s="23" t="s">
-        <v>506</v>
       </c>
       <c r="F13" s="35" t="str">
         <f>VLOOKUP(B13,Lexique!A:F,5,)</f>
@@ -3432,7 +3432,7 @@
         <v>25</v>
       </c>
       <c r="C14" s="29" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="D14" s="23" t="s">
         <v>2</v>
@@ -3457,13 +3457,13 @@
         <v>5</v>
       </c>
       <c r="C15" s="29" t="s">
+        <v>506</v>
+      </c>
+      <c r="D15" s="23" t="s">
         <v>507</v>
       </c>
-      <c r="D15" s="23" t="s">
-        <v>508</v>
-      </c>
       <c r="E15" s="23" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="F15" s="35" t="str">
         <f>VLOOKUP(B15,Lexique!A:F,5,)</f>
@@ -3482,13 +3482,13 @@
         <v>82</v>
       </c>
       <c r="C16" s="29" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="D16" s="44" t="s">
+        <v>606</v>
+      </c>
+      <c r="E16" s="62" t="s">
         <v>607</v>
-      </c>
-      <c r="E16" s="62" t="s">
-        <v>608</v>
       </c>
       <c r="F16" s="35" t="str">
         <f>VLOOKUP(B16,Lexique!A:F,5,)</f>
@@ -3507,13 +3507,13 @@
         <v>25</v>
       </c>
       <c r="C17" s="29" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="D17" s="24" t="s">
         <v>22</v>
       </c>
       <c r="E17" s="25" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="F17" s="35" t="str">
         <f>VLOOKUP(B17,Lexique!A:F,5,)</f>
@@ -3532,13 +3532,13 @@
         <v>25</v>
       </c>
       <c r="C18" s="29" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="D18" s="24" t="s">
         <v>22</v>
       </c>
       <c r="E18" s="25" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="F18" s="35" t="str">
         <f>VLOOKUP(B18,Lexique!A:F,5,)</f>
@@ -3557,13 +3557,13 @@
         <v>25</v>
       </c>
       <c r="C19" s="29" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="D19" s="24" t="s">
         <v>22</v>
       </c>
       <c r="E19" s="25" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="F19" s="35" t="str">
         <f>VLOOKUP(B19,Lexique!A:F,5,)</f>
@@ -3582,13 +3582,13 @@
         <v>82</v>
       </c>
       <c r="C20" s="29" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="D20" s="44" t="s">
+        <v>608</v>
+      </c>
+      <c r="E20" s="62" t="s">
         <v>609</v>
-      </c>
-      <c r="E20" s="62" t="s">
-        <v>610</v>
       </c>
       <c r="F20" s="35" t="str">
         <f>VLOOKUP(B20,Lexique!A:F,5,)</f>
@@ -3607,13 +3607,13 @@
         <v>72</v>
       </c>
       <c r="C21" s="29" t="s">
+        <v>513</v>
+      </c>
+      <c r="D21" s="25" t="s">
         <v>514</v>
       </c>
-      <c r="D21" s="25" t="s">
+      <c r="E21" s="25" t="s">
         <v>515</v>
-      </c>
-      <c r="E21" s="25" t="s">
-        <v>516</v>
       </c>
       <c r="F21" s="35" t="str">
         <f>VLOOKUP(B21,Lexique!A:F,5,)</f>
@@ -3632,13 +3632,13 @@
         <v>76</v>
       </c>
       <c r="C22" s="29" t="s">
+        <v>516</v>
+      </c>
+      <c r="D22" s="23" t="s">
+        <v>605</v>
+      </c>
+      <c r="E22" s="23" t="s">
         <v>517</v>
-      </c>
-      <c r="D22" s="23" t="s">
-        <v>606</v>
-      </c>
-      <c r="E22" s="23" t="s">
-        <v>518</v>
       </c>
       <c r="F22" s="35" t="str">
         <f>VLOOKUP(B22,Lexique!A:F,5,)</f>
@@ -3657,13 +3657,13 @@
         <v>73</v>
       </c>
       <c r="C23" s="29" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="D23" s="23" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="E23" s="23" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="F23" s="35" t="str">
         <f>VLOOKUP(B23,Lexique!A:F,5,)</f>
@@ -3682,13 +3682,13 @@
         <v>72</v>
       </c>
       <c r="C24" s="29" t="s">
+        <v>519</v>
+      </c>
+      <c r="D24" s="23" t="s">
         <v>520</v>
       </c>
-      <c r="D24" s="23" t="s">
-        <v>521</v>
-      </c>
       <c r="E24" s="23" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="F24" s="35" t="str">
         <f>VLOOKUP(B24,Lexique!A:F,5,)</f>
@@ -3707,13 +3707,13 @@
         <v>73</v>
       </c>
       <c r="C25" s="29" t="s">
+        <v>521</v>
+      </c>
+      <c r="D25" s="23" t="s">
         <v>522</v>
       </c>
-      <c r="D25" s="23" t="s">
-        <v>523</v>
-      </c>
       <c r="E25" s="23" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="F25" s="35" t="str">
         <f>VLOOKUP(B25,Lexique!A:F,5,)</f>
@@ -3735,10 +3735,10 @@
         <v>267</v>
       </c>
       <c r="D26" s="23" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="E26" s="23" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="F26" s="35" t="str">
         <f>VLOOKUP(B26,Lexique!A:F,5,)</f>
@@ -3757,13 +3757,13 @@
         <v>73</v>
       </c>
       <c r="C27" s="29" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="D27" s="26" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="E27" s="26" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="F27" s="35" t="str">
         <f>VLOOKUP(B27,Lexique!A:F,5,)</f>
@@ -3782,13 +3782,13 @@
         <v>72</v>
       </c>
       <c r="C28" s="29" t="s">
+        <v>525</v>
+      </c>
+      <c r="D28" s="23" t="s">
         <v>526</v>
       </c>
-      <c r="D28" s="23" t="s">
-        <v>527</v>
-      </c>
       <c r="E28" s="23" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="F28" s="35" t="str">
         <f>VLOOKUP(B28,Lexique!A:F,5,)</f>
@@ -3807,13 +3807,13 @@
         <v>73</v>
       </c>
       <c r="C29" s="29" t="s">
+        <v>527</v>
+      </c>
+      <c r="D29" s="23" t="s">
         <v>528</v>
       </c>
-      <c r="D29" s="23" t="s">
-        <v>529</v>
-      </c>
       <c r="E29" s="23" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="F29" s="35" t="str">
         <f>VLOOKUP(B29,Lexique!A:F,5,)</f>
@@ -3832,13 +3832,13 @@
         <v>73</v>
       </c>
       <c r="C30" s="29" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="D30" s="24" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="E30" s="24" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="F30" s="35" t="str">
         <f>VLOOKUP(B30,Lexique!A:F,5,)</f>
@@ -3857,13 +3857,13 @@
         <v>72</v>
       </c>
       <c r="C31" s="29" t="s">
+        <v>519</v>
+      </c>
+      <c r="D31" s="23" t="s">
         <v>520</v>
       </c>
-      <c r="D31" s="23" t="s">
-        <v>521</v>
-      </c>
       <c r="E31" s="23" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="F31" s="35" t="str">
         <f>VLOOKUP(B31,Lexique!A:F,5,)</f>
@@ -3882,13 +3882,13 @@
         <v>73</v>
       </c>
       <c r="C32" s="29" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="D32" s="24" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E32" s="24" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="F32" s="35" t="str">
         <f>VLOOKUP(B32,Lexique!A:F,5,)</f>
@@ -3907,13 +3907,13 @@
         <v>73</v>
       </c>
       <c r="C33" s="29" t="s">
+        <v>531</v>
+      </c>
+      <c r="D33" s="23" t="s">
         <v>532</v>
       </c>
-      <c r="D33" s="23" t="s">
-        <v>533</v>
-      </c>
       <c r="E33" s="23" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="F33" s="35" t="str">
         <f>VLOOKUP(B33,Lexique!A:F,5,)</f>
@@ -3933,13 +3933,13 @@
         <v>76</v>
       </c>
       <c r="C34" s="32" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="D34" s="23" t="s">
+        <v>610</v>
+      </c>
+      <c r="E34" s="23" t="s">
         <v>611</v>
-      </c>
-      <c r="E34" s="23" t="s">
-        <v>612</v>
       </c>
       <c r="F34" s="35" t="str">
         <f>VLOOKUP(B34,Lexique!A:F,5,)</f>
@@ -3959,13 +3959,13 @@
         <v>76</v>
       </c>
       <c r="C35" s="32" t="s">
+        <v>534</v>
+      </c>
+      <c r="D35" s="23" t="s">
         <v>535</v>
       </c>
-      <c r="D35" s="23" t="s">
+      <c r="E35" s="23" t="s">
         <v>536</v>
-      </c>
-      <c r="E35" s="23" t="s">
-        <v>537</v>
       </c>
       <c r="F35" s="35" t="str">
         <f>VLOOKUP(B35,Lexique!A:F,5,)</f>
@@ -3988,10 +3988,10 @@
         <v>4</v>
       </c>
       <c r="D36" s="27" t="s">
+        <v>537</v>
+      </c>
+      <c r="E36" s="27" t="s">
         <v>538</v>
-      </c>
-      <c r="E36" s="27" t="s">
-        <v>539</v>
       </c>
       <c r="F36" s="35"/>
       <c r="G36" s="35"/>
@@ -4008,10 +4008,10 @@
         <v>5</v>
       </c>
       <c r="D37" s="27" t="s">
+        <v>539</v>
+      </c>
+      <c r="E37" s="27" t="s">
         <v>540</v>
-      </c>
-      <c r="E37" s="27" t="s">
-        <v>541</v>
       </c>
       <c r="F37" s="35"/>
       <c r="G37" s="35"/>
@@ -4027,10 +4027,10 @@
         <v>267</v>
       </c>
       <c r="D38" s="23" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="E38" s="23" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="F38" s="35"/>
       <c r="G38" s="35"/>
@@ -4047,10 +4047,10 @@
         <v>6</v>
       </c>
       <c r="D39" s="27" t="s">
+        <v>541</v>
+      </c>
+      <c r="E39" s="27" t="s">
         <v>542</v>
-      </c>
-      <c r="E39" s="27" t="s">
-        <v>543</v>
       </c>
       <c r="F39" s="35"/>
       <c r="G39" s="35"/>
@@ -4063,13 +4063,13 @@
         <v>70</v>
       </c>
       <c r="C40" s="32" t="s">
+        <v>543</v>
+      </c>
+      <c r="D40" s="27" t="s">
         <v>544</v>
       </c>
-      <c r="D40" s="27" t="s">
+      <c r="E40" s="27" t="s">
         <v>545</v>
-      </c>
-      <c r="E40" s="27" t="s">
-        <v>546</v>
       </c>
       <c r="F40" s="35"/>
       <c r="G40" s="35"/>
@@ -4083,7 +4083,7 @@
         <v>78</v>
       </c>
       <c r="C41" s="29" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D41" s="23" t="s">
         <v>154</v>
@@ -4109,13 +4109,13 @@
         <v>76</v>
       </c>
       <c r="C42" s="32" t="s">
+        <v>546</v>
+      </c>
+      <c r="D42" s="27" t="s">
         <v>547</v>
       </c>
-      <c r="D42" s="27" t="s">
+      <c r="E42" s="27" t="s">
         <v>548</v>
-      </c>
-      <c r="E42" s="27" t="s">
-        <v>549</v>
       </c>
       <c r="F42" s="35"/>
       <c r="G42" s="35"/>
@@ -4129,13 +4129,13 @@
         <v>81</v>
       </c>
       <c r="C43" s="32" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="D43" s="23" t="s">
+        <v>549</v>
+      </c>
+      <c r="E43" s="23" t="s">
         <v>550</v>
-      </c>
-      <c r="E43" s="23" t="s">
-        <v>551</v>
       </c>
       <c r="F43" s="35"/>
       <c r="G43" s="35"/>
@@ -4149,13 +4149,13 @@
         <v>76</v>
       </c>
       <c r="C44" s="32" t="s">
+        <v>551</v>
+      </c>
+      <c r="D44" s="27" t="s">
         <v>552</v>
       </c>
-      <c r="D44" s="27" t="s">
+      <c r="E44" s="27" t="s">
         <v>553</v>
-      </c>
-      <c r="E44" s="27" t="s">
-        <v>554</v>
       </c>
       <c r="F44" s="35"/>
       <c r="G44" s="35"/>
@@ -4169,13 +4169,13 @@
         <v>110</v>
       </c>
       <c r="C45" s="32" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="D45" s="27" t="s">
+        <v>349</v>
+      </c>
+      <c r="E45" s="27" t="s">
         <v>350</v>
-      </c>
-      <c r="E45" s="27" t="s">
-        <v>351</v>
       </c>
       <c r="F45" s="35"/>
       <c r="G45" s="35"/>
@@ -6556,7 +6556,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF8C653E-9E00-4EDF-9978-201805372337}">
   <dimension ref="A1:AM14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
@@ -6733,7 +6733,7 @@
         <v>44027</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>208</v>
@@ -6783,7 +6783,7 @@
         <v>42</v>
       </c>
       <c r="T2" s="14" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="U2" t="str">
         <f>TEXT(_xlfn.CONCAT(Tableau2[[#This Row],[Heure_dep]],":",Tableau2[[#This Row],[min_dep]]), "HH:MM")</f>
@@ -6860,7 +6860,7 @@
         <v>44028</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="F3" s="4" t="s">
         <v>209</v>
@@ -6987,7 +6987,7 @@
         <v>44029</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="F4" s="4" t="s">
         <v>207</v>
@@ -7036,7 +7036,7 @@
         <v>42</v>
       </c>
       <c r="T4" s="14" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="U4" t="str">
         <f>TEXT(_xlfn.CONCAT(Tableau2[[#This Row],[Heure_dep]],":",Tableau2[[#This Row],[min_dep]]), "HH:MM")</f>
@@ -7119,7 +7119,7 @@
         <v>44029</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="F5" s="4" t="s">
         <v>232</v>
@@ -7247,7 +7247,7 @@
         <v>44030</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="F6" s="4" t="s">
         <v>230</v>
@@ -7424,7 +7424,7 @@
         <v>42</v>
       </c>
       <c r="T7" s="14" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="U7" t="str">
         <f>TEXT(_xlfn.CONCAT(Tableau2[[#This Row],[Heure_dep]],":",Tableau2[[#This Row],[min_dep]]), "HH:MM")</f>
@@ -7499,7 +7499,7 @@
         <v>44032</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="F8" s="4" t="s">
         <v>211</v>
@@ -7549,7 +7549,7 @@
         <v>42</v>
       </c>
       <c r="T8" s="14" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="U8" t="str">
         <f>TEXT(_xlfn.CONCAT(Tableau2[[#This Row],[Heure_dep]],":",Tableau2[[#This Row],[min_dep]]), "HH:MM")</f>
@@ -7630,8 +7630,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{371307C5-CDC8-4A0E-8E08-E5295E5C8E14}">
   <dimension ref="A1:G326"/>
   <sheetViews>
-    <sheetView topLeftCell="A33" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="D41" sqref="D41"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
@@ -7680,10 +7680,10 @@
         <v>264</v>
       </c>
       <c r="D2" s="23" t="s">
+        <v>460</v>
+      </c>
+      <c r="E2" s="23" t="s">
         <v>461</v>
-      </c>
-      <c r="E2" s="23" t="s">
-        <v>462</v>
       </c>
       <c r="F2" s="35" t="str">
         <f>VLOOKUP(B2,Lexique!A:F,5,)</f>
@@ -8361,10 +8361,10 @@
         <v>276</v>
       </c>
       <c r="D29" s="23" t="s">
+        <v>355</v>
+      </c>
+      <c r="E29" s="23" t="s">
         <v>356</v>
-      </c>
-      <c r="E29" s="23" t="s">
-        <v>357</v>
       </c>
       <c r="F29" s="35" t="str">
         <f>VLOOKUP(B29,Lexique!A:F,5,)</f>
@@ -8389,7 +8389,7 @@
         <v>280</v>
       </c>
       <c r="E30" s="24" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="F30" s="35" t="str">
         <f>VLOOKUP(B30,Lexique!A:F,5,)</f>
@@ -8509,13 +8509,13 @@
         <v>71</v>
       </c>
       <c r="C35" s="29" t="s">
+        <v>423</v>
+      </c>
+      <c r="D35" s="25" t="s">
         <v>424</v>
       </c>
-      <c r="D35" s="25" t="s">
+      <c r="E35" s="25" t="s">
         <v>425</v>
-      </c>
-      <c r="E35" s="25" t="s">
-        <v>426</v>
       </c>
       <c r="F35" s="35" t="str">
         <f>VLOOKUP(B35,Lexique!A:F,5,)</f>
@@ -8589,10 +8589,10 @@
         <v>302</v>
       </c>
       <c r="D38" s="23" t="s">
+        <v>618</v>
+      </c>
+      <c r="E38" s="23" t="s">
         <v>335</v>
-      </c>
-      <c r="E38" s="23" t="s">
-        <v>336</v>
       </c>
       <c r="F38" s="35" t="str">
         <f>VLOOKUP(B38,Lexique!A:F,5,)</f>
@@ -8614,7 +8614,7 @@
         <v>288</v>
       </c>
       <c r="D39" s="23" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E39" s="23" t="str">
         <f>D39</f>
@@ -8640,7 +8640,7 @@
         <v>289</v>
       </c>
       <c r="D40" s="23" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="E40" s="23" t="str">
         <f>D40</f>
@@ -8666,10 +8666,10 @@
         <v>303</v>
       </c>
       <c r="D41" s="23" t="s">
+        <v>338</v>
+      </c>
+      <c r="E41" s="23" t="s">
         <v>339</v>
-      </c>
-      <c r="E41" s="23" t="s">
-        <v>340</v>
       </c>
       <c r="F41" s="35" t="str">
         <f>VLOOKUP(B41,Lexique!A:F,5,)</f>
@@ -8691,7 +8691,7 @@
         <v>290</v>
       </c>
       <c r="D42" s="23" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="E42" s="23" t="str">
         <f>D42</f>
@@ -8717,7 +8717,7 @@
         <v>291</v>
       </c>
       <c r="D43" s="24" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="E43" s="23" t="str">
         <f t="shared" ref="E43:E49" si="0">D43</f>
@@ -8743,7 +8743,7 @@
         <v>292</v>
       </c>
       <c r="D44" s="23" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="E44" s="23" t="str">
         <f t="shared" si="0"/>
@@ -8769,7 +8769,7 @@
         <v>293</v>
       </c>
       <c r="D45" s="23" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="E45" s="23" t="str">
         <f t="shared" si="0"/>
@@ -8795,7 +8795,7 @@
         <v>294</v>
       </c>
       <c r="D46" s="24" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="E46" s="23" t="str">
         <f t="shared" si="0"/>
@@ -8821,7 +8821,7 @@
         <v>291</v>
       </c>
       <c r="D47" s="26" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="E47" s="23" t="str">
         <f t="shared" si="0"/>
@@ -8847,7 +8847,7 @@
         <v>288</v>
       </c>
       <c r="D48" s="26" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E48" s="23" t="str">
         <f t="shared" si="0"/>
@@ -8873,7 +8873,7 @@
         <v>289</v>
       </c>
       <c r="D49" s="26" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="E49" s="23" t="str">
         <f t="shared" si="0"/>
@@ -8899,10 +8899,10 @@
         <v>304</v>
       </c>
       <c r="D50" s="23" t="s">
+        <v>345</v>
+      </c>
+      <c r="E50" s="23" t="s">
         <v>346</v>
-      </c>
-      <c r="E50" s="23" t="s">
-        <v>347</v>
       </c>
       <c r="F50" s="35" t="str">
         <f>VLOOKUP(B50,Lexique!A:F,5,)</f>
@@ -8924,10 +8924,10 @@
         <v>305</v>
       </c>
       <c r="D51" s="26" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="E51" s="26" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="F51" s="35" t="str">
         <f>VLOOKUP(B51,Lexique!A:F,5,)</f>
@@ -8946,13 +8946,13 @@
         <v>110</v>
       </c>
       <c r="C52" s="32" t="s">
+        <v>348</v>
+      </c>
+      <c r="D52" s="26" t="s">
         <v>349</v>
       </c>
-      <c r="D52" s="26" t="s">
+      <c r="E52" s="26" t="s">
         <v>350</v>
-      </c>
-      <c r="E52" s="26" t="s">
-        <v>351</v>
       </c>
       <c r="F52" s="35" t="str">
         <f>VLOOKUP(B52,Lexique!A:F,5,)</f>
@@ -10140,10 +10140,10 @@
         <v>264</v>
       </c>
       <c r="D2" s="23" t="s">
+        <v>458</v>
+      </c>
+      <c r="E2" s="23" t="s">
         <v>459</v>
-      </c>
-      <c r="E2" s="23" t="s">
-        <v>460</v>
       </c>
       <c r="F2" s="35" t="str">
         <f>VLOOKUP(B2,Lexique!A:F,5,)</f>
@@ -10168,7 +10168,7 @@
         <v>22</v>
       </c>
       <c r="E3" s="23" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="F3" s="35" t="str">
         <f>VLOOKUP(B3,Lexique!A:F,5,)</f>
@@ -10187,13 +10187,13 @@
         <v>72</v>
       </c>
       <c r="C4" s="29" t="s">
+        <v>556</v>
+      </c>
+      <c r="D4" s="23" t="s">
         <v>557</v>
       </c>
-      <c r="D4" s="23" t="s">
-        <v>558</v>
-      </c>
       <c r="E4" s="23" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="F4" s="35" t="str">
         <f>VLOOKUP(B4,Lexique!A:F,5,)</f>
@@ -10212,13 +10212,13 @@
         <v>82</v>
       </c>
       <c r="C5" s="29" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="D5" s="23" t="s">
+        <v>597</v>
+      </c>
+      <c r="E5" s="23" t="s">
         <v>598</v>
-      </c>
-      <c r="E5" s="23" t="s">
-        <v>599</v>
       </c>
       <c r="F5" s="35" t="str">
         <f>VLOOKUP(B5,Lexique!A:F,5,)</f>
@@ -10237,13 +10237,13 @@
         <v>82</v>
       </c>
       <c r="C6" s="29" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="D6" s="23" t="s">
+        <v>595</v>
+      </c>
+      <c r="E6" s="23" t="s">
         <v>596</v>
-      </c>
-      <c r="E6" s="23" t="s">
-        <v>597</v>
       </c>
       <c r="F6" s="35" t="str">
         <f>VLOOKUP(B6,Lexique!A:F,5,)</f>
@@ -10262,7 +10262,7 @@
         <v>79</v>
       </c>
       <c r="C7" s="29" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="D7" s="23" t="s">
         <v>10</v>
@@ -10287,13 +10287,13 @@
         <v>73</v>
       </c>
       <c r="C8" s="29" t="s">
+        <v>561</v>
+      </c>
+      <c r="D8" s="23" t="s">
         <v>562</v>
       </c>
-      <c r="D8" s="23" t="s">
-        <v>563</v>
-      </c>
       <c r="E8" s="23" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="F8" s="35" t="str">
         <f>VLOOKUP(B8,Lexique!A:F,5,)</f>
@@ -10312,10 +10312,10 @@
         <v>5</v>
       </c>
       <c r="C9" s="29" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="D9" s="23" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="E9" s="23" t="str">
         <f>D9</f>
@@ -10338,13 +10338,13 @@
         <v>81</v>
       </c>
       <c r="C10" s="29" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="D10" s="23" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="E10" s="24" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="F10" s="35" t="str">
         <f>VLOOKUP(B10,Lexique!A:F,5,)</f>
@@ -10369,7 +10369,7 @@
         <v>12</v>
       </c>
       <c r="E11" s="23" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="F11" s="35" t="str">
         <f>VLOOKUP(B11,Lexique!A:F,5,)</f>
@@ -10391,10 +10391,10 @@
         <v>267</v>
       </c>
       <c r="D12" s="23" t="s">
+        <v>589</v>
+      </c>
+      <c r="E12" s="23" t="s">
         <v>590</v>
-      </c>
-      <c r="E12" s="23" t="s">
-        <v>591</v>
       </c>
       <c r="F12" s="35" t="str">
         <f>VLOOKUP(B12,Lexique!A:F,5,)</f>
@@ -10414,7 +10414,7 @@
         <v>78</v>
       </c>
       <c r="C13" s="29" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="D13" s="23" t="s">
         <v>155</v>
@@ -10439,13 +10439,13 @@
         <v>72</v>
       </c>
       <c r="C14" s="29" t="s">
+        <v>566</v>
+      </c>
+      <c r="D14" s="25" t="s">
         <v>567</v>
       </c>
-      <c r="D14" s="25" t="s">
-        <v>568</v>
-      </c>
       <c r="E14" s="25" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="F14" s="35" t="str">
         <f>VLOOKUP(B14,Lexique!A:F,5,)</f>
@@ -10464,7 +10464,7 @@
         <v>25</v>
       </c>
       <c r="C15" s="29" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="D15" s="23" t="s">
         <v>2</v>
@@ -10489,7 +10489,7 @@
         <v>25</v>
       </c>
       <c r="C16" s="29" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="D16" s="23" t="s">
         <v>2</v>
@@ -10514,13 +10514,13 @@
         <v>5</v>
       </c>
       <c r="C17" s="29" t="s">
+        <v>568</v>
+      </c>
+      <c r="D17" s="26" t="s">
         <v>569</v>
       </c>
-      <c r="D17" s="26" t="s">
-        <v>570</v>
-      </c>
       <c r="E17" s="25" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="F17" s="35" t="str">
         <f>VLOOKUP(B17,Lexique!A:F,5,)</f>
@@ -10539,13 +10539,13 @@
         <v>70</v>
       </c>
       <c r="C18" s="29" t="s">
+        <v>570</v>
+      </c>
+      <c r="D18" s="23" t="s">
+        <v>586</v>
+      </c>
+      <c r="E18" s="23" t="s">
         <v>571</v>
-      </c>
-      <c r="D18" s="23" t="s">
-        <v>587</v>
-      </c>
-      <c r="E18" s="23" t="s">
-        <v>572</v>
       </c>
       <c r="F18" s="35" t="str">
         <f>VLOOKUP(B18,Lexique!A:F,5,)</f>
@@ -10570,7 +10570,7 @@
         <v>22</v>
       </c>
       <c r="E19" s="23" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="F19" s="35" t="str">
         <f>VLOOKUP(B19,Lexique!A:F,5,)</f>
@@ -10589,13 +10589,13 @@
         <v>152</v>
       </c>
       <c r="C20" s="29" t="s">
+        <v>572</v>
+      </c>
+      <c r="D20" s="25" t="s">
+        <v>572</v>
+      </c>
+      <c r="E20" s="25" t="s">
         <v>573</v>
-      </c>
-      <c r="D20" s="25" t="s">
-        <v>573</v>
-      </c>
-      <c r="E20" s="25" t="s">
-        <v>574</v>
       </c>
       <c r="F20" s="35" t="str">
         <f>VLOOKUP(B20,Lexique!A:F,5,)</f>
@@ -10617,10 +10617,10 @@
         <v>267</v>
       </c>
       <c r="D21" s="23" t="s">
+        <v>591</v>
+      </c>
+      <c r="E21" s="23" t="s">
         <v>592</v>
-      </c>
-      <c r="E21" s="23" t="s">
-        <v>593</v>
       </c>
       <c r="F21" s="35" t="str">
         <f>VLOOKUP(B21,Lexique!A:F,5,)</f>
@@ -10639,7 +10639,7 @@
         <v>25</v>
       </c>
       <c r="C22" s="29" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="D22" s="23" t="s">
         <v>2</v>
@@ -10664,7 +10664,7 @@
         <v>25</v>
       </c>
       <c r="C23" s="29" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="D23" s="23" t="s">
         <v>2</v>
@@ -10689,13 +10689,13 @@
         <v>81</v>
       </c>
       <c r="C24" s="29" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="D24" s="23" t="s">
+        <v>603</v>
+      </c>
+      <c r="E24" s="24" t="s">
         <v>604</v>
-      </c>
-      <c r="E24" s="24" t="s">
-        <v>605</v>
       </c>
       <c r="F24" s="35" t="str">
         <f>VLOOKUP(B24,Lexique!A:F,5,)</f>
@@ -10715,7 +10715,7 @@
         <v>78</v>
       </c>
       <c r="C25" s="29" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="D25" s="25" t="s">
         <v>154</v>
@@ -10740,10 +10740,10 @@
         <v>5</v>
       </c>
       <c r="C26" s="29" t="s">
+        <v>601</v>
+      </c>
+      <c r="D26" s="25" t="s">
         <v>602</v>
-      </c>
-      <c r="D26" s="25" t="s">
-        <v>603</v>
       </c>
       <c r="E26" s="25" t="str">
         <f>D26</f>
@@ -10766,13 +10766,13 @@
         <v>82</v>
       </c>
       <c r="C27" s="29" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="D27" s="23" t="s">
+        <v>593</v>
+      </c>
+      <c r="E27" s="23" t="s">
         <v>594</v>
-      </c>
-      <c r="E27" s="23" t="s">
-        <v>595</v>
       </c>
       <c r="F27" s="35" t="str">
         <f>VLOOKUP(B27,Lexique!A:F,5,)</f>
@@ -10797,7 +10797,7 @@
         <v>22</v>
       </c>
       <c r="E28" s="23" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="F28" s="35" t="str">
         <f>VLOOKUP(B28,Lexique!A:F,5,)</f>
@@ -10816,13 +10816,13 @@
         <v>72</v>
       </c>
       <c r="C29" s="29" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="D29" s="25" t="s">
+        <v>514</v>
+      </c>
+      <c r="E29" s="25" t="s">
         <v>515</v>
-      </c>
-      <c r="E29" s="25" t="s">
-        <v>516</v>
       </c>
       <c r="F29" s="35" t="str">
         <f>VLOOKUP(B29,Lexique!A:F,5,)</f>
@@ -10841,13 +10841,13 @@
         <v>76</v>
       </c>
       <c r="C30" s="29" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="D30" s="23" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="E30" s="23" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="F30" s="35" t="str">
         <f>VLOOKUP(B30,Lexique!A:F,5,)</f>
@@ -10866,13 +10866,13 @@
         <v>73</v>
       </c>
       <c r="C31" s="29" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="D31" s="23" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="E31" s="23" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="F31" s="35" t="str">
         <f>VLOOKUP(B31,Lexique!A:F,5,)</f>
@@ -10891,13 +10891,13 @@
         <v>72</v>
       </c>
       <c r="C32" s="29" t="s">
+        <v>519</v>
+      </c>
+      <c r="D32" s="63" t="s">
         <v>520</v>
       </c>
-      <c r="D32" s="63" t="s">
-        <v>521</v>
-      </c>
       <c r="E32" s="28" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="F32" s="35" t="str">
         <f>VLOOKUP(B32,Lexique!A:F,5,)</f>
@@ -10916,13 +10916,13 @@
         <v>73</v>
       </c>
       <c r="C33" s="29" t="s">
+        <v>521</v>
+      </c>
+      <c r="D33" s="23" t="s">
         <v>522</v>
       </c>
-      <c r="D33" s="23" t="s">
-        <v>523</v>
-      </c>
       <c r="E33" s="23" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="F33" s="35" t="str">
         <f>VLOOKUP(B33,Lexique!A:F,5,)</f>
@@ -10944,10 +10944,10 @@
         <v>267</v>
       </c>
       <c r="D34" s="23" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="E34" s="23" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="F34" s="35" t="str">
         <f>VLOOKUP(B34,Lexique!A:F,5,)</f>
@@ -10966,13 +10966,13 @@
         <v>73</v>
       </c>
       <c r="C35" s="29" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="D35" s="26" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="E35" s="26" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="F35" s="35" t="str">
         <f>VLOOKUP(B35,Lexique!A:F,5,)</f>
@@ -10991,13 +10991,13 @@
         <v>73</v>
       </c>
       <c r="C36" s="29" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="D36" s="23" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="E36" s="23" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="F36" s="35" t="str">
         <f>VLOOKUP(B36,Lexique!A:F,5,)</f>
@@ -11016,13 +11016,13 @@
         <v>72</v>
       </c>
       <c r="C37" s="29" t="s">
+        <v>519</v>
+      </c>
+      <c r="D37" s="23" t="s">
         <v>520</v>
       </c>
-      <c r="D37" s="23" t="s">
-        <v>521</v>
-      </c>
       <c r="E37" s="23" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="F37" s="35" t="str">
         <f>VLOOKUP(B37,Lexique!A:F,5,)</f>
@@ -11041,13 +11041,13 @@
         <v>73</v>
       </c>
       <c r="C38" s="29" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="D38" s="24" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E38" s="24" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="F38" s="35" t="str">
         <f>VLOOKUP(B38,Lexique!A:F,5,)</f>
@@ -11066,13 +11066,13 @@
         <v>73</v>
       </c>
       <c r="C39" s="29" t="s">
+        <v>531</v>
+      </c>
+      <c r="D39" s="23" t="s">
         <v>532</v>
       </c>
-      <c r="D39" s="23" t="s">
-        <v>533</v>
-      </c>
       <c r="E39" s="23" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="F39" s="35" t="str">
         <f>VLOOKUP(B39,Lexique!A:F,5,)</f>
@@ -11091,13 +11091,13 @@
         <v>70</v>
       </c>
       <c r="C40" s="29" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="D40" s="23" t="s">
+        <v>599</v>
+      </c>
+      <c r="E40" s="23" t="s">
         <v>600</v>
-      </c>
-      <c r="E40" s="23" t="s">
-        <v>601</v>
       </c>
       <c r="F40" s="35" t="str">
         <f>VLOOKUP(B40,Lexique!A:F,5,)</f>
@@ -11116,13 +11116,13 @@
         <v>80</v>
       </c>
       <c r="C41" s="34" t="s">
+        <v>581</v>
+      </c>
+      <c r="D41" s="23" t="s">
         <v>582</v>
       </c>
-      <c r="D41" s="23" t="s">
-        <v>583</v>
-      </c>
       <c r="E41" s="23" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="F41" s="35" t="str">
         <f>VLOOKUP(B41,Lexique!A:F,5,)</f>
@@ -11141,13 +11141,13 @@
         <v>110</v>
       </c>
       <c r="C42" s="34" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="D42" s="63" t="s">
+        <v>349</v>
+      </c>
+      <c r="E42" s="27" t="s">
         <v>350</v>
-      </c>
-      <c r="E42" s="27" t="s">
-        <v>351</v>
       </c>
       <c r="F42" s="35" t="str">
         <f>VLOOKUP(B42,Lexique!A:F,5,)</f>
@@ -13176,10 +13176,10 @@
       </c>
       <c r="C2" s="29"/>
       <c r="D2" s="23" t="s">
+        <v>382</v>
+      </c>
+      <c r="E2" s="23" t="s">
         <v>383</v>
-      </c>
-      <c r="E2" s="23" t="s">
-        <v>384</v>
       </c>
       <c r="F2" s="47" t="str">
         <f>VLOOKUP(B2,Lexique!A:F,5,)</f>
@@ -13198,10 +13198,10 @@
         <v>72</v>
       </c>
       <c r="C3" s="29" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="D3" s="23" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="E3" s="23" t="str">
         <f>D3</f>
@@ -13224,13 +13224,13 @@
         <v>75</v>
       </c>
       <c r="C4" s="29" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="D4" s="23" t="s">
+        <v>373</v>
+      </c>
+      <c r="E4" s="23" t="s">
         <v>374</v>
-      </c>
-      <c r="E4" s="23" t="s">
-        <v>375</v>
       </c>
       <c r="F4" s="47" t="str">
         <f>VLOOKUP(B4,Lexique!A:F,5,)</f>
@@ -13249,10 +13249,10 @@
         <v>73</v>
       </c>
       <c r="C5" s="29" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="D5" s="23" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="E5" s="23" t="str">
         <f>D5</f>
@@ -13275,13 +13275,13 @@
         <v>74</v>
       </c>
       <c r="C6" s="29" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="D6" s="23" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="E6" s="23" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="F6" s="47" t="str">
         <f>VLOOKUP(B6,Lexique!A:F,5,)</f>
@@ -13352,13 +13352,13 @@
         <v>73</v>
       </c>
       <c r="C9" s="29" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="D9" s="23" t="s">
+        <v>376</v>
+      </c>
+      <c r="E9" s="23" t="s">
         <v>377</v>
-      </c>
-      <c r="E9" s="23" t="s">
-        <v>378</v>
       </c>
       <c r="F9" s="47" t="str">
         <f>VLOOKUP(B9,Lexique!A:F,5,)</f>
@@ -13377,13 +13377,13 @@
         <v>77</v>
       </c>
       <c r="C10" s="29" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="D10" s="23" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="E10" s="23" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="F10" s="47" t="str">
         <f>VLOOKUP(B10,Lexique!A:F,5,)</f>
@@ -13402,13 +13402,13 @@
         <v>72</v>
       </c>
       <c r="C11" s="29" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="D11" s="49" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="E11" s="23" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="F11" s="47" t="str">
         <f>VLOOKUP(B11,Lexique!A:F,5,)</f>
@@ -13430,10 +13430,10 @@
         <v>333</v>
       </c>
       <c r="D12" s="23" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="E12" s="23" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="F12" s="47" t="str">
         <f>VLOOKUP(B12,Lexique!A:F,5,)</f>
@@ -13452,10 +13452,10 @@
         <v>76</v>
       </c>
       <c r="C13" s="29" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="D13" s="23" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="E13" s="23" t="str">
         <f t="shared" si="0"/>
@@ -13478,10 +13478,10 @@
         <v>72</v>
       </c>
       <c r="C14" s="29" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="D14" s="23" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="E14" s="23" t="str">
         <f t="shared" si="0"/>
@@ -13504,13 +13504,13 @@
         <v>75</v>
       </c>
       <c r="C15" s="29" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="D15" s="23" t="s">
+        <v>373</v>
+      </c>
+      <c r="E15" s="23" t="s">
         <v>374</v>
-      </c>
-      <c r="E15" s="23" t="s">
-        <v>375</v>
       </c>
       <c r="F15" s="47" t="str">
         <f>VLOOKUP(B15,Lexique!A:F,5,)</f>
@@ -13529,10 +13529,10 @@
         <v>73</v>
       </c>
       <c r="C16" s="29" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="D16" s="49" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="E16" s="23" t="str">
         <f t="shared" si="0"/>
@@ -13555,10 +13555,10 @@
         <v>72</v>
       </c>
       <c r="C17" s="29" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="D17" s="50" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="E17" s="23" t="str">
         <f t="shared" si="0"/>
@@ -13581,7 +13581,7 @@
         <v>43</v>
       </c>
       <c r="C18" s="29" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="D18" s="23" t="s">
         <v>199</v>
@@ -15852,10 +15852,10 @@
       </c>
       <c r="C2" s="29"/>
       <c r="D2" s="23" t="s">
+        <v>490</v>
+      </c>
+      <c r="E2" s="23" t="s">
         <v>491</v>
-      </c>
-      <c r="E2" s="23" t="s">
-        <v>492</v>
       </c>
       <c r="F2" s="35" t="str">
         <f>VLOOKUP(B2,Lexique!A:F,5,)</f>
@@ -15874,10 +15874,10 @@
         <v>73</v>
       </c>
       <c r="C3" s="29" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="D3" s="23" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="E3" s="23" t="str">
         <f>D3</f>
@@ -15900,10 +15900,10 @@
         <v>73</v>
       </c>
       <c r="C4" s="29" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="D4" s="23" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="E4" s="23" t="str">
         <f>D4</f>
@@ -15926,13 +15926,13 @@
         <v>75</v>
       </c>
       <c r="C5" s="29" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="D5" s="23" t="s">
+        <v>486</v>
+      </c>
+      <c r="E5" s="23" t="s">
         <v>487</v>
-      </c>
-      <c r="E5" s="23" t="s">
-        <v>488</v>
       </c>
       <c r="F5" s="35" t="str">
         <f>VLOOKUP(B5,Lexique!A:F,5,)</f>
@@ -15976,13 +15976,13 @@
         <v>82</v>
       </c>
       <c r="C7" s="29" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="D7" s="23" t="s">
+        <v>483</v>
+      </c>
+      <c r="E7" s="23" t="s">
         <v>484</v>
-      </c>
-      <c r="E7" s="23" t="s">
-        <v>485</v>
       </c>
       <c r="F7" s="35" t="str">
         <f>VLOOKUP(B7,Lexique!A:F,5,)</f>
@@ -16001,7 +16001,7 @@
         <v>79</v>
       </c>
       <c r="C8" s="29" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="D8" s="23" t="s">
         <v>10</v>
@@ -16026,7 +16026,7 @@
         <v>74</v>
       </c>
       <c r="C9" s="29" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="D9" s="28" t="s">
         <v>165</v>
@@ -16052,7 +16052,7 @@
         <v>81</v>
       </c>
       <c r="C10" s="29" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="D10" s="23" t="s">
         <v>185</v>
@@ -16102,7 +16102,7 @@
         <v>74</v>
       </c>
       <c r="C12" s="29" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="D12" s="28" t="s">
         <v>165</v>
@@ -16153,7 +16153,7 @@
         <v>73</v>
       </c>
       <c r="C14" s="29" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="D14" s="23" t="s">
         <v>188</v>
@@ -16178,7 +16178,7 @@
         <v>73</v>
       </c>
       <c r="C15" s="29" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="D15" s="23" t="s">
         <v>200</v>
@@ -16203,7 +16203,7 @@
         <v>72</v>
       </c>
       <c r="C16" s="29" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="D16" s="24" t="s">
         <v>165</v>
@@ -16253,7 +16253,7 @@
         <v>75</v>
       </c>
       <c r="C18" s="29" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="D18" s="28" t="s">
         <v>165</v>
@@ -16279,7 +16279,7 @@
         <v>81</v>
       </c>
       <c r="C19" s="29" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="D19" s="23" t="s">
         <v>185</v>
@@ -16329,13 +16329,13 @@
         <v>82</v>
       </c>
       <c r="C21" s="29" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="D21" s="23" t="s">
+        <v>481</v>
+      </c>
+      <c r="E21" s="23" t="s">
         <v>482</v>
-      </c>
-      <c r="E21" s="23" t="s">
-        <v>483</v>
       </c>
       <c r="F21" s="35" t="str">
         <f>VLOOKUP(B21,Lexique!A:F,5,)</f>
@@ -16379,13 +16379,13 @@
         <v>75</v>
       </c>
       <c r="C23" s="29" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="D23" s="23" t="s">
+        <v>486</v>
+      </c>
+      <c r="E23" s="23" t="s">
         <v>487</v>
-      </c>
-      <c r="E23" s="23" t="s">
-        <v>488</v>
       </c>
       <c r="F23" s="35" t="str">
         <f>VLOOKUP(B23,Lexique!A:F,5,)</f>
@@ -16404,13 +16404,13 @@
         <v>72</v>
       </c>
       <c r="C24" s="29" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="D24" s="28" t="s">
+        <v>488</v>
+      </c>
+      <c r="E24" s="28" t="s">
         <v>489</v>
-      </c>
-      <c r="E24" s="28" t="s">
-        <v>490</v>
       </c>
       <c r="F24" s="35" t="str">
         <f>VLOOKUP(B24,Lexique!A:F,5,)</f>
@@ -16429,13 +16429,13 @@
         <v>110</v>
       </c>
       <c r="C25" s="29" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="D25" s="23" t="s">
+        <v>492</v>
+      </c>
+      <c r="E25" s="23" t="s">
         <v>493</v>
-      </c>
-      <c r="E25" s="23" t="s">
-        <v>494</v>
       </c>
       <c r="F25" s="35" t="str">
         <f>VLOOKUP(B25,Lexique!A:F,5,)</f>
@@ -16454,10 +16454,10 @@
         <v>73</v>
       </c>
       <c r="C26" s="29" t="s">
+        <v>477</v>
+      </c>
+      <c r="D26" s="23" t="s">
         <v>478</v>
-      </c>
-      <c r="D26" s="23" t="s">
-        <v>479</v>
       </c>
       <c r="E26" s="23" t="str">
         <f>D26</f>
@@ -18657,10 +18657,10 @@
       </c>
       <c r="C2" s="29"/>
       <c r="D2" s="23" t="s">
+        <v>456</v>
+      </c>
+      <c r="E2" s="23" t="s">
         <v>457</v>
-      </c>
-      <c r="E2" s="23" t="s">
-        <v>458</v>
       </c>
       <c r="F2" s="35" t="str">
         <f>VLOOKUP(B2,Lexique!A:F,5,)</f>
@@ -19564,10 +19564,10 @@
         <v>264</v>
       </c>
       <c r="D2" s="23" t="s">
+        <v>385</v>
+      </c>
+      <c r="E2" s="23" t="s">
         <v>386</v>
-      </c>
-      <c r="E2" s="23" t="s">
-        <v>387</v>
       </c>
       <c r="F2" s="35" t="str">
         <f>VLOOKUP(B2,Lexique!A:F,5,)</f>
@@ -19586,10 +19586,10 @@
         <v>73</v>
       </c>
       <c r="C3" s="29" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="D3" s="23" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="E3" s="23" t="str">
         <f>D3</f>
@@ -19612,10 +19612,10 @@
         <v>72</v>
       </c>
       <c r="C4" s="29" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="D4" s="23" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="E4" s="23" t="str">
         <f>D4</f>
@@ -19638,10 +19638,10 @@
         <v>73</v>
       </c>
       <c r="C5" s="29" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="D5" s="23" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="E5" s="23" t="str">
         <f>D5</f>
@@ -19664,10 +19664,10 @@
         <v>72</v>
       </c>
       <c r="C6" s="29" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="D6" s="23" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="E6" s="23" t="str">
         <f>D6</f>
@@ -19690,13 +19690,13 @@
         <v>74</v>
       </c>
       <c r="C7" s="29" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="D7" s="23" t="s">
+        <v>416</v>
+      </c>
+      <c r="E7" s="23" t="s">
         <v>417</v>
-      </c>
-      <c r="E7" s="23" t="s">
-        <v>418</v>
       </c>
       <c r="F7" s="35" t="str">
         <f>VLOOKUP(B7,Lexique!A:F,5,)</f>
@@ -19715,7 +19715,7 @@
         <v>74</v>
       </c>
       <c r="C8" s="29" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="D8" s="23" t="s">
         <v>330</v>
@@ -19744,10 +19744,10 @@
         <v>333</v>
       </c>
       <c r="D9" s="23" t="s">
+        <v>454</v>
+      </c>
+      <c r="E9" s="23" t="s">
         <v>455</v>
-      </c>
-      <c r="E9" s="23" t="s">
-        <v>456</v>
       </c>
       <c r="F9" s="35" t="str">
         <f>VLOOKUP(B9,Lexique!A:F,5,)</f>
@@ -19766,10 +19766,10 @@
         <v>73</v>
       </c>
       <c r="C10" s="29" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="D10" s="23" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="E10" s="24" t="str">
         <f>D10</f>
@@ -19792,10 +19792,10 @@
         <v>73</v>
       </c>
       <c r="C11" s="29" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="D11" s="24" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="E11" s="24" t="str">
         <f>D11</f>
@@ -19818,7 +19818,7 @@
         <v>73</v>
       </c>
       <c r="C12" s="29" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="D12" s="23" t="s">
         <v>330</v>
@@ -19844,7 +19844,7 @@
         <v>72</v>
       </c>
       <c r="C13" s="29" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="D13" s="23" t="s">
         <v>333</v>
@@ -19870,7 +19870,7 @@
         <v>73</v>
       </c>
       <c r="C14" s="29" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="D14" s="25" t="s">
         <v>334</v>
@@ -19896,10 +19896,10 @@
         <v>72</v>
       </c>
       <c r="C15" s="29" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="D15" s="23" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="E15" s="25" t="str">
         <f t="shared" si="0"/>
@@ -19922,10 +19922,10 @@
         <v>73</v>
       </c>
       <c r="C16" s="29" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="D16" s="24" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E16" s="25" t="str">
         <f t="shared" si="0"/>
@@ -19948,10 +19948,10 @@
         <v>73</v>
       </c>
       <c r="C17" s="29" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="D17" s="43" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="E17" s="25" t="str">
         <f t="shared" si="0"/>
@@ -19974,13 +19974,13 @@
         <v>76</v>
       </c>
       <c r="C18" s="29" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="D18" s="23" t="s">
+        <v>449</v>
+      </c>
+      <c r="E18" s="23" t="s">
         <v>450</v>
-      </c>
-      <c r="E18" s="23" t="s">
-        <v>451</v>
       </c>
       <c r="F18" s="35" t="str">
         <f>VLOOKUP(B18,Lexique!A:F,5,)</f>
@@ -20000,13 +20000,13 @@
         <v>76</v>
       </c>
       <c r="C19" s="29" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="D19" s="23" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="E19" s="23" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="F19" s="35" t="str">
         <f>VLOOKUP(B19,Lexique!A:F,5,)</f>
@@ -20026,13 +20026,13 @@
         <v>71</v>
       </c>
       <c r="C20" s="29" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="D20" s="25" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="E20" s="25" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="F20" s="35" t="str">
         <f>VLOOKUP(B20,Lexique!A:F,5,)</f>
@@ -20052,13 +20052,13 @@
         <v>76</v>
       </c>
       <c r="C21" s="29" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="D21" s="23" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="E21" s="23" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F21" s="35" t="str">
         <f>VLOOKUP(B21,Lexique!A:F,5,)</f>
@@ -20078,7 +20078,7 @@
         <v>78</v>
       </c>
       <c r="C22" s="29" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D22" s="23" t="s">
         <v>155</v>
@@ -20104,13 +20104,13 @@
         <v>70</v>
       </c>
       <c r="C23" s="29" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="D23" s="23" t="s">
+        <v>447</v>
+      </c>
+      <c r="E23" s="23" t="s">
         <v>448</v>
-      </c>
-      <c r="E23" s="23" t="s">
-        <v>449</v>
       </c>
       <c r="F23" s="35" t="str">
         <f>VLOOKUP(B23,Lexique!A:F,5,)</f>
@@ -20130,13 +20130,13 @@
         <v>76</v>
       </c>
       <c r="C24" s="29" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="D24" s="23" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="E24" s="23" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="F24" s="35" t="str">
         <f>VLOOKUP(B24,Lexique!A:F,5,)</f>
@@ -20156,13 +20156,13 @@
         <v>71</v>
       </c>
       <c r="C25" s="29" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D25" s="25" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="E25" s="25" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="F25" s="35" t="str">
         <f>VLOOKUP(B25,Lexique!A:F,5,)</f>
@@ -20182,13 +20182,13 @@
         <v>81</v>
       </c>
       <c r="C26" s="29" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="D26" s="23" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="E26" s="23" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="F26" s="35" t="str">
         <f>VLOOKUP(B26,Lexique!A:F,5,)</f>
@@ -20208,13 +20208,13 @@
         <v>76</v>
       </c>
       <c r="C27" s="29" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="D27" s="23" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="E27" s="23" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="F27" s="35" t="str">
         <f>VLOOKUP(B27,Lexique!A:F,5,)</f>
@@ -20234,13 +20234,13 @@
         <v>76</v>
       </c>
       <c r="C28" s="29" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="D28" s="23" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="E28" s="23" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="F28" s="35" t="str">
         <f>VLOOKUP(B28,Lexique!A:F,5,)</f>
@@ -20260,13 +20260,13 @@
         <v>71</v>
       </c>
       <c r="C29" s="29" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="D29" s="25" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="E29" s="25" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="F29" s="35" t="str">
         <f>VLOOKUP(B29,Lexique!A:F,5,)</f>
@@ -20286,13 +20286,13 @@
         <v>70</v>
       </c>
       <c r="C30" s="29" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="D30" s="23" t="s">
+        <v>445</v>
+      </c>
+      <c r="E30" s="23" t="s">
         <v>446</v>
-      </c>
-      <c r="E30" s="23" t="s">
-        <v>447</v>
       </c>
       <c r="F30" s="35" t="str">
         <f>VLOOKUP(B30,Lexique!A:F,5,)</f>
@@ -20312,13 +20312,13 @@
         <v>81</v>
       </c>
       <c r="C31" s="29" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="D31" s="23" t="s">
+        <v>442</v>
+      </c>
+      <c r="E31" s="23" t="s">
         <v>443</v>
-      </c>
-      <c r="E31" s="23" t="s">
-        <v>444</v>
       </c>
       <c r="F31" s="35" t="str">
         <f>VLOOKUP(B31,Lexique!A:F,5,)</f>
@@ -20338,7 +20338,7 @@
         <v>78</v>
       </c>
       <c r="C32" s="29" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="D32" s="23" t="s">
         <v>154</v>
@@ -20364,13 +20364,13 @@
         <v>80</v>
       </c>
       <c r="C33" s="29" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="D33" s="23" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="E33" s="23" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="F33" s="35" t="str">
         <f>VLOOKUP(B33,Lexique!A:F,5,)</f>
@@ -20391,10 +20391,10 @@
       </c>
       <c r="C34" s="29"/>
       <c r="D34" s="26" t="s">
+        <v>349</v>
+      </c>
+      <c r="E34" s="26" t="s">
         <v>350</v>
-      </c>
-      <c r="E34" s="26" t="s">
-        <v>351</v>
       </c>
       <c r="F34" s="35" t="str">
         <f>VLOOKUP(B34,Lexique!A:F,5,)</f>
@@ -20414,7 +20414,7 @@
         <v>43</v>
       </c>
       <c r="C35" s="29" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="D35" s="26" t="s">
         <v>109</v>

</xml_diff>

<commit_message>
Compilation post corrections France et Pierre
</commit_message>
<xml_diff>
--- a/excel/Itineraires.xlsx
+++ b/excel/Itineraires.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brunogauthier/Documents/guide2024/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DB74E8C-F022-3748-A47D-02CFA3F6181B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B15BF596-67E1-0A4B-88D8-DD6508DA573E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" tabRatio="758" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" tabRatio="758" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="23" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1196" uniqueCount="619">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1196" uniqueCount="620">
   <si>
     <t>GPM</t>
   </si>
@@ -713,9 +713,6 @@
     <t>Étape 5 - Boucle Senneterre</t>
   </si>
   <si>
-    <t>Étape 6 - Circuit Urbain</t>
-  </si>
-  <si>
     <t>Étape 7 - Senneterre</t>
   </si>
   <si>
@@ -728,9 +725,6 @@
     <t>Stage 5 - Senneterre Loop</t>
   </si>
   <si>
-    <t>Stage 6 - Urban Circuit</t>
-  </si>
-  <si>
     <t>Stage 7 - Senneterre</t>
   </si>
   <si>
@@ -1899,6 +1893,15 @@
   </si>
   <si>
     <t>Entrée sur le circuit d’arrivée &lt;br/&gt;1er avenue</t>
+  </si>
+  <si>
+    <t>Hôtel de ville</t>
+  </si>
+  <si>
+    <t>Étape 6 - Circuit urbain</t>
+  </si>
+  <si>
+    <t>Stage 6 - Urban circuit</t>
   </si>
 </sst>
 </file>
@@ -3051,27 +3054,27 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A6" s="4" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A7" s="4" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A8" s="4" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A9" s="4" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A10" s="4" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
     </row>
   </sheetData>
@@ -3108,7 +3111,7 @@
         <v>19</v>
       </c>
       <c r="C1" s="39" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="D1" s="40" t="s">
         <v>17</v>
@@ -3117,10 +3120,10 @@
         <v>18</v>
       </c>
       <c r="F1" s="41" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="G1" s="41" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="15" x14ac:dyDescent="0.2">
@@ -3131,13 +3134,13 @@
         <v>63</v>
       </c>
       <c r="C2" s="29" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="D2" s="23" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="E2" s="23" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="F2" s="35" t="str">
         <f>VLOOKUP(B2,Lexique!A:F,5,)</f>
@@ -3156,13 +3159,13 @@
         <v>76</v>
       </c>
       <c r="C3" s="29" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="D3" s="23" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="E3" s="23" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="F3" s="35" t="str">
         <f>VLOOKUP(B3,Lexique!A:F,5,)</f>
@@ -3181,13 +3184,13 @@
         <v>73</v>
       </c>
       <c r="C4" s="29" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="D4" s="23" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="E4" s="23" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="F4" s="35" t="str">
         <f>VLOOKUP(B4,Lexique!A:F,5,)</f>
@@ -3206,13 +3209,13 @@
         <v>75</v>
       </c>
       <c r="C5" s="29" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="D5" s="23" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="E5" s="23" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="F5" s="35" t="str">
         <f>VLOOKUP(B5,Lexique!A:F,5,)</f>
@@ -3231,13 +3234,13 @@
         <v>75</v>
       </c>
       <c r="C6" s="29" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="D6" s="23" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="E6" s="23" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="F6" s="35" t="str">
         <f>VLOOKUP(B6,Lexique!A:F,5,)</f>
@@ -3256,7 +3259,7 @@
         <v>25</v>
       </c>
       <c r="C7" s="29" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="D7" s="23" t="s">
         <v>2</v>
@@ -3281,7 +3284,7 @@
         <v>79</v>
       </c>
       <c r="C8" s="29" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="D8" s="23" t="s">
         <v>10</v>
@@ -3306,7 +3309,7 @@
         <v>25</v>
       </c>
       <c r="C9" s="29" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="D9" s="23" t="s">
         <v>2</v>
@@ -3332,7 +3335,7 @@
         <v>78</v>
       </c>
       <c r="C10" s="29" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="D10" s="23" t="s">
         <v>155</v>
@@ -3357,7 +3360,7 @@
         <v>72</v>
       </c>
       <c r="C11" s="29" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="D11" s="23" t="s">
         <v>165</v>
@@ -3382,7 +3385,7 @@
         <v>76</v>
       </c>
       <c r="C12" s="29" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="D12" s="23" t="s">
         <v>165</v>
@@ -3407,13 +3410,13 @@
         <v>71</v>
       </c>
       <c r="C13" s="29" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="D13" s="23" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="E13" s="23" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="F13" s="35" t="str">
         <f>VLOOKUP(B13,Lexique!A:F,5,)</f>
@@ -3432,7 +3435,7 @@
         <v>25</v>
       </c>
       <c r="C14" s="29" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="D14" s="23" t="s">
         <v>2</v>
@@ -3457,13 +3460,13 @@
         <v>5</v>
       </c>
       <c r="C15" s="29" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="D15" s="23" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="E15" s="23" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="F15" s="35" t="str">
         <f>VLOOKUP(B15,Lexique!A:F,5,)</f>
@@ -3482,13 +3485,13 @@
         <v>82</v>
       </c>
       <c r="C16" s="29" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="D16" s="44" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
       <c r="E16" s="62" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
       <c r="F16" s="35" t="str">
         <f>VLOOKUP(B16,Lexique!A:F,5,)</f>
@@ -3507,13 +3510,13 @@
         <v>25</v>
       </c>
       <c r="C17" s="29" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="D17" s="24" t="s">
         <v>22</v>
       </c>
       <c r="E17" s="25" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="F17" s="35" t="str">
         <f>VLOOKUP(B17,Lexique!A:F,5,)</f>
@@ -3532,13 +3535,13 @@
         <v>25</v>
       </c>
       <c r="C18" s="29" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="D18" s="24" t="s">
         <v>22</v>
       </c>
       <c r="E18" s="25" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="F18" s="35" t="str">
         <f>VLOOKUP(B18,Lexique!A:F,5,)</f>
@@ -3557,13 +3560,13 @@
         <v>25</v>
       </c>
       <c r="C19" s="29" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="D19" s="24" t="s">
         <v>22</v>
       </c>
       <c r="E19" s="25" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="F19" s="35" t="str">
         <f>VLOOKUP(B19,Lexique!A:F,5,)</f>
@@ -3582,13 +3585,13 @@
         <v>82</v>
       </c>
       <c r="C20" s="29" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="D20" s="44" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="E20" s="62" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="F20" s="35" t="str">
         <f>VLOOKUP(B20,Lexique!A:F,5,)</f>
@@ -3607,13 +3610,13 @@
         <v>72</v>
       </c>
       <c r="C21" s="29" t="s">
+        <v>511</v>
+      </c>
+      <c r="D21" s="25" t="s">
+        <v>512</v>
+      </c>
+      <c r="E21" s="25" t="s">
         <v>513</v>
-      </c>
-      <c r="D21" s="25" t="s">
-        <v>514</v>
-      </c>
-      <c r="E21" s="25" t="s">
-        <v>515</v>
       </c>
       <c r="F21" s="35" t="str">
         <f>VLOOKUP(B21,Lexique!A:F,5,)</f>
@@ -3632,13 +3635,13 @@
         <v>76</v>
       </c>
       <c r="C22" s="29" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="D22" s="23" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
       <c r="E22" s="23" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="F22" s="35" t="str">
         <f>VLOOKUP(B22,Lexique!A:F,5,)</f>
@@ -3657,13 +3660,13 @@
         <v>73</v>
       </c>
       <c r="C23" s="29" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="D23" s="23" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="E23" s="23" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="F23" s="35" t="str">
         <f>VLOOKUP(B23,Lexique!A:F,5,)</f>
@@ -3682,13 +3685,13 @@
         <v>72</v>
       </c>
       <c r="C24" s="29" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="D24" s="23" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="E24" s="23" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="F24" s="35" t="str">
         <f>VLOOKUP(B24,Lexique!A:F,5,)</f>
@@ -3707,13 +3710,13 @@
         <v>73</v>
       </c>
       <c r="C25" s="29" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="D25" s="23" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="E25" s="23" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="F25" s="35" t="str">
         <f>VLOOKUP(B25,Lexique!A:F,5,)</f>
@@ -3732,13 +3735,13 @@
         <v>71</v>
       </c>
       <c r="C26" s="29" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="D26" s="23" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="E26" s="23" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="F26" s="35" t="str">
         <f>VLOOKUP(B26,Lexique!A:F,5,)</f>
@@ -3757,13 +3760,13 @@
         <v>73</v>
       </c>
       <c r="C27" s="29" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="D27" s="26" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="E27" s="26" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="F27" s="35" t="str">
         <f>VLOOKUP(B27,Lexique!A:F,5,)</f>
@@ -3782,13 +3785,13 @@
         <v>72</v>
       </c>
       <c r="C28" s="29" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="D28" s="23" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="E28" s="23" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="F28" s="35" t="str">
         <f>VLOOKUP(B28,Lexique!A:F,5,)</f>
@@ -3807,13 +3810,13 @@
         <v>73</v>
       </c>
       <c r="C29" s="29" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="D29" s="23" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="E29" s="23" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="F29" s="35" t="str">
         <f>VLOOKUP(B29,Lexique!A:F,5,)</f>
@@ -3832,13 +3835,13 @@
         <v>73</v>
       </c>
       <c r="C30" s="29" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="D30" s="24" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="E30" s="24" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="F30" s="35" t="str">
         <f>VLOOKUP(B30,Lexique!A:F,5,)</f>
@@ -3857,13 +3860,13 @@
         <v>72</v>
       </c>
       <c r="C31" s="29" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="D31" s="23" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="E31" s="23" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="F31" s="35" t="str">
         <f>VLOOKUP(B31,Lexique!A:F,5,)</f>
@@ -3882,13 +3885,13 @@
         <v>73</v>
       </c>
       <c r="C32" s="29" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="D32" s="24" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="E32" s="24" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="F32" s="35" t="str">
         <f>VLOOKUP(B32,Lexique!A:F,5,)</f>
@@ -3907,13 +3910,13 @@
         <v>73</v>
       </c>
       <c r="C33" s="29" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="D33" s="23" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="E33" s="23" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="F33" s="35" t="str">
         <f>VLOOKUP(B33,Lexique!A:F,5,)</f>
@@ -3933,13 +3936,13 @@
         <v>76</v>
       </c>
       <c r="C34" s="32" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="D34" s="23" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
       <c r="E34" s="23" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
       <c r="F34" s="35" t="str">
         <f>VLOOKUP(B34,Lexique!A:F,5,)</f>
@@ -3959,13 +3962,13 @@
         <v>76</v>
       </c>
       <c r="C35" s="32" t="s">
+        <v>532</v>
+      </c>
+      <c r="D35" s="23" t="s">
+        <v>533</v>
+      </c>
+      <c r="E35" s="23" t="s">
         <v>534</v>
-      </c>
-      <c r="D35" s="23" t="s">
-        <v>535</v>
-      </c>
-      <c r="E35" s="23" t="s">
-        <v>536</v>
       </c>
       <c r="F35" s="35" t="str">
         <f>VLOOKUP(B35,Lexique!A:F,5,)</f>
@@ -3988,10 +3991,10 @@
         <v>4</v>
       </c>
       <c r="D36" s="27" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="E36" s="27" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="F36" s="35"/>
       <c r="G36" s="35"/>
@@ -4008,10 +4011,10 @@
         <v>5</v>
       </c>
       <c r="D37" s="27" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="E37" s="27" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="F37" s="35"/>
       <c r="G37" s="35"/>
@@ -4024,13 +4027,13 @@
         <v>71</v>
       </c>
       <c r="C38" s="32" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="D38" s="23" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="E38" s="23" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="F38" s="35"/>
       <c r="G38" s="35"/>
@@ -4047,10 +4050,10 @@
         <v>6</v>
       </c>
       <c r="D39" s="27" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="E39" s="27" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="F39" s="35"/>
       <c r="G39" s="35"/>
@@ -4063,13 +4066,13 @@
         <v>70</v>
       </c>
       <c r="C40" s="32" t="s">
+        <v>541</v>
+      </c>
+      <c r="D40" s="27" t="s">
+        <v>542</v>
+      </c>
+      <c r="E40" s="27" t="s">
         <v>543</v>
-      </c>
-      <c r="D40" s="27" t="s">
-        <v>544</v>
-      </c>
-      <c r="E40" s="27" t="s">
-        <v>545</v>
       </c>
       <c r="F40" s="35"/>
       <c r="G40" s="35"/>
@@ -4083,7 +4086,7 @@
         <v>78</v>
       </c>
       <c r="C41" s="29" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="D41" s="23" t="s">
         <v>154</v>
@@ -4109,13 +4112,13 @@
         <v>76</v>
       </c>
       <c r="C42" s="32" t="s">
+        <v>544</v>
+      </c>
+      <c r="D42" s="27" t="s">
+        <v>545</v>
+      </c>
+      <c r="E42" s="27" t="s">
         <v>546</v>
-      </c>
-      <c r="D42" s="27" t="s">
-        <v>547</v>
-      </c>
-      <c r="E42" s="27" t="s">
-        <v>548</v>
       </c>
       <c r="F42" s="35"/>
       <c r="G42" s="35"/>
@@ -4129,13 +4132,13 @@
         <v>81</v>
       </c>
       <c r="C43" s="32" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="D43" s="23" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="E43" s="23" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="F43" s="35"/>
       <c r="G43" s="35"/>
@@ -4149,13 +4152,13 @@
         <v>76</v>
       </c>
       <c r="C44" s="32" t="s">
+        <v>549</v>
+      </c>
+      <c r="D44" s="27" t="s">
+        <v>550</v>
+      </c>
+      <c r="E44" s="27" t="s">
         <v>551</v>
-      </c>
-      <c r="D44" s="27" t="s">
-        <v>552</v>
-      </c>
-      <c r="E44" s="27" t="s">
-        <v>553</v>
       </c>
       <c r="F44" s="35"/>
       <c r="G44" s="35"/>
@@ -4169,13 +4172,13 @@
         <v>110</v>
       </c>
       <c r="C45" s="32" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
       <c r="D45" s="27" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="E45" s="27" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="F45" s="35"/>
       <c r="G45" s="35"/>
@@ -4188,7 +4191,7 @@
         <v>43</v>
       </c>
       <c r="C46" s="32" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="D46" s="23" t="s">
         <v>166</v>
@@ -6152,10 +6155,10 @@
         <v>38</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="F1" s="22" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.15">
@@ -6172,10 +6175,10 @@
         <v>40</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.15">
@@ -6212,10 +6215,10 @@
         <v>42</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.15">
@@ -6252,10 +6255,10 @@
         <v>25</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.15">
@@ -6272,10 +6275,10 @@
         <v>5</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.15">
@@ -6292,10 +6295,10 @@
         <v>44</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.15">
@@ -6312,10 +6315,10 @@
         <v>45</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.15">
@@ -6332,10 +6335,10 @@
         <v>46</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="14" x14ac:dyDescent="0.15">
@@ -6352,7 +6355,7 @@
         <v>47</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="F11" t="str">
         <f>Tableau1[[#This Row],[Texte_REF_FR]]</f>
@@ -6373,7 +6376,7 @@
         <v>48</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="F12" t="str">
         <f>Tableau1[[#This Row],[Texte_REF_FR]]</f>
@@ -6394,7 +6397,7 @@
         <v>49</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="F13" t="str">
         <f>Tableau1[[#This Row],[Texte_REF_FR]]</f>
@@ -6415,7 +6418,7 @@
         <v>50</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="F14" t="str">
         <f>Tableau1[[#This Row],[Texte_REF_FR]]</f>
@@ -6436,7 +6439,7 @@
         <v>51</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="F15" t="str">
         <f>Tableau1[[#This Row],[Texte_REF_FR]]</f>
@@ -6457,10 +6460,10 @@
         <v>52</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.15">
@@ -6497,10 +6500,10 @@
         <v>84</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.15">
@@ -6517,10 +6520,10 @@
         <v>112</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.15">
@@ -6537,10 +6540,10 @@
         <v>151</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
   </sheetData>
@@ -6556,8 +6559,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF8C653E-9E00-4EDF-9978-201805372337}">
   <dimension ref="A1:AM14"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" topLeftCell="AB1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="AE22" sqref="AE22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -6733,7 +6736,7 @@
         <v>44027</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>208</v>
@@ -6783,7 +6786,7 @@
         <v>42</v>
       </c>
       <c r="T2" s="14" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="U2" t="str">
         <f>TEXT(_xlfn.CONCAT(Tableau2[[#This Row],[Heure_dep]],":",Tableau2[[#This Row],[min_dep]]), "HH:MM")</f>
@@ -6827,7 +6830,7 @@
         <v>129</v>
       </c>
       <c r="AG2" s="16" t="s">
-        <v>217</v>
+        <v>617</v>
       </c>
       <c r="AH2" s="16" t="str">
         <f>Tableau2[[#This Row],[LieuDepFR]]</f>
@@ -6840,7 +6843,7 @@
         <v>220</v>
       </c>
       <c r="AK2" s="4" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="AL2" s="15"/>
       <c r="AM2" s="15"/>
@@ -6860,7 +6863,7 @@
         <v>44028</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="F3" s="4" t="s">
         <v>209</v>
@@ -6910,7 +6913,7 @@
         <v>42</v>
       </c>
       <c r="T3" s="14" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="U3" t="str">
         <f>TEXT(_xlfn.CONCAT(Tableau2[[#This Row],[Heure_dep]],":",Tableau2[[#This Row],[min_dep]]), "HH:MM")</f>
@@ -6954,7 +6957,7 @@
         <v>126</v>
       </c>
       <c r="AG3" s="16" t="s">
-        <v>217</v>
+        <v>617</v>
       </c>
       <c r="AH3" s="16" t="str">
         <f>Tableau2[[#This Row],[LieuDepFR]]</f>
@@ -6967,7 +6970,7 @@
         <v>221</v>
       </c>
       <c r="AK3" s="4" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="AL3" s="15"/>
       <c r="AM3" s="15"/>
@@ -6987,7 +6990,7 @@
         <v>44029</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="F4" s="4" t="s">
         <v>207</v>
@@ -7036,7 +7039,7 @@
         <v>42</v>
       </c>
       <c r="T4" s="14" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="U4" t="str">
         <f>TEXT(_xlfn.CONCAT(Tableau2[[#This Row],[Heure_dep]],":",Tableau2[[#This Row],[min_dep]]), "HH:MM")</f>
@@ -7119,10 +7122,10 @@
         <v>44029</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="G5" s="19" t="str">
         <f>CONCATENATE(Tableau2[[#This Row],[Distance_totale]]," km")</f>
@@ -7169,7 +7172,7 @@
         <v>44</v>
       </c>
       <c r="T5" s="14" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="U5" t="str">
         <f>TEXT(_xlfn.CONCAT(Tableau2[[#This Row],[Heure_dep]],":",Tableau2[[#This Row],[min_dep]]), "HH:MM")</f>
@@ -7210,14 +7213,14 @@
         <v>140</v>
       </c>
       <c r="AF5" s="16" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="AG5" s="16" t="str">
         <f>Tableau2[[#This Row],[LieuDepFR]]</f>
         <v>Musée minéralogique de l'A-T</v>
       </c>
       <c r="AH5" s="16" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="AI5" s="15" t="str">
         <f>Tableau2[[#This Row],[LieuDepEN]]</f>
@@ -7247,10 +7250,10 @@
         <v>44030</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="G6" s="19" t="str">
         <f>CONCATENATE(Tableau2[[#This Row],[Distance_totale]]," km")</f>
@@ -7297,7 +7300,7 @@
         <v>41</v>
       </c>
       <c r="T6" s="14" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="U6" t="str">
         <f>TEXT(_xlfn.CONCAT(Tableau2[[#This Row],[Heure_dep]],":",Tableau2[[#This Row],[min_dep]]), "HH:MM")</f>
@@ -7338,22 +7341,22 @@
         <v>215</v>
       </c>
       <c r="AF6" s="16" t="s">
-        <v>217</v>
+        <v>617</v>
       </c>
       <c r="AG6" s="16" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="AH6" s="16" t="s">
         <v>219</v>
       </c>
       <c r="AI6" s="16" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="AJ6" s="4" t="s">
         <v>222</v>
       </c>
       <c r="AK6" s="4" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="AL6" s="15"/>
       <c r="AM6" s="15"/>
@@ -7373,7 +7376,7 @@
         <v>44031</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="F7" s="19" t="s">
         <v>210</v>
@@ -7424,7 +7427,7 @@
         <v>42</v>
       </c>
       <c r="T7" s="14" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="U7" t="str">
         <f>TEXT(_xlfn.CONCAT(Tableau2[[#This Row],[Heure_dep]],":",Tableau2[[#This Row],[min_dep]]), "HH:MM")</f>
@@ -7463,11 +7466,11 @@
       </c>
       <c r="AE7" s="16"/>
       <c r="AF7" s="21" t="s">
-        <v>217</v>
+        <v>617</v>
       </c>
       <c r="AG7" s="16" t="str">
         <f>Tableau2[[#This Row],[LieuDepFR]]</f>
-        <v>Hôtel de Ville</v>
+        <v>Hôtel de ville</v>
       </c>
       <c r="AH7" s="16" t="s">
         <v>219</v>
@@ -7476,10 +7479,10 @@
         <v>219</v>
       </c>
       <c r="AJ7" s="4" t="s">
-        <v>223</v>
+        <v>618</v>
       </c>
       <c r="AK7" s="4" t="s">
-        <v>228</v>
+        <v>619</v>
       </c>
       <c r="AL7" s="15"/>
       <c r="AM7" s="15"/>
@@ -7499,7 +7502,7 @@
         <v>44032</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
       <c r="F8" s="4" t="s">
         <v>211</v>
@@ -7549,7 +7552,7 @@
         <v>42</v>
       </c>
       <c r="T8" s="14" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="U8" t="str">
         <f>TEXT(_xlfn.CONCAT(Tableau2[[#This Row],[Heure_dep]],":",Tableau2[[#This Row],[min_dep]]), "HH:MM")</f>
@@ -7590,7 +7593,7 @@
         <v>216</v>
       </c>
       <c r="AF8" s="16" t="s">
-        <v>217</v>
+        <v>617</v>
       </c>
       <c r="AG8" s="16" t="s">
         <v>217</v>
@@ -7602,10 +7605,10 @@
         <v>219</v>
       </c>
       <c r="AJ8" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="AK8" s="4" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="AL8" s="15"/>
       <c r="AM8" s="15"/>
@@ -7630,7 +7633,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{371307C5-CDC8-4A0E-8E08-E5295E5C8E14}">
   <dimension ref="A1:G326"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView topLeftCell="A28" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
@@ -7654,7 +7657,7 @@
         <v>19</v>
       </c>
       <c r="C1" s="39" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="D1" s="40" t="s">
         <v>17</v>
@@ -7663,10 +7666,10 @@
         <v>18</v>
       </c>
       <c r="F1" s="41" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="G1" s="41" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="15" x14ac:dyDescent="0.2">
@@ -7677,13 +7680,13 @@
         <v>63</v>
       </c>
       <c r="C2" s="29" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="D2" s="23" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="E2" s="23" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="F2" s="35" t="str">
         <f>VLOOKUP(B2,Lexique!A:F,5,)</f>
@@ -7702,7 +7705,7 @@
         <v>72</v>
       </c>
       <c r="C3" s="29" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="D3" s="23" t="s">
         <v>147</v>
@@ -7728,7 +7731,7 @@
         <v>73</v>
       </c>
       <c r="C4" s="29" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="D4" s="23" t="s">
         <v>148</v>
@@ -7754,7 +7757,7 @@
         <v>72</v>
       </c>
       <c r="C5" s="29" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="D5" s="23" t="s">
         <v>149</v>
@@ -7780,10 +7783,10 @@
         <v>73</v>
       </c>
       <c r="C6" s="29" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="D6" s="23" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="E6" s="23" t="str">
         <f>D6</f>
@@ -7806,13 +7809,13 @@
         <v>82</v>
       </c>
       <c r="C7" s="29" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="D7" s="23" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="E7" s="23" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="F7" s="35" t="str">
         <f>VLOOKUP(B7,Lexique!A:F,5,)</f>
@@ -7831,7 +7834,7 @@
         <v>79</v>
       </c>
       <c r="C8" s="29" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="D8" s="23" t="s">
         <v>10</v>
@@ -7856,13 +7859,13 @@
         <v>5</v>
       </c>
       <c r="C9" s="29" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="D9" s="23" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="E9" s="23" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="F9" s="35" t="str">
         <f>VLOOKUP(B9,Lexique!A:F,5,)</f>
@@ -7931,13 +7934,13 @@
         <v>5</v>
       </c>
       <c r="C12" s="29" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="D12" s="23" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="E12" s="25" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="F12" s="35" t="str">
         <f>VLOOKUP(B12,Lexique!A:F,5,)</f>
@@ -7981,13 +7984,13 @@
         <v>71</v>
       </c>
       <c r="C14" s="29" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="D14" s="25" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="E14" s="25" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="F14" s="35" t="str">
         <f>VLOOKUP(B14,Lexique!A:F,5,)</f>
@@ -8006,7 +8009,7 @@
         <v>78</v>
       </c>
       <c r="C15" s="29" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="D15" s="23" t="s">
         <v>155</v>
@@ -8056,13 +8059,13 @@
         <v>70</v>
       </c>
       <c r="C17" s="29" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D17" s="43" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="E17" s="43" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="F17" s="35" t="str">
         <f>VLOOKUP(B17,Lexique!A:F,5,)</f>
@@ -8081,10 +8084,10 @@
         <v>5</v>
       </c>
       <c r="C18" s="29" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="D18" s="23" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="E18" s="23" t="s">
         <v>140</v>
@@ -8106,13 +8109,13 @@
         <v>81</v>
       </c>
       <c r="C19" s="29" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="D19" s="23" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="E19" s="23" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="F19" s="35" t="str">
         <f>VLOOKUP(B19,Lexique!A:F,5,)</f>
@@ -8131,13 +8134,13 @@
         <v>5</v>
       </c>
       <c r="C20" s="29" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="D20" s="23" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="E20" s="23" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="F20" s="35" t="str">
         <f>VLOOKUP(B20,Lexique!A:F,5,)</f>
@@ -8156,7 +8159,7 @@
         <v>75</v>
       </c>
       <c r="C21" s="29" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="D21" s="24" t="s">
         <v>165</v>
@@ -8182,7 +8185,7 @@
         <v>75</v>
       </c>
       <c r="C22" s="29" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="D22" s="23" t="s">
         <v>165</v>
@@ -8208,13 +8211,13 @@
         <v>70</v>
       </c>
       <c r="C23" s="29" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="D23" s="43" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="E23" s="43" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="F23" s="35" t="str">
         <f>VLOOKUP(B23,Lexique!A:F,5,)</f>
@@ -8233,13 +8236,13 @@
         <v>5</v>
       </c>
       <c r="C24" s="29" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="D24" s="23" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="E24" s="44" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="F24" s="35" t="str">
         <f>VLOOKUP(B24,Lexique!A:F,5,)</f>
@@ -8258,13 +8261,13 @@
         <v>82</v>
       </c>
       <c r="C25" s="29" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="D25" s="23" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="E25" s="23" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="F25" s="35" t="str">
         <f>VLOOKUP(B25,Lexique!A:F,5,)</f>
@@ -8283,13 +8286,13 @@
         <v>25</v>
       </c>
       <c r="C26" s="29" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="D26" s="23" t="s">
         <v>22</v>
       </c>
       <c r="E26" s="23" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="F26" s="35" t="str">
         <f>VLOOKUP(B26,Lexique!A:F,5,)</f>
@@ -8308,7 +8311,7 @@
         <v>152</v>
       </c>
       <c r="C27" s="29" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="D27" s="23" t="s">
         <v>205</v>
@@ -8333,13 +8336,13 @@
         <v>5</v>
       </c>
       <c r="C28" s="29" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="D28" s="23" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="E28" s="23" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="F28" s="35" t="str">
         <f>VLOOKUP(B28,Lexique!A:F,5,)</f>
@@ -8358,13 +8361,13 @@
         <v>81</v>
       </c>
       <c r="C29" s="29" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="D29" s="23" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="E29" s="23" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="F29" s="35" t="str">
         <f>VLOOKUP(B29,Lexique!A:F,5,)</f>
@@ -8383,13 +8386,13 @@
         <v>25</v>
       </c>
       <c r="C30" s="29" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="D30" s="24" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="E30" s="24" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="F30" s="35" t="str">
         <f>VLOOKUP(B30,Lexique!A:F,5,)</f>
@@ -8408,7 +8411,7 @@
         <v>78</v>
       </c>
       <c r="C31" s="29" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="D31" s="23" t="s">
         <v>154</v>
@@ -8433,13 +8436,13 @@
         <v>5</v>
       </c>
       <c r="C32" s="29" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="D32" s="23" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="E32" s="23" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="F32" s="35" t="str">
         <f>VLOOKUP(B32,Lexique!A:F,5,)</f>
@@ -8458,13 +8461,13 @@
         <v>82</v>
       </c>
       <c r="C33" s="29" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="D33" s="23" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="E33" s="23" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="F33" s="35" t="str">
         <f>VLOOKUP(B33,Lexique!A:F,5,)</f>
@@ -8483,10 +8486,10 @@
         <v>73</v>
       </c>
       <c r="C34" s="29" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="D34" s="23" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="E34" s="23" t="str">
         <f>D34</f>
@@ -8509,13 +8512,13 @@
         <v>71</v>
       </c>
       <c r="C35" s="29" t="s">
+        <v>421</v>
+      </c>
+      <c r="D35" s="25" t="s">
+        <v>422</v>
+      </c>
+      <c r="E35" s="25" t="s">
         <v>423</v>
-      </c>
-      <c r="D35" s="25" t="s">
-        <v>424</v>
-      </c>
-      <c r="E35" s="25" t="s">
-        <v>425</v>
       </c>
       <c r="F35" s="35" t="str">
         <f>VLOOKUP(B35,Lexique!A:F,5,)</f>
@@ -8534,10 +8537,10 @@
         <v>72</v>
       </c>
       <c r="C36" s="29" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="D36" s="23" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="E36" s="23" t="str">
         <f>D36</f>
@@ -8560,10 +8563,10 @@
         <v>73</v>
       </c>
       <c r="C37" s="29" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="D37" s="23" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="E37" s="23" t="str">
         <f>D37</f>
@@ -8586,13 +8589,13 @@
         <v>72</v>
       </c>
       <c r="C38" s="29" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="D38" s="23" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
       <c r="E38" s="23" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="F38" s="35" t="str">
         <f>VLOOKUP(B38,Lexique!A:F,5,)</f>
@@ -8611,10 +8614,10 @@
         <v>73</v>
       </c>
       <c r="C39" s="29" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="D39" s="23" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="E39" s="23" t="str">
         <f>D39</f>
@@ -8637,10 +8640,10 @@
         <v>73</v>
       </c>
       <c r="C40" s="29" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="D40" s="23" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="E40" s="23" t="str">
         <f>D40</f>
@@ -8663,13 +8666,13 @@
         <v>76</v>
       </c>
       <c r="C41" s="29" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="D41" s="23" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="E41" s="23" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="F41" s="35" t="str">
         <f>VLOOKUP(B41,Lexique!A:F,5,)</f>
@@ -8688,10 +8691,10 @@
         <v>73</v>
       </c>
       <c r="C42" s="29" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="D42" s="23" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="E42" s="23" t="str">
         <f>D42</f>
@@ -8714,10 +8717,10 @@
         <v>72</v>
       </c>
       <c r="C43" s="29" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="D43" s="24" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="E43" s="23" t="str">
         <f t="shared" ref="E43:E49" si="0">D43</f>
@@ -8740,10 +8743,10 @@
         <v>73</v>
       </c>
       <c r="C44" s="29" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="D44" s="23" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="E44" s="23" t="str">
         <f t="shared" si="0"/>
@@ -8766,10 +8769,10 @@
         <v>73</v>
       </c>
       <c r="C45" s="29" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="D45" s="23" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="E45" s="23" t="str">
         <f t="shared" si="0"/>
@@ -8792,10 +8795,10 @@
         <v>73</v>
       </c>
       <c r="C46" s="29" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="D46" s="24" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="E46" s="23" t="str">
         <f t="shared" si="0"/>
@@ -8818,10 +8821,10 @@
         <v>72</v>
       </c>
       <c r="C47" s="32" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="D47" s="26" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="E47" s="23" t="str">
         <f t="shared" si="0"/>
@@ -8844,10 +8847,10 @@
         <v>73</v>
       </c>
       <c r="C48" s="32" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="D48" s="26" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="E48" s="23" t="str">
         <f t="shared" si="0"/>
@@ -8870,10 +8873,10 @@
         <v>73</v>
       </c>
       <c r="C49" s="32" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="D49" s="26" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="E49" s="23" t="str">
         <f t="shared" si="0"/>
@@ -8896,13 +8899,13 @@
         <v>76</v>
       </c>
       <c r="C50" s="32" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="D50" s="23" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="E50" s="23" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="F50" s="35" t="str">
         <f>VLOOKUP(B50,Lexique!A:F,5,)</f>
@@ -8921,13 +8924,13 @@
         <v>80</v>
       </c>
       <c r="C51" s="32" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="D51" s="26" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="E51" s="26" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="F51" s="35" t="str">
         <f>VLOOKUP(B51,Lexique!A:F,5,)</f>
@@ -8946,13 +8949,13 @@
         <v>110</v>
       </c>
       <c r="C52" s="32" t="s">
+        <v>346</v>
+      </c>
+      <c r="D52" s="26" t="s">
+        <v>347</v>
+      </c>
+      <c r="E52" s="26" t="s">
         <v>348</v>
-      </c>
-      <c r="D52" s="26" t="s">
-        <v>349</v>
-      </c>
-      <c r="E52" s="26" t="s">
-        <v>350</v>
       </c>
       <c r="F52" s="35" t="str">
         <f>VLOOKUP(B52,Lexique!A:F,5,)</f>
@@ -8971,7 +8974,7 @@
         <v>43</v>
       </c>
       <c r="C53" s="32" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="D53" s="26" t="s">
         <v>109</v>
@@ -10114,7 +10117,7 @@
         <v>19</v>
       </c>
       <c r="C1" s="39" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="D1" s="40" t="s">
         <v>17</v>
@@ -10123,10 +10126,10 @@
         <v>18</v>
       </c>
       <c r="F1" s="41" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="G1" s="41" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="15" x14ac:dyDescent="0.2">
@@ -10137,13 +10140,13 @@
         <v>63</v>
       </c>
       <c r="C2" s="29" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="D2" s="23" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="E2" s="23" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="F2" s="35" t="str">
         <f>VLOOKUP(B2,Lexique!A:F,5,)</f>
@@ -10168,7 +10171,7 @@
         <v>22</v>
       </c>
       <c r="E3" s="23" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="F3" s="35" t="str">
         <f>VLOOKUP(B3,Lexique!A:F,5,)</f>
@@ -10187,13 +10190,13 @@
         <v>72</v>
       </c>
       <c r="C4" s="29" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="D4" s="23" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="E4" s="23" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="F4" s="35" t="str">
         <f>VLOOKUP(B4,Lexique!A:F,5,)</f>
@@ -10212,13 +10215,13 @@
         <v>82</v>
       </c>
       <c r="C5" s="29" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
       <c r="D5" s="23" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
       <c r="E5" s="23" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
       <c r="F5" s="35" t="str">
         <f>VLOOKUP(B5,Lexique!A:F,5,)</f>
@@ -10237,13 +10240,13 @@
         <v>82</v>
       </c>
       <c r="C6" s="29" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="D6" s="23" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="E6" s="23" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
       <c r="F6" s="35" t="str">
         <f>VLOOKUP(B6,Lexique!A:F,5,)</f>
@@ -10262,7 +10265,7 @@
         <v>79</v>
       </c>
       <c r="C7" s="29" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="D7" s="23" t="s">
         <v>10</v>
@@ -10287,13 +10290,13 @@
         <v>73</v>
       </c>
       <c r="C8" s="29" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="D8" s="23" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="E8" s="23" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="F8" s="35" t="str">
         <f>VLOOKUP(B8,Lexique!A:F,5,)</f>
@@ -10312,10 +10315,10 @@
         <v>5</v>
       </c>
       <c r="C9" s="29" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="D9" s="23" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="E9" s="23" t="str">
         <f>D9</f>
@@ -10338,13 +10341,13 @@
         <v>81</v>
       </c>
       <c r="C10" s="29" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="D10" s="23" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="E10" s="24" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
       <c r="F10" s="35" t="str">
         <f>VLOOKUP(B10,Lexique!A:F,5,)</f>
@@ -10369,7 +10372,7 @@
         <v>12</v>
       </c>
       <c r="E11" s="23" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="F11" s="35" t="str">
         <f>VLOOKUP(B11,Lexique!A:F,5,)</f>
@@ -10388,13 +10391,13 @@
         <v>71</v>
       </c>
       <c r="C12" s="29" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="D12" s="23" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
       <c r="E12" s="23" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
       <c r="F12" s="35" t="str">
         <f>VLOOKUP(B12,Lexique!A:F,5,)</f>
@@ -10414,7 +10417,7 @@
         <v>78</v>
       </c>
       <c r="C13" s="29" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
       <c r="D13" s="23" t="s">
         <v>155</v>
@@ -10439,13 +10442,13 @@
         <v>72</v>
       </c>
       <c r="C14" s="29" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
       <c r="D14" s="25" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
       <c r="E14" s="25" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
       <c r="F14" s="35" t="str">
         <f>VLOOKUP(B14,Lexique!A:F,5,)</f>
@@ -10464,7 +10467,7 @@
         <v>25</v>
       </c>
       <c r="C15" s="29" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="D15" s="23" t="s">
         <v>2</v>
@@ -10489,7 +10492,7 @@
         <v>25</v>
       </c>
       <c r="C16" s="29" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="D16" s="23" t="s">
         <v>2</v>
@@ -10514,13 +10517,13 @@
         <v>5</v>
       </c>
       <c r="C17" s="29" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="D17" s="26" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="E17" s="25" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="F17" s="35" t="str">
         <f>VLOOKUP(B17,Lexique!A:F,5,)</f>
@@ -10539,13 +10542,13 @@
         <v>70</v>
       </c>
       <c r="C18" s="29" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
       <c r="D18" s="23" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
       <c r="E18" s="23" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="F18" s="35" t="str">
         <f>VLOOKUP(B18,Lexique!A:F,5,)</f>
@@ -10570,7 +10573,7 @@
         <v>22</v>
       </c>
       <c r="E19" s="23" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="F19" s="35" t="str">
         <f>VLOOKUP(B19,Lexique!A:F,5,)</f>
@@ -10589,13 +10592,13 @@
         <v>152</v>
       </c>
       <c r="C20" s="29" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
       <c r="D20" s="25" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
       <c r="E20" s="25" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
       <c r="F20" s="35" t="str">
         <f>VLOOKUP(B20,Lexique!A:F,5,)</f>
@@ -10614,13 +10617,13 @@
         <v>71</v>
       </c>
       <c r="C21" s="29" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="D21" s="23" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="E21" s="23" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
       <c r="F21" s="35" t="str">
         <f>VLOOKUP(B21,Lexique!A:F,5,)</f>
@@ -10639,7 +10642,7 @@
         <v>25</v>
       </c>
       <c r="C22" s="29" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="D22" s="23" t="s">
         <v>2</v>
@@ -10664,7 +10667,7 @@
         <v>25</v>
       </c>
       <c r="C23" s="29" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
       <c r="D23" s="23" t="s">
         <v>2</v>
@@ -10689,13 +10692,13 @@
         <v>81</v>
       </c>
       <c r="C24" s="29" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="D24" s="23" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="E24" s="24" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="F24" s="35" t="str">
         <f>VLOOKUP(B24,Lexique!A:F,5,)</f>
@@ -10715,7 +10718,7 @@
         <v>78</v>
       </c>
       <c r="C25" s="29" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="D25" s="25" t="s">
         <v>154</v>
@@ -10740,10 +10743,10 @@
         <v>5</v>
       </c>
       <c r="C26" s="29" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="D26" s="25" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
       <c r="E26" s="25" t="str">
         <f>D26</f>
@@ -10766,13 +10769,13 @@
         <v>82</v>
       </c>
       <c r="C27" s="29" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
       <c r="D27" s="23" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
       <c r="E27" s="23" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="F27" s="35" t="str">
         <f>VLOOKUP(B27,Lexique!A:F,5,)</f>
@@ -10797,7 +10800,7 @@
         <v>22</v>
       </c>
       <c r="E28" s="23" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="F28" s="35" t="str">
         <f>VLOOKUP(B28,Lexique!A:F,5,)</f>
@@ -10816,13 +10819,13 @@
         <v>72</v>
       </c>
       <c r="C29" s="29" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="D29" s="25" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="E29" s="25" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="F29" s="35" t="str">
         <f>VLOOKUP(B29,Lexique!A:F,5,)</f>
@@ -10841,13 +10844,13 @@
         <v>76</v>
       </c>
       <c r="C30" s="29" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="D30" s="23" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="E30" s="23" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
       <c r="F30" s="35" t="str">
         <f>VLOOKUP(B30,Lexique!A:F,5,)</f>
@@ -10866,13 +10869,13 @@
         <v>73</v>
       </c>
       <c r="C31" s="29" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="D31" s="23" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="E31" s="23" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="F31" s="35" t="str">
         <f>VLOOKUP(B31,Lexique!A:F,5,)</f>
@@ -10891,13 +10894,13 @@
         <v>72</v>
       </c>
       <c r="C32" s="29" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="D32" s="63" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="E32" s="28" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="F32" s="35" t="str">
         <f>VLOOKUP(B32,Lexique!A:F,5,)</f>
@@ -10916,13 +10919,13 @@
         <v>73</v>
       </c>
       <c r="C33" s="29" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="D33" s="23" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="E33" s="23" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="F33" s="35" t="str">
         <f>VLOOKUP(B33,Lexique!A:F,5,)</f>
@@ -10941,13 +10944,13 @@
         <v>71</v>
       </c>
       <c r="C34" s="29" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="D34" s="23" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="E34" s="23" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="F34" s="35" t="str">
         <f>VLOOKUP(B34,Lexique!A:F,5,)</f>
@@ -10966,13 +10969,13 @@
         <v>73</v>
       </c>
       <c r="C35" s="29" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="D35" s="26" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="E35" s="26" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="F35" s="35" t="str">
         <f>VLOOKUP(B35,Lexique!A:F,5,)</f>
@@ -10991,13 +10994,13 @@
         <v>73</v>
       </c>
       <c r="C36" s="29" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="D36" s="23" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="E36" s="23" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="F36" s="35" t="str">
         <f>VLOOKUP(B36,Lexique!A:F,5,)</f>
@@ -11016,13 +11019,13 @@
         <v>72</v>
       </c>
       <c r="C37" s="29" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="D37" s="23" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="E37" s="23" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="F37" s="35" t="str">
         <f>VLOOKUP(B37,Lexique!A:F,5,)</f>
@@ -11041,13 +11044,13 @@
         <v>73</v>
       </c>
       <c r="C38" s="29" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="D38" s="24" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="E38" s="24" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="F38" s="35" t="str">
         <f>VLOOKUP(B38,Lexique!A:F,5,)</f>
@@ -11066,13 +11069,13 @@
         <v>73</v>
       </c>
       <c r="C39" s="29" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="D39" s="23" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="E39" s="23" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="F39" s="35" t="str">
         <f>VLOOKUP(B39,Lexique!A:F,5,)</f>
@@ -11091,13 +11094,13 @@
         <v>70</v>
       </c>
       <c r="C40" s="29" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
       <c r="D40" s="23" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
       <c r="E40" s="23" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
       <c r="F40" s="35" t="str">
         <f>VLOOKUP(B40,Lexique!A:F,5,)</f>
@@ -11116,13 +11119,13 @@
         <v>80</v>
       </c>
       <c r="C41" s="34" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
       <c r="D41" s="23" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
       <c r="E41" s="23" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
       <c r="F41" s="35" t="str">
         <f>VLOOKUP(B41,Lexique!A:F,5,)</f>
@@ -11141,13 +11144,13 @@
         <v>110</v>
       </c>
       <c r="C42" s="34" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
       <c r="D42" s="63" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="E42" s="27" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="F42" s="35" t="str">
         <f>VLOOKUP(B42,Lexique!A:F,5,)</f>
@@ -11166,7 +11169,7 @@
         <v>43</v>
       </c>
       <c r="C43" s="34" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="D43" s="63" t="s">
         <v>166</v>
@@ -13152,7 +13155,7 @@
         <v>19</v>
       </c>
       <c r="C1" s="39" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="D1" s="40" t="s">
         <v>17</v>
@@ -13161,10 +13164,10 @@
         <v>18</v>
       </c>
       <c r="F1" s="45" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="G1" s="45" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="15" x14ac:dyDescent="0.15">
@@ -13176,10 +13179,10 @@
       </c>
       <c r="C2" s="29"/>
       <c r="D2" s="23" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="E2" s="23" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="F2" s="47" t="str">
         <f>VLOOKUP(B2,Lexique!A:F,5,)</f>
@@ -13198,10 +13201,10 @@
         <v>72</v>
       </c>
       <c r="C3" s="29" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="D3" s="23" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="E3" s="23" t="str">
         <f>D3</f>
@@ -13224,13 +13227,13 @@
         <v>75</v>
       </c>
       <c r="C4" s="29" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="D4" s="23" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="E4" s="23" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="F4" s="47" t="str">
         <f>VLOOKUP(B4,Lexique!A:F,5,)</f>
@@ -13249,10 +13252,10 @@
         <v>73</v>
       </c>
       <c r="C5" s="29" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="D5" s="23" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="E5" s="23" t="str">
         <f>D5</f>
@@ -13275,13 +13278,13 @@
         <v>74</v>
       </c>
       <c r="C6" s="29" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="D6" s="23" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="E6" s="23" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="F6" s="47" t="str">
         <f>VLOOKUP(B6,Lexique!A:F,5,)</f>
@@ -13300,10 +13303,10 @@
         <v>76</v>
       </c>
       <c r="C7" s="29" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="D7" s="23" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="E7" s="23" t="str">
         <f>D7</f>
@@ -13326,10 +13329,10 @@
         <v>73</v>
       </c>
       <c r="C8" s="29" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="D8" s="23" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="E8" s="23" t="str">
         <f t="shared" ref="E8:E17" si="0">D8</f>
@@ -13352,13 +13355,13 @@
         <v>73</v>
       </c>
       <c r="C9" s="29" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="D9" s="23" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="E9" s="23" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="F9" s="47" t="str">
         <f>VLOOKUP(B9,Lexique!A:F,5,)</f>
@@ -13377,13 +13380,13 @@
         <v>77</v>
       </c>
       <c r="C10" s="29" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="D10" s="23" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="E10" s="23" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="F10" s="47" t="str">
         <f>VLOOKUP(B10,Lexique!A:F,5,)</f>
@@ -13402,13 +13405,13 @@
         <v>72</v>
       </c>
       <c r="C11" s="29" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="D11" s="49" t="s">
+        <v>376</v>
+      </c>
+      <c r="E11" s="23" t="s">
         <v>378</v>
-      </c>
-      <c r="E11" s="23" t="s">
-        <v>380</v>
       </c>
       <c r="F11" s="47" t="str">
         <f>VLOOKUP(B11,Lexique!A:F,5,)</f>
@@ -13427,13 +13430,13 @@
         <v>72</v>
       </c>
       <c r="C12" s="29" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="D12" s="23" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="E12" s="23" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="F12" s="47" t="str">
         <f>VLOOKUP(B12,Lexique!A:F,5,)</f>
@@ -13452,10 +13455,10 @@
         <v>76</v>
       </c>
       <c r="C13" s="29" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="D13" s="23" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="E13" s="23" t="str">
         <f t="shared" si="0"/>
@@ -13478,10 +13481,10 @@
         <v>72</v>
       </c>
       <c r="C14" s="29" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="D14" s="23" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="E14" s="23" t="str">
         <f t="shared" si="0"/>
@@ -13504,13 +13507,13 @@
         <v>75</v>
       </c>
       <c r="C15" s="29" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="D15" s="23" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="E15" s="23" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="F15" s="47" t="str">
         <f>VLOOKUP(B15,Lexique!A:F,5,)</f>
@@ -13529,10 +13532,10 @@
         <v>73</v>
       </c>
       <c r="C16" s="29" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="D16" s="49" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="E16" s="23" t="str">
         <f t="shared" si="0"/>
@@ -13555,10 +13558,10 @@
         <v>72</v>
       </c>
       <c r="C17" s="29" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="D17" s="50" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="E17" s="23" t="str">
         <f t="shared" si="0"/>
@@ -13581,7 +13584,7 @@
         <v>43</v>
       </c>
       <c r="C18" s="29" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="D18" s="23" t="s">
         <v>199</v>
@@ -15828,7 +15831,7 @@
         <v>19</v>
       </c>
       <c r="C1" s="39" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="D1" s="40" t="s">
         <v>17</v>
@@ -15837,10 +15840,10 @@
         <v>18</v>
       </c>
       <c r="F1" s="41" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="G1" s="41" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.2">
@@ -15852,10 +15855,10 @@
       </c>
       <c r="C2" s="29"/>
       <c r="D2" s="23" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="E2" s="23" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="F2" s="35" t="str">
         <f>VLOOKUP(B2,Lexique!A:F,5,)</f>
@@ -15874,10 +15877,10 @@
         <v>73</v>
       </c>
       <c r="C3" s="29" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="D3" s="23" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="E3" s="23" t="str">
         <f>D3</f>
@@ -15900,10 +15903,10 @@
         <v>73</v>
       </c>
       <c r="C4" s="29" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="D4" s="23" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="E4" s="23" t="str">
         <f>D4</f>
@@ -15926,13 +15929,13 @@
         <v>75</v>
       </c>
       <c r="C5" s="29" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="D5" s="23" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="E5" s="23" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="F5" s="35" t="str">
         <f>VLOOKUP(B5,Lexique!A:F,5,)</f>
@@ -15951,7 +15954,7 @@
         <v>25</v>
       </c>
       <c r="C6" s="29" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="D6" s="23" t="s">
         <v>22</v>
@@ -15976,13 +15979,13 @@
         <v>82</v>
       </c>
       <c r="C7" s="29" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="D7" s="23" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="E7" s="23" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="F7" s="35" t="str">
         <f>VLOOKUP(B7,Lexique!A:F,5,)</f>
@@ -16001,7 +16004,7 @@
         <v>79</v>
       </c>
       <c r="C8" s="29" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="D8" s="23" t="s">
         <v>10</v>
@@ -16026,7 +16029,7 @@
         <v>74</v>
       </c>
       <c r="C9" s="29" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="D9" s="28" t="s">
         <v>165</v>
@@ -16052,7 +16055,7 @@
         <v>81</v>
       </c>
       <c r="C10" s="29" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="D10" s="23" t="s">
         <v>185</v>
@@ -16102,7 +16105,7 @@
         <v>74</v>
       </c>
       <c r="C12" s="29" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="D12" s="28" t="s">
         <v>165</v>
@@ -16153,7 +16156,7 @@
         <v>73</v>
       </c>
       <c r="C14" s="29" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="D14" s="23" t="s">
         <v>188</v>
@@ -16178,7 +16181,7 @@
         <v>73</v>
       </c>
       <c r="C15" s="29" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="D15" s="23" t="s">
         <v>200</v>
@@ -16203,7 +16206,7 @@
         <v>72</v>
       </c>
       <c r="C16" s="29" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="D16" s="24" t="s">
         <v>165</v>
@@ -16253,7 +16256,7 @@
         <v>75</v>
       </c>
       <c r="C18" s="29" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="D18" s="28" t="s">
         <v>165</v>
@@ -16279,7 +16282,7 @@
         <v>81</v>
       </c>
       <c r="C19" s="29" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="D19" s="23" t="s">
         <v>185</v>
@@ -16329,13 +16332,13 @@
         <v>82</v>
       </c>
       <c r="C21" s="29" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="D21" s="23" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="E21" s="23" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="F21" s="35" t="str">
         <f>VLOOKUP(B21,Lexique!A:F,5,)</f>
@@ -16354,7 +16357,7 @@
         <v>25</v>
       </c>
       <c r="C22" s="29" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="D22" s="23" t="s">
         <v>22</v>
@@ -16379,13 +16382,13 @@
         <v>75</v>
       </c>
       <c r="C23" s="29" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="D23" s="23" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="E23" s="23" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="F23" s="35" t="str">
         <f>VLOOKUP(B23,Lexique!A:F,5,)</f>
@@ -16404,13 +16407,13 @@
         <v>72</v>
       </c>
       <c r="C24" s="29" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="D24" s="28" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="E24" s="28" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="F24" s="35" t="str">
         <f>VLOOKUP(B24,Lexique!A:F,5,)</f>
@@ -16429,13 +16432,13 @@
         <v>110</v>
       </c>
       <c r="C25" s="29" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="D25" s="23" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="E25" s="23" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="F25" s="35" t="str">
         <f>VLOOKUP(B25,Lexique!A:F,5,)</f>
@@ -16454,10 +16457,10 @@
         <v>73</v>
       </c>
       <c r="C26" s="29" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="D26" s="23" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="E26" s="23" t="str">
         <f>D26</f>
@@ -16480,7 +16483,7 @@
         <v>43</v>
       </c>
       <c r="C27" s="29" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="D27" s="23" t="s">
         <v>166</v>
@@ -18633,7 +18636,7 @@
         <v>19</v>
       </c>
       <c r="C1" s="39" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="D1" s="39" t="s">
         <v>17</v>
@@ -18642,10 +18645,10 @@
         <v>18</v>
       </c>
       <c r="F1" s="41" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="G1" s="41" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="15" x14ac:dyDescent="0.2">
@@ -18657,10 +18660,10 @@
       </c>
       <c r="C2" s="29"/>
       <c r="D2" s="23" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="E2" s="23" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="F2" s="35" t="str">
         <f>VLOOKUP(B2,Lexique!A:F,5,)</f>
@@ -19538,7 +19541,7 @@
         <v>19</v>
       </c>
       <c r="C1" s="39" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="D1" s="40" t="s">
         <v>17</v>
@@ -19547,10 +19550,10 @@
         <v>18</v>
       </c>
       <c r="F1" s="41" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="G1" s="41" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="15" x14ac:dyDescent="0.2">
@@ -19561,13 +19564,13 @@
         <v>79</v>
       </c>
       <c r="C2" s="29" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="D2" s="23" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="E2" s="23" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="F2" s="35" t="str">
         <f>VLOOKUP(B2,Lexique!A:F,5,)</f>
@@ -19586,10 +19589,10 @@
         <v>73</v>
       </c>
       <c r="C3" s="29" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="D3" s="23" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="E3" s="23" t="str">
         <f>D3</f>
@@ -19612,10 +19615,10 @@
         <v>72</v>
       </c>
       <c r="C4" s="29" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="D4" s="23" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="E4" s="23" t="str">
         <f>D4</f>
@@ -19638,10 +19641,10 @@
         <v>73</v>
       </c>
       <c r="C5" s="29" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="D5" s="23" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="E5" s="23" t="str">
         <f>D5</f>
@@ -19664,10 +19667,10 @@
         <v>72</v>
       </c>
       <c r="C6" s="29" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="D6" s="23" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="E6" s="23" t="str">
         <f>D6</f>
@@ -19690,13 +19693,13 @@
         <v>74</v>
       </c>
       <c r="C7" s="29" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="D7" s="23" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="E7" s="23" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="F7" s="35" t="str">
         <f>VLOOKUP(B7,Lexique!A:F,5,)</f>
@@ -19715,10 +19718,10 @@
         <v>74</v>
       </c>
       <c r="C8" s="29" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="D8" s="23" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="E8" s="23" t="str">
         <f>D8</f>
@@ -19741,13 +19744,13 @@
         <v>72</v>
       </c>
       <c r="C9" s="29" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="D9" s="23" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="E9" s="23" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="F9" s="35" t="str">
         <f>VLOOKUP(B9,Lexique!A:F,5,)</f>
@@ -19766,10 +19769,10 @@
         <v>73</v>
       </c>
       <c r="C10" s="29" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="D10" s="23" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="E10" s="24" t="str">
         <f>D10</f>
@@ -19792,10 +19795,10 @@
         <v>73</v>
       </c>
       <c r="C11" s="29" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="D11" s="24" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="E11" s="24" t="str">
         <f>D11</f>
@@ -19818,10 +19821,10 @@
         <v>73</v>
       </c>
       <c r="C12" s="29" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="D12" s="23" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="E12" s="25" t="str">
         <f>D12</f>
@@ -19844,10 +19847,10 @@
         <v>72</v>
       </c>
       <c r="C13" s="29" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="D13" s="23" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="E13" s="25" t="str">
         <f t="shared" ref="E13:E17" si="0">D13</f>
@@ -19870,10 +19873,10 @@
         <v>73</v>
       </c>
       <c r="C14" s="29" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="D14" s="25" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="E14" s="25" t="str">
         <f t="shared" si="0"/>
@@ -19896,10 +19899,10 @@
         <v>72</v>
       </c>
       <c r="C15" s="29" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="D15" s="23" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="E15" s="25" t="str">
         <f t="shared" si="0"/>
@@ -19922,10 +19925,10 @@
         <v>73</v>
       </c>
       <c r="C16" s="29" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="D16" s="24" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="E16" s="25" t="str">
         <f t="shared" si="0"/>
@@ -19948,10 +19951,10 @@
         <v>73</v>
       </c>
       <c r="C17" s="29" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="D17" s="43" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="E17" s="25" t="str">
         <f t="shared" si="0"/>
@@ -19974,13 +19977,13 @@
         <v>76</v>
       </c>
       <c r="C18" s="29" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="D18" s="23" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="E18" s="23" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="F18" s="35" t="str">
         <f>VLOOKUP(B18,Lexique!A:F,5,)</f>
@@ -20000,13 +20003,13 @@
         <v>76</v>
       </c>
       <c r="C19" s="29" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="D19" s="23" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="E19" s="23" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="F19" s="35" t="str">
         <f>VLOOKUP(B19,Lexique!A:F,5,)</f>
@@ -20026,13 +20029,13 @@
         <v>71</v>
       </c>
       <c r="C20" s="29" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="D20" s="25" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="E20" s="25" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="F20" s="35" t="str">
         <f>VLOOKUP(B20,Lexique!A:F,5,)</f>
@@ -20052,13 +20055,13 @@
         <v>76</v>
       </c>
       <c r="C21" s="29" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="D21" s="23" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="E21" s="23" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="F21" s="35" t="str">
         <f>VLOOKUP(B21,Lexique!A:F,5,)</f>
@@ -20078,7 +20081,7 @@
         <v>78</v>
       </c>
       <c r="C22" s="29" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="D22" s="23" t="s">
         <v>155</v>
@@ -20104,13 +20107,13 @@
         <v>70</v>
       </c>
       <c r="C23" s="29" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="D23" s="23" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="E23" s="23" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="F23" s="35" t="str">
         <f>VLOOKUP(B23,Lexique!A:F,5,)</f>
@@ -20130,13 +20133,13 @@
         <v>76</v>
       </c>
       <c r="C24" s="29" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="D24" s="23" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="E24" s="23" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="F24" s="35" t="str">
         <f>VLOOKUP(B24,Lexique!A:F,5,)</f>
@@ -20156,13 +20159,13 @@
         <v>71</v>
       </c>
       <c r="C25" s="29" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="D25" s="25" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="E25" s="25" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="F25" s="35" t="str">
         <f>VLOOKUP(B25,Lexique!A:F,5,)</f>
@@ -20182,13 +20185,13 @@
         <v>81</v>
       </c>
       <c r="C26" s="29" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="D26" s="23" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="E26" s="23" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="F26" s="35" t="str">
         <f>VLOOKUP(B26,Lexique!A:F,5,)</f>
@@ -20208,13 +20211,13 @@
         <v>76</v>
       </c>
       <c r="C27" s="29" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="D27" s="23" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="E27" s="23" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="F27" s="35" t="str">
         <f>VLOOKUP(B27,Lexique!A:F,5,)</f>
@@ -20234,13 +20237,13 @@
         <v>76</v>
       </c>
       <c r="C28" s="29" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="D28" s="23" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="E28" s="23" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="F28" s="35" t="str">
         <f>VLOOKUP(B28,Lexique!A:F,5,)</f>
@@ -20260,13 +20263,13 @@
         <v>71</v>
       </c>
       <c r="C29" s="29" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="D29" s="25" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="E29" s="25" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="F29" s="35" t="str">
         <f>VLOOKUP(B29,Lexique!A:F,5,)</f>
@@ -20286,13 +20289,13 @@
         <v>70</v>
       </c>
       <c r="C30" s="29" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="D30" s="23" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="E30" s="23" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="F30" s="35" t="str">
         <f>VLOOKUP(B30,Lexique!A:F,5,)</f>
@@ -20312,13 +20315,13 @@
         <v>81</v>
       </c>
       <c r="C31" s="29" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="D31" s="23" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="E31" s="23" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="F31" s="35" t="str">
         <f>VLOOKUP(B31,Lexique!A:F,5,)</f>
@@ -20338,7 +20341,7 @@
         <v>78</v>
       </c>
       <c r="C32" s="29" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="D32" s="23" t="s">
         <v>154</v>
@@ -20364,13 +20367,13 @@
         <v>80</v>
       </c>
       <c r="C33" s="29" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="D33" s="23" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="E33" s="23" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="F33" s="35" t="str">
         <f>VLOOKUP(B33,Lexique!A:F,5,)</f>
@@ -20391,10 +20394,10 @@
       </c>
       <c r="C34" s="29"/>
       <c r="D34" s="26" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="E34" s="26" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="F34" s="35" t="str">
         <f>VLOOKUP(B34,Lexique!A:F,5,)</f>
@@ -20414,7 +20417,7 @@
         <v>43</v>
       </c>
       <c r="C35" s="29" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="D35" s="26" t="s">
         <v>109</v>

</xml_diff>

<commit_message>
Ajout sprint maire val-sennevilel
</commit_message>
<xml_diff>
--- a/excel/Itineraires.xlsx
+++ b/excel/Itineraires.xlsx
@@ -5,12 +5,12 @@
   <workbookPr date1904="1" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brunogauthier/Documents/guide2024/excel/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christinebeausoleil/Documents/TourAbitibi/Guide/guide2024/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B15BF596-67E1-0A4B-88D8-DD6508DA573E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F1B9273-0EBB-E54B-90D1-78B9C56E3856}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" tabRatio="758" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4340" yWindow="500" windowWidth="24460" windowHeight="17500" tabRatio="758" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="23" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1196" uniqueCount="620">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1199" uniqueCount="622">
   <si>
     <t>GPM</t>
   </si>
@@ -1902,6 +1902,12 @@
   </si>
   <si>
     <t>Stage 6 - Urban circuit</t>
+  </si>
+  <si>
+    <t>Sprint du maire de Senneterre 250$&lt;br/&gt;(Val-Senneville)</t>
+  </si>
+  <si>
+    <t>Senneterre Mayor's sprint 250$&lt;br/&gt;(Val-Senneville)</t>
   </si>
 </sst>
 </file>
@@ -6559,7 +6565,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF8C653E-9E00-4EDF-9978-201805372337}">
   <dimension ref="A1:AM14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AB1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView topLeftCell="AB1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="AE22" sqref="AE22"/>
     </sheetView>
   </sheetViews>
@@ -18611,10 +18617,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA4CF35A-AE95-4D4B-80F8-FB6E5D8CEEB2}">
-  <dimension ref="A1:I47"/>
+  <dimension ref="A1:I48"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
@@ -18868,17 +18874,17 @@
     </row>
     <row r="11" spans="1:9" ht="30" x14ac:dyDescent="0.2">
       <c r="A11" s="30">
-        <v>67.3</v>
+        <v>56.5</v>
       </c>
       <c r="B11" s="29" t="s">
         <v>70</v>
       </c>
       <c r="C11" s="29"/>
       <c r="D11" s="23" t="s">
-        <v>194</v>
+        <v>620</v>
       </c>
       <c r="E11" s="23" t="s">
-        <v>172</v>
+        <v>621</v>
       </c>
       <c r="F11" s="35" t="str">
         <f>VLOOKUP(B11,Lexique!A:F,5,)</f>
@@ -18890,81 +18896,81 @@
       </c>
       <c r="I11" s="6"/>
     </row>
-    <row r="12" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" ht="30" x14ac:dyDescent="0.2">
       <c r="A12" s="30">
-        <v>71</v>
+        <v>67.3</v>
       </c>
       <c r="B12" s="29" t="s">
-        <v>152</v>
+        <v>70</v>
       </c>
       <c r="C12" s="29"/>
       <c r="D12" s="23" t="s">
-        <v>182</v>
+        <v>194</v>
       </c>
       <c r="E12" s="23" t="s">
-        <v>181</v>
+        <v>172</v>
       </c>
       <c r="F12" s="35" t="str">
         <f>VLOOKUP(B12,Lexique!A:F,5,)</f>
-        <v>Zone déchets (sur xxx m)</v>
+        <v>Sprint bonification temps et points&lt;br/&gt; Lieu précis Ville</v>
       </c>
       <c r="G12" s="35" t="str">
         <f>VLOOKUP(B12,Lexique!A:F,6,)</f>
-        <v>Trash zone (on xxx m)</v>
+        <v>Bonification Sprint - times and points&lt;br/&gt; Lieu précis Ville</v>
       </c>
       <c r="I12" s="6"/>
     </row>
     <row r="13" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A13" s="30">
-        <v>72.3</v>
+        <v>71</v>
       </c>
       <c r="B13" s="29" t="s">
-        <v>82</v>
+        <v>152</v>
       </c>
       <c r="C13" s="29"/>
       <c r="D13" s="23" t="s">
-        <v>201</v>
+        <v>182</v>
       </c>
       <c r="E13" s="23" t="s">
-        <v>202</v>
+        <v>181</v>
       </c>
       <c r="F13" s="35" t="str">
         <f>VLOOKUP(B13,Lexique!A:F,5,)</f>
-        <v>Carrefour giratoire, Xe sortie tout droit/droite/gauche&lt;br/&gt;rue</v>
+        <v>Zone déchets (sur xxx m)</v>
       </c>
       <c r="G13" s="35" t="str">
         <f>VLOOKUP(B13,Lexique!A:F,6,)</f>
-        <v>Round about Xnd exit straight ahead/right/left&lt;br&gt; rue</v>
+        <v>Trash zone (on xxx m)</v>
       </c>
       <c r="I13" s="6"/>
     </row>
     <row r="14" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A14" s="30">
-        <v>72.8</v>
+        <v>72.3</v>
       </c>
       <c r="B14" s="29" t="s">
-        <v>25</v>
+        <v>82</v>
       </c>
       <c r="C14" s="29"/>
       <c r="D14" s="23" t="s">
-        <v>22</v>
+        <v>201</v>
       </c>
       <c r="E14" s="23" t="s">
-        <v>173</v>
+        <v>202</v>
       </c>
       <c r="F14" s="35" t="str">
         <f>VLOOKUP(B14,Lexique!A:F,5,)</f>
-        <v>Voie ferrée oblique / Pont de bois</v>
+        <v>Carrefour giratoire, Xe sortie tout droit/droite/gauche&lt;br/&gt;rue</v>
       </c>
       <c r="G14" s="35" t="str">
         <f>VLOOKUP(B14,Lexique!A:F,6,)</f>
-        <v>Oblique railroad crossing / Wooden bridge</v>
+        <v>Round about Xnd exit straight ahead/right/left&lt;br&gt; rue</v>
       </c>
       <c r="I14" s="6"/>
     </row>
     <row r="15" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A15" s="30">
-        <v>73.900000000000006</v>
+        <v>72.8</v>
       </c>
       <c r="B15" s="29" t="s">
         <v>25</v>
@@ -18988,211 +18994,210 @@
     </row>
     <row r="16" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A16" s="30">
-        <v>74.8</v>
+        <v>73.900000000000006</v>
       </c>
       <c r="B16" s="29" t="s">
-        <v>82</v>
+        <v>25</v>
       </c>
       <c r="C16" s="29"/>
       <c r="D16" s="23" t="s">
-        <v>201</v>
+        <v>22</v>
       </c>
       <c r="E16" s="23" t="s">
-        <v>202</v>
+        <v>173</v>
       </c>
       <c r="F16" s="35" t="str">
         <f>VLOOKUP(B16,Lexique!A:F,5,)</f>
-        <v>Carrefour giratoire, Xe sortie tout droit/droite/gauche&lt;br/&gt;rue</v>
+        <v>Voie ferrée oblique / Pont de bois</v>
       </c>
       <c r="G16" s="35" t="str">
         <f>VLOOKUP(B16,Lexique!A:F,6,)</f>
-        <v>Round about Xnd exit straight ahead/right/left&lt;br&gt; rue</v>
+        <v>Oblique railroad crossing / Wooden bridge</v>
       </c>
       <c r="I16" s="6"/>
     </row>
     <row r="17" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A17" s="30">
-        <v>96.1</v>
+        <v>74.8</v>
       </c>
       <c r="B17" s="29" t="s">
-        <v>71</v>
+        <v>82</v>
       </c>
       <c r="C17" s="29"/>
       <c r="D17" s="23" t="s">
-        <v>183</v>
+        <v>201</v>
       </c>
       <c r="E17" s="23" t="s">
-        <v>184</v>
+        <v>202</v>
       </c>
       <c r="F17" s="35" t="str">
         <f>VLOOKUP(B17,Lexique!A:F,5,)</f>
-        <v>Points GPM&lt;br/&gt; Lieu précis Ville</v>
+        <v>Carrefour giratoire, Xe sortie tout droit/droite/gauche&lt;br/&gt;rue</v>
       </c>
       <c r="G17" s="35" t="str">
         <f>VLOOKUP(B17,Lexique!A:F,6,)</f>
-        <v>KOM Points&lt;br/&gt; Lieu précis Ville</v>
+        <v>Round about Xnd exit straight ahead/right/left&lt;br&gt; rue</v>
       </c>
       <c r="I17" s="6"/>
     </row>
     <row r="18" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A18" s="30">
-        <v>103.3</v>
+        <v>96.1</v>
       </c>
       <c r="B18" s="29" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C18" s="29"/>
       <c r="D18" s="23" t="s">
-        <v>195</v>
-      </c>
-      <c r="E18" s="23" t="str">
-        <f>D18</f>
-        <v>Route 113</v>
+        <v>183</v>
+      </c>
+      <c r="E18" s="23" t="s">
+        <v>184</v>
       </c>
       <c r="F18" s="35" t="str">
         <f>VLOOKUP(B18,Lexique!A:F,5,)</f>
-        <v>Nom route / rue</v>
+        <v>Points GPM&lt;br/&gt; Lieu précis Ville</v>
       </c>
       <c r="G18" s="35" t="str">
         <f>VLOOKUP(B18,Lexique!A:F,6,)</f>
-        <v>Nom route / rue</v>
+        <v>KOM Points&lt;br/&gt; Lieu précis Ville</v>
       </c>
       <c r="I18" s="6"/>
     </row>
     <row r="19" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A19" s="30">
-        <v>116.6</v>
+        <v>103.3</v>
       </c>
       <c r="B19" s="29" t="s">
-        <v>5</v>
+        <v>73</v>
       </c>
       <c r="C19" s="29"/>
       <c r="D19" s="23" t="s">
-        <v>174</v>
-      </c>
-      <c r="E19" s="23" t="s">
-        <v>174</v>
+        <v>195</v>
+      </c>
+      <c r="E19" s="23" t="str">
+        <f>D19</f>
+        <v>Route 113</v>
       </c>
       <c r="F19" s="35" t="str">
         <f>VLOOKUP(B19,Lexique!A:F,5,)</f>
-        <v>Ville</v>
+        <v>Nom route / rue</v>
       </c>
       <c r="G19" s="35" t="str">
         <f>VLOOKUP(B19,Lexique!A:F,6,)</f>
-        <v>Ville</v>
+        <v>Nom route / rue</v>
       </c>
       <c r="I19" s="6"/>
     </row>
-    <row r="20" spans="1:9" ht="30" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A20" s="30">
-        <v>117</v>
+        <v>116.6</v>
       </c>
       <c r="B20" s="29" t="s">
-        <v>81</v>
+        <v>5</v>
       </c>
       <c r="C20" s="29"/>
       <c r="D20" s="23" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="E20" s="23" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="F20" s="35" t="str">
         <f>VLOOKUP(B20,Lexique!A:F,5,)</f>
-        <v>Sprint du maire Ville $250&lt;br/&gt; Lieu précis Ville</v>
+        <v>Ville</v>
       </c>
       <c r="G20" s="35" t="str">
         <f>VLOOKUP(B20,Lexique!A:F,6,)</f>
-        <v>Ville Mayor's sprint $250&lt;br/&gt; Lieu précis Ville</v>
+        <v>Ville</v>
       </c>
       <c r="I20" s="6"/>
     </row>
-    <row r="21" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" ht="30" x14ac:dyDescent="0.2">
       <c r="A21" s="30">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="B21" s="29" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="C21" s="29"/>
       <c r="D21" s="23" t="s">
-        <v>154</v>
+        <v>176</v>
       </c>
       <c r="E21" s="23" t="s">
-        <v>153</v>
+        <v>175</v>
       </c>
       <c r="F21" s="35" t="str">
         <f>VLOOKUP(B21,Lexique!A:F,5,)</f>
-        <v>Début du ravitaillement / Fin du ravitaillement</v>
+        <v>Sprint du maire Ville $250&lt;br/&gt; Lieu précis Ville</v>
       </c>
       <c r="G21" s="35" t="str">
         <f>VLOOKUP(B21,Lexique!A:F,6,)</f>
-        <v>Feed open / Feed closed</v>
+        <v>Ville Mayor's sprint $250&lt;br/&gt; Lieu précis Ville</v>
       </c>
       <c r="I21" s="6"/>
     </row>
     <row r="22" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A22" s="30">
-        <v>139</v>
+        <v>125</v>
       </c>
       <c r="B22" s="29" t="s">
-        <v>5</v>
+        <v>78</v>
       </c>
       <c r="C22" s="29"/>
       <c r="D22" s="23" t="s">
-        <v>131</v>
+        <v>154</v>
       </c>
       <c r="E22" s="23" t="s">
-        <v>131</v>
+        <v>153</v>
       </c>
       <c r="F22" s="35" t="str">
         <f>VLOOKUP(B22,Lexique!A:F,5,)</f>
-        <v>Ville</v>
+        <v>Début du ravitaillement / Fin du ravitaillement</v>
       </c>
       <c r="G22" s="35" t="str">
         <f>VLOOKUP(B22,Lexique!A:F,6,)</f>
-        <v>Ville</v>
+        <v>Feed open / Feed closed</v>
       </c>
       <c r="I22" s="6"/>
     </row>
     <row r="23" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A23" s="30">
-        <v>139.30000000000001</v>
+        <v>139</v>
       </c>
       <c r="B23" s="29" t="s">
-        <v>74</v>
+        <v>5</v>
       </c>
       <c r="C23" s="29"/>
       <c r="D23" s="23" t="s">
-        <v>203</v>
+        <v>131</v>
       </c>
       <c r="E23" s="23" t="s">
-        <v>204</v>
+        <v>131</v>
       </c>
       <c r="F23" s="35" t="str">
         <f>VLOOKUP(B23,Lexique!A:F,5,)</f>
-        <v>Nom route / rue</v>
+        <v>Ville</v>
       </c>
       <c r="G23" s="35" t="str">
         <f>VLOOKUP(B23,Lexique!A:F,6,)</f>
-        <v>Nom route / rue</v>
+        <v>Ville</v>
       </c>
       <c r="I23" s="6"/>
     </row>
     <row r="24" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A24" s="30">
-        <v>139.80000000000001</v>
+        <v>139.30000000000001</v>
       </c>
       <c r="B24" s="29" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="C24" s="29"/>
       <c r="D24" s="23" t="s">
-        <v>196</v>
-      </c>
-      <c r="E24" s="23" t="str">
-        <f>D24</f>
-        <v>10e Avenue/ Route 386</v>
+        <v>203</v>
+      </c>
+      <c r="E24" s="23" t="s">
+        <v>204</v>
       </c>
       <c r="F24" s="35" t="str">
         <f>VLOOKUP(B24,Lexique!A:F,5,)</f>
@@ -19206,17 +19211,18 @@
     </row>
     <row r="25" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A25" s="30">
-        <v>140.5</v>
+        <v>139.80000000000001</v>
       </c>
       <c r="B25" s="29" t="s">
         <v>72</v>
       </c>
       <c r="C25" s="29"/>
       <c r="D25" s="23" t="s">
-        <v>177</v>
-      </c>
-      <c r="E25" s="23" t="s">
-        <v>177</v>
+        <v>196</v>
+      </c>
+      <c r="E25" s="23" t="str">
+        <f>D25</f>
+        <v>10e Avenue/ Route 386</v>
       </c>
       <c r="F25" s="35" t="str">
         <f>VLOOKUP(B25,Lexique!A:F,5,)</f>
@@ -19230,17 +19236,17 @@
     </row>
     <row r="26" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A26" s="30">
-        <v>142.1</v>
+        <v>140.5</v>
       </c>
       <c r="B26" s="29" t="s">
         <v>72</v>
       </c>
       <c r="C26" s="29"/>
       <c r="D26" s="23" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E26" s="23" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F26" s="35" t="str">
         <f>VLOOKUP(B26,Lexique!A:F,5,)</f>
@@ -19254,17 +19260,17 @@
     </row>
     <row r="27" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A27" s="30">
-        <v>143.80000000000001</v>
+        <v>142.1</v>
       </c>
       <c r="B27" s="29" t="s">
         <v>72</v>
       </c>
       <c r="C27" s="29"/>
       <c r="D27" s="23" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E27" s="23" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="F27" s="35" t="str">
         <f>VLOOKUP(B27,Lexique!A:F,5,)</f>
@@ -19276,86 +19282,100 @@
       </c>
       <c r="I27" s="6"/>
     </row>
-    <row r="28" spans="1:9" ht="30" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A28" s="30">
-        <v>144.6</v>
+        <v>143.80000000000001</v>
       </c>
       <c r="B28" s="29" t="s">
-        <v>110</v>
+        <v>72</v>
       </c>
       <c r="C28" s="29"/>
       <c r="D28" s="23" t="s">
-        <v>197</v>
+        <v>179</v>
       </c>
       <c r="E28" s="23" t="s">
-        <v>198</v>
+        <v>179</v>
       </c>
       <c r="F28" s="35" t="str">
         <f>VLOOKUP(B28,Lexique!A:F,5,)</f>
-        <v>Déviation de la caravance&lt;br/&gt; À droite/gauche sur rue</v>
+        <v>Nom route / rue</v>
       </c>
       <c r="G28" s="35" t="str">
         <f>VLOOKUP(B28,Lexique!A:F,6,)</f>
-        <v>Caravan bypass&lt;br/&gt;Right/left on rue</v>
+        <v>Nom route / rue</v>
       </c>
       <c r="I28" s="6"/>
     </row>
-    <row r="29" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:9" ht="30" x14ac:dyDescent="0.2">
       <c r="A29" s="30">
-        <v>144.9</v>
+        <v>144.6</v>
       </c>
       <c r="B29" s="29" t="s">
-        <v>75</v>
+        <v>110</v>
       </c>
       <c r="C29" s="29"/>
       <c r="D29" s="23" t="s">
-        <v>180</v>
+        <v>197</v>
       </c>
       <c r="E29" s="23" t="s">
-        <v>180</v>
+        <v>198</v>
       </c>
       <c r="F29" s="35" t="str">
         <f>VLOOKUP(B29,Lexique!A:F,5,)</f>
-        <v>Nom route / rue</v>
+        <v>Déviation de la caravance&lt;br/&gt; À droite/gauche sur rue</v>
       </c>
       <c r="G29" s="35" t="str">
         <f>VLOOKUP(B29,Lexique!A:F,6,)</f>
-        <v>Nom route / rue</v>
+        <v>Caravan bypass&lt;br/&gt;Right/left on rue</v>
       </c>
       <c r="I29" s="6"/>
     </row>
-    <row r="30" spans="1:9" ht="30" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A30" s="30">
-        <v>145</v>
+        <v>144.9</v>
       </c>
       <c r="B30" s="29" t="s">
-        <v>43</v>
+        <v>75</v>
       </c>
       <c r="C30" s="29"/>
       <c r="D30" s="23" t="s">
-        <v>189</v>
+        <v>180</v>
       </c>
       <c r="E30" s="23" t="s">
-        <v>190</v>
+        <v>180</v>
       </c>
       <c r="F30" s="35" t="str">
         <f>VLOOKUP(B30,Lexique!A:F,5,)</f>
-        <v>Arrivée&lt;br/&gt;Bonification en temps et points</v>
+        <v>Nom route / rue</v>
       </c>
       <c r="G30" s="35" t="str">
         <f>VLOOKUP(B30,Lexique!A:F,6,)</f>
+        <v>Nom route / rue</v>
+      </c>
+      <c r="I30" s="6"/>
+    </row>
+    <row r="31" spans="1:9" ht="30" x14ac:dyDescent="0.2">
+      <c r="A31" s="30">
+        <v>145</v>
+      </c>
+      <c r="B31" s="29" t="s">
+        <v>43</v>
+      </c>
+      <c r="C31" s="29"/>
+      <c r="D31" s="23" t="s">
+        <v>189</v>
+      </c>
+      <c r="E31" s="23" t="s">
+        <v>190</v>
+      </c>
+      <c r="F31" s="35" t="str">
+        <f>VLOOKUP(B31,Lexique!A:F,5,)</f>
+        <v>Arrivée&lt;br/&gt;Bonification en temps et points</v>
+      </c>
+      <c r="G31" s="35" t="str">
+        <f>VLOOKUP(B31,Lexique!A:F,6,)</f>
         <v>Finish&lt;br/&gt;Time and points bonus</v>
       </c>
-      <c r="I30" s="6"/>
-    </row>
-    <row r="31" spans="1:9" ht="14" x14ac:dyDescent="0.2">
-      <c r="A31" s="30"/>
-      <c r="B31" s="29"/>
-      <c r="C31" s="29"/>
-      <c r="D31" s="23"/>
-      <c r="E31" s="23"/>
-      <c r="F31" s="35"/>
-      <c r="G31" s="35"/>
       <c r="I31" s="6"/>
     </row>
     <row r="32" spans="1:9" ht="14" x14ac:dyDescent="0.2">
@@ -19448,16 +19468,17 @@
       <c r="G40" s="35"/>
       <c r="I40" s="6"/>
     </row>
-    <row r="41" spans="1:9" ht="47.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="36"/>
-      <c r="B41" s="31"/>
-      <c r="C41" s="32"/>
+    <row r="41" spans="1:9" ht="14" x14ac:dyDescent="0.2">
+      <c r="A41" s="30"/>
+      <c r="B41" s="29"/>
+      <c r="C41" s="29"/>
       <c r="D41" s="23"/>
       <c r="E41" s="23"/>
       <c r="F41" s="35"/>
       <c r="G41" s="35"/>
-    </row>
-    <row r="42" spans="1:9" ht="14" x14ac:dyDescent="0.2">
+      <c r="I41" s="6"/>
+    </row>
+    <row r="42" spans="1:9" ht="47.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="36"/>
       <c r="B42" s="31"/>
       <c r="C42" s="32"/>
@@ -19497,6 +19518,8 @@
       <c r="A46" s="36"/>
       <c r="B46" s="31"/>
       <c r="C46" s="32"/>
+      <c r="D46" s="23"/>
+      <c r="E46" s="23"/>
       <c r="F46" s="35"/>
       <c r="G46" s="35"/>
     </row>
@@ -19506,6 +19529,13 @@
       <c r="C47" s="32"/>
       <c r="F47" s="35"/>
       <c r="G47" s="35"/>
+    </row>
+    <row r="48" spans="1:9" ht="14" x14ac:dyDescent="0.2">
+      <c r="A48" s="36"/>
+      <c r="B48" s="31"/>
+      <c r="C48" s="32"/>
+      <c r="F48" s="35"/>
+      <c r="G48" s="35"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
correction sprint pour mayor
</commit_message>
<xml_diff>
--- a/excel/Itineraires.xlsx
+++ b/excel/Itineraires.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christinebeausoleil/Documents/TourAbitibi/Guide/guide2024/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F1B9273-0EBB-E54B-90D1-78B9C56E3856}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B185EC86-69F4-034F-9660-F52D3CAC330D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4340" yWindow="500" windowWidth="24460" windowHeight="17500" tabRatio="758" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18620,7 +18620,7 @@
   <dimension ref="A1:I48"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A6" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
@@ -18877,7 +18877,7 @@
         <v>56.5</v>
       </c>
       <c r="B11" s="29" t="s">
-        <v>70</v>
+        <v>81</v>
       </c>
       <c r="C11" s="29"/>
       <c r="D11" s="23" t="s">
@@ -18888,11 +18888,11 @@
       </c>
       <c r="F11" s="35" t="str">
         <f>VLOOKUP(B11,Lexique!A:F,5,)</f>
-        <v>Sprint bonification temps et points&lt;br/&gt; Lieu précis Ville</v>
+        <v>Sprint du maire Ville $250&lt;br/&gt; Lieu précis Ville</v>
       </c>
       <c r="G11" s="35" t="str">
         <f>VLOOKUP(B11,Lexique!A:F,6,)</f>
-        <v>Bonification Sprint - times and points&lt;br/&gt; Lieu précis Ville</v>
+        <v>Ville Mayor's sprint $250&lt;br/&gt; Lieu précis Ville</v>
       </c>
       <c r="I11" s="6"/>
     </row>

</xml_diff>

<commit_message>
etape 7 ajustement des sprints
</commit_message>
<xml_diff>
--- a/excel/Itineraires.xlsx
+++ b/excel/Itineraires.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christinebeausoleil/Documents/TourAbitibi/Guide/guide2024/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B185EC86-69F4-034F-9660-F52D3CAC330D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAA94B8B-2D5D-B142-BA73-38371109F5C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4340" yWindow="500" windowWidth="24460" windowHeight="17500" tabRatio="758" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4340" yWindow="500" windowWidth="24460" windowHeight="17500" tabRatio="758" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="23" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1199" uniqueCount="622">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1202" uniqueCount="626">
   <si>
     <t>GPM</t>
   </si>
@@ -1637,39 +1637,12 @@
     <t>2e Avenue</t>
   </si>
   <si>
-    <t>Sprint de la Mairesse 250$ / Mayor Sprint</t>
-  </si>
-  <si>
-    <t>straigth</t>
-  </si>
-  <si>
-    <t>Début 3e tour (8 tours à faire)</t>
-  </si>
-  <si>
-    <t>Start of 3rd lap (8 laps to go)</t>
-  </si>
-  <si>
-    <t>Début 4e tour (7 à faire)&lt;br/&gt;Sprint bonification temps et points</t>
-  </si>
-  <si>
-    <t>Start of 4th lap (7 to go)&lt;br/&gt;Bonfication sprint - times and points</t>
-  </si>
-  <si>
-    <t>Début 5e tour (6 à faire)</t>
-  </si>
-  <si>
-    <t>Start of 5th lap (6 to go)</t>
-  </si>
-  <si>
     <t>Début 6e tour (5 à faire)</t>
   </si>
   <si>
     <t>Start of 6th lap (5 to go)</t>
   </si>
   <si>
-    <t>Sprint Bonif / 7e tour (4 à faire) / 7th lap (4 to go)</t>
-  </si>
-  <si>
     <t>Début 7e tour (4 à faire)&lt;br/&gt;Sprint bonification temps et points</t>
   </si>
   <si>
@@ -1685,12 +1658,6 @@
     <t>Start of 8th lap (3 to go)</t>
   </si>
   <si>
-    <t>Début 9e tour (2 tours à faire)&lt;br/&gt;Sprint de la Mairesse de Senneterre (250$)</t>
-  </si>
-  <si>
-    <t>Start of 9th lap (2 laps to go)&lt;br/&gt;Senneterre Mayor's sprint (250$)</t>
-  </si>
-  <si>
     <t>Dernier passage / last lap</t>
   </si>
   <si>
@@ -1908,6 +1875,51 @@
   </si>
   <si>
     <t>Senneterre Mayor's sprint 250$&lt;br/&gt;(Val-Senneville)</t>
+  </si>
+  <si>
+    <t>Début 4e tour (7 à faire)</t>
+  </si>
+  <si>
+    <t>Start of 4th lap (7 to go)</t>
+  </si>
+  <si>
+    <t>Début 9e tour (2 tours à faire)&lt;br/&gt;Sprint du Maire de Preissac (250$)</t>
+  </si>
+  <si>
+    <t>Start of 9th lap (2 laps to go)&lt;br/&gt;Preissac Mayor's sprint (250$)</t>
+  </si>
+  <si>
+    <t>Start of 3rd lap (8 laps to go)&lt;br/&gt;Bonfication sprint - times and points</t>
+  </si>
+  <si>
+    <t>Start of 5th lap (6 to go)&lt;br/&gt;Preissac Mayor's sprint (250$)</t>
+  </si>
+  <si>
+    <t>Début 5e tour (6 à faire)&lt;br/&gt;Sprint du Maire de Preissac (250$)</t>
+  </si>
+  <si>
+    <t>Début 3e tour (8 tours à faire)&lt;br/&gt;Sprint bonification temps et points</t>
+  </si>
+  <si>
+    <t>Fin du tour 1</t>
+  </si>
+  <si>
+    <t>Fin du tour 2</t>
+  </si>
+  <si>
+    <t>Fin du tour 4</t>
+  </si>
+  <si>
+    <t>fin du tour 5</t>
+  </si>
+  <si>
+    <t>Fin du tour 3</t>
+  </si>
+  <si>
+    <t>fin du tour 6</t>
+  </si>
+  <si>
+    <t>Fin du tour 8</t>
   </si>
 </sst>
 </file>
@@ -3093,15 +3105,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BF2EC7B-8CF4-1449-B844-A73E16F738A4}">
   <dimension ref="A1:G322"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="9.33203125" style="37" customWidth="1"/>
     <col min="2" max="2" width="11.83203125" style="33" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.5" style="34" customWidth="1"/>
+    <col min="3" max="3" width="34.83203125" style="34" customWidth="1"/>
     <col min="4" max="4" width="60.6640625" style="28" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="62.5" style="28" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="43" style="38" bestFit="1" customWidth="1"/>
@@ -3494,10 +3506,10 @@
         <v>506</v>
       </c>
       <c r="D16" s="44" t="s">
-        <v>604</v>
+        <v>593</v>
       </c>
       <c r="E16" s="62" t="s">
-        <v>605</v>
+        <v>594</v>
       </c>
       <c r="F16" s="35" t="str">
         <f>VLOOKUP(B16,Lexique!A:F,5,)</f>
@@ -3594,10 +3606,10 @@
         <v>527</v>
       </c>
       <c r="D20" s="44" t="s">
-        <v>606</v>
+        <v>595</v>
       </c>
       <c r="E20" s="62" t="s">
-        <v>607</v>
+        <v>596</v>
       </c>
       <c r="F20" s="35" t="str">
         <f>VLOOKUP(B20,Lexique!A:F,5,)</f>
@@ -3644,7 +3656,7 @@
         <v>514</v>
       </c>
       <c r="D22" s="23" t="s">
-        <v>603</v>
+        <v>592</v>
       </c>
       <c r="E22" s="23" t="s">
         <v>515</v>
@@ -3942,13 +3954,13 @@
         <v>76</v>
       </c>
       <c r="C34" s="32" t="s">
-        <v>532</v>
+        <v>619</v>
       </c>
       <c r="D34" s="23" t="s">
-        <v>608</v>
+        <v>597</v>
       </c>
       <c r="E34" s="23" t="s">
-        <v>609</v>
+        <v>598</v>
       </c>
       <c r="F34" s="35" t="str">
         <f>VLOOKUP(B34,Lexique!A:F,5,)</f>
@@ -3965,42 +3977,42 @@
         <v>79.599999999999994</v>
       </c>
       <c r="B35" s="31" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="C35" s="32" t="s">
-        <v>532</v>
+        <v>620</v>
       </c>
       <c r="D35" s="23" t="s">
-        <v>533</v>
+        <v>618</v>
       </c>
       <c r="E35" s="23" t="s">
-        <v>534</v>
+        <v>615</v>
       </c>
       <c r="F35" s="35" t="str">
         <f>VLOOKUP(B35,Lexique!A:F,5,)</f>
-        <v>Nom route / rue</v>
+        <v>Sprint bonification temps et points&lt;br/&gt; Lieu précis Ville</v>
       </c>
       <c r="G35" s="35" t="str">
         <f>VLOOKUP(B35,Lexique!A:F,6,)</f>
-        <v>Nom route / rue</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" ht="14" x14ac:dyDescent="0.2">
+        <v>Bonification Sprint - times and points&lt;br/&gt; Lieu précis Ville</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="15" x14ac:dyDescent="0.2">
       <c r="A36" s="37">
         <f>A35+5.175</f>
         <v>84.774999999999991</v>
       </c>
-      <c r="B36" s="31" t="s">
-        <v>70</v>
-      </c>
-      <c r="C36" s="32">
-        <v>4</v>
+      <c r="B36" s="29" t="s">
+        <v>76</v>
+      </c>
+      <c r="C36" s="32" t="s">
+        <v>623</v>
       </c>
       <c r="D36" s="27" t="s">
-        <v>535</v>
+        <v>611</v>
       </c>
       <c r="E36" s="27" t="s">
-        <v>536</v>
+        <v>612</v>
       </c>
       <c r="F36" s="35"/>
       <c r="G36" s="35"/>
@@ -4011,16 +4023,16 @@
         <v>89.949999999999989</v>
       </c>
       <c r="B37" s="31" t="s">
-        <v>76</v>
-      </c>
-      <c r="C37" s="32">
-        <v>5</v>
+        <v>81</v>
+      </c>
+      <c r="C37" s="32" t="s">
+        <v>621</v>
       </c>
       <c r="D37" s="27" t="s">
-        <v>537</v>
+        <v>617</v>
       </c>
       <c r="E37" s="27" t="s">
-        <v>538</v>
+        <v>616</v>
       </c>
       <c r="F37" s="35"/>
       <c r="G37" s="35"/>
@@ -4052,14 +4064,14 @@
       <c r="B39" s="31" t="s">
         <v>76</v>
       </c>
-      <c r="C39" s="32">
-        <v>6</v>
+      <c r="C39" s="32" t="s">
+        <v>622</v>
       </c>
       <c r="D39" s="27" t="s">
-        <v>539</v>
+        <v>531</v>
       </c>
       <c r="E39" s="27" t="s">
-        <v>540</v>
+        <v>532</v>
       </c>
       <c r="F39" s="35"/>
       <c r="G39" s="35"/>
@@ -4072,13 +4084,13 @@
         <v>70</v>
       </c>
       <c r="C40" s="32" t="s">
-        <v>541</v>
+        <v>624</v>
       </c>
       <c r="D40" s="27" t="s">
-        <v>542</v>
+        <v>533</v>
       </c>
       <c r="E40" s="27" t="s">
-        <v>543</v>
+        <v>534</v>
       </c>
       <c r="F40" s="35"/>
       <c r="G40" s="35"/>
@@ -4118,13 +4130,13 @@
         <v>76</v>
       </c>
       <c r="C42" s="32" t="s">
-        <v>544</v>
+        <v>535</v>
       </c>
       <c r="D42" s="27" t="s">
-        <v>545</v>
+        <v>536</v>
       </c>
       <c r="E42" s="27" t="s">
-        <v>546</v>
+        <v>537</v>
       </c>
       <c r="F42" s="35"/>
       <c r="G42" s="35"/>
@@ -4138,13 +4150,13 @@
         <v>81</v>
       </c>
       <c r="C43" s="32" t="s">
-        <v>531</v>
+        <v>625</v>
       </c>
       <c r="D43" s="23" t="s">
-        <v>547</v>
+        <v>613</v>
       </c>
       <c r="E43" s="23" t="s">
-        <v>548</v>
+        <v>614</v>
       </c>
       <c r="F43" s="35"/>
       <c r="G43" s="35"/>
@@ -4158,13 +4170,13 @@
         <v>76</v>
       </c>
       <c r="C44" s="32" t="s">
-        <v>549</v>
+        <v>538</v>
       </c>
       <c r="D44" s="27" t="s">
-        <v>550</v>
+        <v>539</v>
       </c>
       <c r="E44" s="27" t="s">
-        <v>551</v>
+        <v>540</v>
       </c>
       <c r="F44" s="35"/>
       <c r="G44" s="35"/>
@@ -4178,7 +4190,7 @@
         <v>110</v>
       </c>
       <c r="C45" s="32" t="s">
-        <v>552</v>
+        <v>541</v>
       </c>
       <c r="D45" s="27" t="s">
         <v>347</v>
@@ -6742,7 +6754,7 @@
         <v>44027</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>610</v>
+        <v>599</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>208</v>
@@ -6836,7 +6848,7 @@
         <v>129</v>
       </c>
       <c r="AG2" s="16" t="s">
-        <v>617</v>
+        <v>606</v>
       </c>
       <c r="AH2" s="16" t="str">
         <f>Tableau2[[#This Row],[LieuDepFR]]</f>
@@ -6869,7 +6881,7 @@
         <v>44028</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>611</v>
+        <v>600</v>
       </c>
       <c r="F3" s="4" t="s">
         <v>209</v>
@@ -6963,7 +6975,7 @@
         <v>126</v>
       </c>
       <c r="AG3" s="16" t="s">
-        <v>617</v>
+        <v>606</v>
       </c>
       <c r="AH3" s="16" t="str">
         <f>Tableau2[[#This Row],[LieuDepFR]]</f>
@@ -6996,7 +7008,7 @@
         <v>44029</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>612</v>
+        <v>601</v>
       </c>
       <c r="F4" s="4" t="s">
         <v>207</v>
@@ -7128,7 +7140,7 @@
         <v>44029</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>613</v>
+        <v>602</v>
       </c>
       <c r="F5" s="4" t="s">
         <v>230</v>
@@ -7256,7 +7268,7 @@
         <v>44030</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>614</v>
+        <v>603</v>
       </c>
       <c r="F6" s="4" t="s">
         <v>228</v>
@@ -7347,7 +7359,7 @@
         <v>215</v>
       </c>
       <c r="AF6" s="16" t="s">
-        <v>617</v>
+        <v>606</v>
       </c>
       <c r="AG6" s="16" t="s">
         <v>235</v>
@@ -7472,7 +7484,7 @@
       </c>
       <c r="AE7" s="16"/>
       <c r="AF7" s="21" t="s">
-        <v>617</v>
+        <v>606</v>
       </c>
       <c r="AG7" s="16" t="str">
         <f>Tableau2[[#This Row],[LieuDepFR]]</f>
@@ -7485,10 +7497,10 @@
         <v>219</v>
       </c>
       <c r="AJ7" s="4" t="s">
-        <v>618</v>
+        <v>607</v>
       </c>
       <c r="AK7" s="4" t="s">
-        <v>619</v>
+        <v>608</v>
       </c>
       <c r="AL7" s="15"/>
       <c r="AM7" s="15"/>
@@ -7508,7 +7520,7 @@
         <v>44032</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>615</v>
+        <v>604</v>
       </c>
       <c r="F8" s="4" t="s">
         <v>211</v>
@@ -7599,7 +7611,7 @@
         <v>216</v>
       </c>
       <c r="AF8" s="16" t="s">
-        <v>617</v>
+        <v>606</v>
       </c>
       <c r="AG8" s="16" t="s">
         <v>217</v>
@@ -8598,7 +8610,7 @@
         <v>300</v>
       </c>
       <c r="D38" s="23" t="s">
-        <v>616</v>
+        <v>605</v>
       </c>
       <c r="E38" s="23" t="s">
         <v>333</v>
@@ -10177,7 +10189,7 @@
         <v>22</v>
       </c>
       <c r="E3" s="23" t="s">
-        <v>553</v>
+        <v>542</v>
       </c>
       <c r="F3" s="35" t="str">
         <f>VLOOKUP(B3,Lexique!A:F,5,)</f>
@@ -10196,13 +10208,13 @@
         <v>72</v>
       </c>
       <c r="C4" s="29" t="s">
-        <v>554</v>
+        <v>543</v>
       </c>
       <c r="D4" s="23" t="s">
-        <v>555</v>
+        <v>544</v>
       </c>
       <c r="E4" s="23" t="s">
-        <v>555</v>
+        <v>544</v>
       </c>
       <c r="F4" s="35" t="str">
         <f>VLOOKUP(B4,Lexique!A:F,5,)</f>
@@ -10221,13 +10233,13 @@
         <v>82</v>
       </c>
       <c r="C5" s="29" t="s">
-        <v>556</v>
+        <v>545</v>
       </c>
       <c r="D5" s="23" t="s">
-        <v>595</v>
+        <v>584</v>
       </c>
       <c r="E5" s="23" t="s">
-        <v>596</v>
+        <v>585</v>
       </c>
       <c r="F5" s="35" t="str">
         <f>VLOOKUP(B5,Lexique!A:F,5,)</f>
@@ -10246,13 +10258,13 @@
         <v>82</v>
       </c>
       <c r="C6" s="29" t="s">
-        <v>557</v>
+        <v>546</v>
       </c>
       <c r="D6" s="23" t="s">
-        <v>593</v>
+        <v>582</v>
       </c>
       <c r="E6" s="23" t="s">
-        <v>594</v>
+        <v>583</v>
       </c>
       <c r="F6" s="35" t="str">
         <f>VLOOKUP(B6,Lexique!A:F,5,)</f>
@@ -10271,7 +10283,7 @@
         <v>79</v>
       </c>
       <c r="C7" s="29" t="s">
-        <v>558</v>
+        <v>547</v>
       </c>
       <c r="D7" s="23" t="s">
         <v>10</v>
@@ -10296,13 +10308,13 @@
         <v>73</v>
       </c>
       <c r="C8" s="29" t="s">
-        <v>559</v>
+        <v>548</v>
       </c>
       <c r="D8" s="23" t="s">
-        <v>560</v>
+        <v>549</v>
       </c>
       <c r="E8" s="23" t="s">
-        <v>560</v>
+        <v>549</v>
       </c>
       <c r="F8" s="35" t="str">
         <f>VLOOKUP(B8,Lexique!A:F,5,)</f>
@@ -10321,10 +10333,10 @@
         <v>5</v>
       </c>
       <c r="C9" s="29" t="s">
-        <v>581</v>
+        <v>570</v>
       </c>
       <c r="D9" s="23" t="s">
-        <v>581</v>
+        <v>570</v>
       </c>
       <c r="E9" s="23" t="str">
         <f>D9</f>
@@ -10347,13 +10359,13 @@
         <v>81</v>
       </c>
       <c r="C10" s="29" t="s">
-        <v>561</v>
+        <v>550</v>
       </c>
       <c r="D10" s="23" t="s">
-        <v>583</v>
+        <v>572</v>
       </c>
       <c r="E10" s="24" t="s">
-        <v>582</v>
+        <v>571</v>
       </c>
       <c r="F10" s="35" t="str">
         <f>VLOOKUP(B10,Lexique!A:F,5,)</f>
@@ -10378,7 +10390,7 @@
         <v>12</v>
       </c>
       <c r="E11" s="23" t="s">
-        <v>562</v>
+        <v>551</v>
       </c>
       <c r="F11" s="35" t="str">
         <f>VLOOKUP(B11,Lexique!A:F,5,)</f>
@@ -10400,10 +10412,10 @@
         <v>265</v>
       </c>
       <c r="D12" s="23" t="s">
-        <v>587</v>
+        <v>576</v>
       </c>
       <c r="E12" s="23" t="s">
-        <v>588</v>
+        <v>577</v>
       </c>
       <c r="F12" s="35" t="str">
         <f>VLOOKUP(B12,Lexique!A:F,5,)</f>
@@ -10423,7 +10435,7 @@
         <v>78</v>
       </c>
       <c r="C13" s="29" t="s">
-        <v>563</v>
+        <v>552</v>
       </c>
       <c r="D13" s="23" t="s">
         <v>155</v>
@@ -10448,13 +10460,13 @@
         <v>72</v>
       </c>
       <c r="C14" s="29" t="s">
-        <v>564</v>
+        <v>553</v>
       </c>
       <c r="D14" s="25" t="s">
-        <v>565</v>
+        <v>554</v>
       </c>
       <c r="E14" s="25" t="s">
-        <v>565</v>
+        <v>554</v>
       </c>
       <c r="F14" s="35" t="str">
         <f>VLOOKUP(B14,Lexique!A:F,5,)</f>
@@ -10523,13 +10535,13 @@
         <v>5</v>
       </c>
       <c r="C17" s="29" t="s">
-        <v>566</v>
+        <v>555</v>
       </c>
       <c r="D17" s="26" t="s">
-        <v>567</v>
+        <v>556</v>
       </c>
       <c r="E17" s="25" t="s">
-        <v>567</v>
+        <v>556</v>
       </c>
       <c r="F17" s="35" t="str">
         <f>VLOOKUP(B17,Lexique!A:F,5,)</f>
@@ -10548,13 +10560,13 @@
         <v>70</v>
       </c>
       <c r="C18" s="29" t="s">
-        <v>568</v>
+        <v>557</v>
       </c>
       <c r="D18" s="23" t="s">
-        <v>584</v>
+        <v>573</v>
       </c>
       <c r="E18" s="23" t="s">
-        <v>569</v>
+        <v>558</v>
       </c>
       <c r="F18" s="35" t="str">
         <f>VLOOKUP(B18,Lexique!A:F,5,)</f>
@@ -10579,7 +10591,7 @@
         <v>22</v>
       </c>
       <c r="E19" s="23" t="s">
-        <v>553</v>
+        <v>542</v>
       </c>
       <c r="F19" s="35" t="str">
         <f>VLOOKUP(B19,Lexique!A:F,5,)</f>
@@ -10598,13 +10610,13 @@
         <v>152</v>
       </c>
       <c r="C20" s="29" t="s">
-        <v>570</v>
+        <v>559</v>
       </c>
       <c r="D20" s="25" t="s">
-        <v>570</v>
+        <v>559</v>
       </c>
       <c r="E20" s="25" t="s">
-        <v>571</v>
+        <v>560</v>
       </c>
       <c r="F20" s="35" t="str">
         <f>VLOOKUP(B20,Lexique!A:F,5,)</f>
@@ -10626,10 +10638,10 @@
         <v>265</v>
       </c>
       <c r="D21" s="23" t="s">
-        <v>589</v>
+        <v>578</v>
       </c>
       <c r="E21" s="23" t="s">
-        <v>590</v>
+        <v>579</v>
       </c>
       <c r="F21" s="35" t="str">
         <f>VLOOKUP(B21,Lexique!A:F,5,)</f>
@@ -10673,7 +10685,7 @@
         <v>25</v>
       </c>
       <c r="C23" s="29" t="s">
-        <v>572</v>
+        <v>561</v>
       </c>
       <c r="D23" s="23" t="s">
         <v>2</v>
@@ -10698,13 +10710,13 @@
         <v>81</v>
       </c>
       <c r="C24" s="29" t="s">
-        <v>561</v>
+        <v>550</v>
       </c>
       <c r="D24" s="23" t="s">
-        <v>601</v>
+        <v>590</v>
       </c>
       <c r="E24" s="24" t="s">
-        <v>602</v>
+        <v>591</v>
       </c>
       <c r="F24" s="35" t="str">
         <f>VLOOKUP(B24,Lexique!A:F,5,)</f>
@@ -10724,7 +10736,7 @@
         <v>78</v>
       </c>
       <c r="C25" s="29" t="s">
-        <v>573</v>
+        <v>562</v>
       </c>
       <c r="D25" s="25" t="s">
         <v>154</v>
@@ -10749,10 +10761,10 @@
         <v>5</v>
       </c>
       <c r="C26" s="29" t="s">
-        <v>599</v>
+        <v>588</v>
       </c>
       <c r="D26" s="25" t="s">
-        <v>600</v>
+        <v>589</v>
       </c>
       <c r="E26" s="25" t="str">
         <f>D26</f>
@@ -10775,13 +10787,13 @@
         <v>82</v>
       </c>
       <c r="C27" s="29" t="s">
-        <v>574</v>
+        <v>563</v>
       </c>
       <c r="D27" s="23" t="s">
-        <v>591</v>
+        <v>580</v>
       </c>
       <c r="E27" s="23" t="s">
-        <v>592</v>
+        <v>581</v>
       </c>
       <c r="F27" s="35" t="str">
         <f>VLOOKUP(B27,Lexique!A:F,5,)</f>
@@ -10806,7 +10818,7 @@
         <v>22</v>
       </c>
       <c r="E28" s="23" t="s">
-        <v>553</v>
+        <v>542</v>
       </c>
       <c r="F28" s="35" t="str">
         <f>VLOOKUP(B28,Lexique!A:F,5,)</f>
@@ -10825,7 +10837,7 @@
         <v>72</v>
       </c>
       <c r="C29" s="29" t="s">
-        <v>575</v>
+        <v>564</v>
       </c>
       <c r="D29" s="25" t="s">
         <v>512</v>
@@ -10850,13 +10862,13 @@
         <v>76</v>
       </c>
       <c r="C30" s="29" t="s">
-        <v>576</v>
+        <v>565</v>
       </c>
       <c r="D30" s="23" t="s">
         <v>336</v>
       </c>
       <c r="E30" s="23" t="s">
-        <v>586</v>
+        <v>575</v>
       </c>
       <c r="F30" s="35" t="str">
         <f>VLOOKUP(B30,Lexique!A:F,5,)</f>
@@ -11000,7 +11012,7 @@
         <v>73</v>
       </c>
       <c r="C36" s="29" t="s">
-        <v>577</v>
+        <v>566</v>
       </c>
       <c r="D36" s="23" t="s">
         <v>524</v>
@@ -11100,13 +11112,13 @@
         <v>70</v>
       </c>
       <c r="C40" s="29" t="s">
-        <v>578</v>
+        <v>567</v>
       </c>
       <c r="D40" s="23" t="s">
-        <v>597</v>
+        <v>586</v>
       </c>
       <c r="E40" s="23" t="s">
-        <v>598</v>
+        <v>587</v>
       </c>
       <c r="F40" s="35" t="str">
         <f>VLOOKUP(B40,Lexique!A:F,5,)</f>
@@ -11125,13 +11137,13 @@
         <v>80</v>
       </c>
       <c r="C41" s="34" t="s">
-        <v>579</v>
+        <v>568</v>
       </c>
       <c r="D41" s="23" t="s">
-        <v>580</v>
+        <v>569</v>
       </c>
       <c r="E41" s="23" t="s">
-        <v>585</v>
+        <v>574</v>
       </c>
       <c r="F41" s="35" t="str">
         <f>VLOOKUP(B41,Lexique!A:F,5,)</f>
@@ -11150,7 +11162,7 @@
         <v>110</v>
       </c>
       <c r="C42" s="34" t="s">
-        <v>552</v>
+        <v>541</v>
       </c>
       <c r="D42" s="63" t="s">
         <v>347</v>
@@ -15813,7 +15825,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD202D62-DD01-6144-9D35-8AFF416A0F43}">
   <dimension ref="A1:G320"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView topLeftCell="A3" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
@@ -18619,7 +18631,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA4CF35A-AE95-4D4B-80F8-FB6E5D8CEEB2}">
   <dimension ref="A1:I48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView topLeftCell="A6" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
@@ -18881,10 +18893,10 @@
       </c>
       <c r="C11" s="29"/>
       <c r="D11" s="23" t="s">
-        <v>620</v>
+        <v>609</v>
       </c>
       <c r="E11" s="23" t="s">
-        <v>621</v>
+        <v>610</v>
       </c>
       <c r="F11" s="35" t="str">
         <f>VLOOKUP(B11,Lexique!A:F,5,)</f>
@@ -19547,7 +19559,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AEBDB8C-6DC2-3445-97F3-86408AFF8E25}">
   <dimension ref="A1:G321"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView topLeftCell="A11" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Compil guides - ajout sprint maire Preissac
* Tableaux descriptifs
* Élévations
* Cartes complètes
</commit_message>
<xml_diff>
--- a/excel/Itineraires.xlsx
+++ b/excel/Itineraires.xlsx
@@ -5,12 +5,12 @@
   <workbookPr date1904="1" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christinebeausoleil/Documents/TourAbitibi/Guide/guide2024/excel/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brunogauthier/Documents/guide2024/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAA94B8B-2D5D-B142-BA73-38371109F5C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12A15BAE-CA1F-6A43-8A87-7C3C6DA5DBB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4340" yWindow="500" windowWidth="24460" windowHeight="17500" tabRatio="758" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="21140" yWindow="1500" windowWidth="43900" windowHeight="25600" tabRatio="758" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="23" r:id="rId1"/>
@@ -1871,12 +1871,6 @@
     <t>Stage 6 - Urban circuit</t>
   </si>
   <si>
-    <t>Sprint du maire de Senneterre 250$&lt;br/&gt;(Val-Senneville)</t>
-  </si>
-  <si>
-    <t>Senneterre Mayor's sprint 250$&lt;br/&gt;(Val-Senneville)</t>
-  </si>
-  <si>
     <t>Début 4e tour (7 à faire)</t>
   </si>
   <si>
@@ -1920,6 +1914,12 @@
   </si>
   <si>
     <t>Fin du tour 8</t>
+  </si>
+  <si>
+    <t>Sprint du maire de Senneterre 250$&lt;br/&gt;(Chemin Paré - Val-Senneville)</t>
+  </si>
+  <si>
+    <t>Senneterre Mayor's sprint 250$&lt;br/&gt;(Chemin Paré -Val-Senneville)</t>
   </si>
 </sst>
 </file>
@@ -3105,8 +3105,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BF2EC7B-8CF4-1449-B844-A73E16F738A4}">
   <dimension ref="A1:G322"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="C44" sqref="C44"/>
+    <sheetView topLeftCell="A20" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
@@ -3194,7 +3194,7 @@
         <v>Nom route / rue</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" s="30">
         <v>0.31</v>
       </c>
@@ -3244,7 +3244,7 @@
         <v>Nom route / rue</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" ht="15" x14ac:dyDescent="0.2">
       <c r="A6" s="30">
         <v>0.71</v>
       </c>
@@ -3645,7 +3645,7 @@
         <v>Nom route / rue</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="30" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" ht="15" x14ac:dyDescent="0.2">
       <c r="A22" s="30">
         <v>69.25</v>
       </c>
@@ -3770,7 +3770,7 @@
         <v>KOM Points&lt;br/&gt; Lieu précis Ville</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="30" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7" ht="15" x14ac:dyDescent="0.2">
       <c r="A27" s="30">
         <v>70.62</v>
       </c>
@@ -3820,7 +3820,7 @@
         <v>Nom route / rue</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="30" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:7" ht="15" x14ac:dyDescent="0.2">
       <c r="A29" s="30">
         <v>71.98</v>
       </c>
@@ -3954,7 +3954,7 @@
         <v>76</v>
       </c>
       <c r="C34" s="32" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="D34" s="23" t="s">
         <v>597</v>
@@ -3980,13 +3980,13 @@
         <v>70</v>
       </c>
       <c r="C35" s="32" t="s">
-        <v>620</v>
+        <v>618</v>
       </c>
       <c r="D35" s="23" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
       <c r="E35" s="23" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="F35" s="35" t="str">
         <f>VLOOKUP(B35,Lexique!A:F,5,)</f>
@@ -4006,13 +4006,13 @@
         <v>76</v>
       </c>
       <c r="C36" s="32" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
       <c r="D36" s="27" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
       <c r="E36" s="27" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
       <c r="F36" s="35"/>
       <c r="G36" s="35"/>
@@ -4026,13 +4026,13 @@
         <v>81</v>
       </c>
       <c r="C37" s="32" t="s">
-        <v>621</v>
+        <v>619</v>
       </c>
       <c r="D37" s="27" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
       <c r="E37" s="27" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="F37" s="35"/>
       <c r="G37" s="35"/>
@@ -4065,7 +4065,7 @@
         <v>76</v>
       </c>
       <c r="C39" s="32" t="s">
-        <v>622</v>
+        <v>620</v>
       </c>
       <c r="D39" s="27" t="s">
         <v>531</v>
@@ -4084,7 +4084,7 @@
         <v>70</v>
       </c>
       <c r="C40" s="32" t="s">
-        <v>624</v>
+        <v>622</v>
       </c>
       <c r="D40" s="27" t="s">
         <v>533</v>
@@ -4150,13 +4150,13 @@
         <v>81</v>
       </c>
       <c r="C43" s="32" t="s">
-        <v>625</v>
+        <v>623</v>
       </c>
       <c r="D43" s="23" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="E43" s="23" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="F43" s="35"/>
       <c r="G43" s="35"/>
@@ -18631,8 +18631,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA4CF35A-AE95-4D4B-80F8-FB6E5D8CEEB2}">
   <dimension ref="A1:I48"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
@@ -18893,10 +18893,10 @@
       </c>
       <c r="C11" s="29"/>
       <c r="D11" s="23" t="s">
-        <v>609</v>
+        <v>624</v>
       </c>
       <c r="E11" s="23" t="s">
-        <v>610</v>
+        <v>625</v>
       </c>
       <c r="F11" s="35" t="str">
         <f>VLOOKUP(B11,Lexique!A:F,5,)</f>

</xml_diff>

<commit_message>
Corr rue Allard - CLMI
</commit_message>
<xml_diff>
--- a/excel/Itineraires.xlsx
+++ b/excel/Itineraires.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brunogauthier/Documents/guide2024/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12A15BAE-CA1F-6A43-8A87-7C3C6DA5DBB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9271C75-9C79-EC4F-9FDF-ECF6E92435D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21140" yWindow="1500" windowWidth="43900" windowHeight="25600" tabRatio="758" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" tabRatio="758" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="23" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1202" uniqueCount="626">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1204" uniqueCount="626">
   <si>
     <t>GPM</t>
   </si>
@@ -1163,9 +1163,6 @@
     <t>On the right side of the central median</t>
   </si>
   <si>
-    <t>Left of the central median&lt;br/&gt;before the 7th street intersection&lt;br/&gt;Start of counterflow traffic (southbound lane)</t>
-  </si>
-  <si>
     <t>Tour observation Rotary&lt;br/&gt;Stationnement</t>
   </si>
   <si>
@@ -1283,9 +1280,6 @@
     <t>Boulevard des Pins&lt;br/&gt;Sharp turn in the descent</t>
   </si>
   <si>
-    <t>À gauche du terre-plein&lt;br/&gt;avant intersection 7e rue&lt;br/&gt;Début circulation à contre-sens (voie sud)</t>
-  </si>
-  <si>
     <t>À gauche du terre-plein avant interserction&lt;br/&gt;Début circulation à contre-sens (voie est)</t>
   </si>
   <si>
@@ -1920,6 +1914,12 @@
   </si>
   <si>
     <t>Senneterre Mayor's sprint 250$&lt;br/&gt;(Chemin Paré -Val-Senneville)</t>
+  </si>
+  <si>
+    <t>À gauche du terre-plein&lt;br/&gt;intersection 7e rue&lt;br/&gt;Début circulation à contre-sens (voie sud)</t>
+  </si>
+  <si>
+    <t>Left of the central median&lt;br/&gt;7th street intersection&lt;br/&gt;Start of counterflow traffic (southbound lane)</t>
   </si>
 </sst>
 </file>
@@ -3155,10 +3155,10 @@
         <v>262</v>
       </c>
       <c r="D2" s="23" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="E2" s="23" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="F2" s="35" t="str">
         <f>VLOOKUP(B2,Lexique!A:F,5,)</f>
@@ -3177,13 +3177,13 @@
         <v>76</v>
       </c>
       <c r="C3" s="29" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="D3" s="23" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="E3" s="23" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="F3" s="35" t="str">
         <f>VLOOKUP(B3,Lexique!A:F,5,)</f>
@@ -3202,13 +3202,13 @@
         <v>73</v>
       </c>
       <c r="C4" s="29" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="D4" s="23" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="E4" s="23" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="F4" s="35" t="str">
         <f>VLOOKUP(B4,Lexique!A:F,5,)</f>
@@ -3227,13 +3227,13 @@
         <v>75</v>
       </c>
       <c r="C5" s="29" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="D5" s="23" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="E5" s="23" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="F5" s="35" t="str">
         <f>VLOOKUP(B5,Lexique!A:F,5,)</f>
@@ -3252,13 +3252,13 @@
         <v>75</v>
       </c>
       <c r="C6" s="29" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="D6" s="23" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="E6" s="23" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="F6" s="35" t="str">
         <f>VLOOKUP(B6,Lexique!A:F,5,)</f>
@@ -3277,7 +3277,7 @@
         <v>25</v>
       </c>
       <c r="C7" s="29" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="D7" s="23" t="s">
         <v>2</v>
@@ -3327,7 +3327,7 @@
         <v>25</v>
       </c>
       <c r="C9" s="29" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="D9" s="23" t="s">
         <v>2</v>
@@ -3353,7 +3353,7 @@
         <v>78</v>
       </c>
       <c r="C10" s="29" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="D10" s="23" t="s">
         <v>155</v>
@@ -3378,7 +3378,7 @@
         <v>72</v>
       </c>
       <c r="C11" s="29" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="D11" s="23" t="s">
         <v>165</v>
@@ -3403,7 +3403,7 @@
         <v>76</v>
       </c>
       <c r="C12" s="29" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="D12" s="23" t="s">
         <v>165</v>
@@ -3431,10 +3431,10 @@
         <v>265</v>
       </c>
       <c r="D13" s="23" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="E13" s="23" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="F13" s="35" t="str">
         <f>VLOOKUP(B13,Lexique!A:F,5,)</f>
@@ -3453,7 +3453,7 @@
         <v>25</v>
       </c>
       <c r="C14" s="29" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="D14" s="23" t="s">
         <v>2</v>
@@ -3478,13 +3478,13 @@
         <v>5</v>
       </c>
       <c r="C15" s="29" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="D15" s="23" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="E15" s="23" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="F15" s="35" t="str">
         <f>VLOOKUP(B15,Lexique!A:F,5,)</f>
@@ -3503,13 +3503,13 @@
         <v>82</v>
       </c>
       <c r="C16" s="29" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="D16" s="44" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
       <c r="E16" s="62" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="F16" s="35" t="str">
         <f>VLOOKUP(B16,Lexique!A:F,5,)</f>
@@ -3528,13 +3528,13 @@
         <v>25</v>
       </c>
       <c r="C17" s="29" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="D17" s="24" t="s">
         <v>22</v>
       </c>
       <c r="E17" s="25" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="F17" s="35" t="str">
         <f>VLOOKUP(B17,Lexique!A:F,5,)</f>
@@ -3553,13 +3553,13 @@
         <v>25</v>
       </c>
       <c r="C18" s="29" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="D18" s="24" t="s">
         <v>22</v>
       </c>
       <c r="E18" s="25" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="F18" s="35" t="str">
         <f>VLOOKUP(B18,Lexique!A:F,5,)</f>
@@ -3578,13 +3578,13 @@
         <v>25</v>
       </c>
       <c r="C19" s="29" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="D19" s="24" t="s">
         <v>22</v>
       </c>
       <c r="E19" s="25" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="F19" s="35" t="str">
         <f>VLOOKUP(B19,Lexique!A:F,5,)</f>
@@ -3603,13 +3603,13 @@
         <v>82</v>
       </c>
       <c r="C20" s="29" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="D20" s="44" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="E20" s="62" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
       <c r="F20" s="35" t="str">
         <f>VLOOKUP(B20,Lexique!A:F,5,)</f>
@@ -3628,13 +3628,13 @@
         <v>72</v>
       </c>
       <c r="C21" s="29" t="s">
+        <v>509</v>
+      </c>
+      <c r="D21" s="25" t="s">
+        <v>510</v>
+      </c>
+      <c r="E21" s="25" t="s">
         <v>511</v>
-      </c>
-      <c r="D21" s="25" t="s">
-        <v>512</v>
-      </c>
-      <c r="E21" s="25" t="s">
-        <v>513</v>
       </c>
       <c r="F21" s="35" t="str">
         <f>VLOOKUP(B21,Lexique!A:F,5,)</f>
@@ -3653,13 +3653,13 @@
         <v>76</v>
       </c>
       <c r="C22" s="29" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="D22" s="23" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
       <c r="E22" s="23" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="F22" s="35" t="str">
         <f>VLOOKUP(B22,Lexique!A:F,5,)</f>
@@ -3678,7 +3678,7 @@
         <v>73</v>
       </c>
       <c r="C23" s="29" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="D23" s="23" t="s">
         <v>338</v>
@@ -3703,13 +3703,13 @@
         <v>72</v>
       </c>
       <c r="C24" s="29" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="D24" s="23" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="E24" s="23" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="F24" s="35" t="str">
         <f>VLOOKUP(B24,Lexique!A:F,5,)</f>
@@ -3728,13 +3728,13 @@
         <v>73</v>
       </c>
       <c r="C25" s="29" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="D25" s="23" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="E25" s="23" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="F25" s="35" t="str">
         <f>VLOOKUP(B25,Lexique!A:F,5,)</f>
@@ -3756,10 +3756,10 @@
         <v>265</v>
       </c>
       <c r="D26" s="23" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="E26" s="23" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="F26" s="35" t="str">
         <f>VLOOKUP(B26,Lexique!A:F,5,)</f>
@@ -3778,7 +3778,7 @@
         <v>73</v>
       </c>
       <c r="C27" s="29" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="D27" s="26" t="s">
         <v>340</v>
@@ -3803,13 +3803,13 @@
         <v>72</v>
       </c>
       <c r="C28" s="29" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="D28" s="23" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="E28" s="23" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="F28" s="35" t="str">
         <f>VLOOKUP(B28,Lexique!A:F,5,)</f>
@@ -3828,13 +3828,13 @@
         <v>73</v>
       </c>
       <c r="C29" s="29" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="D29" s="23" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="E29" s="23" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="F29" s="35" t="str">
         <f>VLOOKUP(B29,Lexique!A:F,5,)</f>
@@ -3853,13 +3853,13 @@
         <v>73</v>
       </c>
       <c r="C30" s="29" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="D30" s="24" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="E30" s="24" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="F30" s="35" t="str">
         <f>VLOOKUP(B30,Lexique!A:F,5,)</f>
@@ -3878,13 +3878,13 @@
         <v>72</v>
       </c>
       <c r="C31" s="29" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="D31" s="23" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="E31" s="23" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="F31" s="35" t="str">
         <f>VLOOKUP(B31,Lexique!A:F,5,)</f>
@@ -3903,7 +3903,7 @@
         <v>73</v>
       </c>
       <c r="C32" s="29" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D32" s="24" t="s">
         <v>334</v>
@@ -3928,13 +3928,13 @@
         <v>73</v>
       </c>
       <c r="C33" s="29" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="D33" s="23" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="E33" s="23" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="F33" s="35" t="str">
         <f>VLOOKUP(B33,Lexique!A:F,5,)</f>
@@ -3954,13 +3954,13 @@
         <v>76</v>
       </c>
       <c r="C34" s="32" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
       <c r="D34" s="23" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
       <c r="E34" s="23" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
       <c r="F34" s="35" t="str">
         <f>VLOOKUP(B34,Lexique!A:F,5,)</f>
@@ -3980,13 +3980,13 @@
         <v>70</v>
       </c>
       <c r="C35" s="32" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
       <c r="D35" s="23" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="E35" s="23" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="F35" s="35" t="str">
         <f>VLOOKUP(B35,Lexique!A:F,5,)</f>
@@ -4006,13 +4006,13 @@
         <v>76</v>
       </c>
       <c r="C36" s="32" t="s">
-        <v>621</v>
+        <v>619</v>
       </c>
       <c r="D36" s="27" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="E36" s="27" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
       <c r="F36" s="35"/>
       <c r="G36" s="35"/>
@@ -4026,13 +4026,13 @@
         <v>81</v>
       </c>
       <c r="C37" s="32" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="D37" s="27" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="E37" s="27" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="F37" s="35"/>
       <c r="G37" s="35"/>
@@ -4048,10 +4048,10 @@
         <v>265</v>
       </c>
       <c r="D38" s="23" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="E38" s="23" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="F38" s="35"/>
       <c r="G38" s="35"/>
@@ -4065,13 +4065,13 @@
         <v>76</v>
       </c>
       <c r="C39" s="32" t="s">
-        <v>620</v>
+        <v>618</v>
       </c>
       <c r="D39" s="27" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="E39" s="27" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="F39" s="35"/>
       <c r="G39" s="35"/>
@@ -4084,13 +4084,13 @@
         <v>70</v>
       </c>
       <c r="C40" s="32" t="s">
-        <v>622</v>
+        <v>620</v>
       </c>
       <c r="D40" s="27" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="E40" s="27" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="F40" s="35"/>
       <c r="G40" s="35"/>
@@ -4104,7 +4104,7 @@
         <v>78</v>
       </c>
       <c r="C41" s="29" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="D41" s="23" t="s">
         <v>154</v>
@@ -4130,13 +4130,13 @@
         <v>76</v>
       </c>
       <c r="C42" s="32" t="s">
+        <v>533</v>
+      </c>
+      <c r="D42" s="27" t="s">
+        <v>534</v>
+      </c>
+      <c r="E42" s="27" t="s">
         <v>535</v>
-      </c>
-      <c r="D42" s="27" t="s">
-        <v>536</v>
-      </c>
-      <c r="E42" s="27" t="s">
-        <v>537</v>
       </c>
       <c r="F42" s="35"/>
       <c r="G42" s="35"/>
@@ -4150,13 +4150,13 @@
         <v>81</v>
       </c>
       <c r="C43" s="32" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
       <c r="D43" s="23" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
       <c r="E43" s="23" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
       <c r="F43" s="35"/>
       <c r="G43" s="35"/>
@@ -4170,13 +4170,13 @@
         <v>76</v>
       </c>
       <c r="C44" s="32" t="s">
+        <v>536</v>
+      </c>
+      <c r="D44" s="27" t="s">
+        <v>537</v>
+      </c>
+      <c r="E44" s="27" t="s">
         <v>538</v>
-      </c>
-      <c r="D44" s="27" t="s">
-        <v>539</v>
-      </c>
-      <c r="E44" s="27" t="s">
-        <v>540</v>
       </c>
       <c r="F44" s="35"/>
       <c r="G44" s="35"/>
@@ -4190,7 +4190,7 @@
         <v>110</v>
       </c>
       <c r="C45" s="32" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="D45" s="27" t="s">
         <v>347</v>
@@ -6754,7 +6754,7 @@
         <v>44027</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>208</v>
@@ -6848,7 +6848,7 @@
         <v>129</v>
       </c>
       <c r="AG2" s="16" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
       <c r="AH2" s="16" t="str">
         <f>Tableau2[[#This Row],[LieuDepFR]]</f>
@@ -6881,7 +6881,7 @@
         <v>44028</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
       <c r="F3" s="4" t="s">
         <v>209</v>
@@ -6975,7 +6975,7 @@
         <v>126</v>
       </c>
       <c r="AG3" s="16" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
       <c r="AH3" s="16" t="str">
         <f>Tableau2[[#This Row],[LieuDepFR]]</f>
@@ -7008,7 +7008,7 @@
         <v>44029</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="F4" s="4" t="s">
         <v>207</v>
@@ -7140,7 +7140,7 @@
         <v>44029</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
       <c r="F5" s="4" t="s">
         <v>230</v>
@@ -7268,7 +7268,7 @@
         <v>44030</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="F6" s="4" t="s">
         <v>228</v>
@@ -7359,7 +7359,7 @@
         <v>215</v>
       </c>
       <c r="AF6" s="16" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
       <c r="AG6" s="16" t="s">
         <v>235</v>
@@ -7445,7 +7445,7 @@
         <v>42</v>
       </c>
       <c r="T7" s="14" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="U7" t="str">
         <f>TEXT(_xlfn.CONCAT(Tableau2[[#This Row],[Heure_dep]],":",Tableau2[[#This Row],[min_dep]]), "HH:MM")</f>
@@ -7484,7 +7484,7 @@
       </c>
       <c r="AE7" s="16"/>
       <c r="AF7" s="21" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
       <c r="AG7" s="16" t="str">
         <f>Tableau2[[#This Row],[LieuDepFR]]</f>
@@ -7497,10 +7497,10 @@
         <v>219</v>
       </c>
       <c r="AJ7" s="4" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
       <c r="AK7" s="4" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="AL7" s="15"/>
       <c r="AM7" s="15"/>
@@ -7520,7 +7520,7 @@
         <v>44032</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="F8" s="4" t="s">
         <v>211</v>
@@ -7570,7 +7570,7 @@
         <v>42</v>
       </c>
       <c r="T8" s="14" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="U8" t="str">
         <f>TEXT(_xlfn.CONCAT(Tableau2[[#This Row],[Heure_dep]],":",Tableau2[[#This Row],[min_dep]]), "HH:MM")</f>
@@ -7611,7 +7611,7 @@
         <v>216</v>
       </c>
       <c r="AF8" s="16" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
       <c r="AG8" s="16" t="s">
         <v>217</v>
@@ -7701,10 +7701,10 @@
         <v>262</v>
       </c>
       <c r="D2" s="23" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="E2" s="23" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="F2" s="35" t="str">
         <f>VLOOKUP(B2,Lexique!A:F,5,)</f>
@@ -8530,13 +8530,13 @@
         <v>71</v>
       </c>
       <c r="C35" s="29" t="s">
+        <v>419</v>
+      </c>
+      <c r="D35" s="25" t="s">
+        <v>420</v>
+      </c>
+      <c r="E35" s="25" t="s">
         <v>421</v>
-      </c>
-      <c r="D35" s="25" t="s">
-        <v>422</v>
-      </c>
-      <c r="E35" s="25" t="s">
-        <v>423</v>
       </c>
       <c r="F35" s="35" t="str">
         <f>VLOOKUP(B35,Lexique!A:F,5,)</f>
@@ -8610,7 +8610,7 @@
         <v>300</v>
       </c>
       <c r="D38" s="23" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
       <c r="E38" s="23" t="s">
         <v>333</v>
@@ -8948,7 +8948,7 @@
         <v>345</v>
       </c>
       <c r="E51" s="26" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="F51" s="35" t="str">
         <f>VLOOKUP(B51,Lexique!A:F,5,)</f>
@@ -10161,10 +10161,10 @@
         <v>262</v>
       </c>
       <c r="D2" s="23" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="E2" s="23" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="F2" s="35" t="str">
         <f>VLOOKUP(B2,Lexique!A:F,5,)</f>
@@ -10189,7 +10189,7 @@
         <v>22</v>
       </c>
       <c r="E3" s="23" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="F3" s="35" t="str">
         <f>VLOOKUP(B3,Lexique!A:F,5,)</f>
@@ -10208,13 +10208,13 @@
         <v>72</v>
       </c>
       <c r="C4" s="29" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="D4" s="23" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
       <c r="E4" s="23" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
       <c r="F4" s="35" t="str">
         <f>VLOOKUP(B4,Lexique!A:F,5,)</f>
@@ -10233,13 +10233,13 @@
         <v>82</v>
       </c>
       <c r="C5" s="29" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
       <c r="D5" s="23" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
       <c r="E5" s="23" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="F5" s="35" t="str">
         <f>VLOOKUP(B5,Lexique!A:F,5,)</f>
@@ -10258,13 +10258,13 @@
         <v>82</v>
       </c>
       <c r="C6" s="29" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="D6" s="23" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
       <c r="E6" s="23" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="F6" s="35" t="str">
         <f>VLOOKUP(B6,Lexique!A:F,5,)</f>
@@ -10283,7 +10283,7 @@
         <v>79</v>
       </c>
       <c r="C7" s="29" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="D7" s="23" t="s">
         <v>10</v>
@@ -10308,13 +10308,13 @@
         <v>73</v>
       </c>
       <c r="C8" s="29" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
       <c r="D8" s="23" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="E8" s="23" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="F8" s="35" t="str">
         <f>VLOOKUP(B8,Lexique!A:F,5,)</f>
@@ -10333,10 +10333,10 @@
         <v>5</v>
       </c>
       <c r="C9" s="29" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
       <c r="D9" s="23" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
       <c r="E9" s="23" t="str">
         <f>D9</f>
@@ -10359,13 +10359,13 @@
         <v>81</v>
       </c>
       <c r="C10" s="29" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="D10" s="23" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
       <c r="E10" s="24" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="F10" s="35" t="str">
         <f>VLOOKUP(B10,Lexique!A:F,5,)</f>
@@ -10390,7 +10390,7 @@
         <v>12</v>
       </c>
       <c r="E11" s="23" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
       <c r="F11" s="35" t="str">
         <f>VLOOKUP(B11,Lexique!A:F,5,)</f>
@@ -10412,10 +10412,10 @@
         <v>265</v>
       </c>
       <c r="D12" s="23" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
       <c r="E12" s="23" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="F12" s="35" t="str">
         <f>VLOOKUP(B12,Lexique!A:F,5,)</f>
@@ -10435,7 +10435,7 @@
         <v>78</v>
       </c>
       <c r="C13" s="29" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="D13" s="23" t="s">
         <v>155</v>
@@ -10460,13 +10460,13 @@
         <v>72</v>
       </c>
       <c r="C14" s="29" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="D14" s="25" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
       <c r="E14" s="25" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
       <c r="F14" s="35" t="str">
         <f>VLOOKUP(B14,Lexique!A:F,5,)</f>
@@ -10485,7 +10485,7 @@
         <v>25</v>
       </c>
       <c r="C15" s="29" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="D15" s="23" t="s">
         <v>2</v>
@@ -10510,7 +10510,7 @@
         <v>25</v>
       </c>
       <c r="C16" s="29" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="D16" s="23" t="s">
         <v>2</v>
@@ -10535,13 +10535,13 @@
         <v>5</v>
       </c>
       <c r="C17" s="29" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="D17" s="26" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="E17" s="25" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="F17" s="35" t="str">
         <f>VLOOKUP(B17,Lexique!A:F,5,)</f>
@@ -10560,13 +10560,13 @@
         <v>70</v>
       </c>
       <c r="C18" s="29" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="D18" s="23" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
       <c r="E18" s="23" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
       <c r="F18" s="35" t="str">
         <f>VLOOKUP(B18,Lexique!A:F,5,)</f>
@@ -10591,7 +10591,7 @@
         <v>22</v>
       </c>
       <c r="E19" s="23" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="F19" s="35" t="str">
         <f>VLOOKUP(B19,Lexique!A:F,5,)</f>
@@ -10610,13 +10610,13 @@
         <v>152</v>
       </c>
       <c r="C20" s="29" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="D20" s="25" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="E20" s="25" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="F20" s="35" t="str">
         <f>VLOOKUP(B20,Lexique!A:F,5,)</f>
@@ -10638,10 +10638,10 @@
         <v>265</v>
       </c>
       <c r="D21" s="23" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="E21" s="23" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="F21" s="35" t="str">
         <f>VLOOKUP(B21,Lexique!A:F,5,)</f>
@@ -10660,7 +10660,7 @@
         <v>25</v>
       </c>
       <c r="C22" s="29" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="D22" s="23" t="s">
         <v>2</v>
@@ -10685,7 +10685,7 @@
         <v>25</v>
       </c>
       <c r="C23" s="29" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="D23" s="23" t="s">
         <v>2</v>
@@ -10710,13 +10710,13 @@
         <v>81</v>
       </c>
       <c r="C24" s="29" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="D24" s="23" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
       <c r="E24" s="24" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="F24" s="35" t="str">
         <f>VLOOKUP(B24,Lexique!A:F,5,)</f>
@@ -10736,7 +10736,7 @@
         <v>78</v>
       </c>
       <c r="C25" s="29" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="D25" s="25" t="s">
         <v>154</v>
@@ -10761,10 +10761,10 @@
         <v>5</v>
       </c>
       <c r="C26" s="29" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
       <c r="D26" s="25" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
       <c r="E26" s="25" t="str">
         <f>D26</f>
@@ -10787,13 +10787,13 @@
         <v>82</v>
       </c>
       <c r="C27" s="29" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="D27" s="23" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
       <c r="E27" s="23" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
       <c r="F27" s="35" t="str">
         <f>VLOOKUP(B27,Lexique!A:F,5,)</f>
@@ -10818,7 +10818,7 @@
         <v>22</v>
       </c>
       <c r="E28" s="23" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="F28" s="35" t="str">
         <f>VLOOKUP(B28,Lexique!A:F,5,)</f>
@@ -10837,13 +10837,13 @@
         <v>72</v>
       </c>
       <c r="C29" s="29" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="D29" s="25" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="E29" s="25" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="F29" s="35" t="str">
         <f>VLOOKUP(B29,Lexique!A:F,5,)</f>
@@ -10862,13 +10862,13 @@
         <v>76</v>
       </c>
       <c r="C30" s="29" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
       <c r="D30" s="23" t="s">
         <v>336</v>
       </c>
       <c r="E30" s="23" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="F30" s="35" t="str">
         <f>VLOOKUP(B30,Lexique!A:F,5,)</f>
@@ -10887,7 +10887,7 @@
         <v>73</v>
       </c>
       <c r="C31" s="29" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="D31" s="23" t="s">
         <v>338</v>
@@ -10912,13 +10912,13 @@
         <v>72</v>
       </c>
       <c r="C32" s="29" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="D32" s="63" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="E32" s="28" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="F32" s="35" t="str">
         <f>VLOOKUP(B32,Lexique!A:F,5,)</f>
@@ -10937,13 +10937,13 @@
         <v>73</v>
       </c>
       <c r="C33" s="29" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="D33" s="23" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="E33" s="23" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="F33" s="35" t="str">
         <f>VLOOKUP(B33,Lexique!A:F,5,)</f>
@@ -10965,10 +10965,10 @@
         <v>265</v>
       </c>
       <c r="D34" s="23" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="E34" s="23" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="F34" s="35" t="str">
         <f>VLOOKUP(B34,Lexique!A:F,5,)</f>
@@ -10987,7 +10987,7 @@
         <v>73</v>
       </c>
       <c r="C35" s="29" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="D35" s="26" t="s">
         <v>340</v>
@@ -11012,13 +11012,13 @@
         <v>73</v>
       </c>
       <c r="C36" s="29" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
       <c r="D36" s="23" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="E36" s="23" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="F36" s="35" t="str">
         <f>VLOOKUP(B36,Lexique!A:F,5,)</f>
@@ -11037,13 +11037,13 @@
         <v>72</v>
       </c>
       <c r="C37" s="29" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="D37" s="23" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="E37" s="23" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="F37" s="35" t="str">
         <f>VLOOKUP(B37,Lexique!A:F,5,)</f>
@@ -11062,7 +11062,7 @@
         <v>73</v>
       </c>
       <c r="C38" s="29" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D38" s="24" t="s">
         <v>334</v>
@@ -11087,13 +11087,13 @@
         <v>73</v>
       </c>
       <c r="C39" s="29" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="D39" s="23" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="E39" s="23" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="F39" s="35" t="str">
         <f>VLOOKUP(B39,Lexique!A:F,5,)</f>
@@ -11112,13 +11112,13 @@
         <v>70</v>
       </c>
       <c r="C40" s="29" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
       <c r="D40" s="23" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
       <c r="E40" s="23" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
       <c r="F40" s="35" t="str">
         <f>VLOOKUP(B40,Lexique!A:F,5,)</f>
@@ -11137,13 +11137,13 @@
         <v>80</v>
       </c>
       <c r="C41" s="34" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="D41" s="23" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="E41" s="23" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
       <c r="F41" s="35" t="str">
         <f>VLOOKUP(B41,Lexique!A:F,5,)</f>
@@ -11162,7 +11162,7 @@
         <v>110</v>
       </c>
       <c r="C42" s="34" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="D42" s="63" t="s">
         <v>347</v>
@@ -13147,10 +13147,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D75B715-9E33-8E4E-9ACA-D6CC0A1B5E86}">
-  <dimension ref="A1:G325"/>
+  <dimension ref="A1:G326"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
@@ -13197,10 +13197,10 @@
       </c>
       <c r="C2" s="29"/>
       <c r="D2" s="23" t="s">
+        <v>379</v>
+      </c>
+      <c r="E2" s="23" t="s">
         <v>380</v>
-      </c>
-      <c r="E2" s="23" t="s">
-        <v>381</v>
       </c>
       <c r="F2" s="47" t="str">
         <f>VLOOKUP(B2,Lexique!A:F,5,)</f>
@@ -13213,20 +13213,21 @@
     </row>
     <row r="3" spans="1:7" ht="15" x14ac:dyDescent="0.15">
       <c r="A3" s="30">
-        <v>0.83</v>
+        <v>0.6</v>
       </c>
       <c r="B3" s="29" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C3" s="29" t="s">
-        <v>358</v>
-      </c>
-      <c r="D3" s="23" t="s">
-        <v>358</v>
+        <v>367</v>
+      </c>
+      <c r="D3" s="23" t="str">
+        <f>C3</f>
+        <v>Rue Allard</v>
       </c>
       <c r="E3" s="23" t="str">
         <f>D3</f>
-        <v>Boulevard Dennisson</v>
+        <v>Rue Allard</v>
       </c>
       <c r="F3" s="47" t="str">
         <f>VLOOKUP(B3,Lexique!A:F,5,)</f>
@@ -13239,19 +13240,20 @@
     </row>
     <row r="4" spans="1:7" ht="15" x14ac:dyDescent="0.15">
       <c r="A4" s="30">
-        <v>0.98</v>
+        <v>0.83</v>
       </c>
       <c r="B4" s="29" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C4" s="29" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="D4" s="23" t="s">
-        <v>371</v>
-      </c>
-      <c r="E4" s="23" t="s">
-        <v>372</v>
+        <v>358</v>
+      </c>
+      <c r="E4" s="23" t="str">
+        <f>D4</f>
+        <v>Boulevard Dennisson</v>
       </c>
       <c r="F4" s="47" t="str">
         <f>VLOOKUP(B4,Lexique!A:F,5,)</f>
@@ -13264,20 +13266,19 @@
     </row>
     <row r="5" spans="1:7" ht="15" x14ac:dyDescent="0.15">
       <c r="A5" s="30">
-        <v>1.69</v>
+        <v>0.98</v>
       </c>
       <c r="B5" s="29" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C5" s="29" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="D5" s="23" t="s">
-        <v>364</v>
-      </c>
-      <c r="E5" s="23" t="str">
-        <f>D5</f>
-        <v>Rue Self</v>
+        <v>371</v>
+      </c>
+      <c r="E5" s="23" t="s">
+        <v>372</v>
       </c>
       <c r="F5" s="47" t="str">
         <f>VLOOKUP(B5,Lexique!A:F,5,)</f>
@@ -13288,21 +13289,22 @@
         <v>Nom route / rue</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:7" ht="15" x14ac:dyDescent="0.15">
       <c r="A6" s="30">
-        <v>2.58</v>
+        <v>1.69</v>
       </c>
       <c r="B6" s="29" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C6" s="29" t="s">
-        <v>370</v>
+        <v>360</v>
       </c>
       <c r="D6" s="23" t="s">
-        <v>413</v>
-      </c>
-      <c r="E6" s="23" t="s">
-        <v>373</v>
+        <v>364</v>
+      </c>
+      <c r="E6" s="23" t="str">
+        <f>D6</f>
+        <v>Rue Self</v>
       </c>
       <c r="F6" s="47" t="str">
         <f>VLOOKUP(B6,Lexique!A:F,5,)</f>
@@ -13313,22 +13315,21 @@
         <v>Nom route / rue</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:7" ht="30" x14ac:dyDescent="0.15">
       <c r="A7" s="30">
-        <v>2.7</v>
+        <v>2.58</v>
       </c>
       <c r="B7" s="29" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C7" s="29" t="s">
-        <v>331</v>
+        <v>370</v>
       </c>
       <c r="D7" s="23" t="s">
-        <v>331</v>
-      </c>
-      <c r="E7" s="23" t="str">
-        <f>D7</f>
-        <v>Boulevard des Pins</v>
+        <v>624</v>
+      </c>
+      <c r="E7" s="23" t="s">
+        <v>625</v>
       </c>
       <c r="F7" s="47" t="str">
         <f>VLOOKUP(B7,Lexique!A:F,5,)</f>
@@ -13341,20 +13342,20 @@
     </row>
     <row r="8" spans="1:7" ht="15" x14ac:dyDescent="0.15">
       <c r="A8" s="30">
-        <v>3.71</v>
+        <v>2.7</v>
       </c>
       <c r="B8" s="29" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="C8" s="29" t="s">
-        <v>328</v>
+        <v>331</v>
       </c>
       <c r="D8" s="23" t="s">
-        <v>328</v>
+        <v>331</v>
       </c>
       <c r="E8" s="23" t="str">
-        <f t="shared" ref="E8:E17" si="0">D8</f>
-        <v>Boulevard Sabourin</v>
+        <f>D8</f>
+        <v>Boulevard des Pins</v>
       </c>
       <c r="F8" s="47" t="str">
         <f>VLOOKUP(B8,Lexique!A:F,5,)</f>
@@ -13367,19 +13368,20 @@
     </row>
     <row r="9" spans="1:7" ht="15" x14ac:dyDescent="0.15">
       <c r="A9" s="30">
-        <v>4.04</v>
+        <v>3.71</v>
       </c>
       <c r="B9" s="29" t="s">
         <v>73</v>
       </c>
       <c r="C9" s="29" t="s">
-        <v>361</v>
+        <v>328</v>
       </c>
       <c r="D9" s="23" t="s">
-        <v>374</v>
-      </c>
-      <c r="E9" s="23" t="s">
-        <v>375</v>
+        <v>328</v>
+      </c>
+      <c r="E9" s="23" t="str">
+        <f t="shared" ref="E9:E18" si="0">D9</f>
+        <v>Boulevard Sabourin</v>
       </c>
       <c r="F9" s="47" t="str">
         <f>VLOOKUP(B9,Lexique!A:F,5,)</f>
@@ -13392,69 +13394,69 @@
     </row>
     <row r="10" spans="1:7" ht="15" x14ac:dyDescent="0.15">
       <c r="A10" s="30">
-        <v>4.1399999999999997</v>
+        <v>4.04</v>
       </c>
       <c r="B10" s="29" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C10" s="29" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="D10" s="23" t="s">
-        <v>362</v>
+        <v>373</v>
       </c>
       <c r="E10" s="23" t="s">
-        <v>379</v>
+        <v>374</v>
       </c>
       <c r="F10" s="47" t="str">
         <f>VLOOKUP(B10,Lexique!A:F,5,)</f>
-        <v>Demi-tour</v>
+        <v>Nom route / rue</v>
       </c>
       <c r="G10" s="47" t="str">
         <f>VLOOKUP(B10,Lexique!A:F,6,)</f>
-        <v>U-turn</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.15">
+        <v>Nom route / rue</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="15" x14ac:dyDescent="0.15">
       <c r="A11" s="30">
-        <v>4.24</v>
+        <v>4.1399999999999997</v>
       </c>
       <c r="B11" s="29" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="C11" s="29" t="s">
-        <v>363</v>
-      </c>
-      <c r="D11" s="49" t="s">
-        <v>376</v>
+        <v>362</v>
+      </c>
+      <c r="D11" s="23" t="s">
+        <v>362</v>
       </c>
       <c r="E11" s="23" t="s">
         <v>378</v>
       </c>
       <c r="F11" s="47" t="str">
         <f>VLOOKUP(B11,Lexique!A:F,5,)</f>
-        <v>Nom route / rue</v>
+        <v>Demi-tour</v>
       </c>
       <c r="G11" s="47" t="str">
         <f>VLOOKUP(B11,Lexique!A:F,6,)</f>
-        <v>Nom route / rue</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="15" x14ac:dyDescent="0.15">
+        <v>U-turn</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="30" x14ac:dyDescent="0.15">
       <c r="A12" s="30">
-        <v>4.54</v>
+        <v>4.24</v>
       </c>
       <c r="B12" s="29" t="s">
         <v>72</v>
       </c>
       <c r="C12" s="29" t="s">
-        <v>331</v>
-      </c>
-      <c r="D12" s="23" t="s">
-        <v>382</v>
+        <v>363</v>
+      </c>
+      <c r="D12" s="49" t="s">
+        <v>375</v>
       </c>
       <c r="E12" s="23" t="s">
-        <v>412</v>
+        <v>377</v>
       </c>
       <c r="F12" s="47" t="str">
         <f>VLOOKUP(B12,Lexique!A:F,5,)</f>
@@ -13467,72 +13469,72 @@
     </row>
     <row r="13" spans="1:7" ht="15" x14ac:dyDescent="0.15">
       <c r="A13" s="30">
+        <v>4.54</v>
+      </c>
+      <c r="B13" s="29" t="s">
+        <v>72</v>
+      </c>
+      <c r="C13" s="29" t="s">
+        <v>331</v>
+      </c>
+      <c r="D13" s="23" t="s">
+        <v>381</v>
+      </c>
+      <c r="E13" s="23" t="s">
+        <v>411</v>
+      </c>
+      <c r="F13" s="47" t="str">
+        <f>VLOOKUP(B13,Lexique!A:F,5,)</f>
+        <v>Nom route / rue</v>
+      </c>
+      <c r="G13" s="47" t="str">
+        <f>VLOOKUP(B13,Lexique!A:F,6,)</f>
+        <v>Nom route / rue</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="15" x14ac:dyDescent="0.15">
+      <c r="A14" s="30">
         <v>5.54</v>
       </c>
-      <c r="B13" s="29" t="s">
+      <c r="B14" s="29" t="s">
         <v>76</v>
       </c>
-      <c r="C13" s="29" t="s">
+      <c r="C14" s="29" t="s">
         <v>364</v>
       </c>
-      <c r="D13" s="23" t="s">
+      <c r="D14" s="23" t="s">
         <v>364</v>
       </c>
-      <c r="E13" s="23" t="str">
+      <c r="E14" s="23" t="str">
         <f t="shared" si="0"/>
         <v>Rue Self</v>
       </c>
-      <c r="F13" s="47" t="str">
-        <f>VLOOKUP(B13,Lexique!A:F,5,)</f>
-        <v>Nom route / rue</v>
-      </c>
-      <c r="G13" s="47" t="str">
-        <f>VLOOKUP(B13,Lexique!A:F,6,)</f>
-        <v>Nom route / rue</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="30" x14ac:dyDescent="0.15">
-      <c r="A14" s="30">
+      <c r="F14" s="47" t="str">
+        <f>VLOOKUP(B14,Lexique!A:F,5,)</f>
+        <v>Nom route / rue</v>
+      </c>
+      <c r="G14" s="47" t="str">
+        <f>VLOOKUP(B14,Lexique!A:F,6,)</f>
+        <v>Nom route / rue</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="30" x14ac:dyDescent="0.15">
+      <c r="A15" s="30">
         <v>6.54</v>
       </c>
-      <c r="B14" s="29" t="s">
+      <c r="B15" s="29" t="s">
         <v>72</v>
       </c>
-      <c r="C14" s="29" t="s">
+      <c r="C15" s="29" t="s">
         <v>365</v>
       </c>
-      <c r="D14" s="23" t="s">
+      <c r="D15" s="23" t="s">
         <v>358</v>
       </c>
-      <c r="E14" s="23" t="str">
+      <c r="E15" s="23" t="str">
         <f t="shared" si="0"/>
         <v>Boulevard Dennisson</v>
       </c>
-      <c r="F14" s="47" t="str">
-        <f>VLOOKUP(B14,Lexique!A:F,5,)</f>
-        <v>Nom route / rue</v>
-      </c>
-      <c r="G14" s="47" t="str">
-        <f>VLOOKUP(B14,Lexique!A:F,6,)</f>
-        <v>Nom route / rue</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="15" x14ac:dyDescent="0.15">
-      <c r="A15" s="30">
-        <v>6.95</v>
-      </c>
-      <c r="B15" s="29" t="s">
-        <v>75</v>
-      </c>
-      <c r="C15" s="29" t="s">
-        <v>366</v>
-      </c>
-      <c r="D15" s="23" t="s">
-        <v>371</v>
-      </c>
-      <c r="E15" s="23" t="s">
-        <v>372</v>
-      </c>
       <c r="F15" s="47" t="str">
         <f>VLOOKUP(B15,Lexique!A:F,5,)</f>
         <v>Nom route / rue</v>
@@ -13544,96 +13546,112 @@
     </row>
     <row r="16" spans="1:7" ht="15" x14ac:dyDescent="0.15">
       <c r="A16" s="30">
+        <v>6.95</v>
+      </c>
+      <c r="B16" s="29" t="s">
+        <v>75</v>
+      </c>
+      <c r="C16" s="29" t="s">
+        <v>366</v>
+      </c>
+      <c r="D16" s="23" t="s">
+        <v>371</v>
+      </c>
+      <c r="E16" s="23" t="s">
+        <v>372</v>
+      </c>
+      <c r="F16" s="47" t="str">
+        <f>VLOOKUP(B16,Lexique!A:F,5,)</f>
+        <v>Nom route / rue</v>
+      </c>
+      <c r="G16" s="47" t="str">
+        <f>VLOOKUP(B16,Lexique!A:F,6,)</f>
+        <v>Nom route / rue</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="15" x14ac:dyDescent="0.15">
+      <c r="A17" s="30">
         <v>7.4</v>
       </c>
-      <c r="B16" s="29" t="s">
+      <c r="B17" s="29" t="s">
         <v>73</v>
       </c>
-      <c r="C16" s="29" t="s">
+      <c r="C17" s="29" t="s">
         <v>367</v>
       </c>
-      <c r="D16" s="49" t="s">
+      <c r="D17" s="49" t="s">
         <v>367</v>
       </c>
-      <c r="E16" s="23" t="str">
+      <c r="E17" s="23" t="str">
         <f t="shared" si="0"/>
         <v>Rue Allard</v>
       </c>
-      <c r="F16" s="47" t="str">
-        <f>VLOOKUP(B16,Lexique!A:F,5,)</f>
-        <v>Nom route / rue</v>
-      </c>
-      <c r="G16" s="47" t="str">
-        <f>VLOOKUP(B16,Lexique!A:F,6,)</f>
-        <v>Nom route / rue</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="15" x14ac:dyDescent="0.15">
-      <c r="A17" s="30">
+      <c r="F17" s="47" t="str">
+        <f>VLOOKUP(B17,Lexique!A:F,5,)</f>
+        <v>Nom route / rue</v>
+      </c>
+      <c r="G17" s="47" t="str">
+        <f>VLOOKUP(B17,Lexique!A:F,6,)</f>
+        <v>Nom route / rue</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="15" x14ac:dyDescent="0.15">
+      <c r="A18" s="30">
         <v>7.66</v>
       </c>
-      <c r="B17" s="29" t="s">
+      <c r="B18" s="29" t="s">
         <v>72</v>
       </c>
-      <c r="C17" s="29" t="s">
+      <c r="C18" s="29" t="s">
         <v>368</v>
       </c>
-      <c r="D17" s="50" t="s">
-        <v>377</v>
-      </c>
-      <c r="E17" s="23" t="str">
+      <c r="D18" s="50" t="s">
+        <v>376</v>
+      </c>
+      <c r="E18" s="23" t="str">
         <f t="shared" si="0"/>
         <v>Avenue Perreault</v>
       </c>
-      <c r="F17" s="47" t="str">
-        <f>VLOOKUP(B17,Lexique!A:F,5,)</f>
-        <v>Nom route / rue</v>
-      </c>
-      <c r="G17" s="47" t="str">
-        <f>VLOOKUP(B17,Lexique!A:F,6,)</f>
-        <v>Nom route / rue</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="15" x14ac:dyDescent="0.15">
-      <c r="A18" s="30">
-        <v>8.3000000000000007</v>
-      </c>
-      <c r="B18" s="29" t="s">
-        <v>43</v>
-      </c>
-      <c r="C18" s="29" t="s">
-        <v>369</v>
-      </c>
-      <c r="D18" s="23" t="s">
-        <v>199</v>
-      </c>
-      <c r="E18" s="23" t="s">
-        <v>43</v>
-      </c>
       <c r="F18" s="47" t="str">
         <f>VLOOKUP(B18,Lexique!A:F,5,)</f>
-        <v>Arrivée&lt;br/&gt;Bonification en temps et points</v>
+        <v>Nom route / rue</v>
       </c>
       <c r="G18" s="47" t="str">
         <f>VLOOKUP(B18,Lexique!A:F,6,)</f>
+        <v>Nom route / rue</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="15" x14ac:dyDescent="0.15">
+      <c r="A19" s="30">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="B19" s="29" t="s">
+        <v>43</v>
+      </c>
+      <c r="C19" s="29" t="s">
+        <v>369</v>
+      </c>
+      <c r="D19" s="23" t="s">
+        <v>199</v>
+      </c>
+      <c r="E19" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="F19" s="47" t="str">
+        <f>VLOOKUP(B19,Lexique!A:F,5,)</f>
+        <v>Arrivée&lt;br/&gt;Bonification en temps et points</v>
+      </c>
+      <c r="G19" s="47" t="str">
+        <f>VLOOKUP(B19,Lexique!A:F,6,)</f>
         <v>Finish&lt;br/&gt;Time and points bonus</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" ht="14" x14ac:dyDescent="0.15">
-      <c r="A19" s="30"/>
-      <c r="B19" s="29"/>
-      <c r="C19" s="29"/>
-      <c r="D19" s="23"/>
-      <c r="E19" s="23"/>
-      <c r="F19" s="47"/>
-      <c r="G19" s="47"/>
     </row>
     <row r="20" spans="1:7" ht="14" x14ac:dyDescent="0.15">
       <c r="A20" s="30"/>
       <c r="B20" s="29"/>
       <c r="C20" s="29"/>
-      <c r="D20" s="49"/>
-      <c r="E20" s="49"/>
+      <c r="D20" s="23"/>
+      <c r="E20" s="23"/>
       <c r="F20" s="47"/>
       <c r="G20" s="47"/>
     </row>
@@ -13641,8 +13659,8 @@
       <c r="A21" s="30"/>
       <c r="B21" s="29"/>
       <c r="C21" s="29"/>
-      <c r="D21" s="23"/>
-      <c r="E21" s="23"/>
+      <c r="D21" s="49"/>
+      <c r="E21" s="49"/>
       <c r="F21" s="47"/>
       <c r="G21" s="47"/>
     </row>
@@ -13650,8 +13668,8 @@
       <c r="A22" s="30"/>
       <c r="B22" s="29"/>
       <c r="C22" s="29"/>
-      <c r="D22" s="50"/>
-      <c r="E22" s="50"/>
+      <c r="D22" s="23"/>
+      <c r="E22" s="23"/>
       <c r="F22" s="47"/>
       <c r="G22" s="47"/>
     </row>
@@ -13659,8 +13677,8 @@
       <c r="A23" s="30"/>
       <c r="B23" s="29"/>
       <c r="C23" s="29"/>
-      <c r="D23" s="23"/>
-      <c r="E23" s="44"/>
+      <c r="D23" s="50"/>
+      <c r="E23" s="50"/>
       <c r="F23" s="47"/>
       <c r="G23" s="47"/>
     </row>
@@ -13669,7 +13687,7 @@
       <c r="B24" s="29"/>
       <c r="C24" s="29"/>
       <c r="D24" s="23"/>
-      <c r="E24" s="23"/>
+      <c r="E24" s="44"/>
       <c r="F24" s="47"/>
       <c r="G24" s="47"/>
     </row>
@@ -13713,8 +13731,8 @@
       <c r="A29" s="30"/>
       <c r="B29" s="29"/>
       <c r="C29" s="29"/>
-      <c r="D29" s="49"/>
-      <c r="E29" s="49"/>
+      <c r="D29" s="23"/>
+      <c r="E29" s="23"/>
       <c r="F29" s="47"/>
       <c r="G29" s="47"/>
     </row>
@@ -13722,8 +13740,8 @@
       <c r="A30" s="30"/>
       <c r="B30" s="29"/>
       <c r="C30" s="29"/>
-      <c r="D30" s="23"/>
-      <c r="E30" s="23"/>
+      <c r="D30" s="49"/>
+      <c r="E30" s="49"/>
       <c r="F30" s="47"/>
       <c r="G30" s="47"/>
     </row>
@@ -13830,7 +13848,7 @@
       <c r="A42" s="30"/>
       <c r="B42" s="29"/>
       <c r="C42" s="29"/>
-      <c r="D42" s="49"/>
+      <c r="D42" s="23"/>
       <c r="E42" s="23"/>
       <c r="F42" s="47"/>
       <c r="G42" s="47"/>
@@ -13839,7 +13857,7 @@
       <c r="A43" s="30"/>
       <c r="B43" s="29"/>
       <c r="C43" s="29"/>
-      <c r="D43" s="23"/>
+      <c r="D43" s="49"/>
       <c r="E43" s="23"/>
       <c r="F43" s="47"/>
       <c r="G43" s="47"/>
@@ -13857,16 +13875,16 @@
       <c r="A45" s="30"/>
       <c r="B45" s="29"/>
       <c r="C45" s="29"/>
-      <c r="D45" s="49"/>
+      <c r="D45" s="23"/>
       <c r="E45" s="23"/>
       <c r="F45" s="47"/>
       <c r="G45" s="47"/>
     </row>
     <row r="46" spans="1:7" ht="14" x14ac:dyDescent="0.15">
-      <c r="A46" s="51"/>
-      <c r="B46" s="52"/>
-      <c r="C46" s="53"/>
-      <c r="D46" s="54"/>
+      <c r="A46" s="30"/>
+      <c r="B46" s="29"/>
+      <c r="C46" s="29"/>
+      <c r="D46" s="49"/>
       <c r="E46" s="23"/>
       <c r="F46" s="47"/>
       <c r="G46" s="47"/>
@@ -13893,7 +13911,7 @@
       <c r="A49" s="51"/>
       <c r="B49" s="52"/>
       <c r="C49" s="53"/>
-      <c r="D49" s="23"/>
+      <c r="D49" s="54"/>
       <c r="E49" s="23"/>
       <c r="F49" s="47"/>
       <c r="G49" s="47"/>
@@ -13902,8 +13920,8 @@
       <c r="A50" s="51"/>
       <c r="B50" s="52"/>
       <c r="C50" s="53"/>
-      <c r="D50" s="54"/>
-      <c r="E50" s="54"/>
+      <c r="D50" s="23"/>
+      <c r="E50" s="23"/>
       <c r="F50" s="47"/>
       <c r="G50" s="47"/>
     </row>
@@ -13925,9 +13943,14 @@
       <c r="F52" s="47"/>
       <c r="G52" s="47"/>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="D53" s="58"/>
-      <c r="E53" s="58"/>
+    <row r="53" spans="1:7" ht="14" x14ac:dyDescent="0.15">
+      <c r="A53" s="51"/>
+      <c r="B53" s="52"/>
+      <c r="C53" s="53"/>
+      <c r="D53" s="54"/>
+      <c r="E53" s="54"/>
+      <c r="F53" s="47"/>
+      <c r="G53" s="47"/>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.15">
       <c r="D54" s="58"/>
@@ -13969,10 +13992,7 @@
       <c r="D63" s="58"/>
       <c r="E63" s="58"/>
     </row>
-    <row r="64" spans="1:7" s="59" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A64" s="55"/>
-      <c r="B64" s="56"/>
-      <c r="C64" s="57"/>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.15">
       <c r="D64" s="58"/>
       <c r="E64" s="58"/>
     </row>
@@ -15802,6 +15822,13 @@
       <c r="C325" s="57"/>
       <c r="D325" s="58"/>
       <c r="E325" s="58"/>
+    </row>
+    <row r="326" spans="1:5" s="59" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A326" s="55"/>
+      <c r="B326" s="56"/>
+      <c r="C326" s="57"/>
+      <c r="D326" s="58"/>
+      <c r="E326" s="58"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -15873,10 +15900,10 @@
       </c>
       <c r="C2" s="29"/>
       <c r="D2" s="23" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="E2" s="23" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="F2" s="35" t="str">
         <f>VLOOKUP(B2,Lexique!A:F,5,)</f>
@@ -15895,10 +15922,10 @@
         <v>73</v>
       </c>
       <c r="C3" s="29" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="D3" s="23" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="E3" s="23" t="str">
         <f>D3</f>
@@ -15921,10 +15948,10 @@
         <v>73</v>
       </c>
       <c r="C4" s="29" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="D4" s="23" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="E4" s="23" t="str">
         <f>D4</f>
@@ -15947,13 +15974,13 @@
         <v>75</v>
       </c>
       <c r="C5" s="29" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="D5" s="23" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="E5" s="23" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="F5" s="35" t="str">
         <f>VLOOKUP(B5,Lexique!A:F,5,)</f>
@@ -15997,13 +16024,13 @@
         <v>82</v>
       </c>
       <c r="C7" s="29" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="D7" s="23" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="E7" s="23" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="F7" s="35" t="str">
         <f>VLOOKUP(B7,Lexique!A:F,5,)</f>
@@ -16022,7 +16049,7 @@
         <v>79</v>
       </c>
       <c r="C8" s="29" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="D8" s="23" t="s">
         <v>10</v>
@@ -16047,7 +16074,7 @@
         <v>74</v>
       </c>
       <c r="C9" s="29" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="D9" s="28" t="s">
         <v>165</v>
@@ -16073,7 +16100,7 @@
         <v>81</v>
       </c>
       <c r="C10" s="29" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="D10" s="23" t="s">
         <v>185</v>
@@ -16123,7 +16150,7 @@
         <v>74</v>
       </c>
       <c r="C12" s="29" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="D12" s="28" t="s">
         <v>165</v>
@@ -16174,7 +16201,7 @@
         <v>73</v>
       </c>
       <c r="C14" s="29" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="D14" s="23" t="s">
         <v>188</v>
@@ -16199,7 +16226,7 @@
         <v>73</v>
       </c>
       <c r="C15" s="29" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="D15" s="23" t="s">
         <v>200</v>
@@ -16224,7 +16251,7 @@
         <v>72</v>
       </c>
       <c r="C16" s="29" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="D16" s="24" t="s">
         <v>165</v>
@@ -16274,7 +16301,7 @@
         <v>75</v>
       </c>
       <c r="C18" s="29" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="D18" s="28" t="s">
         <v>165</v>
@@ -16300,7 +16327,7 @@
         <v>81</v>
       </c>
       <c r="C19" s="29" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="D19" s="23" t="s">
         <v>185</v>
@@ -16350,13 +16377,13 @@
         <v>82</v>
       </c>
       <c r="C21" s="29" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="D21" s="23" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="E21" s="23" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="F21" s="35" t="str">
         <f>VLOOKUP(B21,Lexique!A:F,5,)</f>
@@ -16400,13 +16427,13 @@
         <v>75</v>
       </c>
       <c r="C23" s="29" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="D23" s="23" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="E23" s="23" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="F23" s="35" t="str">
         <f>VLOOKUP(B23,Lexique!A:F,5,)</f>
@@ -16425,13 +16452,13 @@
         <v>72</v>
       </c>
       <c r="C24" s="29" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="D24" s="28" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="E24" s="28" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="F24" s="35" t="str">
         <f>VLOOKUP(B24,Lexique!A:F,5,)</f>
@@ -16450,13 +16477,13 @@
         <v>110</v>
       </c>
       <c r="C25" s="29" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="D25" s="23" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="E25" s="23" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="F25" s="35" t="str">
         <f>VLOOKUP(B25,Lexique!A:F,5,)</f>
@@ -16475,10 +16502,10 @@
         <v>73</v>
       </c>
       <c r="C26" s="29" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="D26" s="23" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="E26" s="23" t="str">
         <f>D26</f>
@@ -18631,7 +18658,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA4CF35A-AE95-4D4B-80F8-FB6E5D8CEEB2}">
   <dimension ref="A1:I48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
@@ -18678,10 +18705,10 @@
       </c>
       <c r="C2" s="29"/>
       <c r="D2" s="23" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="E2" s="23" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="F2" s="35" t="str">
         <f>VLOOKUP(B2,Lexique!A:F,5,)</f>
@@ -18893,10 +18920,10 @@
       </c>
       <c r="C11" s="29"/>
       <c r="D11" s="23" t="s">
-        <v>624</v>
+        <v>622</v>
       </c>
       <c r="E11" s="23" t="s">
-        <v>625</v>
+        <v>623</v>
       </c>
       <c r="F11" s="35" t="str">
         <f>VLOOKUP(B11,Lexique!A:F,5,)</f>
@@ -19609,10 +19636,10 @@
         <v>262</v>
       </c>
       <c r="D2" s="23" t="s">
+        <v>382</v>
+      </c>
+      <c r="E2" s="23" t="s">
         <v>383</v>
-      </c>
-      <c r="E2" s="23" t="s">
-        <v>384</v>
       </c>
       <c r="F2" s="35" t="str">
         <f>VLOOKUP(B2,Lexique!A:F,5,)</f>
@@ -19631,7 +19658,7 @@
         <v>73</v>
       </c>
       <c r="C3" s="29" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="D3" s="23" t="s">
         <v>338</v>
@@ -19657,7 +19684,7 @@
         <v>72</v>
       </c>
       <c r="C4" s="29" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="D4" s="23" t="s">
         <v>339</v>
@@ -19683,10 +19710,10 @@
         <v>73</v>
       </c>
       <c r="C5" s="29" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="D5" s="23" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="E5" s="23" t="str">
         <f>D5</f>
@@ -19709,10 +19736,10 @@
         <v>72</v>
       </c>
       <c r="C6" s="29" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="D6" s="23" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="E6" s="23" t="str">
         <f>D6</f>
@@ -19735,13 +19762,13 @@
         <v>74</v>
       </c>
       <c r="C7" s="29" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="D7" s="23" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="E7" s="23" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="F7" s="35" t="str">
         <f>VLOOKUP(B7,Lexique!A:F,5,)</f>
@@ -19760,7 +19787,7 @@
         <v>74</v>
       </c>
       <c r="C8" s="29" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="D8" s="23" t="s">
         <v>328</v>
@@ -19789,10 +19816,10 @@
         <v>331</v>
       </c>
       <c r="D9" s="23" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="E9" s="23" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="F9" s="35" t="str">
         <f>VLOOKUP(B9,Lexique!A:F,5,)</f>
@@ -19811,10 +19838,10 @@
         <v>73</v>
       </c>
       <c r="C10" s="29" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="D10" s="23" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="E10" s="24" t="str">
         <f>D10</f>
@@ -19837,10 +19864,10 @@
         <v>73</v>
       </c>
       <c r="C11" s="29" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="D11" s="24" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="E11" s="24" t="str">
         <f>D11</f>
@@ -19863,7 +19890,7 @@
         <v>73</v>
       </c>
       <c r="C12" s="29" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="D12" s="23" t="s">
         <v>328</v>
@@ -19889,7 +19916,7 @@
         <v>72</v>
       </c>
       <c r="C13" s="29" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="D13" s="23" t="s">
         <v>331</v>
@@ -19915,7 +19942,7 @@
         <v>73</v>
       </c>
       <c r="C14" s="29" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="D14" s="25" t="s">
         <v>332</v>
@@ -19941,7 +19968,7 @@
         <v>72</v>
       </c>
       <c r="C15" s="29" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="D15" s="23" t="s">
         <v>339</v>
@@ -19967,7 +19994,7 @@
         <v>73</v>
       </c>
       <c r="C16" s="29" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="D16" s="24" t="s">
         <v>334</v>
@@ -19993,7 +20020,7 @@
         <v>73</v>
       </c>
       <c r="C17" s="29" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="D17" s="43" t="s">
         <v>335</v>
@@ -20019,13 +20046,13 @@
         <v>76</v>
       </c>
       <c r="C18" s="29" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="D18" s="23" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="E18" s="23" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="F18" s="35" t="str">
         <f>VLOOKUP(B18,Lexique!A:F,5,)</f>
@@ -20045,13 +20072,13 @@
         <v>76</v>
       </c>
       <c r="C19" s="29" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="D19" s="23" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="E19" s="23" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="F19" s="35" t="str">
         <f>VLOOKUP(B19,Lexique!A:F,5,)</f>
@@ -20071,13 +20098,13 @@
         <v>71</v>
       </c>
       <c r="C20" s="29" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D20" s="25" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="E20" s="25" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="F20" s="35" t="str">
         <f>VLOOKUP(B20,Lexique!A:F,5,)</f>
@@ -20097,13 +20124,13 @@
         <v>76</v>
       </c>
       <c r="C21" s="29" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="D21" s="23" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="E21" s="23" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="F21" s="35" t="str">
         <f>VLOOKUP(B21,Lexique!A:F,5,)</f>
@@ -20123,7 +20150,7 @@
         <v>78</v>
       </c>
       <c r="C22" s="29" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="D22" s="23" t="s">
         <v>155</v>
@@ -20149,13 +20176,13 @@
         <v>70</v>
       </c>
       <c r="C23" s="29" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="D23" s="23" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="E23" s="23" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="F23" s="35" t="str">
         <f>VLOOKUP(B23,Lexique!A:F,5,)</f>
@@ -20175,13 +20202,13 @@
         <v>76</v>
       </c>
       <c r="C24" s="29" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="D24" s="23" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="E24" s="23" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="F24" s="35" t="str">
         <f>VLOOKUP(B24,Lexique!A:F,5,)</f>
@@ -20201,13 +20228,13 @@
         <v>71</v>
       </c>
       <c r="C25" s="29" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="D25" s="25" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="E25" s="25" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="F25" s="35" t="str">
         <f>VLOOKUP(B25,Lexique!A:F,5,)</f>
@@ -20227,13 +20254,13 @@
         <v>81</v>
       </c>
       <c r="C26" s="29" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="D26" s="23" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="E26" s="23" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="F26" s="35" t="str">
         <f>VLOOKUP(B26,Lexique!A:F,5,)</f>
@@ -20253,13 +20280,13 @@
         <v>76</v>
       </c>
       <c r="C27" s="29" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="D27" s="23" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="E27" s="23" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="F27" s="35" t="str">
         <f>VLOOKUP(B27,Lexique!A:F,5,)</f>
@@ -20279,13 +20306,13 @@
         <v>76</v>
       </c>
       <c r="C28" s="29" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="D28" s="23" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="E28" s="23" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="F28" s="35" t="str">
         <f>VLOOKUP(B28,Lexique!A:F,5,)</f>
@@ -20305,13 +20332,13 @@
         <v>71</v>
       </c>
       <c r="C29" s="29" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="D29" s="25" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="E29" s="25" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="F29" s="35" t="str">
         <f>VLOOKUP(B29,Lexique!A:F,5,)</f>
@@ -20331,13 +20358,13 @@
         <v>70</v>
       </c>
       <c r="C30" s="29" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="D30" s="23" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="E30" s="23" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="F30" s="35" t="str">
         <f>VLOOKUP(B30,Lexique!A:F,5,)</f>
@@ -20357,13 +20384,13 @@
         <v>81</v>
       </c>
       <c r="C31" s="29" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="D31" s="23" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="E31" s="23" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="F31" s="35" t="str">
         <f>VLOOKUP(B31,Lexique!A:F,5,)</f>
@@ -20383,7 +20410,7 @@
         <v>78</v>
       </c>
       <c r="C32" s="29" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="D32" s="23" t="s">
         <v>154</v>
@@ -20409,13 +20436,13 @@
         <v>80</v>
       </c>
       <c r="C33" s="29" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="D33" s="23" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="E33" s="23" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="F33" s="35" t="str">
         <f>VLOOKUP(B33,Lexique!A:F,5,)</f>
@@ -20459,7 +20486,7 @@
         <v>43</v>
       </c>
       <c r="C35" s="29" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="D35" s="26" t="s">
         <v>109</v>

</xml_diff>

<commit_message>
Ajout page détail radio-tour et corrections repas
</commit_message>
<xml_diff>
--- a/excel/Itineraires.xlsx
+++ b/excel/Itineraires.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brunogauthier/Documents/guide2024/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9271C75-9C79-EC4F-9FDF-ECF6E92435D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{750F8CE9-F36A-CB46-BD8A-F5B3D7B64A3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" tabRatio="758" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" tabRatio="758" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="23" r:id="rId1"/>
@@ -572,9 +572,6 @@
     <t>Senneterre Mayor's sprint 250$&lt;br/&gt;(Camping le Huard)</t>
   </si>
   <si>
-    <t>Sprint du maire de Senneterre 250$&lt;br/&gt;(Camping le Huard)</t>
-  </si>
-  <si>
     <t>Rue du Parc</t>
   </si>
   <si>
@@ -1355,12 +1352,6 @@
     <t>Start of 3rd lap (1 laps to go)</t>
   </si>
   <si>
-    <t>Début 7e tour (6 tours à faire)&lt;br/&gt;Sprint de la Mairesse de Val-d'Or (250$)</t>
-  </si>
-  <si>
-    <t>Début 11e tour (2 tours à faire)&lt;br/&gt;Sprint de la Mairesse de Val-d'Or (250$)</t>
-  </si>
-  <si>
     <t>Start of 11th lap (2 laps to go)&lt;br/&gt;Val-d'Or Mayor's sprint (250$)</t>
   </si>
   <si>
@@ -1871,9 +1862,6 @@
     <t>Start of 4th lap (7 to go)</t>
   </si>
   <si>
-    <t>Début 9e tour (2 tours à faire)&lt;br/&gt;Sprint du Maire de Preissac (250$)</t>
-  </si>
-  <si>
     <t>Start of 9th lap (2 laps to go)&lt;br/&gt;Preissac Mayor's sprint (250$)</t>
   </si>
   <si>
@@ -1883,9 +1871,6 @@
     <t>Start of 5th lap (6 to go)&lt;br/&gt;Preissac Mayor's sprint (250$)</t>
   </si>
   <si>
-    <t>Début 5e tour (6 à faire)&lt;br/&gt;Sprint du Maire de Preissac (250$)</t>
-  </si>
-  <si>
     <t>Début 3e tour (8 tours à faire)&lt;br/&gt;Sprint bonification temps et points</t>
   </si>
   <si>
@@ -1910,9 +1895,6 @@
     <t>Fin du tour 8</t>
   </si>
   <si>
-    <t>Sprint du maire de Senneterre 250$&lt;br/&gt;(Chemin Paré - Val-Senneville)</t>
-  </si>
-  <si>
     <t>Senneterre Mayor's sprint 250$&lt;br/&gt;(Chemin Paré -Val-Senneville)</t>
   </si>
   <si>
@@ -1920,6 +1902,24 @@
   </si>
   <si>
     <t>Left of the central median&lt;br/&gt;7th street intersection&lt;br/&gt;Start of counterflow traffic (southbound lane)</t>
+  </si>
+  <si>
+    <t>Sprint du maire de Senneterre 250$ &lt;br/&gt;(Camping le Huard)</t>
+  </si>
+  <si>
+    <t>Sprint du maire de Senneterre 250$ &lt;br/&gt;(Chemin Paré - Val-Senneville)</t>
+  </si>
+  <si>
+    <t>Début 7e tour (6 tours à faire)&lt;br/&gt;Sprint de la Mairesse de Val-d'Or 250$</t>
+  </si>
+  <si>
+    <t>Début 11e tour (2 tours à faire)&lt;br/&gt;Sprint de la Mairesse de Val-d'Or 250$</t>
+  </si>
+  <si>
+    <t>Début 5e tour (6 à faire)&lt;br/&gt;Sprint du Maire de Preissac 250$</t>
+  </si>
+  <si>
+    <t>Début 9e tour (2 tours à faire)&lt;br/&gt;Sprint du Maire de Preissac 250$</t>
   </si>
 </sst>
 </file>
@@ -3072,27 +3072,27 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A6" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A7" s="4" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A8" s="4" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A9" s="4" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A10" s="4" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
   </sheetData>
@@ -3105,8 +3105,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BF2EC7B-8CF4-1449-B844-A73E16F738A4}">
   <dimension ref="A1:G322"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="D44" sqref="D44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
@@ -3129,7 +3129,7 @@
         <v>19</v>
       </c>
       <c r="C1" s="39" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="D1" s="40" t="s">
         <v>17</v>
@@ -3138,10 +3138,10 @@
         <v>18</v>
       </c>
       <c r="F1" s="41" t="s">
+        <v>304</v>
+      </c>
+      <c r="G1" s="41" t="s">
         <v>305</v>
-      </c>
-      <c r="G1" s="41" t="s">
-        <v>306</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="15" x14ac:dyDescent="0.2">
@@ -3152,13 +3152,13 @@
         <v>63</v>
       </c>
       <c r="C2" s="29" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D2" s="23" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
       <c r="E2" s="23" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
       <c r="F2" s="35" t="str">
         <f>VLOOKUP(B2,Lexique!A:F,5,)</f>
@@ -3177,13 +3177,13 @@
         <v>76</v>
       </c>
       <c r="C3" s="29" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="D3" s="23" t="s">
-        <v>492</v>
+        <v>489</v>
       </c>
       <c r="E3" s="23" t="s">
-        <v>492</v>
+        <v>489</v>
       </c>
       <c r="F3" s="35" t="str">
         <f>VLOOKUP(B3,Lexique!A:F,5,)</f>
@@ -3202,13 +3202,13 @@
         <v>73</v>
       </c>
       <c r="C4" s="29" t="s">
-        <v>493</v>
+        <v>490</v>
       </c>
       <c r="D4" s="23" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
       <c r="E4" s="23" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
       <c r="F4" s="35" t="str">
         <f>VLOOKUP(B4,Lexique!A:F,5,)</f>
@@ -3227,13 +3227,13 @@
         <v>75</v>
       </c>
       <c r="C5" s="29" t="s">
-        <v>495</v>
+        <v>492</v>
       </c>
       <c r="D5" s="23" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
       <c r="E5" s="23" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
       <c r="F5" s="35" t="str">
         <f>VLOOKUP(B5,Lexique!A:F,5,)</f>
@@ -3252,13 +3252,13 @@
         <v>75</v>
       </c>
       <c r="C6" s="29" t="s">
-        <v>496</v>
+        <v>493</v>
       </c>
       <c r="D6" s="23" t="s">
-        <v>497</v>
+        <v>494</v>
       </c>
       <c r="E6" s="23" t="s">
-        <v>497</v>
+        <v>494</v>
       </c>
       <c r="F6" s="35" t="str">
         <f>VLOOKUP(B6,Lexique!A:F,5,)</f>
@@ -3277,7 +3277,7 @@
         <v>25</v>
       </c>
       <c r="C7" s="29" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="D7" s="23" t="s">
         <v>2</v>
@@ -3302,7 +3302,7 @@
         <v>79</v>
       </c>
       <c r="C8" s="29" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="D8" s="23" t="s">
         <v>10</v>
@@ -3327,7 +3327,7 @@
         <v>25</v>
       </c>
       <c r="C9" s="29" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="D9" s="23" t="s">
         <v>2</v>
@@ -3353,7 +3353,7 @@
         <v>78</v>
       </c>
       <c r="C10" s="29" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
       <c r="D10" s="23" t="s">
         <v>155</v>
@@ -3378,7 +3378,7 @@
         <v>72</v>
       </c>
       <c r="C11" s="29" t="s">
-        <v>495</v>
+        <v>492</v>
       </c>
       <c r="D11" s="23" t="s">
         <v>165</v>
@@ -3403,7 +3403,7 @@
         <v>76</v>
       </c>
       <c r="C12" s="29" t="s">
-        <v>499</v>
+        <v>496</v>
       </c>
       <c r="D12" s="23" t="s">
         <v>165</v>
@@ -3428,13 +3428,13 @@
         <v>71</v>
       </c>
       <c r="C13" s="29" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D13" s="23" t="s">
-        <v>500</v>
+        <v>497</v>
       </c>
       <c r="E13" s="23" t="s">
-        <v>501</v>
+        <v>498</v>
       </c>
       <c r="F13" s="35" t="str">
         <f>VLOOKUP(B13,Lexique!A:F,5,)</f>
@@ -3453,7 +3453,7 @@
         <v>25</v>
       </c>
       <c r="C14" s="29" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="D14" s="23" t="s">
         <v>2</v>
@@ -3478,13 +3478,13 @@
         <v>5</v>
       </c>
       <c r="C15" s="29" t="s">
-        <v>502</v>
+        <v>499</v>
       </c>
       <c r="D15" s="23" t="s">
-        <v>503</v>
+        <v>500</v>
       </c>
       <c r="E15" s="23" t="s">
-        <v>503</v>
+        <v>500</v>
       </c>
       <c r="F15" s="35" t="str">
         <f>VLOOKUP(B15,Lexique!A:F,5,)</f>
@@ -3503,13 +3503,13 @@
         <v>82</v>
       </c>
       <c r="C16" s="29" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="D16" s="44" t="s">
-        <v>591</v>
+        <v>588</v>
       </c>
       <c r="E16" s="62" t="s">
-        <v>592</v>
+        <v>589</v>
       </c>
       <c r="F16" s="35" t="str">
         <f>VLOOKUP(B16,Lexique!A:F,5,)</f>
@@ -3528,13 +3528,13 @@
         <v>25</v>
       </c>
       <c r="C17" s="29" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
       <c r="D17" s="24" t="s">
         <v>22</v>
       </c>
       <c r="E17" s="25" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
       <c r="F17" s="35" t="str">
         <f>VLOOKUP(B17,Lexique!A:F,5,)</f>
@@ -3553,13 +3553,13 @@
         <v>25</v>
       </c>
       <c r="C18" s="29" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
       <c r="D18" s="24" t="s">
         <v>22</v>
       </c>
       <c r="E18" s="25" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
       <c r="F18" s="35" t="str">
         <f>VLOOKUP(B18,Lexique!A:F,5,)</f>
@@ -3578,13 +3578,13 @@
         <v>25</v>
       </c>
       <c r="C19" s="29" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
       <c r="D19" s="24" t="s">
         <v>22</v>
       </c>
       <c r="E19" s="25" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
       <c r="F19" s="35" t="str">
         <f>VLOOKUP(B19,Lexique!A:F,5,)</f>
@@ -3603,13 +3603,13 @@
         <v>82</v>
       </c>
       <c r="C20" s="29" t="s">
-        <v>525</v>
+        <v>522</v>
       </c>
       <c r="D20" s="44" t="s">
-        <v>593</v>
+        <v>590</v>
       </c>
       <c r="E20" s="62" t="s">
-        <v>594</v>
+        <v>591</v>
       </c>
       <c r="F20" s="35" t="str">
         <f>VLOOKUP(B20,Lexique!A:F,5,)</f>
@@ -3628,13 +3628,13 @@
         <v>72</v>
       </c>
       <c r="C21" s="29" t="s">
-        <v>509</v>
+        <v>506</v>
       </c>
       <c r="D21" s="25" t="s">
-        <v>510</v>
+        <v>507</v>
       </c>
       <c r="E21" s="25" t="s">
-        <v>511</v>
+        <v>508</v>
       </c>
       <c r="F21" s="35" t="str">
         <f>VLOOKUP(B21,Lexique!A:F,5,)</f>
@@ -3653,13 +3653,13 @@
         <v>76</v>
       </c>
       <c r="C22" s="29" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
       <c r="D22" s="23" t="s">
-        <v>590</v>
+        <v>587</v>
       </c>
       <c r="E22" s="23" t="s">
-        <v>513</v>
+        <v>510</v>
       </c>
       <c r="F22" s="35" t="str">
         <f>VLOOKUP(B22,Lexique!A:F,5,)</f>
@@ -3678,13 +3678,13 @@
         <v>73</v>
       </c>
       <c r="C23" s="29" t="s">
-        <v>514</v>
+        <v>511</v>
       </c>
       <c r="D23" s="23" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="E23" s="23" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="F23" s="35" t="str">
         <f>VLOOKUP(B23,Lexique!A:F,5,)</f>
@@ -3703,13 +3703,13 @@
         <v>72</v>
       </c>
       <c r="C24" s="29" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
       <c r="D24" s="23" t="s">
-        <v>516</v>
+        <v>513</v>
       </c>
       <c r="E24" s="23" t="s">
-        <v>516</v>
+        <v>513</v>
       </c>
       <c r="F24" s="35" t="str">
         <f>VLOOKUP(B24,Lexique!A:F,5,)</f>
@@ -3728,13 +3728,13 @@
         <v>73</v>
       </c>
       <c r="C25" s="29" t="s">
-        <v>517</v>
+        <v>514</v>
       </c>
       <c r="D25" s="23" t="s">
-        <v>518</v>
+        <v>515</v>
       </c>
       <c r="E25" s="23" t="s">
-        <v>518</v>
+        <v>515</v>
       </c>
       <c r="F25" s="35" t="str">
         <f>VLOOKUP(B25,Lexique!A:F,5,)</f>
@@ -3753,13 +3753,13 @@
         <v>71</v>
       </c>
       <c r="C26" s="29" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D26" s="23" t="s">
-        <v>519</v>
+        <v>516</v>
       </c>
       <c r="E26" s="23" t="s">
-        <v>519</v>
+        <v>516</v>
       </c>
       <c r="F26" s="35" t="str">
         <f>VLOOKUP(B26,Lexique!A:F,5,)</f>
@@ -3778,13 +3778,13 @@
         <v>73</v>
       </c>
       <c r="C27" s="29" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
       <c r="D27" s="26" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="E27" s="26" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="F27" s="35" t="str">
         <f>VLOOKUP(B27,Lexique!A:F,5,)</f>
@@ -3803,13 +3803,13 @@
         <v>72</v>
       </c>
       <c r="C28" s="29" t="s">
-        <v>521</v>
+        <v>518</v>
       </c>
       <c r="D28" s="23" t="s">
-        <v>522</v>
+        <v>519</v>
       </c>
       <c r="E28" s="23" t="s">
-        <v>522</v>
+        <v>519</v>
       </c>
       <c r="F28" s="35" t="str">
         <f>VLOOKUP(B28,Lexique!A:F,5,)</f>
@@ -3828,13 +3828,13 @@
         <v>73</v>
       </c>
       <c r="C29" s="29" t="s">
-        <v>523</v>
+        <v>520</v>
       </c>
       <c r="D29" s="23" t="s">
-        <v>524</v>
+        <v>521</v>
       </c>
       <c r="E29" s="23" t="s">
-        <v>524</v>
+        <v>521</v>
       </c>
       <c r="F29" s="35" t="str">
         <f>VLOOKUP(B29,Lexique!A:F,5,)</f>
@@ -3853,13 +3853,13 @@
         <v>73</v>
       </c>
       <c r="C30" s="29" t="s">
-        <v>525</v>
+        <v>522</v>
       </c>
       <c r="D30" s="24" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="E30" s="24" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="F30" s="35" t="str">
         <f>VLOOKUP(B30,Lexique!A:F,5,)</f>
@@ -3878,13 +3878,13 @@
         <v>72</v>
       </c>
       <c r="C31" s="29" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
       <c r="D31" s="23" t="s">
-        <v>516</v>
+        <v>513</v>
       </c>
       <c r="E31" s="23" t="s">
-        <v>516</v>
+        <v>513</v>
       </c>
       <c r="F31" s="35" t="str">
         <f>VLOOKUP(B31,Lexique!A:F,5,)</f>
@@ -3903,13 +3903,13 @@
         <v>73</v>
       </c>
       <c r="C32" s="29" t="s">
-        <v>526</v>
+        <v>523</v>
       </c>
       <c r="D32" s="24" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="E32" s="24" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="F32" s="35" t="str">
         <f>VLOOKUP(B32,Lexique!A:F,5,)</f>
@@ -3928,13 +3928,13 @@
         <v>73</v>
       </c>
       <c r="C33" s="29" t="s">
-        <v>527</v>
+        <v>524</v>
       </c>
       <c r="D33" s="23" t="s">
-        <v>528</v>
+        <v>525</v>
       </c>
       <c r="E33" s="23" t="s">
-        <v>528</v>
+        <v>525</v>
       </c>
       <c r="F33" s="35" t="str">
         <f>VLOOKUP(B33,Lexique!A:F,5,)</f>
@@ -3954,13 +3954,13 @@
         <v>76</v>
       </c>
       <c r="C34" s="32" t="s">
-        <v>615</v>
+        <v>610</v>
       </c>
       <c r="D34" s="23" t="s">
-        <v>595</v>
+        <v>592</v>
       </c>
       <c r="E34" s="23" t="s">
-        <v>596</v>
+        <v>593</v>
       </c>
       <c r="F34" s="35" t="str">
         <f>VLOOKUP(B34,Lexique!A:F,5,)</f>
@@ -3980,13 +3980,13 @@
         <v>70</v>
       </c>
       <c r="C35" s="32" t="s">
-        <v>616</v>
+        <v>611</v>
       </c>
       <c r="D35" s="23" t="s">
-        <v>614</v>
+        <v>609</v>
       </c>
       <c r="E35" s="23" t="s">
-        <v>611</v>
+        <v>607</v>
       </c>
       <c r="F35" s="35" t="str">
         <f>VLOOKUP(B35,Lexique!A:F,5,)</f>
@@ -4006,13 +4006,13 @@
         <v>76</v>
       </c>
       <c r="C36" s="32" t="s">
-        <v>619</v>
+        <v>614</v>
       </c>
       <c r="D36" s="27" t="s">
-        <v>607</v>
+        <v>604</v>
       </c>
       <c r="E36" s="27" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
       <c r="F36" s="35"/>
       <c r="G36" s="35"/>
@@ -4026,13 +4026,13 @@
         <v>81</v>
       </c>
       <c r="C37" s="32" t="s">
-        <v>617</v>
+        <v>612</v>
       </c>
       <c r="D37" s="27" t="s">
-        <v>613</v>
+        <v>624</v>
       </c>
       <c r="E37" s="27" t="s">
-        <v>612</v>
+        <v>608</v>
       </c>
       <c r="F37" s="35"/>
       <c r="G37" s="35"/>
@@ -4045,13 +4045,13 @@
         <v>71</v>
       </c>
       <c r="C38" s="32" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D38" s="23" t="s">
-        <v>519</v>
+        <v>516</v>
       </c>
       <c r="E38" s="23" t="s">
-        <v>519</v>
+        <v>516</v>
       </c>
       <c r="F38" s="35"/>
       <c r="G38" s="35"/>
@@ -4065,13 +4065,13 @@
         <v>76</v>
       </c>
       <c r="C39" s="32" t="s">
-        <v>618</v>
+        <v>613</v>
       </c>
       <c r="D39" s="27" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
       <c r="E39" s="27" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
       <c r="F39" s="35"/>
       <c r="G39" s="35"/>
@@ -4084,13 +4084,13 @@
         <v>70</v>
       </c>
       <c r="C40" s="32" t="s">
-        <v>620</v>
+        <v>615</v>
       </c>
       <c r="D40" s="27" t="s">
-        <v>531</v>
+        <v>528</v>
       </c>
       <c r="E40" s="27" t="s">
-        <v>532</v>
+        <v>529</v>
       </c>
       <c r="F40" s="35"/>
       <c r="G40" s="35"/>
@@ -4104,7 +4104,7 @@
         <v>78</v>
       </c>
       <c r="C41" s="29" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
       <c r="D41" s="23" t="s">
         <v>154</v>
@@ -4130,13 +4130,13 @@
         <v>76</v>
       </c>
       <c r="C42" s="32" t="s">
-        <v>533</v>
+        <v>530</v>
       </c>
       <c r="D42" s="27" t="s">
-        <v>534</v>
+        <v>531</v>
       </c>
       <c r="E42" s="27" t="s">
-        <v>535</v>
+        <v>532</v>
       </c>
       <c r="F42" s="35"/>
       <c r="G42" s="35"/>
@@ -4150,13 +4150,13 @@
         <v>81</v>
       </c>
       <c r="C43" s="32" t="s">
-        <v>621</v>
+        <v>616</v>
       </c>
       <c r="D43" s="23" t="s">
-        <v>609</v>
+        <v>625</v>
       </c>
       <c r="E43" s="23" t="s">
-        <v>610</v>
+        <v>606</v>
       </c>
       <c r="F43" s="35"/>
       <c r="G43" s="35"/>
@@ -4170,13 +4170,13 @@
         <v>76</v>
       </c>
       <c r="C44" s="32" t="s">
-        <v>536</v>
+        <v>533</v>
       </c>
       <c r="D44" s="27" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
       <c r="E44" s="27" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
       <c r="F44" s="35"/>
       <c r="G44" s="35"/>
@@ -4190,13 +4190,13 @@
         <v>110</v>
       </c>
       <c r="C45" s="32" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
       <c r="D45" s="27" t="s">
+        <v>346</v>
+      </c>
+      <c r="E45" s="27" t="s">
         <v>347</v>
-      </c>
-      <c r="E45" s="27" t="s">
-        <v>348</v>
       </c>
       <c r="F45" s="35"/>
       <c r="G45" s="35"/>
@@ -4209,7 +4209,7 @@
         <v>43</v>
       </c>
       <c r="C46" s="32" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D46" s="23" t="s">
         <v>166</v>
@@ -6173,10 +6173,10 @@
         <v>38</v>
       </c>
       <c r="E1" s="3" t="s">
+        <v>236</v>
+      </c>
+      <c r="F1" s="22" t="s">
         <v>237</v>
-      </c>
-      <c r="F1" s="22" t="s">
-        <v>238</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.15">
@@ -6193,10 +6193,10 @@
         <v>40</v>
       </c>
       <c r="E2" s="4" t="s">
+        <v>238</v>
+      </c>
+      <c r="F2" s="4" t="s">
         <v>239</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>240</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.15">
@@ -6233,10 +6233,10 @@
         <v>42</v>
       </c>
       <c r="E4" s="4" t="s">
+        <v>240</v>
+      </c>
+      <c r="F4" s="4" t="s">
         <v>241</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>242</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.15">
@@ -6273,10 +6273,10 @@
         <v>25</v>
       </c>
       <c r="E6" s="4" t="s">
+        <v>243</v>
+      </c>
+      <c r="F6" s="4" t="s">
         <v>244</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>245</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.15">
@@ -6293,10 +6293,10 @@
         <v>5</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.15">
@@ -6313,10 +6313,10 @@
         <v>44</v>
       </c>
       <c r="E8" s="4" t="s">
+        <v>245</v>
+      </c>
+      <c r="F8" s="4" t="s">
         <v>246</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>247</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.15">
@@ -6333,10 +6333,10 @@
         <v>45</v>
       </c>
       <c r="E9" s="4" t="s">
+        <v>247</v>
+      </c>
+      <c r="F9" s="4" t="s">
         <v>248</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>249</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.15">
@@ -6353,10 +6353,10 @@
         <v>46</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="14" x14ac:dyDescent="0.15">
@@ -6373,7 +6373,7 @@
         <v>47</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="F11" t="str">
         <f>Tableau1[[#This Row],[Texte_REF_FR]]</f>
@@ -6394,7 +6394,7 @@
         <v>48</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="F12" t="str">
         <f>Tableau1[[#This Row],[Texte_REF_FR]]</f>
@@ -6415,7 +6415,7 @@
         <v>49</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="F13" t="str">
         <f>Tableau1[[#This Row],[Texte_REF_FR]]</f>
@@ -6436,7 +6436,7 @@
         <v>50</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="F14" t="str">
         <f>Tableau1[[#This Row],[Texte_REF_FR]]</f>
@@ -6457,7 +6457,7 @@
         <v>51</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="F15" t="str">
         <f>Tableau1[[#This Row],[Texte_REF_FR]]</f>
@@ -6478,10 +6478,10 @@
         <v>52</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.15">
@@ -6518,10 +6518,10 @@
         <v>84</v>
       </c>
       <c r="E18" s="4" t="s">
+        <v>252</v>
+      </c>
+      <c r="F18" s="4" t="s">
         <v>253</v>
-      </c>
-      <c r="F18" s="4" t="s">
-        <v>254</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.15">
@@ -6538,10 +6538,10 @@
         <v>112</v>
       </c>
       <c r="E19" s="4" t="s">
+        <v>254</v>
+      </c>
+      <c r="F19" s="4" t="s">
         <v>255</v>
-      </c>
-      <c r="F19" s="4" t="s">
-        <v>256</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.15">
@@ -6558,10 +6558,10 @@
         <v>151</v>
       </c>
       <c r="E20" s="4" t="s">
+        <v>256</v>
+      </c>
+      <c r="F20" s="4" t="s">
         <v>257</v>
-      </c>
-      <c r="F20" s="4" t="s">
-        <v>258</v>
       </c>
     </row>
   </sheetData>
@@ -6754,10 +6754,10 @@
         <v>44027</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>597</v>
+        <v>594</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="G2" s="19" t="str">
         <f>CONCATENATE(Tableau2[[#This Row],[Distance_Route]], " km + (",Tableau2[[#This Row],[Nb_tours]]," x ",Tableau2[[#This Row],[KM_par_tours]]," km) = ",Tableau2[[#This Row],[Distance_totale]]," km")</f>
@@ -6804,7 +6804,7 @@
         <v>42</v>
       </c>
       <c r="T2" s="14" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="U2" t="str">
         <f>TEXT(_xlfn.CONCAT(Tableau2[[#This Row],[Heure_dep]],":",Tableau2[[#This Row],[min_dep]]), "HH:MM")</f>
@@ -6836,32 +6836,32 @@
         <v>0.81022727272727268</v>
       </c>
       <c r="AC2" s="16" t="s">
+        <v>211</v>
+      </c>
+      <c r="AD2" s="16" t="s">
         <v>212</v>
       </c>
-      <c r="AD2" s="16" t="s">
+      <c r="AE2" s="16" t="s">
         <v>213</v>
-      </c>
-      <c r="AE2" s="16" t="s">
-        <v>214</v>
       </c>
       <c r="AF2" s="16" t="s">
         <v>129</v>
       </c>
       <c r="AG2" s="16" t="s">
-        <v>604</v>
+        <v>601</v>
       </c>
       <c r="AH2" s="16" t="str">
         <f>Tableau2[[#This Row],[LieuDepFR]]</f>
         <v>CEGEP</v>
       </c>
       <c r="AI2" s="16" t="s">
+        <v>218</v>
+      </c>
+      <c r="AJ2" s="4" t="s">
         <v>219</v>
       </c>
-      <c r="AJ2" s="4" t="s">
-        <v>220</v>
-      </c>
       <c r="AK2" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="AL2" s="15"/>
       <c r="AM2" s="15"/>
@@ -6881,10 +6881,10 @@
         <v>44028</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>598</v>
+        <v>595</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="G3" s="19" t="str">
         <f>CONCATENATE(Tableau2[[#This Row],[Distance_Route]], " km + (",Tableau2[[#This Row],[Nb_tours]]," x ",Tableau2[[#This Row],[KM_par_tours]]," km) = ",Tableau2[[#This Row],[Distance_totale]]," km")</f>
@@ -6931,7 +6931,7 @@
         <v>42</v>
       </c>
       <c r="T3" s="14" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="U3" t="str">
         <f>TEXT(_xlfn.CONCAT(Tableau2[[#This Row],[Heure_dep]],":",Tableau2[[#This Row],[min_dep]]), "HH:MM")</f>
@@ -6966,7 +6966,7 @@
         <v>123</v>
       </c>
       <c r="AD3" s="16" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="AE3" s="16" t="s">
         <v>135</v>
@@ -6975,20 +6975,20 @@
         <v>126</v>
       </c>
       <c r="AG3" s="16" t="s">
-        <v>604</v>
+        <v>601</v>
       </c>
       <c r="AH3" s="16" t="str">
         <f>Tableau2[[#This Row],[LieuDepFR]]</f>
         <v>Cathédrale</v>
       </c>
       <c r="AI3" s="16" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="AJ3" s="4" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="AK3" s="4" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="AL3" s="15"/>
       <c r="AM3" s="15"/>
@@ -7008,10 +7008,10 @@
         <v>44029</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>599</v>
+        <v>596</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="G4" s="19" t="str">
         <f>CONCATENATE(Tableau2[[#This Row],[Distance_totale]]," km")</f>
@@ -7057,7 +7057,7 @@
         <v>42</v>
       </c>
       <c r="T4" s="14" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="U4" t="str">
         <f>TEXT(_xlfn.CONCAT(Tableau2[[#This Row],[Heure_dep]],":",Tableau2[[#This Row],[min_dep]]), "HH:MM")</f>
@@ -7089,14 +7089,14 @@
         <v>0.382518115942029</v>
       </c>
       <c r="AC4" s="16" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="AD4" s="16" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="AE4" s="16"/>
       <c r="AF4" s="16" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="AG4" s="16" t="str">
         <f>Tableau2[[#This Row],[LieuDepFR]]</f>
@@ -7140,10 +7140,10 @@
         <v>44029</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>600</v>
+        <v>597</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="G5" s="19" t="str">
         <f>CONCATENATE(Tableau2[[#This Row],[Distance_totale]]," km")</f>
@@ -7190,7 +7190,7 @@
         <v>44</v>
       </c>
       <c r="T5" s="14" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="U5" t="str">
         <f>TEXT(_xlfn.CONCAT(Tableau2[[#This Row],[Heure_dep]],":",Tableau2[[#This Row],[min_dep]]), "HH:MM")</f>
@@ -7231,14 +7231,14 @@
         <v>140</v>
       </c>
       <c r="AF5" s="16" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="AG5" s="16" t="str">
         <f>Tableau2[[#This Row],[LieuDepFR]]</f>
         <v>Musée minéralogique de l'A-T</v>
       </c>
       <c r="AH5" s="16" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="AI5" s="15" t="str">
         <f>Tableau2[[#This Row],[LieuDepEN]]</f>
@@ -7268,10 +7268,10 @@
         <v>44030</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>601</v>
+        <v>598</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G6" s="19" t="str">
         <f>CONCATENATE(Tableau2[[#This Row],[Distance_totale]]," km")</f>
@@ -7318,7 +7318,7 @@
         <v>41</v>
       </c>
       <c r="T6" s="14" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="U6" t="str">
         <f>TEXT(_xlfn.CONCAT(Tableau2[[#This Row],[Heure_dep]],":",Tableau2[[#This Row],[min_dep]]), "HH:MM")</f>
@@ -7356,25 +7356,25 @@
         <v>131</v>
       </c>
       <c r="AE6" s="16" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="AF6" s="16" t="s">
-        <v>604</v>
+        <v>601</v>
       </c>
       <c r="AG6" s="16" t="s">
+        <v>234</v>
+      </c>
+      <c r="AH6" s="16" t="s">
+        <v>218</v>
+      </c>
+      <c r="AI6" s="16" t="s">
         <v>235</v>
       </c>
-      <c r="AH6" s="16" t="s">
-        <v>219</v>
-      </c>
-      <c r="AI6" s="16" t="s">
-        <v>236</v>
-      </c>
       <c r="AJ6" s="4" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="AK6" s="4" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="AL6" s="15"/>
       <c r="AM6" s="15"/>
@@ -7394,10 +7394,10 @@
         <v>44031</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="F7" s="19" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="G7" s="19" t="str">
         <f>CONCATENATE(Tableau2[[#This Row],[Nb_tours]], " x ",Tableau2[[#This Row],[KM_par_tours]], " km = ",Tableau2[[#This Row],[Distance_totale]]," km")</f>
@@ -7445,7 +7445,7 @@
         <v>42</v>
       </c>
       <c r="T7" s="14" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
       <c r="U7" t="str">
         <f>TEXT(_xlfn.CONCAT(Tableau2[[#This Row],[Heure_dep]],":",Tableau2[[#This Row],[min_dep]]), "HH:MM")</f>
@@ -7477,30 +7477,30 @@
         <v>0.80568181818181817</v>
       </c>
       <c r="AC7" s="16" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="AD7" s="16" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="AE7" s="16"/>
       <c r="AF7" s="21" t="s">
-        <v>604</v>
+        <v>601</v>
       </c>
       <c r="AG7" s="16" t="str">
         <f>Tableau2[[#This Row],[LieuDepFR]]</f>
         <v>Hôtel de ville</v>
       </c>
       <c r="AH7" s="16" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="AI7" s="16" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="AJ7" s="4" t="s">
-        <v>605</v>
+        <v>602</v>
       </c>
       <c r="AK7" s="4" t="s">
-        <v>606</v>
+        <v>603</v>
       </c>
       <c r="AL7" s="15"/>
       <c r="AM7" s="15"/>
@@ -7520,10 +7520,10 @@
         <v>44032</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>602</v>
+        <v>599</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="G8" s="19" t="str">
         <f>CONCATENATE(Tableau2[[#This Row],[Distance_Route]], " km + (",Tableau2[[#This Row],[Nb_tours]]," x ",Tableau2[[#This Row],[KM_par_tours]]," km) = ",Tableau2[[#This Row],[Distance_totale]]," km")</f>
@@ -7570,7 +7570,7 @@
         <v>42</v>
       </c>
       <c r="T8" s="14" t="s">
-        <v>490</v>
+        <v>487</v>
       </c>
       <c r="U8" t="str">
         <f>TEXT(_xlfn.CONCAT(Tableau2[[#This Row],[Heure_dep]],":",Tableau2[[#This Row],[min_dep]]), "HH:MM")</f>
@@ -7605,28 +7605,28 @@
         <v>131</v>
       </c>
       <c r="AD8" s="16" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="AE8" s="16" t="s">
+        <v>215</v>
+      </c>
+      <c r="AF8" s="16" t="s">
+        <v>601</v>
+      </c>
+      <c r="AG8" s="16" t="s">
         <v>216</v>
       </c>
-      <c r="AF8" s="16" t="s">
-        <v>604</v>
-      </c>
-      <c r="AG8" s="16" t="s">
-        <v>217</v>
-      </c>
       <c r="AH8" s="16" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="AI8" s="16" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="AJ8" s="4" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="AK8" s="4" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="AL8" s="15"/>
       <c r="AM8" s="15"/>
@@ -7675,7 +7675,7 @@
         <v>19</v>
       </c>
       <c r="C1" s="39" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="D1" s="40" t="s">
         <v>17</v>
@@ -7684,10 +7684,10 @@
         <v>18</v>
       </c>
       <c r="F1" s="41" t="s">
+        <v>304</v>
+      </c>
+      <c r="G1" s="41" t="s">
         <v>305</v>
-      </c>
-      <c r="G1" s="41" t="s">
-        <v>306</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="15" x14ac:dyDescent="0.2">
@@ -7698,13 +7698,13 @@
         <v>63</v>
       </c>
       <c r="C2" s="29" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D2" s="23" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
       <c r="E2" s="23" t="s">
-        <v>457</v>
+        <v>454</v>
       </c>
       <c r="F2" s="35" t="str">
         <f>VLOOKUP(B2,Lexique!A:F,5,)</f>
@@ -7723,7 +7723,7 @@
         <v>72</v>
       </c>
       <c r="C3" s="29" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D3" s="23" t="s">
         <v>147</v>
@@ -7749,7 +7749,7 @@
         <v>73</v>
       </c>
       <c r="C4" s="29" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D4" s="23" t="s">
         <v>148</v>
@@ -7775,7 +7775,7 @@
         <v>72</v>
       </c>
       <c r="C5" s="29" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="D5" s="23" t="s">
         <v>149</v>
@@ -7801,10 +7801,10 @@
         <v>73</v>
       </c>
       <c r="C6" s="29" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="D6" s="23" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="E6" s="23" t="str">
         <f>D6</f>
@@ -7827,13 +7827,13 @@
         <v>82</v>
       </c>
       <c r="C7" s="29" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D7" s="23" t="s">
+        <v>307</v>
+      </c>
+      <c r="E7" s="23" t="s">
         <v>308</v>
-      </c>
-      <c r="E7" s="23" t="s">
-        <v>309</v>
       </c>
       <c r="F7" s="35" t="str">
         <f>VLOOKUP(B7,Lexique!A:F,5,)</f>
@@ -7852,7 +7852,7 @@
         <v>79</v>
       </c>
       <c r="C8" s="29" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="D8" s="23" t="s">
         <v>10</v>
@@ -7877,13 +7877,13 @@
         <v>5</v>
       </c>
       <c r="C9" s="29" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D9" s="23" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="E9" s="23" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="F9" s="35" t="str">
         <f>VLOOKUP(B9,Lexique!A:F,5,)</f>
@@ -7952,13 +7952,13 @@
         <v>5</v>
       </c>
       <c r="C12" s="29" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="D12" s="23" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="E12" s="25" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="F12" s="35" t="str">
         <f>VLOOKUP(B12,Lexique!A:F,5,)</f>
@@ -8002,13 +8002,13 @@
         <v>71</v>
       </c>
       <c r="C14" s="29" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D14" s="25" t="s">
+        <v>310</v>
+      </c>
+      <c r="E14" s="25" t="s">
         <v>311</v>
-      </c>
-      <c r="E14" s="25" t="s">
-        <v>312</v>
       </c>
       <c r="F14" s="35" t="str">
         <f>VLOOKUP(B14,Lexique!A:F,5,)</f>
@@ -8027,7 +8027,7 @@
         <v>78</v>
       </c>
       <c r="C15" s="29" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="D15" s="23" t="s">
         <v>155</v>
@@ -8077,13 +8077,13 @@
         <v>70</v>
       </c>
       <c r="C17" s="29" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D17" s="43" t="s">
+        <v>313</v>
+      </c>
+      <c r="E17" s="43" t="s">
         <v>314</v>
-      </c>
-      <c r="E17" s="43" t="s">
-        <v>315</v>
       </c>
       <c r="F17" s="35" t="str">
         <f>VLOOKUP(B17,Lexique!A:F,5,)</f>
@@ -8102,10 +8102,10 @@
         <v>5</v>
       </c>
       <c r="C18" s="29" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D18" s="23" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="E18" s="23" t="s">
         <v>140</v>
@@ -8127,13 +8127,13 @@
         <v>81</v>
       </c>
       <c r="C19" s="29" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D19" s="23" t="s">
+        <v>316</v>
+      </c>
+      <c r="E19" s="23" t="s">
         <v>317</v>
-      </c>
-      <c r="E19" s="23" t="s">
-        <v>318</v>
       </c>
       <c r="F19" s="35" t="str">
         <f>VLOOKUP(B19,Lexique!A:F,5,)</f>
@@ -8152,13 +8152,13 @@
         <v>5</v>
       </c>
       <c r="C20" s="29" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D20" s="23" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="E20" s="23" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="F20" s="35" t="str">
         <f>VLOOKUP(B20,Lexique!A:F,5,)</f>
@@ -8177,7 +8177,7 @@
         <v>75</v>
       </c>
       <c r="C21" s="29" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D21" s="24" t="s">
         <v>165</v>
@@ -8203,7 +8203,7 @@
         <v>75</v>
       </c>
       <c r="C22" s="29" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D22" s="23" t="s">
         <v>165</v>
@@ -8229,13 +8229,13 @@
         <v>70</v>
       </c>
       <c r="C23" s="29" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D23" s="43" t="s">
+        <v>319</v>
+      </c>
+      <c r="E23" s="43" t="s">
         <v>320</v>
-      </c>
-      <c r="E23" s="43" t="s">
-        <v>321</v>
       </c>
       <c r="F23" s="35" t="str">
         <f>VLOOKUP(B23,Lexique!A:F,5,)</f>
@@ -8254,13 +8254,13 @@
         <v>5</v>
       </c>
       <c r="C24" s="29" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D24" s="23" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="E24" s="44" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="F24" s="35" t="str">
         <f>VLOOKUP(B24,Lexique!A:F,5,)</f>
@@ -8279,13 +8279,13 @@
         <v>82</v>
       </c>
       <c r="C25" s="29" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="D25" s="23" t="s">
+        <v>322</v>
+      </c>
+      <c r="E25" s="23" t="s">
         <v>323</v>
-      </c>
-      <c r="E25" s="23" t="s">
-        <v>324</v>
       </c>
       <c r="F25" s="35" t="str">
         <f>VLOOKUP(B25,Lexique!A:F,5,)</f>
@@ -8304,13 +8304,13 @@
         <v>25</v>
       </c>
       <c r="C26" s="29" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D26" s="23" t="s">
         <v>22</v>
       </c>
       <c r="E26" s="23" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="F26" s="35" t="str">
         <f>VLOOKUP(B26,Lexique!A:F,5,)</f>
@@ -8329,13 +8329,13 @@
         <v>152</v>
       </c>
       <c r="C27" s="29" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D27" s="23" t="s">
+        <v>204</v>
+      </c>
+      <c r="E27" s="23" t="s">
         <v>205</v>
-      </c>
-      <c r="E27" s="23" t="s">
-        <v>206</v>
       </c>
       <c r="F27" s="35" t="str">
         <f>VLOOKUP(B27,Lexique!A:F,5,)</f>
@@ -8354,13 +8354,13 @@
         <v>5</v>
       </c>
       <c r="C28" s="29" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D28" s="23" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="E28" s="23" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="F28" s="35" t="str">
         <f>VLOOKUP(B28,Lexique!A:F,5,)</f>
@@ -8379,13 +8379,13 @@
         <v>81</v>
       </c>
       <c r="C29" s="29" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D29" s="23" t="s">
+        <v>352</v>
+      </c>
+      <c r="E29" s="23" t="s">
         <v>353</v>
-      </c>
-      <c r="E29" s="23" t="s">
-        <v>354</v>
       </c>
       <c r="F29" s="35" t="str">
         <f>VLOOKUP(B29,Lexique!A:F,5,)</f>
@@ -8404,13 +8404,13 @@
         <v>25</v>
       </c>
       <c r="C30" s="29" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D30" s="24" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="E30" s="24" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="F30" s="35" t="str">
         <f>VLOOKUP(B30,Lexique!A:F,5,)</f>
@@ -8429,7 +8429,7 @@
         <v>78</v>
       </c>
       <c r="C31" s="29" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D31" s="23" t="s">
         <v>154</v>
@@ -8454,13 +8454,13 @@
         <v>5</v>
       </c>
       <c r="C32" s="29" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D32" s="23" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="E32" s="23" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="F32" s="35" t="str">
         <f>VLOOKUP(B32,Lexique!A:F,5,)</f>
@@ -8479,13 +8479,13 @@
         <v>82</v>
       </c>
       <c r="C33" s="29" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="D33" s="23" t="s">
+        <v>328</v>
+      </c>
+      <c r="E33" s="23" t="s">
         <v>329</v>
-      </c>
-      <c r="E33" s="23" t="s">
-        <v>330</v>
       </c>
       <c r="F33" s="35" t="str">
         <f>VLOOKUP(B33,Lexique!A:F,5,)</f>
@@ -8504,10 +8504,10 @@
         <v>73</v>
       </c>
       <c r="C34" s="29" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D34" s="23" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="E34" s="23" t="str">
         <f>D34</f>
@@ -8530,13 +8530,13 @@
         <v>71</v>
       </c>
       <c r="C35" s="29" t="s">
+        <v>418</v>
+      </c>
+      <c r="D35" s="25" t="s">
         <v>419</v>
       </c>
-      <c r="D35" s="25" t="s">
+      <c r="E35" s="25" t="s">
         <v>420</v>
-      </c>
-      <c r="E35" s="25" t="s">
-        <v>421</v>
       </c>
       <c r="F35" s="35" t="str">
         <f>VLOOKUP(B35,Lexique!A:F,5,)</f>
@@ -8555,10 +8555,10 @@
         <v>72</v>
       </c>
       <c r="C36" s="29" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D36" s="23" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="E36" s="23" t="str">
         <f>D36</f>
@@ -8581,10 +8581,10 @@
         <v>73</v>
       </c>
       <c r="C37" s="29" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D37" s="23" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="E37" s="23" t="str">
         <f>D37</f>
@@ -8607,13 +8607,13 @@
         <v>72</v>
       </c>
       <c r="C38" s="29" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="D38" s="23" t="s">
-        <v>603</v>
+        <v>600</v>
       </c>
       <c r="E38" s="23" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="F38" s="35" t="str">
         <f>VLOOKUP(B38,Lexique!A:F,5,)</f>
@@ -8632,10 +8632,10 @@
         <v>73</v>
       </c>
       <c r="C39" s="29" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D39" s="23" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="E39" s="23" t="str">
         <f>D39</f>
@@ -8658,10 +8658,10 @@
         <v>73</v>
       </c>
       <c r="C40" s="29" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="D40" s="23" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E40" s="23" t="str">
         <f>D40</f>
@@ -8684,13 +8684,13 @@
         <v>76</v>
       </c>
       <c r="C41" s="29" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D41" s="23" t="s">
+        <v>335</v>
+      </c>
+      <c r="E41" s="23" t="s">
         <v>336</v>
-      </c>
-      <c r="E41" s="23" t="s">
-        <v>337</v>
       </c>
       <c r="F41" s="35" t="str">
         <f>VLOOKUP(B41,Lexique!A:F,5,)</f>
@@ -8709,10 +8709,10 @@
         <v>73</v>
       </c>
       <c r="C42" s="29" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="D42" s="23" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="E42" s="23" t="str">
         <f>D42</f>
@@ -8735,10 +8735,10 @@
         <v>72</v>
       </c>
       <c r="C43" s="29" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="D43" s="24" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="E43" s="23" t="str">
         <f t="shared" ref="E43:E49" si="0">D43</f>
@@ -8761,10 +8761,10 @@
         <v>73</v>
       </c>
       <c r="C44" s="29" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D44" s="23" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="E44" s="23" t="str">
         <f t="shared" si="0"/>
@@ -8787,10 +8787,10 @@
         <v>73</v>
       </c>
       <c r="C45" s="29" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="D45" s="23" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="E45" s="23" t="str">
         <f t="shared" si="0"/>
@@ -8813,10 +8813,10 @@
         <v>73</v>
       </c>
       <c r="C46" s="29" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="D46" s="24" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="E46" s="23" t="str">
         <f t="shared" si="0"/>
@@ -8839,10 +8839,10 @@
         <v>72</v>
       </c>
       <c r="C47" s="32" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="D47" s="26" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="E47" s="23" t="str">
         <f t="shared" si="0"/>
@@ -8865,10 +8865,10 @@
         <v>73</v>
       </c>
       <c r="C48" s="32" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D48" s="26" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="E48" s="23" t="str">
         <f t="shared" si="0"/>
@@ -8891,10 +8891,10 @@
         <v>73</v>
       </c>
       <c r="C49" s="32" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="D49" s="26" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E49" s="23" t="str">
         <f t="shared" si="0"/>
@@ -8917,13 +8917,13 @@
         <v>76</v>
       </c>
       <c r="C50" s="32" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="D50" s="23" t="s">
+        <v>342</v>
+      </c>
+      <c r="E50" s="23" t="s">
         <v>343</v>
-      </c>
-      <c r="E50" s="23" t="s">
-        <v>344</v>
       </c>
       <c r="F50" s="35" t="str">
         <f>VLOOKUP(B50,Lexique!A:F,5,)</f>
@@ -8942,13 +8942,13 @@
         <v>80</v>
       </c>
       <c r="C51" s="32" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D51" s="26" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="E51" s="26" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F51" s="35" t="str">
         <f>VLOOKUP(B51,Lexique!A:F,5,)</f>
@@ -8967,13 +8967,13 @@
         <v>110</v>
       </c>
       <c r="C52" s="32" t="s">
+        <v>345</v>
+      </c>
+      <c r="D52" s="26" t="s">
         <v>346</v>
       </c>
-      <c r="D52" s="26" t="s">
+      <c r="E52" s="26" t="s">
         <v>347</v>
-      </c>
-      <c r="E52" s="26" t="s">
-        <v>348</v>
       </c>
       <c r="F52" s="35" t="str">
         <f>VLOOKUP(B52,Lexique!A:F,5,)</f>
@@ -8992,7 +8992,7 @@
         <v>43</v>
       </c>
       <c r="C53" s="32" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D53" s="26" t="s">
         <v>109</v>
@@ -10135,7 +10135,7 @@
         <v>19</v>
       </c>
       <c r="C1" s="39" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="D1" s="40" t="s">
         <v>17</v>
@@ -10144,10 +10144,10 @@
         <v>18</v>
       </c>
       <c r="F1" s="41" t="s">
+        <v>304</v>
+      </c>
+      <c r="G1" s="41" t="s">
         <v>305</v>
-      </c>
-      <c r="G1" s="41" t="s">
-        <v>306</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="15" x14ac:dyDescent="0.2">
@@ -10158,13 +10158,13 @@
         <v>63</v>
       </c>
       <c r="C2" s="29" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D2" s="23" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
       <c r="E2" s="23" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
       <c r="F2" s="35" t="str">
         <f>VLOOKUP(B2,Lexique!A:F,5,)</f>
@@ -10189,7 +10189,7 @@
         <v>22</v>
       </c>
       <c r="E3" s="23" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
       <c r="F3" s="35" t="str">
         <f>VLOOKUP(B3,Lexique!A:F,5,)</f>
@@ -10208,13 +10208,13 @@
         <v>72</v>
       </c>
       <c r="C4" s="29" t="s">
-        <v>541</v>
+        <v>538</v>
       </c>
       <c r="D4" s="23" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E4" s="23" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="F4" s="35" t="str">
         <f>VLOOKUP(B4,Lexique!A:F,5,)</f>
@@ -10233,13 +10233,13 @@
         <v>82</v>
       </c>
       <c r="C5" s="29" t="s">
-        <v>543</v>
+        <v>540</v>
       </c>
       <c r="D5" s="23" t="s">
-        <v>582</v>
+        <v>579</v>
       </c>
       <c r="E5" s="23" t="s">
-        <v>583</v>
+        <v>580</v>
       </c>
       <c r="F5" s="35" t="str">
         <f>VLOOKUP(B5,Lexique!A:F,5,)</f>
@@ -10258,13 +10258,13 @@
         <v>82</v>
       </c>
       <c r="C6" s="29" t="s">
-        <v>544</v>
+        <v>541</v>
       </c>
       <c r="D6" s="23" t="s">
-        <v>580</v>
+        <v>577</v>
       </c>
       <c r="E6" s="23" t="s">
-        <v>581</v>
+        <v>578</v>
       </c>
       <c r="F6" s="35" t="str">
         <f>VLOOKUP(B6,Lexique!A:F,5,)</f>
@@ -10283,7 +10283,7 @@
         <v>79</v>
       </c>
       <c r="C7" s="29" t="s">
-        <v>545</v>
+        <v>542</v>
       </c>
       <c r="D7" s="23" t="s">
         <v>10</v>
@@ -10308,13 +10308,13 @@
         <v>73</v>
       </c>
       <c r="C8" s="29" t="s">
-        <v>546</v>
+        <v>543</v>
       </c>
       <c r="D8" s="23" t="s">
-        <v>547</v>
+        <v>544</v>
       </c>
       <c r="E8" s="23" t="s">
-        <v>547</v>
+        <v>544</v>
       </c>
       <c r="F8" s="35" t="str">
         <f>VLOOKUP(B8,Lexique!A:F,5,)</f>
@@ -10333,10 +10333,10 @@
         <v>5</v>
       </c>
       <c r="C9" s="29" t="s">
-        <v>568</v>
+        <v>565</v>
       </c>
       <c r="D9" s="23" t="s">
-        <v>568</v>
+        <v>565</v>
       </c>
       <c r="E9" s="23" t="str">
         <f>D9</f>
@@ -10359,13 +10359,13 @@
         <v>81</v>
       </c>
       <c r="C10" s="29" t="s">
-        <v>548</v>
+        <v>545</v>
       </c>
       <c r="D10" s="23" t="s">
-        <v>570</v>
+        <v>567</v>
       </c>
       <c r="E10" s="24" t="s">
-        <v>569</v>
+        <v>566</v>
       </c>
       <c r="F10" s="35" t="str">
         <f>VLOOKUP(B10,Lexique!A:F,5,)</f>
@@ -10390,7 +10390,7 @@
         <v>12</v>
       </c>
       <c r="E11" s="23" t="s">
-        <v>549</v>
+        <v>546</v>
       </c>
       <c r="F11" s="35" t="str">
         <f>VLOOKUP(B11,Lexique!A:F,5,)</f>
@@ -10409,13 +10409,13 @@
         <v>71</v>
       </c>
       <c r="C12" s="29" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D12" s="23" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="E12" s="23" t="s">
-        <v>575</v>
+        <v>572</v>
       </c>
       <c r="F12" s="35" t="str">
         <f>VLOOKUP(B12,Lexique!A:F,5,)</f>
@@ -10435,7 +10435,7 @@
         <v>78</v>
       </c>
       <c r="C13" s="29" t="s">
-        <v>550</v>
+        <v>547</v>
       </c>
       <c r="D13" s="23" t="s">
         <v>155</v>
@@ -10460,13 +10460,13 @@
         <v>72</v>
       </c>
       <c r="C14" s="29" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="D14" s="25" t="s">
-        <v>552</v>
+        <v>549</v>
       </c>
       <c r="E14" s="25" t="s">
-        <v>552</v>
+        <v>549</v>
       </c>
       <c r="F14" s="35" t="str">
         <f>VLOOKUP(B14,Lexique!A:F,5,)</f>
@@ -10485,7 +10485,7 @@
         <v>25</v>
       </c>
       <c r="C15" s="29" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="D15" s="23" t="s">
         <v>2</v>
@@ -10510,7 +10510,7 @@
         <v>25</v>
       </c>
       <c r="C16" s="29" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="D16" s="23" t="s">
         <v>2</v>
@@ -10535,13 +10535,13 @@
         <v>5</v>
       </c>
       <c r="C17" s="29" t="s">
-        <v>553</v>
+        <v>550</v>
       </c>
       <c r="D17" s="26" t="s">
-        <v>554</v>
+        <v>551</v>
       </c>
       <c r="E17" s="25" t="s">
-        <v>554</v>
+        <v>551</v>
       </c>
       <c r="F17" s="35" t="str">
         <f>VLOOKUP(B17,Lexique!A:F,5,)</f>
@@ -10560,13 +10560,13 @@
         <v>70</v>
       </c>
       <c r="C18" s="29" t="s">
-        <v>555</v>
+        <v>552</v>
       </c>
       <c r="D18" s="23" t="s">
-        <v>571</v>
+        <v>568</v>
       </c>
       <c r="E18" s="23" t="s">
-        <v>556</v>
+        <v>553</v>
       </c>
       <c r="F18" s="35" t="str">
         <f>VLOOKUP(B18,Lexique!A:F,5,)</f>
@@ -10591,7 +10591,7 @@
         <v>22</v>
       </c>
       <c r="E19" s="23" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
       <c r="F19" s="35" t="str">
         <f>VLOOKUP(B19,Lexique!A:F,5,)</f>
@@ -10610,13 +10610,13 @@
         <v>152</v>
       </c>
       <c r="C20" s="29" t="s">
-        <v>557</v>
+        <v>554</v>
       </c>
       <c r="D20" s="25" t="s">
-        <v>557</v>
+        <v>554</v>
       </c>
       <c r="E20" s="25" t="s">
-        <v>558</v>
+        <v>555</v>
       </c>
       <c r="F20" s="35" t="str">
         <f>VLOOKUP(B20,Lexique!A:F,5,)</f>
@@ -10635,13 +10635,13 @@
         <v>71</v>
       </c>
       <c r="C21" s="29" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D21" s="23" t="s">
-        <v>576</v>
+        <v>573</v>
       </c>
       <c r="E21" s="23" t="s">
-        <v>577</v>
+        <v>574</v>
       </c>
       <c r="F21" s="35" t="str">
         <f>VLOOKUP(B21,Lexique!A:F,5,)</f>
@@ -10660,7 +10660,7 @@
         <v>25</v>
       </c>
       <c r="C22" s="29" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="D22" s="23" t="s">
         <v>2</v>
@@ -10685,7 +10685,7 @@
         <v>25</v>
       </c>
       <c r="C23" s="29" t="s">
-        <v>559</v>
+        <v>556</v>
       </c>
       <c r="D23" s="23" t="s">
         <v>2</v>
@@ -10710,13 +10710,13 @@
         <v>81</v>
       </c>
       <c r="C24" s="29" t="s">
-        <v>548</v>
+        <v>545</v>
       </c>
       <c r="D24" s="23" t="s">
-        <v>588</v>
+        <v>585</v>
       </c>
       <c r="E24" s="24" t="s">
-        <v>589</v>
+        <v>586</v>
       </c>
       <c r="F24" s="35" t="str">
         <f>VLOOKUP(B24,Lexique!A:F,5,)</f>
@@ -10736,7 +10736,7 @@
         <v>78</v>
       </c>
       <c r="C25" s="29" t="s">
-        <v>560</v>
+        <v>557</v>
       </c>
       <c r="D25" s="25" t="s">
         <v>154</v>
@@ -10761,10 +10761,10 @@
         <v>5</v>
       </c>
       <c r="C26" s="29" t="s">
-        <v>586</v>
+        <v>583</v>
       </c>
       <c r="D26" s="25" t="s">
-        <v>587</v>
+        <v>584</v>
       </c>
       <c r="E26" s="25" t="str">
         <f>D26</f>
@@ -10787,13 +10787,13 @@
         <v>82</v>
       </c>
       <c r="C27" s="29" t="s">
-        <v>561</v>
+        <v>558</v>
       </c>
       <c r="D27" s="23" t="s">
-        <v>578</v>
+        <v>575</v>
       </c>
       <c r="E27" s="23" t="s">
-        <v>579</v>
+        <v>576</v>
       </c>
       <c r="F27" s="35" t="str">
         <f>VLOOKUP(B27,Lexique!A:F,5,)</f>
@@ -10818,7 +10818,7 @@
         <v>22</v>
       </c>
       <c r="E28" s="23" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
       <c r="F28" s="35" t="str">
         <f>VLOOKUP(B28,Lexique!A:F,5,)</f>
@@ -10837,13 +10837,13 @@
         <v>72</v>
       </c>
       <c r="C29" s="29" t="s">
-        <v>562</v>
+        <v>559</v>
       </c>
       <c r="D29" s="25" t="s">
-        <v>510</v>
+        <v>507</v>
       </c>
       <c r="E29" s="25" t="s">
-        <v>511</v>
+        <v>508</v>
       </c>
       <c r="F29" s="35" t="str">
         <f>VLOOKUP(B29,Lexique!A:F,5,)</f>
@@ -10862,13 +10862,13 @@
         <v>76</v>
       </c>
       <c r="C30" s="29" t="s">
-        <v>563</v>
+        <v>560</v>
       </c>
       <c r="D30" s="23" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E30" s="23" t="s">
-        <v>573</v>
+        <v>570</v>
       </c>
       <c r="F30" s="35" t="str">
         <f>VLOOKUP(B30,Lexique!A:F,5,)</f>
@@ -10887,13 +10887,13 @@
         <v>73</v>
       </c>
       <c r="C31" s="29" t="s">
-        <v>514</v>
+        <v>511</v>
       </c>
       <c r="D31" s="23" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="E31" s="23" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="F31" s="35" t="str">
         <f>VLOOKUP(B31,Lexique!A:F,5,)</f>
@@ -10912,13 +10912,13 @@
         <v>72</v>
       </c>
       <c r="C32" s="29" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
       <c r="D32" s="63" t="s">
-        <v>516</v>
+        <v>513</v>
       </c>
       <c r="E32" s="28" t="s">
-        <v>516</v>
+        <v>513</v>
       </c>
       <c r="F32" s="35" t="str">
         <f>VLOOKUP(B32,Lexique!A:F,5,)</f>
@@ -10937,13 +10937,13 @@
         <v>73</v>
       </c>
       <c r="C33" s="29" t="s">
-        <v>517</v>
+        <v>514</v>
       </c>
       <c r="D33" s="23" t="s">
-        <v>518</v>
+        <v>515</v>
       </c>
       <c r="E33" s="23" t="s">
-        <v>518</v>
+        <v>515</v>
       </c>
       <c r="F33" s="35" t="str">
         <f>VLOOKUP(B33,Lexique!A:F,5,)</f>
@@ -10962,13 +10962,13 @@
         <v>71</v>
       </c>
       <c r="C34" s="29" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D34" s="23" t="s">
-        <v>519</v>
+        <v>516</v>
       </c>
       <c r="E34" s="23" t="s">
-        <v>519</v>
+        <v>516</v>
       </c>
       <c r="F34" s="35" t="str">
         <f>VLOOKUP(B34,Lexique!A:F,5,)</f>
@@ -10987,13 +10987,13 @@
         <v>73</v>
       </c>
       <c r="C35" s="29" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
       <c r="D35" s="26" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="E35" s="26" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="F35" s="35" t="str">
         <f>VLOOKUP(B35,Lexique!A:F,5,)</f>
@@ -11012,13 +11012,13 @@
         <v>73</v>
       </c>
       <c r="C36" s="29" t="s">
-        <v>564</v>
+        <v>561</v>
       </c>
       <c r="D36" s="23" t="s">
-        <v>522</v>
+        <v>519</v>
       </c>
       <c r="E36" s="23" t="s">
-        <v>522</v>
+        <v>519</v>
       </c>
       <c r="F36" s="35" t="str">
         <f>VLOOKUP(B36,Lexique!A:F,5,)</f>
@@ -11037,13 +11037,13 @@
         <v>72</v>
       </c>
       <c r="C37" s="29" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
       <c r="D37" s="23" t="s">
-        <v>516</v>
+        <v>513</v>
       </c>
       <c r="E37" s="23" t="s">
-        <v>516</v>
+        <v>513</v>
       </c>
       <c r="F37" s="35" t="str">
         <f>VLOOKUP(B37,Lexique!A:F,5,)</f>
@@ -11062,13 +11062,13 @@
         <v>73</v>
       </c>
       <c r="C38" s="29" t="s">
-        <v>526</v>
+        <v>523</v>
       </c>
       <c r="D38" s="24" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="E38" s="24" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="F38" s="35" t="str">
         <f>VLOOKUP(B38,Lexique!A:F,5,)</f>
@@ -11087,13 +11087,13 @@
         <v>73</v>
       </c>
       <c r="C39" s="29" t="s">
-        <v>527</v>
+        <v>524</v>
       </c>
       <c r="D39" s="23" t="s">
-        <v>528</v>
+        <v>525</v>
       </c>
       <c r="E39" s="23" t="s">
-        <v>528</v>
+        <v>525</v>
       </c>
       <c r="F39" s="35" t="str">
         <f>VLOOKUP(B39,Lexique!A:F,5,)</f>
@@ -11112,13 +11112,13 @@
         <v>70</v>
       </c>
       <c r="C40" s="29" t="s">
-        <v>565</v>
+        <v>562</v>
       </c>
       <c r="D40" s="23" t="s">
-        <v>584</v>
+        <v>581</v>
       </c>
       <c r="E40" s="23" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="F40" s="35" t="str">
         <f>VLOOKUP(B40,Lexique!A:F,5,)</f>
@@ -11137,13 +11137,13 @@
         <v>80</v>
       </c>
       <c r="C41" s="34" t="s">
-        <v>566</v>
+        <v>563</v>
       </c>
       <c r="D41" s="23" t="s">
-        <v>567</v>
+        <v>564</v>
       </c>
       <c r="E41" s="23" t="s">
-        <v>572</v>
+        <v>569</v>
       </c>
       <c r="F41" s="35" t="str">
         <f>VLOOKUP(B41,Lexique!A:F,5,)</f>
@@ -11162,13 +11162,13 @@
         <v>110</v>
       </c>
       <c r="C42" s="34" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
       <c r="D42" s="63" t="s">
+        <v>346</v>
+      </c>
+      <c r="E42" s="27" t="s">
         <v>347</v>
-      </c>
-      <c r="E42" s="27" t="s">
-        <v>348</v>
       </c>
       <c r="F42" s="35" t="str">
         <f>VLOOKUP(B42,Lexique!A:F,5,)</f>
@@ -11187,7 +11187,7 @@
         <v>43</v>
       </c>
       <c r="C43" s="34" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D43" s="63" t="s">
         <v>166</v>
@@ -13149,7 +13149,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D75B715-9E33-8E4E-9ACA-D6CC0A1B5E86}">
   <dimension ref="A1:G326"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
@@ -13173,7 +13173,7 @@
         <v>19</v>
       </c>
       <c r="C1" s="39" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="D1" s="40" t="s">
         <v>17</v>
@@ -13182,10 +13182,10 @@
         <v>18</v>
       </c>
       <c r="F1" s="45" t="s">
+        <v>304</v>
+      </c>
+      <c r="G1" s="45" t="s">
         <v>305</v>
-      </c>
-      <c r="G1" s="45" t="s">
-        <v>306</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="15" x14ac:dyDescent="0.15">
@@ -13197,10 +13197,10 @@
       </c>
       <c r="C2" s="29"/>
       <c r="D2" s="23" t="s">
+        <v>378</v>
+      </c>
+      <c r="E2" s="23" t="s">
         <v>379</v>
-      </c>
-      <c r="E2" s="23" t="s">
-        <v>380</v>
       </c>
       <c r="F2" s="47" t="str">
         <f>VLOOKUP(B2,Lexique!A:F,5,)</f>
@@ -13219,7 +13219,7 @@
         <v>73</v>
       </c>
       <c r="C3" s="29" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="D3" s="23" t="str">
         <f>C3</f>
@@ -13246,10 +13246,10 @@
         <v>72</v>
       </c>
       <c r="C4" s="29" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="D4" s="23" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="E4" s="23" t="str">
         <f>D4</f>
@@ -13272,13 +13272,13 @@
         <v>75</v>
       </c>
       <c r="C5" s="29" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="D5" s="23" t="s">
+        <v>370</v>
+      </c>
+      <c r="E5" s="23" t="s">
         <v>371</v>
-      </c>
-      <c r="E5" s="23" t="s">
-        <v>372</v>
       </c>
       <c r="F5" s="47" t="str">
         <f>VLOOKUP(B5,Lexique!A:F,5,)</f>
@@ -13297,10 +13297,10 @@
         <v>73</v>
       </c>
       <c r="C6" s="29" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="D6" s="23" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="E6" s="23" t="str">
         <f>D6</f>
@@ -13323,13 +13323,13 @@
         <v>74</v>
       </c>
       <c r="C7" s="29" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="D7" s="23" t="s">
-        <v>624</v>
+        <v>618</v>
       </c>
       <c r="E7" s="23" t="s">
-        <v>625</v>
+        <v>619</v>
       </c>
       <c r="F7" s="47" t="str">
         <f>VLOOKUP(B7,Lexique!A:F,5,)</f>
@@ -13348,10 +13348,10 @@
         <v>76</v>
       </c>
       <c r="C8" s="29" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D8" s="23" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="E8" s="23" t="str">
         <f>D8</f>
@@ -13374,10 +13374,10 @@
         <v>73</v>
       </c>
       <c r="C9" s="29" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="D9" s="23" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="E9" s="23" t="str">
         <f t="shared" ref="E9:E18" si="0">D9</f>
@@ -13400,13 +13400,13 @@
         <v>73</v>
       </c>
       <c r="C10" s="29" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="D10" s="23" t="s">
+        <v>372</v>
+      </c>
+      <c r="E10" s="23" t="s">
         <v>373</v>
-      </c>
-      <c r="E10" s="23" t="s">
-        <v>374</v>
       </c>
       <c r="F10" s="47" t="str">
         <f>VLOOKUP(B10,Lexique!A:F,5,)</f>
@@ -13425,13 +13425,13 @@
         <v>77</v>
       </c>
       <c r="C11" s="29" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="D11" s="23" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="E11" s="23" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="F11" s="47" t="str">
         <f>VLOOKUP(B11,Lexique!A:F,5,)</f>
@@ -13450,13 +13450,13 @@
         <v>72</v>
       </c>
       <c r="C12" s="29" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="D12" s="49" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="E12" s="23" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="F12" s="47" t="str">
         <f>VLOOKUP(B12,Lexique!A:F,5,)</f>
@@ -13475,13 +13475,13 @@
         <v>72</v>
       </c>
       <c r="C13" s="29" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D13" s="23" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="E13" s="23" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="F13" s="47" t="str">
         <f>VLOOKUP(B13,Lexique!A:F,5,)</f>
@@ -13500,10 +13500,10 @@
         <v>76</v>
       </c>
       <c r="C14" s="29" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="D14" s="23" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="E14" s="23" t="str">
         <f t="shared" si="0"/>
@@ -13526,10 +13526,10 @@
         <v>72</v>
       </c>
       <c r="C15" s="29" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="D15" s="23" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="E15" s="23" t="str">
         <f t="shared" si="0"/>
@@ -13552,13 +13552,13 @@
         <v>75</v>
       </c>
       <c r="C16" s="29" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="D16" s="23" t="s">
+        <v>370</v>
+      </c>
+      <c r="E16" s="23" t="s">
         <v>371</v>
-      </c>
-      <c r="E16" s="23" t="s">
-        <v>372</v>
       </c>
       <c r="F16" s="47" t="str">
         <f>VLOOKUP(B16,Lexique!A:F,5,)</f>
@@ -13577,10 +13577,10 @@
         <v>73</v>
       </c>
       <c r="C17" s="29" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="D17" s="49" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="E17" s="23" t="str">
         <f t="shared" si="0"/>
@@ -13603,10 +13603,10 @@
         <v>72</v>
       </c>
       <c r="C18" s="29" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="D18" s="50" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="E18" s="23" t="str">
         <f t="shared" si="0"/>
@@ -13629,10 +13629,10 @@
         <v>43</v>
       </c>
       <c r="C19" s="29" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="D19" s="23" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E19" s="23" t="s">
         <v>43</v>
@@ -15876,7 +15876,7 @@
         <v>19</v>
       </c>
       <c r="C1" s="39" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="D1" s="40" t="s">
         <v>17</v>
@@ -15885,10 +15885,10 @@
         <v>18</v>
       </c>
       <c r="F1" s="41" t="s">
+        <v>304</v>
+      </c>
+      <c r="G1" s="41" t="s">
         <v>305</v>
-      </c>
-      <c r="G1" s="41" t="s">
-        <v>306</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.2">
@@ -15900,10 +15900,10 @@
       </c>
       <c r="C2" s="29"/>
       <c r="D2" s="23" t="s">
-        <v>486</v>
+        <v>483</v>
       </c>
       <c r="E2" s="23" t="s">
-        <v>487</v>
+        <v>484</v>
       </c>
       <c r="F2" s="35" t="str">
         <f>VLOOKUP(B2,Lexique!A:F,5,)</f>
@@ -15922,10 +15922,10 @@
         <v>73</v>
       </c>
       <c r="C3" s="29" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
       <c r="D3" s="23" t="s">
-        <v>476</v>
+        <v>473</v>
       </c>
       <c r="E3" s="23" t="str">
         <f>D3</f>
@@ -15948,10 +15948,10 @@
         <v>73</v>
       </c>
       <c r="C4" s="29" t="s">
-        <v>459</v>
+        <v>456</v>
       </c>
       <c r="D4" s="23" t="s">
-        <v>481</v>
+        <v>478</v>
       </c>
       <c r="E4" s="23" t="str">
         <f>D4</f>
@@ -15974,13 +15974,13 @@
         <v>75</v>
       </c>
       <c r="C5" s="29" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
       <c r="D5" s="23" t="s">
-        <v>482</v>
+        <v>479</v>
       </c>
       <c r="E5" s="23" t="s">
-        <v>483</v>
+        <v>480</v>
       </c>
       <c r="F5" s="35" t="str">
         <f>VLOOKUP(B5,Lexique!A:F,5,)</f>
@@ -15999,7 +15999,7 @@
         <v>25</v>
       </c>
       <c r="C6" s="29" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D6" s="23" t="s">
         <v>22</v>
@@ -16024,13 +16024,13 @@
         <v>82</v>
       </c>
       <c r="C7" s="29" t="s">
-        <v>461</v>
+        <v>458</v>
       </c>
       <c r="D7" s="23" t="s">
-        <v>479</v>
+        <v>476</v>
       </c>
       <c r="E7" s="23" t="s">
-        <v>480</v>
+        <v>477</v>
       </c>
       <c r="F7" s="35" t="str">
         <f>VLOOKUP(B7,Lexique!A:F,5,)</f>
@@ -16049,7 +16049,7 @@
         <v>79</v>
       </c>
       <c r="C8" s="29" t="s">
-        <v>462</v>
+        <v>459</v>
       </c>
       <c r="D8" s="23" t="s">
         <v>10</v>
@@ -16074,7 +16074,7 @@
         <v>74</v>
       </c>
       <c r="C9" s="29" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="D9" s="28" t="s">
         <v>165</v>
@@ -16100,13 +16100,13 @@
         <v>81</v>
       </c>
       <c r="C10" s="29" t="s">
-        <v>464</v>
+        <v>461</v>
       </c>
       <c r="D10" s="23" t="s">
+        <v>184</v>
+      </c>
+      <c r="E10" s="23" t="s">
         <v>185</v>
-      </c>
-      <c r="E10" s="23" t="s">
-        <v>186</v>
       </c>
       <c r="F10" s="35" t="str">
         <f>VLOOKUP(B10,Lexique!A:F,5,)</f>
@@ -16125,13 +16125,13 @@
         <v>5</v>
       </c>
       <c r="C11" s="29" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D11" s="23" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E11" s="23" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="F11" s="35" t="str">
         <f>VLOOKUP(B11,Lexique!A:F,5,)</f>
@@ -16150,7 +16150,7 @@
         <v>74</v>
       </c>
       <c r="C12" s="29" t="s">
-        <v>465</v>
+        <v>462</v>
       </c>
       <c r="D12" s="28" t="s">
         <v>165</v>
@@ -16201,13 +16201,13 @@
         <v>73</v>
       </c>
       <c r="C14" s="29" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
       <c r="D14" s="23" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E14" s="23" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F14" s="35" t="str">
         <f>VLOOKUP(B14,Lexique!A:F,5,)</f>
@@ -16226,13 +16226,13 @@
         <v>73</v>
       </c>
       <c r="C15" s="29" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="D15" s="23" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E15" s="24" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="F15" s="35" t="str">
         <f>VLOOKUP(B15,Lexique!A:F,5,)</f>
@@ -16251,7 +16251,7 @@
         <v>72</v>
       </c>
       <c r="C16" s="29" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
       <c r="D16" s="24" t="s">
         <v>165</v>
@@ -16276,13 +16276,13 @@
         <v>5</v>
       </c>
       <c r="C17" s="29" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D17" s="23" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E17" s="25" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="F17" s="35" t="str">
         <f>VLOOKUP(B17,Lexique!A:F,5,)</f>
@@ -16301,7 +16301,7 @@
         <v>75</v>
       </c>
       <c r="C18" s="29" t="s">
-        <v>469</v>
+        <v>466</v>
       </c>
       <c r="D18" s="28" t="s">
         <v>165</v>
@@ -16327,13 +16327,13 @@
         <v>81</v>
       </c>
       <c r="C19" s="29" t="s">
-        <v>464</v>
+        <v>461</v>
       </c>
       <c r="D19" s="23" t="s">
+        <v>184</v>
+      </c>
+      <c r="E19" s="25" t="s">
         <v>185</v>
-      </c>
-      <c r="E19" s="25" t="s">
-        <v>186</v>
       </c>
       <c r="F19" s="35" t="str">
         <f>VLOOKUP(B19,Lexique!A:F,5,)</f>
@@ -16377,13 +16377,13 @@
         <v>82</v>
       </c>
       <c r="C21" s="29" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
       <c r="D21" s="23" t="s">
-        <v>477</v>
+        <v>474</v>
       </c>
       <c r="E21" s="23" t="s">
-        <v>478</v>
+        <v>475</v>
       </c>
       <c r="F21" s="35" t="str">
         <f>VLOOKUP(B21,Lexique!A:F,5,)</f>
@@ -16402,7 +16402,7 @@
         <v>25</v>
       </c>
       <c r="C22" s="29" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D22" s="23" t="s">
         <v>22</v>
@@ -16427,13 +16427,13 @@
         <v>75</v>
       </c>
       <c r="C23" s="29" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
       <c r="D23" s="23" t="s">
-        <v>482</v>
+        <v>479</v>
       </c>
       <c r="E23" s="23" t="s">
-        <v>483</v>
+        <v>480</v>
       </c>
       <c r="F23" s="35" t="str">
         <f>VLOOKUP(B23,Lexique!A:F,5,)</f>
@@ -16452,13 +16452,13 @@
         <v>72</v>
       </c>
       <c r="C24" s="29" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
       <c r="D24" s="28" t="s">
-        <v>484</v>
+        <v>481</v>
       </c>
       <c r="E24" s="28" t="s">
-        <v>485</v>
+        <v>482</v>
       </c>
       <c r="F24" s="35" t="str">
         <f>VLOOKUP(B24,Lexique!A:F,5,)</f>
@@ -16477,13 +16477,13 @@
         <v>110</v>
       </c>
       <c r="C25" s="29" t="s">
-        <v>472</v>
+        <v>469</v>
       </c>
       <c r="D25" s="23" t="s">
-        <v>488</v>
+        <v>485</v>
       </c>
       <c r="E25" s="23" t="s">
-        <v>489</v>
+        <v>486</v>
       </c>
       <c r="F25" s="35" t="str">
         <f>VLOOKUP(B25,Lexique!A:F,5,)</f>
@@ -16502,10 +16502,10 @@
         <v>73</v>
       </c>
       <c r="C26" s="29" t="s">
-        <v>473</v>
+        <v>470</v>
       </c>
       <c r="D26" s="23" t="s">
-        <v>474</v>
+        <v>471</v>
       </c>
       <c r="E26" s="23" t="str">
         <f>D26</f>
@@ -16528,7 +16528,7 @@
         <v>43</v>
       </c>
       <c r="C27" s="29" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D27" s="23" t="s">
         <v>166</v>
@@ -18658,8 +18658,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA4CF35A-AE95-4D4B-80F8-FB6E5D8CEEB2}">
   <dimension ref="A1:I48"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView topLeftCell="A5" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
@@ -18681,7 +18681,7 @@
         <v>19</v>
       </c>
       <c r="C1" s="39" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="D1" s="39" t="s">
         <v>17</v>
@@ -18690,10 +18690,10 @@
         <v>18</v>
       </c>
       <c r="F1" s="41" t="s">
+        <v>304</v>
+      </c>
+      <c r="G1" s="41" t="s">
         <v>305</v>
-      </c>
-      <c r="G1" s="41" t="s">
-        <v>306</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="15" x14ac:dyDescent="0.2">
@@ -18705,10 +18705,10 @@
       </c>
       <c r="C2" s="29"/>
       <c r="D2" s="23" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
       <c r="E2" s="23" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
       <c r="F2" s="35" t="str">
         <f>VLOOKUP(B2,Lexique!A:F,5,)</f>
@@ -18729,10 +18729,10 @@
       </c>
       <c r="C3" s="29"/>
       <c r="D3" s="23" t="s">
+        <v>190</v>
+      </c>
+      <c r="E3" s="23" t="s">
         <v>191</v>
-      </c>
-      <c r="E3" s="23" t="s">
-        <v>192</v>
       </c>
       <c r="F3" s="35" t="str">
         <f>VLOOKUP(B3,Lexique!A:F,5,)</f>
@@ -18823,7 +18823,7 @@
       </c>
       <c r="C7" s="29"/>
       <c r="D7" s="23" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E7" s="23" t="str">
         <f>D7</f>
@@ -18920,10 +18920,10 @@
       </c>
       <c r="C11" s="29"/>
       <c r="D11" s="23" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="E11" s="23" t="s">
-        <v>623</v>
+        <v>617</v>
       </c>
       <c r="F11" s="35" t="str">
         <f>VLOOKUP(B11,Lexique!A:F,5,)</f>
@@ -18944,7 +18944,7 @@
       </c>
       <c r="C12" s="29"/>
       <c r="D12" s="23" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E12" s="23" t="s">
         <v>172</v>
@@ -18968,10 +18968,10 @@
       </c>
       <c r="C13" s="29"/>
       <c r="D13" s="23" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E13" s="23" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F13" s="35" t="str">
         <f>VLOOKUP(B13,Lexique!A:F,5,)</f>
@@ -18992,10 +18992,10 @@
       </c>
       <c r="C14" s="29"/>
       <c r="D14" s="23" t="s">
+        <v>200</v>
+      </c>
+      <c r="E14" s="23" t="s">
         <v>201</v>
-      </c>
-      <c r="E14" s="23" t="s">
-        <v>202</v>
       </c>
       <c r="F14" s="35" t="str">
         <f>VLOOKUP(B14,Lexique!A:F,5,)</f>
@@ -19064,10 +19064,10 @@
       </c>
       <c r="C17" s="29"/>
       <c r="D17" s="23" t="s">
+        <v>200</v>
+      </c>
+      <c r="E17" s="23" t="s">
         <v>201</v>
-      </c>
-      <c r="E17" s="23" t="s">
-        <v>202</v>
       </c>
       <c r="F17" s="35" t="str">
         <f>VLOOKUP(B17,Lexique!A:F,5,)</f>
@@ -19088,10 +19088,10 @@
       </c>
       <c r="C18" s="29"/>
       <c r="D18" s="23" t="s">
+        <v>182</v>
+      </c>
+      <c r="E18" s="23" t="s">
         <v>183</v>
-      </c>
-      <c r="E18" s="23" t="s">
-        <v>184</v>
       </c>
       <c r="F18" s="35" t="str">
         <f>VLOOKUP(B18,Lexique!A:F,5,)</f>
@@ -19112,7 +19112,7 @@
       </c>
       <c r="C19" s="29"/>
       <c r="D19" s="23" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E19" s="23" t="str">
         <f>D19</f>
@@ -19161,7 +19161,7 @@
       </c>
       <c r="C21" s="29"/>
       <c r="D21" s="23" t="s">
-        <v>176</v>
+        <v>620</v>
       </c>
       <c r="E21" s="23" t="s">
         <v>175</v>
@@ -19233,10 +19233,10 @@
       </c>
       <c r="C24" s="29"/>
       <c r="D24" s="23" t="s">
+        <v>202</v>
+      </c>
+      <c r="E24" s="23" t="s">
         <v>203</v>
-      </c>
-      <c r="E24" s="23" t="s">
-        <v>204</v>
       </c>
       <c r="F24" s="35" t="str">
         <f>VLOOKUP(B24,Lexique!A:F,5,)</f>
@@ -19257,7 +19257,7 @@
       </c>
       <c r="C25" s="29"/>
       <c r="D25" s="23" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E25" s="23" t="str">
         <f>D25</f>
@@ -19282,10 +19282,10 @@
       </c>
       <c r="C26" s="29"/>
       <c r="D26" s="23" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E26" s="23" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="F26" s="35" t="str">
         <f>VLOOKUP(B26,Lexique!A:F,5,)</f>
@@ -19306,10 +19306,10 @@
       </c>
       <c r="C27" s="29"/>
       <c r="D27" s="23" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E27" s="23" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F27" s="35" t="str">
         <f>VLOOKUP(B27,Lexique!A:F,5,)</f>
@@ -19330,10 +19330,10 @@
       </c>
       <c r="C28" s="29"/>
       <c r="D28" s="23" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E28" s="23" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="F28" s="35" t="str">
         <f>VLOOKUP(B28,Lexique!A:F,5,)</f>
@@ -19354,10 +19354,10 @@
       </c>
       <c r="C29" s="29"/>
       <c r="D29" s="23" t="s">
+        <v>196</v>
+      </c>
+      <c r="E29" s="23" t="s">
         <v>197</v>
-      </c>
-      <c r="E29" s="23" t="s">
-        <v>198</v>
       </c>
       <c r="F29" s="35" t="str">
         <f>VLOOKUP(B29,Lexique!A:F,5,)</f>
@@ -19378,10 +19378,10 @@
       </c>
       <c r="C30" s="29"/>
       <c r="D30" s="23" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E30" s="23" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="F30" s="35" t="str">
         <f>VLOOKUP(B30,Lexique!A:F,5,)</f>
@@ -19402,10 +19402,10 @@
       </c>
       <c r="C31" s="29"/>
       <c r="D31" s="23" t="s">
+        <v>188</v>
+      </c>
+      <c r="E31" s="23" t="s">
         <v>189</v>
-      </c>
-      <c r="E31" s="23" t="s">
-        <v>190</v>
       </c>
       <c r="F31" s="35" t="str">
         <f>VLOOKUP(B31,Lexique!A:F,5,)</f>
@@ -19587,7 +19587,7 @@
   <dimension ref="A1:G321"/>
   <sheetViews>
     <sheetView topLeftCell="A11" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
@@ -19610,7 +19610,7 @@
         <v>19</v>
       </c>
       <c r="C1" s="39" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="D1" s="40" t="s">
         <v>17</v>
@@ -19619,10 +19619,10 @@
         <v>18</v>
       </c>
       <c r="F1" s="41" t="s">
+        <v>304</v>
+      </c>
+      <c r="G1" s="41" t="s">
         <v>305</v>
-      </c>
-      <c r="G1" s="41" t="s">
-        <v>306</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="15" x14ac:dyDescent="0.2">
@@ -19633,13 +19633,13 @@
         <v>79</v>
       </c>
       <c r="C2" s="29" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D2" s="23" t="s">
+        <v>381</v>
+      </c>
+      <c r="E2" s="23" t="s">
         <v>382</v>
-      </c>
-      <c r="E2" s="23" t="s">
-        <v>383</v>
       </c>
       <c r="F2" s="35" t="str">
         <f>VLOOKUP(B2,Lexique!A:F,5,)</f>
@@ -19658,10 +19658,10 @@
         <v>73</v>
       </c>
       <c r="C3" s="29" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="D3" s="23" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="E3" s="23" t="str">
         <f>D3</f>
@@ -19684,10 +19684,10 @@
         <v>72</v>
       </c>
       <c r="C4" s="29" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="D4" s="23" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="E4" s="23" t="str">
         <f>D4</f>
@@ -19710,10 +19710,10 @@
         <v>73</v>
       </c>
       <c r="C5" s="29" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="D5" s="23" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="E5" s="23" t="str">
         <f>D5</f>
@@ -19736,10 +19736,10 @@
         <v>72</v>
       </c>
       <c r="C6" s="29" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="D6" s="23" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="E6" s="23" t="str">
         <f>D6</f>
@@ -19762,13 +19762,13 @@
         <v>74</v>
       </c>
       <c r="C7" s="29" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="D7" s="23" t="s">
+        <v>411</v>
+      </c>
+      <c r="E7" s="23" t="s">
         <v>412</v>
-      </c>
-      <c r="E7" s="23" t="s">
-        <v>413</v>
       </c>
       <c r="F7" s="35" t="str">
         <f>VLOOKUP(B7,Lexique!A:F,5,)</f>
@@ -19787,10 +19787,10 @@
         <v>74</v>
       </c>
       <c r="C8" s="29" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="D8" s="23" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="E8" s="23" t="str">
         <f>D8</f>
@@ -19813,13 +19813,13 @@
         <v>72</v>
       </c>
       <c r="C9" s="29" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D9" s="23" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
       <c r="E9" s="23" t="s">
-        <v>451</v>
+        <v>448</v>
       </c>
       <c r="F9" s="35" t="str">
         <f>VLOOKUP(B9,Lexique!A:F,5,)</f>
@@ -19838,10 +19838,10 @@
         <v>73</v>
       </c>
       <c r="C10" s="29" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="D10" s="23" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="E10" s="24" t="str">
         <f>D10</f>
@@ -19864,10 +19864,10 @@
         <v>73</v>
       </c>
       <c r="C11" s="29" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="D11" s="24" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="E11" s="24" t="str">
         <f>D11</f>
@@ -19890,10 +19890,10 @@
         <v>73</v>
       </c>
       <c r="C12" s="29" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="D12" s="23" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="E12" s="25" t="str">
         <f>D12</f>
@@ -19916,10 +19916,10 @@
         <v>72</v>
       </c>
       <c r="C13" s="29" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="D13" s="23" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="E13" s="25" t="str">
         <f t="shared" ref="E13:E17" si="0">D13</f>
@@ -19942,10 +19942,10 @@
         <v>73</v>
       </c>
       <c r="C14" s="29" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="D14" s="25" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="E14" s="25" t="str">
         <f t="shared" si="0"/>
@@ -19968,10 +19968,10 @@
         <v>72</v>
       </c>
       <c r="C15" s="29" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="D15" s="23" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="E15" s="25" t="str">
         <f t="shared" si="0"/>
@@ -19994,10 +19994,10 @@
         <v>73</v>
       </c>
       <c r="C16" s="29" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="D16" s="24" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="E16" s="25" t="str">
         <f t="shared" si="0"/>
@@ -20020,10 +20020,10 @@
         <v>73</v>
       </c>
       <c r="C17" s="29" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="D17" s="43" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E17" s="25" t="str">
         <f t="shared" si="0"/>
@@ -20046,13 +20046,13 @@
         <v>76</v>
       </c>
       <c r="C18" s="29" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="D18" s="23" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
       <c r="E18" s="23" t="s">
-        <v>446</v>
+        <v>443</v>
       </c>
       <c r="F18" s="35" t="str">
         <f>VLOOKUP(B18,Lexique!A:F,5,)</f>
@@ -20072,13 +20072,13 @@
         <v>76</v>
       </c>
       <c r="C19" s="29" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="D19" s="23" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="E19" s="23" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="F19" s="35" t="str">
         <f>VLOOKUP(B19,Lexique!A:F,5,)</f>
@@ -20098,13 +20098,13 @@
         <v>71</v>
       </c>
       <c r="C20" s="29" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="D20" s="25" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="E20" s="25" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="F20" s="35" t="str">
         <f>VLOOKUP(B20,Lexique!A:F,5,)</f>
@@ -20124,13 +20124,13 @@
         <v>76</v>
       </c>
       <c r="C21" s="29" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="D21" s="23" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="E21" s="23" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="F21" s="35" t="str">
         <f>VLOOKUP(B21,Lexique!A:F,5,)</f>
@@ -20150,7 +20150,7 @@
         <v>78</v>
       </c>
       <c r="C22" s="29" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
       <c r="D22" s="23" t="s">
         <v>155</v>
@@ -20176,13 +20176,13 @@
         <v>70</v>
       </c>
       <c r="C23" s="29" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="D23" s="23" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
       <c r="E23" s="23" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="F23" s="35" t="str">
         <f>VLOOKUP(B23,Lexique!A:F,5,)</f>
@@ -20202,13 +20202,13 @@
         <v>76</v>
       </c>
       <c r="C24" s="29" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="D24" s="23" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="E24" s="23" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="F24" s="35" t="str">
         <f>VLOOKUP(B24,Lexique!A:F,5,)</f>
@@ -20228,13 +20228,13 @@
         <v>71</v>
       </c>
       <c r="C25" s="29" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="D25" s="25" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="E25" s="25" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="F25" s="35" t="str">
         <f>VLOOKUP(B25,Lexique!A:F,5,)</f>
@@ -20254,13 +20254,13 @@
         <v>81</v>
       </c>
       <c r="C26" s="29" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="D26" s="23" t="s">
+        <v>622</v>
+      </c>
+      <c r="E26" s="23" t="s">
         <v>437</v>
-      </c>
-      <c r="E26" s="23" t="s">
-        <v>440</v>
       </c>
       <c r="F26" s="35" t="str">
         <f>VLOOKUP(B26,Lexique!A:F,5,)</f>
@@ -20280,13 +20280,13 @@
         <v>76</v>
       </c>
       <c r="C27" s="29" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="D27" s="23" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="E27" s="23" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="F27" s="35" t="str">
         <f>VLOOKUP(B27,Lexique!A:F,5,)</f>
@@ -20306,13 +20306,13 @@
         <v>76</v>
       </c>
       <c r="C28" s="29" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="D28" s="23" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="E28" s="23" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="F28" s="35" t="str">
         <f>VLOOKUP(B28,Lexique!A:F,5,)</f>
@@ -20332,13 +20332,13 @@
         <v>71</v>
       </c>
       <c r="C29" s="29" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="D29" s="25" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="E29" s="25" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="F29" s="35" t="str">
         <f>VLOOKUP(B29,Lexique!A:F,5,)</f>
@@ -20358,13 +20358,13 @@
         <v>70</v>
       </c>
       <c r="C30" s="29" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="D30" s="23" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
       <c r="E30" s="23" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
       <c r="F30" s="35" t="str">
         <f>VLOOKUP(B30,Lexique!A:F,5,)</f>
@@ -20384,13 +20384,13 @@
         <v>81</v>
       </c>
       <c r="C31" s="29" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="D31" s="23" t="s">
-        <v>438</v>
+        <v>623</v>
       </c>
       <c r="E31" s="23" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="F31" s="35" t="str">
         <f>VLOOKUP(B31,Lexique!A:F,5,)</f>
@@ -20410,7 +20410,7 @@
         <v>78</v>
       </c>
       <c r="C32" s="29" t="s">
-        <v>448</v>
+        <v>445</v>
       </c>
       <c r="D32" s="23" t="s">
         <v>154</v>
@@ -20436,13 +20436,13 @@
         <v>80</v>
       </c>
       <c r="C33" s="29" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="D33" s="23" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="E33" s="23" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="F33" s="35" t="str">
         <f>VLOOKUP(B33,Lexique!A:F,5,)</f>
@@ -20463,10 +20463,10 @@
       </c>
       <c r="C34" s="29"/>
       <c r="D34" s="26" t="s">
+        <v>346</v>
+      </c>
+      <c r="E34" s="26" t="s">
         <v>347</v>
-      </c>
-      <c r="E34" s="26" t="s">
-        <v>348</v>
       </c>
       <c r="F34" s="35" t="str">
         <f>VLOOKUP(B34,Lexique!A:F,5,)</f>
@@ -20486,7 +20486,7 @@
         <v>43</v>
       </c>
       <c r="C35" s="29" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="D35" s="26" t="s">
         <v>109</v>

</xml_diff>

<commit_message>
MAJ nb coureurs CLMI
</commit_message>
<xml_diff>
--- a/excel/Itineraires.xlsx
+++ b/excel/Itineraires.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brunogauthier/Documents/guide2024/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{750F8CE9-F36A-CB46-BD8A-F5B3D7B64A3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE4B23B6-7A45-DF4B-86C3-E62E1148C8E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" tabRatio="758" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" tabRatio="758" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="23" r:id="rId1"/>
@@ -3025,7 +3025,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3050,8 +3050,7 @@
         <v>36</v>
       </c>
       <c r="B2">
-        <f>6*16</f>
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="C2" s="17">
         <v>6.9444444444444447E-4</v>
@@ -3105,7 +3104,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BF2EC7B-8CF4-1449-B844-A73E16F738A4}">
   <dimension ref="A1:G322"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView topLeftCell="A20" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="D44" sqref="D44"/>
     </sheetView>
   </sheetViews>
@@ -6577,7 +6576,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF8C653E-9E00-4EDF-9978-201805372337}">
   <dimension ref="A1:AM14"/>
   <sheetViews>
-    <sheetView topLeftCell="AB1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="W1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="AE22" sqref="AE22"/>
     </sheetView>
   </sheetViews>
@@ -7118,11 +7117,11 @@
       </c>
       <c r="AL4" s="15" t="str">
         <f>TEXT(Tableau2[[#This Row],[Depart]]+(Notes!$B$2+10)*Notes!$C$2,"HH:MM")</f>
-        <v>10:46</v>
+        <v>10:38</v>
       </c>
       <c r="AM4" s="15" t="str">
         <f>TEXT(Tableau2[[#This Row],[KM_Total]]/Tableau2[[#This Row],[Vit_moy]]/24+Tableau2[[#This Row],[DerDep]],"HH:MM")</f>
-        <v>10:56</v>
+        <v>10:48</v>
       </c>
     </row>
     <row r="5" spans="1:39" x14ac:dyDescent="0.15">

</xml_diff>